<commit_message>
Make summarizeAcrossScenariosUnion.bat echo easier to understand and update scenario set
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8626437E-27F3-4BB5-9F6A-92AB7B5AE869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0B6FE5-4288-42E7-998D-C550023C5C70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="3900" windowWidth="17235" windowHeight="15375" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
+    <workbookView xWindow="6765" yWindow="3975" windowWidth="17235" windowHeight="15375" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="61">
   <si>
     <t>EEJ</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Proposed Plan</t>
   </si>
   <si>
-    <t>2040_06_694_Amd1</t>
-  </si>
-  <si>
     <t>Big Cities</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>2035_06_697</t>
   </si>
   <si>
-    <t>2035_06_694_Amd1</t>
-  </si>
-  <si>
     <t>2035_06_693</t>
   </si>
   <si>
@@ -204,6 +198,24 @@
   </si>
   <si>
     <t>running</t>
+  </si>
+  <si>
+    <t>2050_TM152_DBP_PlusCrossing_03</t>
+  </si>
+  <si>
+    <t>2035_TM152_DBP_Plus_03</t>
+  </si>
+  <si>
+    <t>2035_TM152_DBP_NoProject_03</t>
+  </si>
+  <si>
+    <t>2050_TM152_DBP_NoProject_03</t>
+  </si>
+  <si>
+    <t>2035_06_694_Amd2</t>
+  </si>
+  <si>
+    <t>2040_06_694_Amd2</t>
   </si>
 </sst>
 </file>
@@ -690,11 +702,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A0CDBDA-1D45-4767-94B1-99049134204D}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -706,144 +718,144 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="8">
         <v>2005</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" s="11">
         <v>2010</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="5">
         <v>2015</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" s="15">
         <v>2020</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B6" s="15">
         <v>2020</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="15">
         <v>2020</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8" s="15">
         <v>2020</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>2</v>
@@ -852,16 +864,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="15">
         <v>2020</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>0</v>
@@ -870,70 +882,70 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="21">
         <v>2035</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F10" s="22"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" s="21">
         <v>2035</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" s="22"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="21">
         <v>2035</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" s="22"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" s="21">
         <v>2035</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E13" s="22" t="s">
         <v>2</v>
@@ -942,16 +954,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" s="21">
         <v>2035</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E14" s="22" t="s">
         <v>0</v>
@@ -960,70 +972,70 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" s="18">
         <v>2040</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" s="19"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" s="18">
         <v>2040</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" s="18">
         <v>2040</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" s="19"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B18" s="18">
         <v>2040</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>2</v>
@@ -1032,7 +1044,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B19" s="24">
         <v>2040</v>
@@ -1041,7 +1053,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>0</v>
@@ -1050,342 +1062,420 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B20" s="27">
         <v>2005</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B21" s="2">
         <v>2015</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="30" t="s">
-        <v>30</v>
-      </c>
       <c r="E22" s="30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F22" s="30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="31" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B23" s="29">
         <v>2035</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" s="30"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="31" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B24" s="29">
         <v>2035</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" s="30"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="31" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B25" s="29">
         <v>2035</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" s="30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="20" t="s">
-        <v>28</v>
+      <c r="A26" s="31" t="s">
+        <v>26</v>
       </c>
       <c r="B26" s="29">
         <v>2035</v>
       </c>
-      <c r="C26" s="30" t="s">
-        <v>35</v>
+      <c r="C26" s="31" t="s">
+        <v>57</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="30"/>
+        <v>7</v>
+      </c>
+      <c r="F26" s="30" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B27" s="29">
         <v>2035</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F27" s="30"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B28" s="29">
         <v>2035</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F28" s="30"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B29" s="29">
         <v>2035</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F29" s="30"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B30" s="29">
         <v>2035</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="F30" s="30" t="s">
-        <v>45</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F30" s="30"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="33">
-        <v>2050</v>
-      </c>
-      <c r="C31" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="D31" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="E31" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="34" t="s">
-        <v>45</v>
+      <c r="A31" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" s="30" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" s="33">
-        <v>2050</v>
-      </c>
-      <c r="C32" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="E32" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="F32" s="34" t="s">
+      <c r="A32" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C32" s="30" t="s">
         <v>56</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" s="30" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B33" s="33">
         <v>2050</v>
       </c>
       <c r="C33" s="34" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E33" s="34" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="F33" s="34"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B34" s="33">
         <v>2050</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E34" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F34" s="34"/>
+        <v>7</v>
+      </c>
+      <c r="F34" s="34" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B35" s="33">
         <v>2050</v>
       </c>
       <c r="C35" s="34" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E35" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" s="34"/>
+        <v>7</v>
+      </c>
+      <c r="F35" s="34" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B36" s="33">
         <v>2050</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D36" s="34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E36" s="34" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F36" s="34"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B37" s="33">
         <v>2050</v>
       </c>
       <c r="C37" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37" s="34"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="33">
+        <v>2050</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F38" s="34"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="33">
+        <v>2050</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F39" s="34"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="33">
+        <v>2050</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40" s="34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="33">
+        <v>2050</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F41" s="34" t="s">
         <v>54</v>
-      </c>
-      <c r="D37" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="E37" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="F37" s="34" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add columns for urbansim directories to ModelRuns.xlsx and .csv
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0B6FE5-4288-42E7-998D-C550023C5C70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C895958-B370-4215-B2C9-AB830CE7FBCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6765" yWindow="3975" windowWidth="17235" windowHeight="15375" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
+    <workbookView xWindow="4530" yWindow="1185" windowWidth="16200" windowHeight="9360" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="70">
   <si>
     <t>EEJ</t>
   </si>
@@ -216,6 +216,33 @@
   </si>
   <si>
     <t>2040_06_694_Amd2</t>
+  </si>
+  <si>
+    <t>urbansim_path</t>
+  </si>
+  <si>
+    <t>urbansim_runid</t>
+  </si>
+  <si>
+    <t>2050_TM152_DBP_PlusCrossing_04</t>
+  </si>
+  <si>
+    <t>run56</t>
+  </si>
+  <si>
+    <t>run977</t>
+  </si>
+  <si>
+    <t>run72</t>
+  </si>
+  <si>
+    <t>"Blueprint Basic (s21)\v1.5.1\v1.5.1.2 (to 2050)"</t>
+  </si>
+  <si>
+    <t>"Blueprint Plus Crossing (s23)\v1.5.2"</t>
+  </si>
+  <si>
+    <t>"Blueprint Basic (s21)\v1.5.1\v1.5.1.1 (only to 2035)"</t>
   </si>
 </sst>
 </file>
@@ -322,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -382,6 +409,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,21 +732,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A0CDBDA-1D45-4767-94B1-99049134204D}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="29.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="5" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="15" style="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -733,10 +764,16 @@
         <v>22</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
@@ -753,8 +790,10 @@
         <v>18</v>
       </c>
       <c r="F2" s="9"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="8"/>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
@@ -771,8 +810,10 @@
         <v>18</v>
       </c>
       <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="11"/>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>25</v>
       </c>
@@ -789,8 +830,10 @@
         <v>18</v>
       </c>
       <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>25</v>
       </c>
@@ -807,8 +850,10 @@
         <v>7</v>
       </c>
       <c r="F5" s="16"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="15"/>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>25</v>
       </c>
@@ -825,8 +870,10 @@
         <v>5</v>
       </c>
       <c r="F6" s="16"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="15"/>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>25</v>
       </c>
@@ -843,8 +890,10 @@
         <v>3</v>
       </c>
       <c r="F7" s="16"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>25</v>
       </c>
@@ -861,8 +910,10 @@
         <v>2</v>
       </c>
       <c r="F8" s="16"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="15"/>
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>25</v>
       </c>
@@ -879,8 +930,10 @@
         <v>0</v>
       </c>
       <c r="F9" s="16"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="15"/>
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>25</v>
       </c>
@@ -897,8 +950,10 @@
         <v>7</v>
       </c>
       <c r="F10" s="22"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="21"/>
+      <c r="H10" s="22"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>25</v>
       </c>
@@ -915,8 +970,10 @@
         <v>5</v>
       </c>
       <c r="F11" s="22"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="21"/>
+      <c r="H11" s="22"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>25</v>
       </c>
@@ -933,8 +990,10 @@
         <v>3</v>
       </c>
       <c r="F12" s="22"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="21"/>
+      <c r="H12" s="22"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>25</v>
       </c>
@@ -951,8 +1010,10 @@
         <v>2</v>
       </c>
       <c r="F13" s="22"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="21"/>
+      <c r="H13" s="22"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>25</v>
       </c>
@@ -969,8 +1030,10 @@
         <v>0</v>
       </c>
       <c r="F14" s="22"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="21"/>
+      <c r="H14" s="22"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>25</v>
       </c>
@@ -987,8 +1050,10 @@
         <v>7</v>
       </c>
       <c r="F15" s="19"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="18"/>
+      <c r="H15" s="19"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>25</v>
       </c>
@@ -1005,8 +1070,10 @@
         <v>5</v>
       </c>
       <c r="F16" s="19"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="18"/>
+      <c r="H16" s="19"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>25</v>
       </c>
@@ -1023,8 +1090,10 @@
         <v>3</v>
       </c>
       <c r="F17" s="19"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="18"/>
+      <c r="H17" s="19"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>25</v>
       </c>
@@ -1041,8 +1110,10 @@
         <v>2</v>
       </c>
       <c r="F18" s="19"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="18"/>
+      <c r="H18" s="19"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>25</v>
       </c>
@@ -1059,8 +1130,10 @@
         <v>0</v>
       </c>
       <c r="F19" s="25"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="24"/>
+      <c r="H19" s="25"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
         <v>26</v>
       </c>
@@ -1076,11 +1149,13 @@
       <c r="E20" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="F20" s="28"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
         <v>26</v>
       </c>
@@ -1096,11 +1171,13 @@
       <c r="E21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="1"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
         <v>26</v>
       </c>
@@ -1116,11 +1193,13 @@
       <c r="E22" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="30" t="s">
+      <c r="F22" s="30"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="31" t="s">
         <v>26</v>
       </c>
@@ -1137,8 +1216,10 @@
         <v>7</v>
       </c>
       <c r="F23" s="30"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" s="29"/>
+      <c r="H23" s="30"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="31" t="s">
         <v>26</v>
       </c>
@@ -1155,8 +1236,10 @@
         <v>7</v>
       </c>
       <c r="F24" s="30"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" s="29"/>
+      <c r="H24" s="30"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="31" t="s">
         <v>26</v>
       </c>
@@ -1172,11 +1255,13 @@
       <c r="E25" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="30" t="s">
+      <c r="F25" s="30"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="31" t="s">
         <v>26</v>
       </c>
@@ -1192,11 +1277,13 @@
       <c r="E26" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="30" t="s">
+      <c r="F26" s="30"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="30" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
         <v>26</v>
       </c>
@@ -1213,8 +1300,10 @@
         <v>35</v>
       </c>
       <c r="F27" s="30"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" s="29"/>
+      <c r="H27" s="30"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
         <v>26</v>
       </c>
@@ -1231,8 +1320,10 @@
         <v>35</v>
       </c>
       <c r="F28" s="30"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" s="29"/>
+      <c r="H28" s="30"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
         <v>26</v>
       </c>
@@ -1249,8 +1340,10 @@
         <v>38</v>
       </c>
       <c r="F29" s="30"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" s="29"/>
+      <c r="H29" s="30"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
         <v>26</v>
       </c>
@@ -1267,8 +1360,10 @@
         <v>38</v>
       </c>
       <c r="F30" s="30"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" s="29"/>
+      <c r="H30" s="30"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
         <v>26</v>
       </c>
@@ -1285,10 +1380,16 @@
         <v>38</v>
       </c>
       <c r="F31" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="H31" s="30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
         <v>26</v>
       </c>
@@ -1305,10 +1406,16 @@
         <v>38</v>
       </c>
       <c r="F32" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="G32" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="H32" s="30" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="32" t="s">
         <v>26</v>
       </c>
@@ -1325,8 +1432,10 @@
         <v>7</v>
       </c>
       <c r="F33" s="34"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" s="33"/>
+      <c r="H33" s="34"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
         <v>26</v>
       </c>
@@ -1342,11 +1451,13 @@
       <c r="E34" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="34" t="s">
+      <c r="F34" s="34"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
         <v>26</v>
       </c>
@@ -1362,11 +1473,13 @@
       <c r="E35" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="34" t="s">
+      <c r="F35" s="34"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="34" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
         <v>26</v>
       </c>
@@ -1383,8 +1496,10 @@
         <v>35</v>
       </c>
       <c r="F36" s="34"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36" s="33"/>
+      <c r="H36" s="34"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="32" t="s">
         <v>26</v>
       </c>
@@ -1401,8 +1516,10 @@
         <v>35</v>
       </c>
       <c r="F37" s="34"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37" s="33"/>
+      <c r="H37" s="34"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="32" t="s">
         <v>26</v>
       </c>
@@ -1419,8 +1536,10 @@
         <v>38</v>
       </c>
       <c r="F38" s="34"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38" s="33"/>
+      <c r="H38" s="34"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
         <v>26</v>
       </c>
@@ -1437,8 +1556,10 @@
         <v>38</v>
       </c>
       <c r="F39" s="34"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39" s="33"/>
+      <c r="H39" s="34"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="32" t="s">
         <v>26</v>
       </c>
@@ -1455,10 +1576,16 @@
         <v>38</v>
       </c>
       <c r="F40" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="G40" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="H40" s="34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="32" t="s">
         <v>26</v>
       </c>
@@ -1475,11 +1602,44 @@
         <v>38</v>
       </c>
       <c r="F41" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="G41" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="H41" s="34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="33">
+        <v>2050</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F42" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="G42" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="H42" s="34" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update a couple runs as complete (current)
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C895958-B370-4215-B2C9-AB830CE7FBCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13E4BE8-7001-4133-A0A6-EE8E9A3321F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4530" yWindow="1185" windowWidth="16200" windowHeight="9360" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
+    <workbookView xWindow="7725" yWindow="4905" windowWidth="28800" windowHeight="15435" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -736,7 +736,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1453,9 +1453,7 @@
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="33"/>
-      <c r="H34" s="34" t="s">
-        <v>43</v>
-      </c>
+      <c r="H34" s="34"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
@@ -1473,10 +1471,14 @@
       <c r="E35" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="34"/>
-      <c r="G35" s="33"/>
+      <c r="F35" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="G35" s="33" t="s">
+        <v>66</v>
+      </c>
       <c r="H35" s="34" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1581,9 +1583,7 @@
       <c r="G40" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="H40" s="34" t="s">
-        <v>43</v>
-      </c>
+      <c r="H40" s="34"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="32" t="s">
@@ -1608,7 +1608,7 @@
         <v>64</v>
       </c>
       <c r="H41" s="34" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixing - 2050 NoProject 03 isn't done
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13E4BE8-7001-4133-A0A6-EE8E9A3321F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3C940F-FBDA-43BB-A5BD-01EDF951AA76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7725" yWindow="4905" windowWidth="28800" windowHeight="15435" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="70">
   <si>
     <t>EEJ</t>
   </si>
@@ -736,7 +736,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G43" sqref="G43"/>
+      <selection pane="bottomLeft" activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1453,7 +1453,9 @@
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="33"/>
-      <c r="H34" s="34"/>
+      <c r="H34" s="34" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
@@ -1478,7 +1480,7 @@
         <v>66</v>
       </c>
       <c r="H35" s="34" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updating since 2035_TM152_DBP_Plus_03 is complete
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3C940F-FBDA-43BB-A5BD-01EDF951AA76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4EC8D3-6132-4463-907B-A218867413AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7725" yWindow="4905" windowWidth="28800" windowHeight="15435" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="70">
   <si>
     <t>EEJ</t>
   </si>
@@ -736,7 +736,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H35" sqref="H35"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1385,9 +1385,7 @@
       <c r="G31" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="H31" s="30" t="s">
-        <v>43</v>
-      </c>
+      <c r="H31" s="30"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
@@ -1412,7 +1410,7 @@
         <v>66</v>
       </c>
       <c r="H32" s="30" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
2050_TM152_DBP_NoProject_04 is complete and now current 2050 noproject
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535EAE67-C3B6-4ED3-9E21-95EEC34AA27C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCC81E4-182C-48D8-BFFD-51515FD399D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7725" yWindow="4905" windowWidth="28800" windowHeight="15435" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="71">
   <si>
     <t>EEJ</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>"Blueprint Basic (s21)\v1.5.1\v1.5.1.1 (only to 2035)"</t>
+  </si>
+  <si>
+    <t>2050_TM152_DBP_NoProject_04</t>
   </si>
 </sst>
 </file>
@@ -732,11 +735,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A0CDBDA-1D45-4767-94B1-99049134204D}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
+      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1451,9 +1454,7 @@
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="33"/>
-      <c r="H34" s="34" t="s">
-        <v>43</v>
-      </c>
+      <c r="H34" s="34"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
@@ -1477,9 +1478,7 @@
       <c r="G35" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="H35" s="34" t="s">
-        <v>54</v>
-      </c>
+      <c r="H35" s="34"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
@@ -1489,17 +1488,23 @@
         <v>2050</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="D36" s="34" t="s">
         <v>34</v>
       </c>
       <c r="E36" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F36" s="34"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="34"/>
+        <v>7</v>
+      </c>
+      <c r="F36" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="G36" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="H36" s="34" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="32" t="s">
@@ -1509,7 +1514,7 @@
         <v>2050</v>
       </c>
       <c r="C37" s="34" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D37" s="34" t="s">
         <v>34</v>
@@ -1529,13 +1534,13 @@
         <v>2050</v>
       </c>
       <c r="C38" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D38" s="34" t="s">
         <v>34</v>
       </c>
       <c r="E38" s="34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F38" s="34"/>
       <c r="G38" s="33"/>
@@ -1549,7 +1554,7 @@
         <v>2050</v>
       </c>
       <c r="C39" s="34" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D39" s="34" t="s">
         <v>34</v>
@@ -1569,7 +1574,7 @@
         <v>2050</v>
       </c>
       <c r="C40" s="34" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D40" s="34" t="s">
         <v>34</v>
@@ -1577,12 +1582,8 @@
       <c r="E40" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="F40" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="G40" s="33" t="s">
-        <v>64</v>
-      </c>
+      <c r="F40" s="34"/>
+      <c r="G40" s="33"/>
       <c r="H40" s="34"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1593,7 +1594,7 @@
         <v>2050</v>
       </c>
       <c r="C41" s="34" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D41" s="34" t="s">
         <v>34</v>
@@ -1617,7 +1618,7 @@
         <v>2050</v>
       </c>
       <c r="C42" s="34" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D42" s="34" t="s">
         <v>34</v>
@@ -1626,12 +1627,36 @@
         <v>38</v>
       </c>
       <c r="F42" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="G42" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="H42" s="34"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" s="33">
+        <v>2050</v>
+      </c>
+      <c r="C43" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="G42" s="33" t="s">
+      <c r="G43" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="H42" s="34" t="s">
+      <c r="H43" s="34" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add newest runs (2035_TM152_DBP_Plus_04, 2050_TM152_DBP_PlusCrossing_05)
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCC81E4-182C-48D8-BFFD-51515FD399D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACCB430-1A4C-4D91-90D5-2BD960EB2988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7725" yWindow="4905" windowWidth="28800" windowHeight="15435" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
+    <workbookView xWindow="10410" yWindow="5295" windowWidth="28800" windowHeight="15435" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="75">
   <si>
     <t>EEJ</t>
   </si>
@@ -246,6 +246,18 @@
   </si>
   <si>
     <t>2050_TM152_DBP_NoProject_04</t>
+  </si>
+  <si>
+    <t>2050_TM152_DBP_PlusCrossing_05</t>
+  </si>
+  <si>
+    <t>"Blueprint Plus Crossing (s23)\v1.5.5"</t>
+  </si>
+  <si>
+    <t>run998</t>
+  </si>
+  <si>
+    <t>2035_TM152_DBP_Plus_04</t>
   </si>
 </sst>
 </file>
@@ -735,18 +747,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A0CDBDA-1D45-4767-94B1-99049134204D}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="29.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="6" width="15" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="40.28515625" customWidth="1"/>
     <col min="7" max="7" width="15" style="35" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1412,29 +1425,33 @@
       <c r="G32" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="H32" s="30" t="s">
+      <c r="H32" s="30"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C33" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="G33" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="H33" s="30" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="33">
-        <v>2050</v>
-      </c>
-      <c r="C33" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="D33" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33" s="34"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="34"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
@@ -1444,7 +1461,7 @@
         <v>2050</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D34" s="34" t="s">
         <v>34</v>
@@ -1464,7 +1481,7 @@
         <v>2050</v>
       </c>
       <c r="C35" s="34" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D35" s="34" t="s">
         <v>34</v>
@@ -1472,12 +1489,8 @@
       <c r="E35" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="G35" s="33" t="s">
-        <v>66</v>
-      </c>
+      <c r="F35" s="34"/>
+      <c r="G35" s="33"/>
       <c r="H35" s="34"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1488,7 +1501,7 @@
         <v>2050</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D36" s="34" t="s">
         <v>34</v>
@@ -1502,9 +1515,7 @@
       <c r="G36" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="H36" s="34" t="s">
-        <v>43</v>
-      </c>
+      <c r="H36" s="34"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="32" t="s">
@@ -1514,17 +1525,23 @@
         <v>2050</v>
       </c>
       <c r="C37" s="34" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="D37" s="34" t="s">
         <v>34</v>
       </c>
       <c r="E37" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F37" s="34"/>
-      <c r="G37" s="33"/>
-      <c r="H37" s="34"/>
+        <v>7</v>
+      </c>
+      <c r="F37" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="G37" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="H37" s="34" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="32" t="s">
@@ -1534,7 +1551,7 @@
         <v>2050</v>
       </c>
       <c r="C38" s="34" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D38" s="34" t="s">
         <v>34</v>
@@ -1554,13 +1571,13 @@
         <v>2050</v>
       </c>
       <c r="C39" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D39" s="34" t="s">
         <v>34</v>
       </c>
       <c r="E39" s="34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F39" s="34"/>
       <c r="G39" s="33"/>
@@ -1574,7 +1591,7 @@
         <v>2050</v>
       </c>
       <c r="C40" s="34" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D40" s="34" t="s">
         <v>34</v>
@@ -1594,7 +1611,7 @@
         <v>2050</v>
       </c>
       <c r="C41" s="34" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D41" s="34" t="s">
         <v>34</v>
@@ -1602,12 +1619,8 @@
       <c r="E41" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="F41" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="G41" s="33" t="s">
-        <v>64</v>
-      </c>
+      <c r="F41" s="34"/>
+      <c r="G41" s="33"/>
       <c r="H41" s="34"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1618,7 +1631,7 @@
         <v>2050</v>
       </c>
       <c r="C42" s="34" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D42" s="34" t="s">
         <v>34</v>
@@ -1642,7 +1655,7 @@
         <v>2050</v>
       </c>
       <c r="C43" s="34" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D43" s="34" t="s">
         <v>34</v>
@@ -1651,12 +1664,60 @@
         <v>38</v>
       </c>
       <c r="F43" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="G43" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="H43" s="34"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="33">
+        <v>2050</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E44" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="G43" s="33" t="s">
+      <c r="G44" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="H43" s="34" t="s">
+      <c r="H44" s="34"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="33">
+        <v>2050</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E45" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F45" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="G45" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="H45" s="34" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added _06 and _07 series of model runs
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACCB430-1A4C-4D91-90D5-2BD960EB2988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802EBD40-B634-4FCA-B189-BD18B95167F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10410" yWindow="5295" windowWidth="28800" windowHeight="15435" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
+    <workbookView xWindow="10590" yWindow="5565" windowWidth="20730" windowHeight="12690" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="88">
   <si>
     <t>EEJ</t>
   </si>
@@ -197,9 +197,6 @@
     <t>2050_TM152_DBP_NoProject_01</t>
   </si>
   <si>
-    <t>running</t>
-  </si>
-  <si>
     <t>2050_TM152_DBP_PlusCrossing_03</t>
   </si>
   <si>
@@ -258,6 +255,48 @@
   </si>
   <si>
     <t>2035_TM152_DBP_Plus_04</t>
+  </si>
+  <si>
+    <t>2035_TM152_DBP_Plus_06</t>
+  </si>
+  <si>
+    <t>2035_TM152_DBP_Plus_07</t>
+  </si>
+  <si>
+    <t>"Blueprint Plus Crossing (s23)\v1.6 (all strategies)"</t>
+  </si>
+  <si>
+    <t>run90</t>
+  </si>
+  <si>
+    <t>"Blueprint Plus Crossing (s23)\v1.7 (strategies + BASIS-hybrid)"</t>
+  </si>
+  <si>
+    <t>run92</t>
+  </si>
+  <si>
+    <t>2035_TM152_DBP_NoProject_06</t>
+  </si>
+  <si>
+    <t>2035_TM152_DBP_NoProject_07</t>
+  </si>
+  <si>
+    <t>2035_TM152_DBP_NoProject_04</t>
+  </si>
+  <si>
+    <t>2050_TM152_DBP_NoProject_06</t>
+  </si>
+  <si>
+    <t>2050_TM152_DBP_NoProject_07</t>
+  </si>
+  <si>
+    <t>RTP2022</t>
+  </si>
+  <si>
+    <t>2050_TM152_DBP_PlusCrossing_06</t>
+  </si>
+  <si>
+    <t>2050_TM152_DBP_PlusCrossing_07</t>
   </si>
 </sst>
 </file>
@@ -747,11 +786,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A0CDBDA-1D45-4767-94B1-99049134204D}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -780,10 +819,10 @@
         <v>22</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>42</v>
@@ -1017,7 +1056,7 @@
         <v>2035</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>29</v>
@@ -1117,7 +1156,7 @@
         <v>2040</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>29</v>
@@ -1273,9 +1312,7 @@
       </c>
       <c r="F25" s="30"/>
       <c r="G25" s="29"/>
-      <c r="H25" s="30" t="s">
-        <v>43</v>
-      </c>
+      <c r="H25" s="30"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="31" t="s">
@@ -1285,7 +1322,7 @@
         <v>2035</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D26" s="30" t="s">
         <v>34</v>
@@ -1295,68 +1332,80 @@
       </c>
       <c r="F26" s="30"/>
       <c r="G26" s="29"/>
-      <c r="H26" s="30" t="s">
-        <v>54</v>
-      </c>
+      <c r="H26" s="30"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="31" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="29">
         <v>2035</v>
       </c>
-      <c r="C27" s="30" t="s">
-        <v>33</v>
+      <c r="C27" s="31" t="s">
+        <v>82</v>
       </c>
       <c r="D27" s="30" t="s">
         <v>34</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="30"/>
-      <c r="G27" s="29"/>
+        <v>7</v>
+      </c>
+      <c r="F27" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" s="29" t="s">
+        <v>72</v>
+      </c>
       <c r="H27" s="30"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="31" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="29">
         <v>2035</v>
       </c>
-      <c r="C28" s="30" t="s">
-        <v>46</v>
+      <c r="C28" s="31" t="s">
+        <v>80</v>
       </c>
       <c r="D28" s="30" t="s">
         <v>34</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="F28" s="30"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="30"/>
+        <v>7</v>
+      </c>
+      <c r="F28" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="G28" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="H28" s="30" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="31" t="s">
         <v>26</v>
       </c>
       <c r="B29" s="29">
         <v>2035</v>
       </c>
-      <c r="C29" s="30" t="s">
-        <v>47</v>
+      <c r="C29" s="31" t="s">
+        <v>81</v>
       </c>
       <c r="D29" s="30" t="s">
         <v>34</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="F29" s="30"/>
-      <c r="G29" s="29"/>
+        <v>7</v>
+      </c>
+      <c r="F29" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="G29" s="29" t="s">
+        <v>79</v>
+      </c>
       <c r="H29" s="30"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1367,13 +1416,13 @@
         <v>2035</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D30" s="30" t="s">
         <v>34</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F30" s="30"/>
       <c r="G30" s="29"/>
@@ -1387,20 +1436,16 @@
         <v>2035</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D31" s="30" t="s">
         <v>34</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="F31" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="G31" s="29" t="s">
-        <v>65</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F31" s="30"/>
+      <c r="G31" s="29"/>
       <c r="H31" s="30"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1411,7 +1456,7 @@
         <v>2035</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D32" s="30" t="s">
         <v>34</v>
@@ -1419,12 +1464,8 @@
       <c r="E32" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F32" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="G32" s="29" t="s">
-        <v>66</v>
-      </c>
+      <c r="F32" s="30"/>
+      <c r="G32" s="29"/>
       <c r="H32" s="30"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1435,7 +1476,7 @@
         <v>2035</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="D33" s="30" t="s">
         <v>34</v>
@@ -1443,125 +1484,131 @@
       <c r="E33" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F33" s="30" t="s">
+      <c r="F33" s="30"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="30"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F34" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="G34" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="H34" s="30"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="H35" s="30"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C36" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="G36" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="G33" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="H33" s="30" t="s">
+      <c r="H36" s="30"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F37" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="G37" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="H37" s="30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="33">
-        <v>2050</v>
-      </c>
-      <c r="C34" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="D34" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" s="34"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="34"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="33">
-        <v>2050</v>
-      </c>
-      <c r="C35" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35" s="34"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="34"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="33">
-        <v>2050</v>
-      </c>
-      <c r="C36" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="D36" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="G36" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="H36" s="34"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="33">
-        <v>2050</v>
-      </c>
-      <c r="C37" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="D37" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E37" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="G37" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="H37" s="34" t="s">
-        <v>43</v>
-      </c>
-    </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="33">
-        <v>2050</v>
-      </c>
-      <c r="C38" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D38" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F38" s="34"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="34"/>
+      <c r="A38" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F38" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="G38" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="H38" s="30"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
@@ -1571,13 +1618,13 @@
         <v>2050</v>
       </c>
       <c r="C39" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D39" s="34" t="s">
         <v>34</v>
       </c>
       <c r="E39" s="34" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="F39" s="34"/>
       <c r="G39" s="33"/>
@@ -1591,13 +1638,13 @@
         <v>2050</v>
       </c>
       <c r="C40" s="34" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D40" s="34" t="s">
         <v>34</v>
       </c>
       <c r="E40" s="34" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="F40" s="34"/>
       <c r="G40" s="33"/>
@@ -1611,16 +1658,20 @@
         <v>2050</v>
       </c>
       <c r="C41" s="34" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="D41" s="34" t="s">
         <v>34</v>
       </c>
       <c r="E41" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F41" s="34"/>
-      <c r="G41" s="33"/>
+        <v>7</v>
+      </c>
+      <c r="F41" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="G41" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="H41" s="34"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1631,19 +1682,19 @@
         <v>2050</v>
       </c>
       <c r="C42" s="34" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="D42" s="34" t="s">
         <v>34</v>
       </c>
       <c r="E42" s="34" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="F42" s="34" t="s">
         <v>67</v>
       </c>
       <c r="G42" s="33" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H42" s="34"/>
     </row>
@@ -1655,21 +1706,23 @@
         <v>2050</v>
       </c>
       <c r="C43" s="34" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="D43" s="34" t="s">
         <v>34</v>
       </c>
       <c r="E43" s="34" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="F43" s="34" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="G43" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="H43" s="34"/>
+        <v>77</v>
+      </c>
+      <c r="H43" s="34" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="32" t="s">
@@ -1679,19 +1732,19 @@
         <v>2050</v>
       </c>
       <c r="C44" s="34" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="D44" s="34" t="s">
         <v>34</v>
       </c>
       <c r="E44" s="34" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="F44" s="34" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="G44" s="33" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="H44" s="34"/>
     </row>
@@ -1703,23 +1756,223 @@
         <v>2050</v>
       </c>
       <c r="C45" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D45" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E45" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F45" s="34"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="34"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="33">
+        <v>2050</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E46" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F46" s="34"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="34"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="33">
+        <v>2050</v>
+      </c>
+      <c r="C47" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E47" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F47" s="34"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="34"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="33">
+        <v>2050</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D48" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E48" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F48" s="34"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="34"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="33">
+        <v>2050</v>
+      </c>
+      <c r="C49" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F49" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="G49" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="H49" s="34"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="33">
+        <v>2050</v>
+      </c>
+      <c r="C50" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F50" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="G50" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="H50" s="34"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="33">
+        <v>2050</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D51" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F51" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="G51" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="H51" s="34"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="33">
+        <v>2050</v>
+      </c>
+      <c r="C52" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F52" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="D45" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E45" s="34" t="s">
+      <c r="G52" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="H52" s="34"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="33">
+        <v>2050</v>
+      </c>
+      <c r="C53" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D53" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E53" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="F45" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="G45" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="H45" s="34" t="s">
+      <c r="F53" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="G53" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="H53" s="34" t="s">
         <v>43</v>
       </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" s="33">
+        <v>2051</v>
+      </c>
+      <c r="C54" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D54" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E54" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F54" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="G54" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="H54" s="34"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Fix typo and removed 2035_TM152_DBP_NoProject_04
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802EBD40-B634-4FCA-B189-BD18B95167F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5925DC8D-05EE-49A9-A745-E89A6E962541}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10590" yWindow="5565" windowWidth="20730" windowHeight="12690" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
+    <workbookView xWindow="10875" yWindow="6180" windowWidth="20730" windowHeight="12690" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="86">
   <si>
     <t>EEJ</t>
   </si>
@@ -281,16 +281,10 @@
     <t>2035_TM152_DBP_NoProject_07</t>
   </si>
   <si>
-    <t>2035_TM152_DBP_NoProject_04</t>
-  </si>
-  <si>
     <t>2050_TM152_DBP_NoProject_06</t>
   </si>
   <si>
     <t>2050_TM152_DBP_NoProject_07</t>
-  </si>
-  <si>
-    <t>RTP2022</t>
   </si>
   <si>
     <t>2050_TM152_DBP_PlusCrossing_06</t>
@@ -786,11 +780,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A0CDBDA-1D45-4767-94B1-99049134204D}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H55" sqref="H55"/>
+      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1342,7 +1336,7 @@
         <v>2035</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D27" s="30" t="s">
         <v>34</v>
@@ -1351,12 +1345,14 @@
         <v>7</v>
       </c>
       <c r="F27" s="30" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="G27" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="H27" s="30"/>
+        <v>77</v>
+      </c>
+      <c r="H27" s="30" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="31" t="s">
@@ -1366,7 +1362,7 @@
         <v>2035</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D28" s="30" t="s">
         <v>34</v>
@@ -1375,37 +1371,31 @@
         <v>7</v>
       </c>
       <c r="F28" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G28" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="H28" s="30" t="s">
-        <v>43</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="H28" s="30"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="20" t="s">
         <v>26</v>
       </c>
       <c r="B29" s="29">
         <v>2035</v>
       </c>
-      <c r="C29" s="31" t="s">
-        <v>81</v>
+      <c r="C29" s="30" t="s">
+        <v>33</v>
       </c>
       <c r="D29" s="30" t="s">
         <v>34</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="G29" s="29" t="s">
-        <v>79</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F29" s="30"/>
+      <c r="G29" s="29"/>
       <c r="H29" s="30"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1416,7 +1406,7 @@
         <v>2035</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D30" s="30" t="s">
         <v>34</v>
@@ -1436,13 +1426,13 @@
         <v>2035</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D31" s="30" t="s">
         <v>34</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F31" s="30"/>
       <c r="G31" s="29"/>
@@ -1456,7 +1446,7 @@
         <v>2035</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D32" s="30" t="s">
         <v>34</v>
@@ -1476,7 +1466,7 @@
         <v>2035</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D33" s="30" t="s">
         <v>34</v>
@@ -1484,8 +1474,12 @@
       <c r="E33" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F33" s="30"/>
-      <c r="G33" s="29"/>
+      <c r="F33" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="G33" s="29" t="s">
+        <v>64</v>
+      </c>
       <c r="H33" s="30"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1496,7 +1490,7 @@
         <v>2035</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D34" s="30" t="s">
         <v>34</v>
@@ -1505,10 +1499,10 @@
         <v>38</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G34" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H34" s="30"/>
     </row>
@@ -1520,7 +1514,7 @@
         <v>2035</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="D35" s="30" t="s">
         <v>34</v>
@@ -1529,10 +1523,10 @@
         <v>38</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="G35" s="29" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="H35" s="30"/>
     </row>
@@ -1544,7 +1538,7 @@
         <v>2035</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D36" s="30" t="s">
         <v>34</v>
@@ -1553,12 +1547,14 @@
         <v>38</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="G36" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="H36" s="30"/>
+        <v>77</v>
+      </c>
+      <c r="H36" s="30" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
@@ -1568,7 +1564,7 @@
         <v>2035</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D37" s="30" t="s">
         <v>34</v>
@@ -1577,38 +1573,32 @@
         <v>38</v>
       </c>
       <c r="F37" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G37" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="H37" s="30" t="s">
-        <v>43</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="H37" s="30"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C38" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="D38" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="F38" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="G38" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="H38" s="30"/>
+      <c r="A38" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="33">
+        <v>2050</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="34"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="34"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
@@ -1618,7 +1608,7 @@
         <v>2050</v>
       </c>
       <c r="C39" s="34" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D39" s="34" t="s">
         <v>34</v>
@@ -1638,7 +1628,7 @@
         <v>2050</v>
       </c>
       <c r="C40" s="34" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D40" s="34" t="s">
         <v>34</v>
@@ -1646,8 +1636,12 @@
       <c r="E40" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="F40" s="34"/>
-      <c r="G40" s="33"/>
+      <c r="F40" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="G40" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="H40" s="34"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1658,7 +1652,7 @@
         <v>2050</v>
       </c>
       <c r="C41" s="34" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="D41" s="34" t="s">
         <v>34</v>
@@ -1682,7 +1676,7 @@
         <v>2050</v>
       </c>
       <c r="C42" s="34" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="D42" s="34" t="s">
         <v>34</v>
@@ -1691,12 +1685,14 @@
         <v>7</v>
       </c>
       <c r="F42" s="34" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="G42" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="H42" s="34"/>
+        <v>77</v>
+      </c>
+      <c r="H42" s="34" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="32" t="s">
@@ -1715,14 +1711,12 @@
         <v>7</v>
       </c>
       <c r="F43" s="34" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G43" s="33" t="s">
-        <v>77</v>
-      </c>
-      <c r="H43" s="34" t="s">
-        <v>43</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="H43" s="34"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="32" t="s">
@@ -1732,20 +1726,16 @@
         <v>2050</v>
       </c>
       <c r="C44" s="34" t="s">
-        <v>84</v>
+        <v>36</v>
       </c>
       <c r="D44" s="34" t="s">
         <v>34</v>
       </c>
       <c r="E44" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="G44" s="33" t="s">
-        <v>79</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F44" s="34"/>
+      <c r="G44" s="33"/>
       <c r="H44" s="34"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -1756,7 +1746,7 @@
         <v>2050</v>
       </c>
       <c r="C45" s="34" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D45" s="34" t="s">
         <v>34</v>
@@ -1776,13 +1766,13 @@
         <v>2050</v>
       </c>
       <c r="C46" s="34" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D46" s="34" t="s">
         <v>34</v>
       </c>
       <c r="E46" s="34" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F46" s="34"/>
       <c r="G46" s="33"/>
@@ -1796,7 +1786,7 @@
         <v>2050</v>
       </c>
       <c r="C47" s="34" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D47" s="34" t="s">
         <v>34</v>
@@ -1816,7 +1806,7 @@
         <v>2050</v>
       </c>
       <c r="C48" s="34" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="D48" s="34" t="s">
         <v>34</v>
@@ -1824,8 +1814,12 @@
       <c r="E48" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="F48" s="34"/>
-      <c r="G48" s="33"/>
+      <c r="F48" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="G48" s="33" t="s">
+        <v>63</v>
+      </c>
       <c r="H48" s="34"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -1836,7 +1830,7 @@
         <v>2050</v>
       </c>
       <c r="C49" s="34" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D49" s="34" t="s">
         <v>34</v>
@@ -1860,7 +1854,7 @@
         <v>2050</v>
       </c>
       <c r="C50" s="34" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D50" s="34" t="s">
         <v>34</v>
@@ -1869,10 +1863,10 @@
         <v>38</v>
       </c>
       <c r="F50" s="34" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G50" s="33" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H50" s="34"/>
     </row>
@@ -1884,7 +1878,7 @@
         <v>2050</v>
       </c>
       <c r="C51" s="34" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D51" s="34" t="s">
         <v>34</v>
@@ -1893,10 +1887,10 @@
         <v>38</v>
       </c>
       <c r="F51" s="34" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="G51" s="33" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="H51" s="34"/>
     </row>
@@ -1908,7 +1902,7 @@
         <v>2050</v>
       </c>
       <c r="C52" s="34" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="D52" s="34" t="s">
         <v>34</v>
@@ -1917,22 +1911,24 @@
         <v>38</v>
       </c>
       <c r="F52" s="34" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="G52" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="H52" s="34"/>
+        <v>77</v>
+      </c>
+      <c r="H52" s="34" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="32" t="s">
         <v>26</v>
       </c>
       <c r="B53" s="33">
-        <v>2050</v>
+        <v>2051</v>
       </c>
       <c r="C53" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D53" s="34" t="s">
         <v>34</v>
@@ -1941,38 +1937,12 @@
         <v>38</v>
       </c>
       <c r="F53" s="34" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G53" s="33" t="s">
-        <v>77</v>
-      </c>
-      <c r="H53" s="34" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="B54" s="33">
-        <v>2051</v>
-      </c>
-      <c r="C54" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="D54" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E54" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F54" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="G54" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="H54" s="34"/>
+      <c r="H53" s="34"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Fix one more fill down typo
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5925DC8D-05EE-49A9-A745-E89A6E962541}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC69E25-164D-41DF-ADAC-F68D1DF1530F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10875" yWindow="6180" windowWidth="20730" windowHeight="12690" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
   </bookViews>
@@ -784,7 +784,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
+      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1925,7 +1925,7 @@
         <v>26</v>
       </c>
       <c r="B53" s="33">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="C53" s="34" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
Updated for completed 08 series runs (3 out of 4)
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC69E25-164D-41DF-ADAC-F68D1DF1530F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1ABE4E2-28A1-4551-91DE-422AFEA7EE55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10875" yWindow="6180" windowWidth="20730" windowHeight="12690" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
+    <workbookView xWindow="5190" yWindow="2835" windowWidth="27375" windowHeight="16245" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="93">
   <si>
     <t>EEJ</t>
   </si>
@@ -291,6 +291,27 @@
   </si>
   <si>
     <t>2050_TM152_DBP_PlusCrossing_07</t>
+  </si>
+  <si>
+    <t>running</t>
+  </si>
+  <si>
+    <t>"Blueprint Plus Crossing (s23)\v1.7.1- FINAL DRAFT BLUEPRINT"</t>
+  </si>
+  <si>
+    <t>run98</t>
+  </si>
+  <si>
+    <t>2035_TM152_DBP_NoProject_08</t>
+  </si>
+  <si>
+    <t>2035_TM152_DBP_Plus_08</t>
+  </si>
+  <si>
+    <t>2050_TM152_DBP_NoProject_08</t>
+  </si>
+  <si>
+    <t>2050_TM152_DBP_PlusCrossing_08</t>
   </si>
 </sst>
 </file>
@@ -397,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -451,7 +472,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -460,6 +480,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -780,11 +824,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A0CDBDA-1D45-4767-94B1-99049134204D}">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -793,7 +837,7 @@
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="40.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15" style="35" customWidth="1"/>
+    <col min="7" max="7" width="15" style="34" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -1249,700 +1293,798 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C23" s="31" t="s">
+      <c r="A23" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C23" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="30" t="s">
+      <c r="D23" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="30"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="30"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="22"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C24" s="31" t="s">
+      <c r="A24" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C24" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="30" t="s">
+      <c r="D24" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="30"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="30"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="22"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C25" s="31" t="s">
+      <c r="A25" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C25" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="30" t="s">
+      <c r="D25" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="30"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="30"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="22"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C26" s="31" t="s">
+      <c r="A26" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C26" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E26" s="30" t="s">
+      <c r="D26" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="30"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="30"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="22"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C27" s="31" t="s">
+      <c r="A27" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C27" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="D27" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27" s="30" t="s">
+      <c r="D27" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="30" t="s">
+      <c r="F27" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="G27" s="29" t="s">
+      <c r="G27" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="H27" s="30" t="s">
+      <c r="H27" s="22" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C28" s="31" t="s">
+      <c r="A28" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C28" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D28" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="30" t="s">
+      <c r="D28" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="30" t="s">
+      <c r="F28" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="G28" s="29" t="s">
+      <c r="G28" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="H28" s="30"/>
+      <c r="H28" s="22"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C29" s="30" t="s">
+      <c r="A29" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="36">
+        <v>2035</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="H29" s="37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C30" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" s="30" t="s">
+      <c r="D30" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="30"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="30"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C30" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="F30" s="30"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="30"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="40"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C31" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D31" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="F31" s="30"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="30"/>
+      <c r="B31" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="22"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="22"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C32" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="30" t="s">
+      <c r="B32" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F32" s="30"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="30"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="22"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C33" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D33" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="30" t="s">
+      <c r="B33" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F33" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="G33" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="H33" s="30"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="22"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C34" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="D34" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="30" t="s">
+      <c r="B34" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F34" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="G34" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="H34" s="30"/>
+      <c r="F34" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="G34" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="H34" s="22"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C35" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" s="30" t="s">
+      <c r="B35" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F35" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="G35" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="H35" s="30"/>
+      <c r="F35" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="H35" s="22"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C36" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="D36" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="30" t="s">
+      <c r="B36" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F36" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="G36" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="H36" s="30" t="s">
-        <v>43</v>
-      </c>
+      <c r="F36" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G36" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H36" s="22"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C37" s="30" t="s">
+      <c r="B37" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G37" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="H37" s="22"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C38" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E37" s="30" t="s">
+      <c r="D38" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F37" s="30" t="s">
+      <c r="F38" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="G37" s="29" t="s">
+      <c r="G38" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="H37" s="30"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="33">
+      <c r="H38" s="22"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="36">
+        <v>2035</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="F39" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="G39" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="H39" s="37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="42">
         <v>2050</v>
       </c>
-      <c r="C38" s="34" t="s">
+      <c r="C40" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" s="34" t="s">
+      <c r="D40" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F38" s="34"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="34"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="33">
+      <c r="F40" s="43"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="43"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="44">
         <v>2050</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="C41" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="D39" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E39" s="34" t="s">
+      <c r="D41" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F39" s="34"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="34"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="33">
+      <c r="F41" s="45"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="45"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="44">
         <v>2050</v>
       </c>
-      <c r="C40" s="34" t="s">
+      <c r="C42" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E40" s="34" t="s">
+      <c r="D42" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F40" s="34" t="s">
+      <c r="F42" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="G40" s="33" t="s">
+      <c r="G42" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="H40" s="34"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B41" s="33">
+      <c r="H42" s="45"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" s="44">
         <v>2050</v>
       </c>
-      <c r="C41" s="34" t="s">
+      <c r="C43" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="D41" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E41" s="34" t="s">
+      <c r="D43" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F41" s="34" t="s">
+      <c r="F43" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="G41" s="33" t="s">
+      <c r="G43" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="H41" s="34"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42" s="33">
+      <c r="H43" s="45"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="44">
         <v>2050</v>
       </c>
-      <c r="C42" s="34" t="s">
+      <c r="C44" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="D42" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E42" s="34" t="s">
+      <c r="D44" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E44" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F42" s="34" t="s">
+      <c r="F44" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="G42" s="33" t="s">
+      <c r="G44" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="H42" s="34" t="s">
+      <c r="H44" s="45"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C45" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E45" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="G45" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="H45" s="45"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C46" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="D46" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E46" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="G46" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="H46" s="48" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" s="33">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="42">
         <v>2050</v>
       </c>
-      <c r="C43" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="D43" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E43" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" s="34" t="s">
+      <c r="C47" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E47" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="F47" s="43"/>
+      <c r="G47" s="42"/>
+      <c r="H47" s="43"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C48" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="D48" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E48" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="F48" s="48"/>
+      <c r="G48" s="47"/>
+      <c r="H48" s="48"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C49" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F49" s="33"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="33"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C50" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F50" s="33"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="33"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C51" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F51" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G51" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="H51" s="33"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C52" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D52" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F52" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G52" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="H52" s="33"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C53" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D53" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E53" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F53" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="G53" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="H53" s="33"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C54" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D54" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E54" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F54" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="G54" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H54" s="33"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C55" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D55" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E55" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F55" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="G55" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H55" s="33"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C56" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="D56" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E56" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F56" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="G43" s="33" t="s">
+      <c r="G56" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="H43" s="34"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B44" s="33">
+      <c r="H56" s="33"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" s="32">
         <v>2050</v>
       </c>
-      <c r="C44" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D44" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E44" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F44" s="34"/>
-      <c r="G44" s="33"/>
-      <c r="H44" s="34"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" s="33">
-        <v>2050</v>
-      </c>
-      <c r="C45" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="D45" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E45" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F45" s="34"/>
-      <c r="G45" s="33"/>
-      <c r="H45" s="34"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B46" s="33">
-        <v>2050</v>
-      </c>
-      <c r="C46" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="D46" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E46" s="34" t="s">
+      <c r="C57" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D57" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E57" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F46" s="34"/>
-      <c r="G46" s="33"/>
-      <c r="H46" s="34"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47" s="33">
-        <v>2050</v>
-      </c>
-      <c r="C47" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="D47" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E47" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F47" s="34"/>
-      <c r="G47" s="33"/>
-      <c r="H47" s="34"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B48" s="33">
-        <v>2050</v>
-      </c>
-      <c r="C48" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="D48" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E48" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F48" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="G48" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="H48" s="34"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B49" s="33">
-        <v>2050</v>
-      </c>
-      <c r="C49" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="D49" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E49" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F49" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="G49" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="H49" s="34"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50" s="33">
-        <v>2050</v>
-      </c>
-      <c r="C50" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D50" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E50" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F50" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="G50" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="H50" s="34"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B51" s="33">
-        <v>2050</v>
-      </c>
-      <c r="C51" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="D51" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E51" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F51" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="G51" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="H51" s="34"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B52" s="33">
-        <v>2050</v>
-      </c>
-      <c r="C52" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="D52" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E52" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F52" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="G52" s="33" t="s">
-        <v>77</v>
-      </c>
-      <c r="H52" s="34" t="s">
+      <c r="F57" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="G57" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H57" s="33" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B53" s="33">
-        <v>2050</v>
-      </c>
-      <c r="C53" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="D53" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E53" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F53" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="G53" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="H53" s="34"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Updating for completion of 2035_TM152_DBP_NoProject_08
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1ABE4E2-28A1-4551-91DE-422AFEA7EE55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF896E1-FA4C-40CE-BDF2-7E0207681AC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5190" yWindow="2835" windowWidth="27375" windowHeight="16245" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="16200" windowHeight="9360" xr2:uid="{BDD2923F-CBFD-4599-A62A-2F09FCF1F8BF}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="92">
   <si>
     <t>EEJ</t>
   </si>
@@ -291,9 +291,6 @@
   </si>
   <si>
     <t>2050_TM152_DBP_PlusCrossing_07</t>
-  </si>
-  <si>
-    <t>running</t>
   </si>
   <si>
     <t>"Blueprint Plus Crossing (s23)\v1.7.1- FINAL DRAFT BLUEPRINT"</t>
@@ -828,7 +825,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
+      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1394,9 +1391,7 @@
       <c r="G27" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="H27" s="22" t="s">
-        <v>43</v>
-      </c>
+      <c r="H27" s="22"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
@@ -1430,7 +1425,7 @@
         <v>2035</v>
       </c>
       <c r="C29" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D29" s="37" t="s">
         <v>34</v>
@@ -1439,13 +1434,13 @@
         <v>7</v>
       </c>
       <c r="F29" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="G29" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="G29" s="36" t="s">
-        <v>88</v>
-      </c>
       <c r="H29" s="37" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1656,7 +1651,7 @@
         <v>2035</v>
       </c>
       <c r="C39" s="37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D39" s="37" t="s">
         <v>34</v>
@@ -1665,10 +1660,10 @@
         <v>38</v>
       </c>
       <c r="F39" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="G39" s="36" t="s">
         <v>87</v>
-      </c>
-      <c r="G39" s="36" t="s">
-        <v>88</v>
       </c>
       <c r="H39" s="37" t="s">
         <v>43</v>
@@ -1818,7 +1813,7 @@
         <v>2050</v>
       </c>
       <c r="C46" s="48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D46" s="48" t="s">
         <v>34</v>
@@ -1827,10 +1822,10 @@
         <v>7</v>
       </c>
       <c r="F46" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="G46" s="47" t="s">
         <v>87</v>
-      </c>
-      <c r="G46" s="47" t="s">
-        <v>88</v>
       </c>
       <c r="H46" s="48" t="s">
         <v>43</v>
@@ -2068,7 +2063,7 @@
         <v>2050</v>
       </c>
       <c r="C57" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D57" s="33" t="s">
         <v>34</v>
@@ -2077,10 +2072,10 @@
         <v>38</v>
       </c>
       <c r="F57" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="G57" s="32" t="s">
         <v>87</v>
-      </c>
-      <c r="G57" s="32" t="s">
-        <v>88</v>
       </c>
       <c r="H57" s="33" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
New 2035 and 2050 Final Blueprint runs
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bespin\Documents\GitHub\travel-model-one\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="98">
   <si>
     <t>EEJ</t>
   </si>
@@ -317,6 +317,15 @@
   </si>
   <si>
     <t>2035_TM152_DBP_Plus_08_TollingX2</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_Plus_01</t>
+  </si>
+  <si>
+    <t>FinalBlueprint</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_PlusCrossing_01</t>
   </si>
 </sst>
 </file>
@@ -517,8 +526,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <mruColors>
       <color rgb="FFE4C9FF"/>
@@ -833,14 +870,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
@@ -849,7 +886,7 @@
     <col min="7" max="7" width="15" style="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -875,7 +912,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
@@ -895,7 +932,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
@@ -915,7 +952,7 @@
       <c r="G3" s="11"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>25</v>
       </c>
@@ -935,7 +972,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>25</v>
       </c>
@@ -955,7 +992,7 @@
       <c r="G5" s="15"/>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>25</v>
       </c>
@@ -975,7 +1012,7 @@
       <c r="G6" s="15"/>
       <c r="H6" s="16"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>25</v>
       </c>
@@ -995,7 +1032,7 @@
       <c r="G7" s="15"/>
       <c r="H7" s="16"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>25</v>
       </c>
@@ -1015,7 +1052,7 @@
       <c r="G8" s="15"/>
       <c r="H8" s="16"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>25</v>
       </c>
@@ -1035,7 +1072,7 @@
       <c r="G9" s="15"/>
       <c r="H9" s="16"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>25</v>
       </c>
@@ -1055,7 +1092,7 @@
       <c r="G10" s="21"/>
       <c r="H10" s="22"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>25</v>
       </c>
@@ -1075,7 +1112,7 @@
       <c r="G11" s="21"/>
       <c r="H11" s="22"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>25</v>
       </c>
@@ -1095,7 +1132,7 @@
       <c r="G12" s="21"/>
       <c r="H12" s="22"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>25</v>
       </c>
@@ -1115,7 +1152,7 @@
       <c r="G13" s="21"/>
       <c r="H13" s="22"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>25</v>
       </c>
@@ -1135,7 +1172,7 @@
       <c r="G14" s="21"/>
       <c r="H14" s="22"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>25</v>
       </c>
@@ -1155,7 +1192,7 @@
       <c r="G15" s="18"/>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>25</v>
       </c>
@@ -1175,7 +1212,7 @@
       <c r="G16" s="18"/>
       <c r="H16" s="19"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>25</v>
       </c>
@@ -1195,7 +1232,7 @@
       <c r="G17" s="18"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>25</v>
       </c>
@@ -1215,7 +1252,7 @@
       <c r="G18" s="18"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>25</v>
       </c>
@@ -1235,7 +1272,7 @@
       <c r="G19" s="24"/>
       <c r="H19" s="25"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
         <v>26</v>
       </c>
@@ -1257,7 +1294,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
         <v>26</v>
       </c>
@@ -1279,7 +1316,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>26</v>
       </c>
@@ -1305,7 +1342,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>26</v>
       </c>
@@ -1327,7 +1364,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
         <v>26</v>
       </c>
@@ -1347,7 +1384,7 @@
       <c r="G24" s="21"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
         <v>26</v>
       </c>
@@ -1367,7 +1404,7 @@
       <c r="G25" s="21"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
         <v>26</v>
       </c>
@@ -1387,7 +1424,7 @@
       <c r="G26" s="21"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
         <v>26</v>
       </c>
@@ -1407,7 +1444,7 @@
       <c r="G27" s="21"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
         <v>26</v>
       </c>
@@ -1431,7 +1468,7 @@
       </c>
       <c r="H28" s="22"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
         <v>26</v>
       </c>
@@ -1455,7 +1492,7 @@
       </c>
       <c r="H29" s="22"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="35" t="s">
         <v>26</v>
       </c>
@@ -1481,7 +1518,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="38" t="s">
         <v>26</v>
       </c>
@@ -1501,7 +1538,7 @@
       <c r="G31" s="39"/>
       <c r="H31" s="40"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
         <v>26</v>
       </c>
@@ -1521,7 +1558,7 @@
       <c r="G32" s="21"/>
       <c r="H32" s="22"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
         <v>26</v>
       </c>
@@ -1541,7 +1578,7 @@
       <c r="G33" s="21"/>
       <c r="H33" s="22"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
         <v>26</v>
       </c>
@@ -1561,7 +1598,7 @@
       <c r="G34" s="21"/>
       <c r="H34" s="22"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
         <v>26</v>
       </c>
@@ -1585,7 +1622,7 @@
       </c>
       <c r="H35" s="22"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
         <v>26</v>
       </c>
@@ -1609,7 +1646,7 @@
       </c>
       <c r="H36" s="22"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
         <v>26</v>
       </c>
@@ -1633,7 +1670,7 @@
       </c>
       <c r="H37" s="22"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
         <v>26</v>
       </c>
@@ -1657,7 +1694,7 @@
       </c>
       <c r="H38" s="22"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
         <v>26</v>
       </c>
@@ -1681,7 +1718,7 @@
       </c>
       <c r="H39" s="22"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
         <v>26</v>
       </c>
@@ -1707,7 +1744,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="35" t="s">
         <v>26</v>
       </c>
@@ -1733,7 +1770,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="35" t="s">
         <v>26</v>
       </c>
@@ -1759,47 +1796,53 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A43" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" s="42">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" s="36">
+        <v>2035</v>
+      </c>
+      <c r="C43" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="D43" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="E43" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="G43" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="H43" s="37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="42">
         <v>2050</v>
       </c>
-      <c r="C43" s="43" t="s">
+      <c r="C44" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E43" s="43" t="s">
+      <c r="D44" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E44" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F43" s="43"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="43"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A44" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B44" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C44" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="D44" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E44" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="45"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="45"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F44" s="43"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="43"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="31" t="s">
         <v>26</v>
       </c>
@@ -1807,7 +1850,7 @@
         <v>2050</v>
       </c>
       <c r="C45" s="45" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D45" s="45" t="s">
         <v>34</v>
@@ -1815,15 +1858,11 @@
       <c r="E45" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F45" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="G45" s="44" t="s">
-        <v>65</v>
-      </c>
+      <c r="F45" s="45"/>
+      <c r="G45" s="44"/>
       <c r="H45" s="45"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="31" t="s">
         <v>26</v>
       </c>
@@ -1831,7 +1870,7 @@
         <v>2050</v>
       </c>
       <c r="C46" s="45" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D46" s="45" t="s">
         <v>34</v>
@@ -1847,7 +1886,7 @@
       </c>
       <c r="H46" s="45"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="31" t="s">
         <v>26</v>
       </c>
@@ -1855,7 +1894,7 @@
         <v>2050</v>
       </c>
       <c r="C47" s="45" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="D47" s="45" t="s">
         <v>34</v>
@@ -1864,14 +1903,14 @@
         <v>7</v>
       </c>
       <c r="F47" s="45" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="G47" s="44" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="H47" s="45"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="31" t="s">
         <v>26</v>
       </c>
@@ -1879,7 +1918,7 @@
         <v>2050</v>
       </c>
       <c r="C48" s="45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D48" s="45" t="s">
         <v>34</v>
@@ -1888,100 +1927,104 @@
         <v>7</v>
       </c>
       <c r="F48" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="G48" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="H48" s="45"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C49" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="D49" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="G48" s="44" t="s">
+      <c r="G49" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="H48" s="45"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A49" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B49" s="47">
+      <c r="H49" s="45"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="47">
         <v>2050</v>
       </c>
-      <c r="C49" s="48" t="s">
+      <c r="C50" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="D49" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E49" s="48" t="s">
+      <c r="D50" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F49" s="48" t="s">
+      <c r="F50" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="G49" s="47" t="s">
+      <c r="G50" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="H49" s="48" t="s">
+      <c r="H50" s="48" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A50" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50" s="42">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="42">
         <v>2050</v>
       </c>
-      <c r="C50" s="43" t="s">
+      <c r="C51" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D50" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E50" s="43" t="s">
+      <c r="D51" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="F50" s="43"/>
-      <c r="G50" s="42"/>
-      <c r="H50" s="43"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A51" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B51" s="47">
+      <c r="F51" s="43"/>
+      <c r="G51" s="42"/>
+      <c r="H51" s="43"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="47">
         <v>2050</v>
       </c>
-      <c r="C51" s="48" t="s">
+      <c r="C52" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="D51" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E51" s="48" t="s">
+      <c r="D52" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F51" s="48"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="48"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A52" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B52" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C52" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D52" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E52" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F52" s="33"/>
-      <c r="G52" s="32"/>
-      <c r="H52" s="33"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F52" s="48"/>
+      <c r="G52" s="47"/>
+      <c r="H52" s="48"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="31" t="s">
         <v>26</v>
       </c>
@@ -1989,7 +2032,7 @@
         <v>2050</v>
       </c>
       <c r="C53" s="33" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D53" s="33" t="s">
         <v>34</v>
@@ -2001,7 +2044,7 @@
       <c r="G53" s="32"/>
       <c r="H53" s="33"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="31" t="s">
         <v>26</v>
       </c>
@@ -2009,7 +2052,7 @@
         <v>2050</v>
       </c>
       <c r="C54" s="33" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D54" s="33" t="s">
         <v>34</v>
@@ -2017,15 +2060,11 @@
       <c r="E54" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F54" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G54" s="32" t="s">
-        <v>63</v>
-      </c>
+      <c r="F54" s="33"/>
+      <c r="G54" s="32"/>
       <c r="H54" s="33"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="31" t="s">
         <v>26</v>
       </c>
@@ -2033,7 +2072,7 @@
         <v>2050</v>
       </c>
       <c r="C55" s="33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D55" s="33" t="s">
         <v>34</v>
@@ -2049,7 +2088,7 @@
       </c>
       <c r="H55" s="33"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="31" t="s">
         <v>26</v>
       </c>
@@ -2057,7 +2096,7 @@
         <v>2050</v>
       </c>
       <c r="C56" s="33" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D56" s="33" t="s">
         <v>34</v>
@@ -2066,14 +2105,14 @@
         <v>38</v>
       </c>
       <c r="F56" s="33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G56" s="32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H56" s="33"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="31" t="s">
         <v>26</v>
       </c>
@@ -2081,7 +2120,7 @@
         <v>2050</v>
       </c>
       <c r="C57" s="33" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D57" s="33" t="s">
         <v>34</v>
@@ -2090,14 +2129,14 @@
         <v>38</v>
       </c>
       <c r="F57" s="33" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G57" s="32" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H57" s="33"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="31" t="s">
         <v>26</v>
       </c>
@@ -2105,7 +2144,7 @@
         <v>2050</v>
       </c>
       <c r="C58" s="33" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D58" s="33" t="s">
         <v>34</v>
@@ -2114,14 +2153,14 @@
         <v>38</v>
       </c>
       <c r="F58" s="33" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G58" s="32" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H58" s="33"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="31" t="s">
         <v>26</v>
       </c>
@@ -2129,7 +2168,7 @@
         <v>2050</v>
       </c>
       <c r="C59" s="33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D59" s="33" t="s">
         <v>34</v>
@@ -2138,14 +2177,14 @@
         <v>38</v>
       </c>
       <c r="F59" s="33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G59" s="32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H59" s="33"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="31" t="s">
         <v>26</v>
       </c>
@@ -2153,7 +2192,7 @@
         <v>2050</v>
       </c>
       <c r="C60" s="33" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D60" s="33" t="s">
         <v>34</v>
@@ -2162,12 +2201,62 @@
         <v>38</v>
       </c>
       <c r="F60" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="G60" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="H60" s="33"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C61" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D61" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E61" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F61" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="G60" s="32" t="s">
+      <c r="G61" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="H60" s="33" t="s">
+      <c r="H61" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C62" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="D62" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="E62" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="F62" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="G62" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="H62" s="43" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix mislabeling of FBP 2035 NoProject rundir
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727C2CA1-1876-4267-9241-F1E4A84BD5C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C0E6ED-4A8F-4FF6-8CF0-8CEA0BBE2EDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17955" yWindow="1740" windowWidth="19305" windowHeight="17190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="114">
   <si>
     <t>EEJ</t>
   </si>
@@ -364,6 +364,9 @@
   </si>
   <si>
     <t>2050_TM152_FBP_PlusCrossing_06</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_NoProject_06</t>
   </si>
 </sst>
 </file>
@@ -921,8 +924,8 @@
   <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1592,7 +1595,7 @@
         <v>2035</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="D32" s="25" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
added FBP run v08 for 2035 and 2050
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C0E6ED-4A8F-4FF6-8CF0-8CEA0BBE2EDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17955" yWindow="1740" windowWidth="19305" windowHeight="17190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17955" yWindow="1740" windowWidth="19305" windowHeight="17190"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="118">
   <si>
     <t>EEJ</t>
   </si>
@@ -367,12 +366,24 @@
   </si>
   <si>
     <t>2035_TM152_FBP_NoProject_06</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_PlusCrossing_08</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_Plus_08</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_NoProject_08</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_NoProject_08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -473,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -573,6 +584,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,7 +614,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -920,15 +932,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H78"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
@@ -937,7 +949,7 @@
     <col min="7" max="7" width="15" style="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -963,7 +975,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
@@ -983,7 +995,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
@@ -1003,7 +1015,7 @@
       <c r="G3" s="11"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="13" t="s">
         <v>25</v>
       </c>
@@ -1023,7 +1035,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="14" t="s">
         <v>25</v>
       </c>
@@ -1043,7 +1055,7 @@
       <c r="G5" s="15"/>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="14" t="s">
         <v>25</v>
       </c>
@@ -1063,7 +1075,7 @@
       <c r="G6" s="15"/>
       <c r="H6" s="16"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="14" t="s">
         <v>25</v>
       </c>
@@ -1083,7 +1095,7 @@
       <c r="G7" s="15"/>
       <c r="H7" s="16"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="14" t="s">
         <v>25</v>
       </c>
@@ -1103,7 +1115,7 @@
       <c r="G8" s="15"/>
       <c r="H8" s="16"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="14" t="s">
         <v>25</v>
       </c>
@@ -1123,7 +1135,7 @@
       <c r="G9" s="15"/>
       <c r="H9" s="16"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="20" t="s">
         <v>25</v>
       </c>
@@ -1143,7 +1155,7 @@
       <c r="G10" s="21"/>
       <c r="H10" s="22"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="20" t="s">
         <v>25</v>
       </c>
@@ -1163,7 +1175,7 @@
       <c r="G11" s="21"/>
       <c r="H11" s="22"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="20" t="s">
         <v>25</v>
       </c>
@@ -1183,7 +1195,7 @@
       <c r="G12" s="21"/>
       <c r="H12" s="22"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="20" t="s">
         <v>25</v>
       </c>
@@ -1203,7 +1215,7 @@
       <c r="G13" s="21"/>
       <c r="H13" s="22"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="20" t="s">
         <v>25</v>
       </c>
@@ -1223,7 +1235,7 @@
       <c r="G14" s="21"/>
       <c r="H14" s="22"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="17" t="s">
         <v>25</v>
       </c>
@@ -1243,7 +1255,7 @@
       <c r="G15" s="18"/>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" s="17" t="s">
         <v>25</v>
       </c>
@@ -1263,7 +1275,7 @@
       <c r="G16" s="18"/>
       <c r="H16" s="19"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" s="17" t="s">
         <v>25</v>
       </c>
@@ -1283,7 +1295,7 @@
       <c r="G17" s="18"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" s="17" t="s">
         <v>25</v>
       </c>
@@ -1303,7 +1315,7 @@
       <c r="G18" s="18"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19" s="23" t="s">
         <v>25</v>
       </c>
@@ -1323,7 +1335,7 @@
       <c r="G19" s="24"/>
       <c r="H19" s="25"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A20" s="26" t="s">
         <v>26</v>
       </c>
@@ -1345,7 +1357,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21" s="13" t="s">
         <v>26</v>
       </c>
@@ -1367,7 +1379,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A22" s="10" t="s">
         <v>26</v>
       </c>
@@ -1393,7 +1405,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" s="20" t="s">
         <v>26</v>
       </c>
@@ -1413,7 +1425,7 @@
       <c r="G23" s="29"/>
       <c r="H23" s="29"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24" s="20" t="s">
         <v>26</v>
       </c>
@@ -1435,7 +1447,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A25" s="20" t="s">
         <v>26</v>
       </c>
@@ -1455,7 +1467,7 @@
       <c r="G25" s="21"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A26" s="20" t="s">
         <v>26</v>
       </c>
@@ -1475,7 +1487,7 @@
       <c r="G26" s="21"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A27" s="20" t="s">
         <v>26</v>
       </c>
@@ -1495,7 +1507,7 @@
       <c r="G27" s="21"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A28" s="20" t="s">
         <v>26</v>
       </c>
@@ -1515,7 +1527,7 @@
       <c r="G28" s="21"/>
       <c r="H28" s="22"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A29" s="20" t="s">
         <v>26</v>
       </c>
@@ -1539,7 +1551,7 @@
       </c>
       <c r="H29" s="22"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A30" s="20" t="s">
         <v>26</v>
       </c>
@@ -1563,125 +1575,129 @@
       </c>
       <c r="H30" s="22"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="36">
-        <v>2035</v>
-      </c>
-      <c r="C31" s="35" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A31" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C31" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="D31" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="37" t="s">
+      <c r="D31" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="37" t="s">
+      <c r="F31" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="G31" s="36" t="s">
+      <c r="G31" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="H31" s="37"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C32" s="25" t="s">
+      <c r="H31" s="22"/>
+    </row>
+    <row r="32" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="53">
+        <v>2035</v>
+      </c>
+      <c r="C32" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="D32" s="25" t="s">
+      <c r="D32" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="E32" s="25" t="s">
+      <c r="E32" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="25" t="s">
+      <c r="F32" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="G32" s="24" t="s">
+      <c r="G32" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="H32" s="25" t="s">
+      <c r="H32" s="54"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A33" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="G33" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="H33" s="25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="39">
-        <v>2035</v>
-      </c>
-      <c r="C33" s="40" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A34" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C34" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="40" t="s">
+      <c r="D34" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F33" s="40"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="40"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="36">
-        <v>2035</v>
-      </c>
-      <c r="C34" s="37" t="s">
+      <c r="F34" s="40"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="40"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A35" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="36">
+        <v>2035</v>
+      </c>
+      <c r="C35" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="37" t="s">
+      <c r="D35" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="F34" s="37"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="37"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C35" s="22" t="s">
+      <c r="F35" s="37"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="37"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A36" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C36" s="22" t="s">
         <v>47</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F35" s="22"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="22"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C36" s="22" t="s">
-        <v>37</v>
       </c>
       <c r="D36" s="22" t="s">
         <v>34</v>
@@ -1693,7 +1709,7 @@
       <c r="G36" s="21"/>
       <c r="H36" s="22"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A37" s="20" t="s">
         <v>26</v>
       </c>
@@ -1701,167 +1717,165 @@
         <v>2035</v>
       </c>
       <c r="C37" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F37" s="22"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="22"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A38" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C38" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D37" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F37" s="22" t="s">
+      <c r="D38" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F38" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="G37" s="21" t="s">
+      <c r="G38" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="H37" s="22"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C38" s="22" t="s">
+      <c r="H38" s="22"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A39" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C39" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F38" s="22" t="s">
+      <c r="D39" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F39" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="G38" s="21" t="s">
+      <c r="G39" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="H38" s="22"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C39" s="22" t="s">
+      <c r="H39" s="22"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A40" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C40" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="D39" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F39" s="22" t="s">
+      <c r="D40" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="G39" s="21" t="s">
+      <c r="G40" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="H39" s="22"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C40" s="22" t="s">
+      <c r="H40" s="22"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A41" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C41" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="D40" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E40" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F40" s="22" t="s">
+      <c r="D41" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F41" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="G40" s="21" t="s">
+      <c r="G41" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="H40" s="22"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B41" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C41" s="22" t="s">
+      <c r="H41" s="22"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A42" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C42" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="D41" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E41" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F41" s="22" t="s">
+      <c r="D42" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F42" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="G41" s="21" t="s">
+      <c r="G42" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="H41" s="22"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C42" s="22" t="s">
+      <c r="H42" s="22"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A43" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C43" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E42" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F42" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="G42" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="H42" s="22"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C43" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="D43" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E43" s="30" t="s">
+      <c r="D43" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" s="22" t="s">
         <v>38</v>
       </c>
       <c r="F43" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="G43" s="29" t="s">
+      <c r="G43" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="H43" s="30"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H43" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A44" s="51" t="s">
         <v>26</v>
       </c>
@@ -1869,7 +1883,7 @@
         <v>2035</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D44" s="30" t="s">
         <v>34</v>
@@ -1885,31 +1899,31 @@
       </c>
       <c r="H44" s="30"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C45" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="D45" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E45" s="22" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A45" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C45" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E45" s="30" t="s">
         <v>38</v>
       </c>
       <c r="F45" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="G45" s="21" t="s">
+      <c r="G45" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="H45" s="22"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H45" s="30"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A46" s="20" t="s">
         <v>26</v>
       </c>
@@ -1917,7 +1931,7 @@
         <v>2035</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D46" s="22" t="s">
         <v>34</v>
@@ -1933,7 +1947,7 @@
       </c>
       <c r="H46" s="22"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A47" s="20" t="s">
         <v>26</v>
       </c>
@@ -1941,7 +1955,7 @@
         <v>2035</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D47" s="22" t="s">
         <v>34</v>
@@ -1957,7 +1971,7 @@
       </c>
       <c r="H47" s="22"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A48" s="20" t="s">
         <v>26</v>
       </c>
@@ -1965,7 +1979,7 @@
         <v>2035</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D48" s="22" t="s">
         <v>34</v>
@@ -1981,129 +1995,135 @@
       </c>
       <c r="H48" s="22"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B49" s="53">
-        <v>2035</v>
-      </c>
-      <c r="C49" s="54" t="s">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A49" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C49" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F49" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G49" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="H49" s="22"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A50" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="53">
+        <v>2035</v>
+      </c>
+      <c r="C50" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="D49" s="54" t="s">
+      <c r="D50" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="E49" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F49" s="54" t="s">
+      <c r="E50" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F50" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="G49" s="53" t="s">
+      <c r="G50" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="H49" s="54"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50" s="24">
-        <v>2035</v>
-      </c>
-      <c r="C50" s="25" t="s">
+      <c r="H50" s="54"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A51" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C51" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="D50" s="25" t="s">
+      <c r="D51" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="E50" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F50" s="25" t="s">
+      <c r="E51" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F51" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="G50" s="24" t="s">
+      <c r="G51" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="H50" s="25" t="s">
+      <c r="H51" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B51" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C51" s="43" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A52" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="24">
+        <v>2035</v>
+      </c>
+      <c r="C52" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="E52" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F52" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="G52" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="H52" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A53" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C53" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D51" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E51" s="43" t="s">
+      <c r="D53" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E53" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F51" s="43"/>
-      <c r="G51" s="42"/>
-      <c r="H51" s="43"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B52" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C52" s="45" t="s">
+      <c r="F53" s="43"/>
+      <c r="G53" s="42"/>
+      <c r="H53" s="43"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A54" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C54" s="45" t="s">
         <v>53</v>
-      </c>
-      <c r="D52" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E52" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F52" s="45"/>
-      <c r="G52" s="44"/>
-      <c r="H52" s="45"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B53" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C53" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="D53" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E53" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F53" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="G53" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="H53" s="45"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B54" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C54" s="45" t="s">
-        <v>69</v>
       </c>
       <c r="D54" s="45" t="s">
         <v>34</v>
@@ -2111,15 +2131,11 @@
       <c r="E54" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F54" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="G54" s="44" t="s">
-        <v>65</v>
-      </c>
+      <c r="F54" s="45"/>
+      <c r="G54" s="44"/>
       <c r="H54" s="45"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A55" s="31" t="s">
         <v>26</v>
       </c>
@@ -2127,7 +2143,7 @@
         <v>2050</v>
       </c>
       <c r="C55" s="45" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="D55" s="45" t="s">
         <v>34</v>
@@ -2136,14 +2152,14 @@
         <v>7</v>
       </c>
       <c r="F55" s="45" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="G55" s="44" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="H55" s="45"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A56" s="31" t="s">
         <v>26</v>
       </c>
@@ -2151,7 +2167,7 @@
         <v>2050</v>
       </c>
       <c r="C56" s="45" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="D56" s="45" t="s">
         <v>34</v>
@@ -2160,446 +2176,446 @@
         <v>7</v>
       </c>
       <c r="F56" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="G56" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="H56" s="45"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A57" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C57" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="D57" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E57" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F57" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="G57" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="H57" s="45"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A58" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C58" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="D58" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E58" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F58" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="G56" s="44" t="s">
+      <c r="G58" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="H56" s="45"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B57" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C57" s="48" t="s">
+      <c r="H58" s="45"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A59" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C59" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="D57" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E57" s="48" t="s">
+      <c r="D59" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E59" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F57" s="48" t="s">
+      <c r="F59" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="G57" s="47" t="s">
+      <c r="G59" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="H57" s="48" t="s">
+      <c r="H59" s="48"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A60" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B60" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D60" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="E60" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F60" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="G60" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H60" s="19"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A61" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C61" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D61" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E61" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F61" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G61" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="H61" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B58" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C58" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="D58" s="54" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A62" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C62" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D62" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="E58" s="19" t="s">
+      <c r="E62" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F58" s="19" t="s">
+      <c r="F62" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G62" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="H62" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A63" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C63" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="D63" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E63" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="F63" s="43"/>
+      <c r="G63" s="42"/>
+      <c r="H63" s="43"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A64" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B64" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C64" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="D64" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E64" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="F64" s="48"/>
+      <c r="G64" s="47"/>
+      <c r="H64" s="48"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A65" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B65" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C65" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D65" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E65" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F65" s="33"/>
+      <c r="G65" s="32"/>
+      <c r="H65" s="33"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A66" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B66" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C66" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D66" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E66" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F66" s="33"/>
+      <c r="G66" s="32"/>
+      <c r="H66" s="33"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A67" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C67" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D67" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E67" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F67" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G67" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="H67" s="33"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A68" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C68" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D68" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E68" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F68" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G68" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="H68" s="33"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A69" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B69" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C69" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D69" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E69" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F69" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="G69" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="H69" s="33"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A70" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B70" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C70" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D70" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E70" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F70" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="G70" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H70" s="33"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A71" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C71" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D71" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E71" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F71" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="G71" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H71" s="33"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A72" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B72" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C72" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="D72" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E72" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F72" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="G58" s="56" t="s">
+      <c r="G72" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="H58" s="19"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B59" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C59" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="D59" s="25" t="s">
+      <c r="H72" s="33"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A73" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B73" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C73" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D73" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E73" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F73" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="G73" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="H73" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A74" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74" s="53">
+        <v>2050</v>
+      </c>
+      <c r="C74" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="D74" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="E59" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F59" s="19" t="s">
+      <c r="E74" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F74" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="G59" s="18" t="s">
+      <c r="G74" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="H59" s="19" t="s">
+      <c r="H74" s="54" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B60" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C60" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="D60" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E60" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="F60" s="43"/>
-      <c r="G60" s="42"/>
-      <c r="H60" s="43"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B61" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C61" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="D61" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E61" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="F61" s="48"/>
-      <c r="G61" s="47"/>
-      <c r="H61" s="48"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B62" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C62" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D62" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E62" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F62" s="33"/>
-      <c r="G62" s="32"/>
-      <c r="H62" s="33"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B63" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C63" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D63" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E63" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F63" s="33"/>
-      <c r="G63" s="32"/>
-      <c r="H63" s="33"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B64" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C64" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="D64" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E64" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F64" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G64" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="H64" s="33"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B65" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C65" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D65" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E65" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F65" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G65" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="H65" s="33"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B66" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C66" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="D66" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E66" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F66" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="G66" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="H66" s="33"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B67" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C67" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D67" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E67" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F67" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="G67" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="H67" s="33"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B68" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C68" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="D68" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E68" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F68" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="G68" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="H68" s="33"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B69" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C69" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="D69" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E69" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F69" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="G69" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="H69" s="33"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B70" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C70" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="D70" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E70" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F70" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="G70" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="H70" s="33" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B71" s="53">
-        <v>2050</v>
-      </c>
-      <c r="C71" s="54" t="s">
-        <v>97</v>
-      </c>
-      <c r="D71" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="E71" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F71" s="54" t="s">
-        <v>86</v>
-      </c>
-      <c r="G71" s="53" t="s">
-        <v>87</v>
-      </c>
-      <c r="H71" s="54" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B72" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C72" s="55" t="s">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A75" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B75" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C75" s="55" t="s">
         <v>106</v>
-      </c>
-      <c r="D72" s="55" t="s">
-        <v>96</v>
-      </c>
-      <c r="E72" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F72" s="55" t="s">
-        <v>86</v>
-      </c>
-      <c r="G72" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="H72" s="55"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B73" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C73" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="D73" s="55" t="s">
-        <v>96</v>
-      </c>
-      <c r="E73" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F73" s="55" t="s">
-        <v>86</v>
-      </c>
-      <c r="G73" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="H73" s="55"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B74" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C74" s="55" t="s">
-        <v>108</v>
-      </c>
-      <c r="D74" s="55" t="s">
-        <v>96</v>
-      </c>
-      <c r="E74" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F74" s="55" t="s">
-        <v>86</v>
-      </c>
-      <c r="G74" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="H74" s="55"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B75" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C75" s="55" t="s">
-        <v>109</v>
       </c>
       <c r="D75" s="55" t="s">
         <v>96</v>
@@ -2615,7 +2631,7 @@
       </c>
       <c r="H75" s="55"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A76" s="55" t="s">
         <v>26</v>
       </c>
@@ -2623,7 +2639,7 @@
         <v>2050</v>
       </c>
       <c r="C76" s="55" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D76" s="55" t="s">
         <v>96</v>
@@ -2639,7 +2655,7 @@
       </c>
       <c r="H76" s="55"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A77" s="55" t="s">
         <v>26</v>
       </c>
@@ -2647,7 +2663,7 @@
         <v>2050</v>
       </c>
       <c r="C77" s="55" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D77" s="55" t="s">
         <v>96</v>
@@ -2655,15 +2671,15 @@
       <c r="E77" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F77" s="19" t="s">
-        <v>78</v>
+      <c r="F77" s="55" t="s">
+        <v>86</v>
       </c>
       <c r="G77" s="56" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="H77" s="55"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A78" s="55" t="s">
         <v>26</v>
       </c>
@@ -2671,7 +2687,7 @@
         <v>2050</v>
       </c>
       <c r="C78" s="55" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D78" s="55" t="s">
         <v>96</v>
@@ -2685,7 +2701,105 @@
       <c r="G78" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="H78" s="55" t="s">
+      <c r="H78" s="55"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A79" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B79" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C79" s="55" t="s">
+        <v>110</v>
+      </c>
+      <c r="D79" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="E79" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F79" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="G79" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="H79" s="55"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A80" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B80" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C80" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="D80" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="E80" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F80" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="G80" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H80" s="55"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A81" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B81" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C81" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="D81" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="E81" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F81" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="G81" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="H81" s="55" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A82" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B82" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C82" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="D82" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="E82" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F82" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="G82" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="H82" s="55" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removing 2050_TM152_FBP_PlusCrossing_01 from current
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC6C138-1554-4328-AD48-4E6656831DD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17955" yWindow="1740" windowWidth="19305" windowHeight="17190"/>
+    <workbookView xWindow="15690" yWindow="2760" windowWidth="21510" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="118">
   <si>
     <t>EEJ</t>
   </si>
@@ -383,7 +384,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -614,7 +615,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -932,15 +933,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I73" sqref="I73"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
@@ -949,7 +950,7 @@
     <col min="7" max="7" width="15" style="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -975,7 +976,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
@@ -995,7 +996,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
@@ -1015,7 +1016,7 @@
       <c r="G3" s="11"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>25</v>
       </c>
@@ -1035,7 +1036,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>25</v>
       </c>
@@ -1055,7 +1056,7 @@
       <c r="G5" s="15"/>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>25</v>
       </c>
@@ -1075,7 +1076,7 @@
       <c r="G6" s="15"/>
       <c r="H6" s="16"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>25</v>
       </c>
@@ -1095,7 +1096,7 @@
       <c r="G7" s="15"/>
       <c r="H7" s="16"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>25</v>
       </c>
@@ -1115,7 +1116,7 @@
       <c r="G8" s="15"/>
       <c r="H8" s="16"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>25</v>
       </c>
@@ -1135,7 +1136,7 @@
       <c r="G9" s="15"/>
       <c r="H9" s="16"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>25</v>
       </c>
@@ -1155,7 +1156,7 @@
       <c r="G10" s="21"/>
       <c r="H10" s="22"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>25</v>
       </c>
@@ -1175,7 +1176,7 @@
       <c r="G11" s="21"/>
       <c r="H11" s="22"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>25</v>
       </c>
@@ -1195,7 +1196,7 @@
       <c r="G12" s="21"/>
       <c r="H12" s="22"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>25</v>
       </c>
@@ -1215,7 +1216,7 @@
       <c r="G13" s="21"/>
       <c r="H13" s="22"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>25</v>
       </c>
@@ -1235,7 +1236,7 @@
       <c r="G14" s="21"/>
       <c r="H14" s="22"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>25</v>
       </c>
@@ -1255,7 +1256,7 @@
       <c r="G15" s="18"/>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>25</v>
       </c>
@@ -1275,7 +1276,7 @@
       <c r="G16" s="18"/>
       <c r="H16" s="19"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>25</v>
       </c>
@@ -1295,7 +1296,7 @@
       <c r="G17" s="18"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>25</v>
       </c>
@@ -1315,7 +1316,7 @@
       <c r="G18" s="18"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>25</v>
       </c>
@@ -1335,7 +1336,7 @@
       <c r="G19" s="24"/>
       <c r="H19" s="25"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
         <v>26</v>
       </c>
@@ -1357,7 +1358,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
         <v>26</v>
       </c>
@@ -1379,7 +1380,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>26</v>
       </c>
@@ -1405,7 +1406,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>26</v>
       </c>
@@ -1425,7 +1426,7 @@
       <c r="G23" s="29"/>
       <c r="H23" s="29"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
         <v>26</v>
       </c>
@@ -1447,7 +1448,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
         <v>26</v>
       </c>
@@ -1467,7 +1468,7 @@
       <c r="G25" s="21"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
         <v>26</v>
       </c>
@@ -1487,7 +1488,7 @@
       <c r="G26" s="21"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
         <v>26</v>
       </c>
@@ -1507,7 +1508,7 @@
       <c r="G27" s="21"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
         <v>26</v>
       </c>
@@ -1527,7 +1528,7 @@
       <c r="G28" s="21"/>
       <c r="H28" s="22"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
         <v>26</v>
       </c>
@@ -1551,7 +1552,7 @@
       </c>
       <c r="H29" s="22"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
         <v>26</v>
       </c>
@@ -1575,7 +1576,7 @@
       </c>
       <c r="H30" s="22"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
         <v>26</v>
       </c>
@@ -1599,7 +1600,7 @@
       </c>
       <c r="H31" s="22"/>
     </row>
-    <row r="32" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="52" t="s">
         <v>26</v>
       </c>
@@ -1623,7 +1624,7 @@
       </c>
       <c r="H32" s="54"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>26</v>
       </c>
@@ -1649,7 +1650,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="38" t="s">
         <v>26</v>
       </c>
@@ -1669,7 +1670,7 @@
       <c r="G34" s="39"/>
       <c r="H34" s="40"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="35" t="s">
         <v>26</v>
       </c>
@@ -1689,7 +1690,7 @@
       <c r="G35" s="36"/>
       <c r="H35" s="37"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
         <v>26</v>
       </c>
@@ -1709,7 +1710,7 @@
       <c r="G36" s="21"/>
       <c r="H36" s="22"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
         <v>26</v>
       </c>
@@ -1729,7 +1730,7 @@
       <c r="G37" s="21"/>
       <c r="H37" s="22"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
         <v>26</v>
       </c>
@@ -1753,7 +1754,7 @@
       </c>
       <c r="H38" s="22"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
         <v>26</v>
       </c>
@@ -1777,7 +1778,7 @@
       </c>
       <c r="H39" s="22"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
         <v>26</v>
       </c>
@@ -1801,7 +1802,7 @@
       </c>
       <c r="H40" s="22"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
         <v>26</v>
       </c>
@@ -1825,7 +1826,7 @@
       </c>
       <c r="H41" s="22"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
         <v>26</v>
       </c>
@@ -1849,7 +1850,7 @@
       </c>
       <c r="H42" s="22"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
         <v>26</v>
       </c>
@@ -1875,7 +1876,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="51" t="s">
         <v>26</v>
       </c>
@@ -1899,7 +1900,7 @@
       </c>
       <c r="H44" s="30"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="51" t="s">
         <v>26</v>
       </c>
@@ -1923,7 +1924,7 @@
       </c>
       <c r="H45" s="30"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
         <v>26</v>
       </c>
@@ -1947,7 +1948,7 @@
       </c>
       <c r="H46" s="22"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
         <v>26</v>
       </c>
@@ -1971,7 +1972,7 @@
       </c>
       <c r="H47" s="22"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="s">
         <v>26</v>
       </c>
@@ -1995,7 +1996,7 @@
       </c>
       <c r="H48" s="22"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
         <v>26</v>
       </c>
@@ -2019,7 +2020,7 @@
       </c>
       <c r="H49" s="22"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="52" t="s">
         <v>26</v>
       </c>
@@ -2043,7 +2044,7 @@
       </c>
       <c r="H50" s="54"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
         <v>26</v>
       </c>
@@ -2069,7 +2070,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="23" t="s">
         <v>26</v>
       </c>
@@ -2095,7 +2096,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="41" t="s">
         <v>26</v>
       </c>
@@ -2115,7 +2116,7 @@
       <c r="G53" s="42"/>
       <c r="H53" s="43"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="31" t="s">
         <v>26</v>
       </c>
@@ -2135,7 +2136,7 @@
       <c r="G54" s="44"/>
       <c r="H54" s="45"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="31" t="s">
         <v>26</v>
       </c>
@@ -2159,7 +2160,7 @@
       </c>
       <c r="H55" s="45"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="31" t="s">
         <v>26</v>
       </c>
@@ -2183,7 +2184,7 @@
       </c>
       <c r="H56" s="45"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="31" t="s">
         <v>26</v>
       </c>
@@ -2207,7 +2208,7 @@
       </c>
       <c r="H57" s="45"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="31" t="s">
         <v>26</v>
       </c>
@@ -2231,7 +2232,7 @@
       </c>
       <c r="H58" s="45"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="46" t="s">
         <v>26</v>
       </c>
@@ -2255,7 +2256,7 @@
       </c>
       <c r="H59" s="48"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="17" t="s">
         <v>26</v>
       </c>
@@ -2279,7 +2280,7 @@
       </c>
       <c r="H60" s="19"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="17" t="s">
         <v>26</v>
       </c>
@@ -2305,7 +2306,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="17" t="s">
         <v>26</v>
       </c>
@@ -2331,7 +2332,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="41" t="s">
         <v>26</v>
       </c>
@@ -2351,7 +2352,7 @@
       <c r="G63" s="42"/>
       <c r="H63" s="43"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="46" t="s">
         <v>26</v>
       </c>
@@ -2371,7 +2372,7 @@
       <c r="G64" s="47"/>
       <c r="H64" s="48"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="31" t="s">
         <v>26</v>
       </c>
@@ -2391,7 +2392,7 @@
       <c r="G65" s="32"/>
       <c r="H65" s="33"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="31" t="s">
         <v>26</v>
       </c>
@@ -2411,7 +2412,7 @@
       <c r="G66" s="32"/>
       <c r="H66" s="33"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="31" t="s">
         <v>26</v>
       </c>
@@ -2435,7 +2436,7 @@
       </c>
       <c r="H67" s="33"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="31" t="s">
         <v>26</v>
       </c>
@@ -2459,7 +2460,7 @@
       </c>
       <c r="H68" s="33"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="31" t="s">
         <v>26</v>
       </c>
@@ -2483,7 +2484,7 @@
       </c>
       <c r="H69" s="33"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="31" t="s">
         <v>26</v>
       </c>
@@ -2507,7 +2508,7 @@
       </c>
       <c r="H70" s="33"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="31" t="s">
         <v>26</v>
       </c>
@@ -2531,7 +2532,7 @@
       </c>
       <c r="H71" s="33"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="31" t="s">
         <v>26</v>
       </c>
@@ -2555,7 +2556,7 @@
       </c>
       <c r="H72" s="33"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="31" t="s">
         <v>26</v>
       </c>
@@ -2581,7 +2582,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="52" t="s">
         <v>26</v>
       </c>
@@ -2603,11 +2604,9 @@
       <c r="G74" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="H74" s="54" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H74" s="54"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="55" t="s">
         <v>26</v>
       </c>
@@ -2631,7 +2630,7 @@
       </c>
       <c r="H75" s="55"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="55" t="s">
         <v>26</v>
       </c>
@@ -2655,7 +2654,7 @@
       </c>
       <c r="H76" s="55"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="55" t="s">
         <v>26</v>
       </c>
@@ -2679,7 +2678,7 @@
       </c>
       <c r="H77" s="55"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="55" t="s">
         <v>26</v>
       </c>
@@ -2703,7 +2702,7 @@
       </c>
       <c r="H78" s="55"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="55" t="s">
         <v>26</v>
       </c>
@@ -2727,7 +2726,7 @@
       </c>
       <c r="H79" s="55"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="55" t="s">
         <v>26</v>
       </c>
@@ -2751,7 +2750,7 @@
       </c>
       <c r="H80" s="55"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="55" t="s">
         <v>26</v>
       </c>
@@ -2777,7 +2776,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="55" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Added most recent runs
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC6C138-1554-4328-AD48-4E6656831DD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3495FC-0C02-4DF4-AC72-B3810C332089}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15690" yWindow="2760" windowWidth="21510" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6900" yWindow="945" windowWidth="21510" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="120">
   <si>
     <t>EEJ</t>
   </si>
@@ -375,10 +375,16 @@
     <t>2035_TM152_FBP_Plus_08</t>
   </si>
   <si>
-    <t>2050_TM152_FBP_NoProject_08</t>
-  </si>
-  <si>
     <t>2035_TM152_FBP_NoProject_08</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_PlusCrossing_10</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_Plus_09</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_Plus_10</t>
   </si>
 </sst>
 </file>
@@ -934,11 +940,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H77" sqref="H77"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1632,7 +1638,7 @@
         <v>2035</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D33" s="25" t="s">
         <v>96</v>
@@ -2066,99 +2072,101 @@
       <c r="G51" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="H51" s="19" t="s">
+      <c r="H51" s="19"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E52" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F52" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G52" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="H52" s="19"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C53" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F53" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="H53" s="19"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="24">
+        <v>2035</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="D54" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="E54" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F54" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="G54" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="H54" s="25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B52" s="24">
-        <v>2035</v>
-      </c>
-      <c r="C52" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="D52" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="E52" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F52" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="G52" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="H52" s="25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B53" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C53" s="43" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C55" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D53" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E53" s="43" t="s">
+      <c r="D55" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E55" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F53" s="43"/>
-      <c r="G53" s="42"/>
-      <c r="H53" s="43"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B54" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C54" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="D54" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E54" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F54" s="45"/>
-      <c r="G54" s="44"/>
-      <c r="H54" s="45"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B55" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C55" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="D55" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E55" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F55" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="G55" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="H55" s="45"/>
+      <c r="F55" s="43"/>
+      <c r="G55" s="42"/>
+      <c r="H55" s="43"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="31" t="s">
@@ -2168,7 +2176,7 @@
         <v>2050</v>
       </c>
       <c r="C56" s="45" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D56" s="45" t="s">
         <v>34</v>
@@ -2176,12 +2184,8 @@
       <c r="E56" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F56" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="G56" s="44" t="s">
-        <v>65</v>
-      </c>
+      <c r="F56" s="45"/>
+      <c r="G56" s="44"/>
       <c r="H56" s="45"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -2192,7 +2196,7 @@
         <v>2050</v>
       </c>
       <c r="C57" s="45" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="D57" s="45" t="s">
         <v>34</v>
@@ -2201,10 +2205,10 @@
         <v>7</v>
       </c>
       <c r="F57" s="45" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="G57" s="44" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="H57" s="45"/>
     </row>
@@ -2216,7 +2220,7 @@
         <v>2050</v>
       </c>
       <c r="C58" s="45" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="D58" s="45" t="s">
         <v>34</v>
@@ -2225,86 +2229,84 @@
         <v>7</v>
       </c>
       <c r="F58" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="G58" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="H58" s="45"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C59" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="D59" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E59" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F59" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="G59" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="H59" s="45"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B60" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C60" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="D60" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E60" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F60" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="G58" s="44" t="s">
+      <c r="G60" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="H58" s="45"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B59" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C59" s="48" t="s">
+      <c r="H60" s="45"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C61" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="D59" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E59" s="48" t="s">
+      <c r="D61" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E61" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F59" s="48" t="s">
+      <c r="F61" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="G59" s="47" t="s">
+      <c r="G61" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="H59" s="48"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B60" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C60" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="D60" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="E60" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F60" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="G60" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="H60" s="19"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B61" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C61" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="D61" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E61" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F61" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G61" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="H61" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H61" s="48"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="17" t="s">
@@ -2314,83 +2316,87 @@
         <v>2050</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="D62" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D62" s="54" t="s">
         <v>96</v>
       </c>
       <c r="E62" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F62" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="G62" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H62" s="19"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C63" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D63" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F63" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="G62" s="18" t="s">
+      <c r="G63" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="H62" s="19" t="s">
+      <c r="H63" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B63" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C63" s="43" t="s">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B64" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C64" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D63" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E63" s="43" t="s">
+      <c r="D64" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E64" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="F63" s="43"/>
-      <c r="G63" s="42"/>
-      <c r="H63" s="43"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B64" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C64" s="48" t="s">
+      <c r="F64" s="43"/>
+      <c r="G64" s="42"/>
+      <c r="H64" s="43"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B65" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C65" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="D64" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E64" s="48" t="s">
+      <c r="D65" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E65" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F64" s="48"/>
-      <c r="G64" s="47"/>
-      <c r="H64" s="48"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B65" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C65" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D65" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E65" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F65" s="33"/>
-      <c r="G65" s="32"/>
-      <c r="H65" s="33"/>
+      <c r="F65" s="48"/>
+      <c r="G65" s="47"/>
+      <c r="H65" s="48"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="31" t="s">
@@ -2400,7 +2406,7 @@
         <v>2050</v>
       </c>
       <c r="C66" s="33" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D66" s="33" t="s">
         <v>34</v>
@@ -2420,7 +2426,7 @@
         <v>2050</v>
       </c>
       <c r="C67" s="33" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D67" s="33" t="s">
         <v>34</v>
@@ -2428,12 +2434,8 @@
       <c r="E67" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F67" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G67" s="32" t="s">
-        <v>63</v>
-      </c>
+      <c r="F67" s="33"/>
+      <c r="G67" s="32"/>
       <c r="H67" s="33"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -2444,7 +2446,7 @@
         <v>2050</v>
       </c>
       <c r="C68" s="33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D68" s="33" t="s">
         <v>34</v>
@@ -2468,7 +2470,7 @@
         <v>2050</v>
       </c>
       <c r="C69" s="33" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D69" s="33" t="s">
         <v>34</v>
@@ -2477,10 +2479,10 @@
         <v>38</v>
       </c>
       <c r="F69" s="33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G69" s="32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H69" s="33"/>
     </row>
@@ -2492,7 +2494,7 @@
         <v>2050</v>
       </c>
       <c r="C70" s="33" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D70" s="33" t="s">
         <v>34</v>
@@ -2501,10 +2503,10 @@
         <v>38</v>
       </c>
       <c r="F70" s="33" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G70" s="32" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H70" s="33"/>
     </row>
@@ -2516,7 +2518,7 @@
         <v>2050</v>
       </c>
       <c r="C71" s="33" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D71" s="33" t="s">
         <v>34</v>
@@ -2525,10 +2527,10 @@
         <v>38</v>
       </c>
       <c r="F71" s="33" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G71" s="32" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H71" s="33"/>
     </row>
@@ -2540,7 +2542,7 @@
         <v>2050</v>
       </c>
       <c r="C72" s="33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D72" s="33" t="s">
         <v>34</v>
@@ -2549,10 +2551,10 @@
         <v>38</v>
       </c>
       <c r="F72" s="33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G72" s="32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H72" s="33"/>
     </row>
@@ -2564,71 +2566,71 @@
         <v>2050</v>
       </c>
       <c r="C73" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="D73" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E73" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F73" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="G73" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="H73" s="33"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C74" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="D73" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E73" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F73" s="33" t="s">
+      <c r="D74" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E74" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F74" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="G73" s="32" t="s">
+      <c r="G74" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="H73" s="33" t="s">
+      <c r="H74" s="33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B74" s="53">
-        <v>2050</v>
-      </c>
-      <c r="C74" s="54" t="s">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B75" s="53">
+        <v>2050</v>
+      </c>
+      <c r="C75" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="D74" s="54" t="s">
+      <c r="D75" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="E74" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F74" s="54" t="s">
+      <c r="E75" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F75" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="G74" s="53" t="s">
+      <c r="G75" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="H74" s="54"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B75" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C75" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="D75" s="55" t="s">
-        <v>96</v>
-      </c>
-      <c r="E75" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F75" s="55" t="s">
-        <v>86</v>
-      </c>
-      <c r="G75" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="H75" s="55"/>
+      <c r="H75" s="54"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="55" t="s">
@@ -2638,7 +2640,7 @@
         <v>2050</v>
       </c>
       <c r="C76" s="55" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D76" s="55" t="s">
         <v>96</v>
@@ -2662,7 +2664,7 @@
         <v>2050</v>
       </c>
       <c r="C77" s="55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D77" s="55" t="s">
         <v>96</v>
@@ -2686,7 +2688,7 @@
         <v>2050</v>
       </c>
       <c r="C78" s="55" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D78" s="55" t="s">
         <v>96</v>
@@ -2710,7 +2712,7 @@
         <v>2050</v>
       </c>
       <c r="C79" s="55" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D79" s="55" t="s">
         <v>96</v>
@@ -2734,7 +2736,7 @@
         <v>2050</v>
       </c>
       <c r="C80" s="55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D80" s="55" t="s">
         <v>96</v>
@@ -2742,11 +2744,11 @@
       <c r="E80" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F80" s="19" t="s">
-        <v>78</v>
+      <c r="F80" s="55" t="s">
+        <v>86</v>
       </c>
       <c r="G80" s="56" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="H80" s="55"/>
     </row>
@@ -2758,7 +2760,7 @@
         <v>2050</v>
       </c>
       <c r="C81" s="55" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D81" s="55" t="s">
         <v>96</v>
@@ -2766,15 +2768,13 @@
       <c r="E81" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F81" s="55" t="s">
-        <v>86</v>
+      <c r="F81" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="G81" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="H81" s="55" t="s">
-        <v>43</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="H81" s="55"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="55" t="s">
@@ -2784,7 +2784,7 @@
         <v>2050</v>
       </c>
       <c r="C82" s="55" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D82" s="55" t="s">
         <v>96</v>
@@ -2798,7 +2798,55 @@
       <c r="G82" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="H82" s="55" t="s">
+      <c r="H82" s="55"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B83" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C83" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="D83" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="E83" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F83" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="G83" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="H83" s="55"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B84" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C84" s="55" t="s">
+        <v>117</v>
+      </c>
+      <c r="D84" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="E84" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F84" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="G84" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="H84" s="55" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add v11 run set, demote 2020 DBP from current
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3495FC-0C02-4DF4-AC72-B3810C332089}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB897648-A177-40E7-B4D5-D2880A60FA2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="945" windowWidth="21510" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6000" yWindow="1710" windowWidth="22230" windowHeight="16890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="126">
   <si>
     <t>EEJ</t>
   </si>
@@ -228,9 +228,6 @@
     <t>"Blueprint Basic (s21)\v1.5.1\v1.5.1.2 (to 2050)"</t>
   </si>
   <si>
-    <t>"Blueprint Plus Crossing (s23)\v1.5.2"</t>
-  </si>
-  <si>
     <t>"Blueprint Basic (s21)\v1.5.1\v1.5.1.1 (only to 2035)"</t>
   </si>
   <si>
@@ -240,9 +237,6 @@
     <t>2050_TM152_DBP_PlusCrossing_05</t>
   </si>
   <si>
-    <t>"Blueprint Plus Crossing (s23)\v1.5.5"</t>
-  </si>
-  <si>
     <t>run998</t>
   </si>
   <si>
@@ -255,15 +249,9 @@
     <t>2035_TM152_DBP_Plus_07</t>
   </si>
   <si>
-    <t>"Blueprint Plus Crossing (s23)\v1.6 (all strategies)"</t>
-  </si>
-  <si>
     <t>run90</t>
   </si>
   <si>
-    <t>"Blueprint Plus Crossing (s23)\v1.7 (strategies + BASIS-hybrid)"</t>
-  </si>
-  <si>
     <t>run92</t>
   </si>
   <si>
@@ -285,9 +273,6 @@
     <t>2050_TM152_DBP_PlusCrossing_07</t>
   </si>
   <si>
-    <t>"Blueprint Plus Crossing (s23)\v1.7.1- FINAL DRAFT BLUEPRINT"</t>
-  </si>
-  <si>
     <t>run98</t>
   </si>
   <si>
@@ -385,6 +370,39 @@
   </si>
   <si>
     <t>2035_TM152_FBP_Plus_10</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_Plus_11</t>
+  </si>
+  <si>
+    <t>"Draft Blueprint runs\Blueprint Plus Crossing (s23)\v1.7.1- FINAL DRAFT BLUEPRINT"</t>
+  </si>
+  <si>
+    <t>"Draft Blueprint runs\Blueprint Plus Crossing (s23)\v1.6 (all strategies)"</t>
+  </si>
+  <si>
+    <t>"Draft Blueprint runs\Blueprint Plus Crossing (s23)\v1.7 (strategies + BASIS-hybrid)"</t>
+  </si>
+  <si>
+    <t>"Draft Blueprint runs\Blueprint Plus Crossing (s23)\v1.5.2"</t>
+  </si>
+  <si>
+    <t>"Draft Blueprint runs\Blueprint Plus Crossing (s23)\v1.5.5"</t>
+  </si>
+  <si>
+    <t>"Final Blueprint runs\Final Blueprint (s24)\BAUS v2.16 (not using)"</t>
+  </si>
+  <si>
+    <t>run261</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_NoProject_11</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_NoProject_11</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_PlusCrossing_11</t>
   </si>
 </sst>
 </file>
@@ -940,11 +958,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H84"/>
+  <dimension ref="A1:H88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -952,7 +970,7 @@
     <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="40.28515625" customWidth="1"/>
+    <col min="6" max="6" width="70.85546875" customWidth="1"/>
     <col min="7" max="7" width="15" style="34" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1394,7 +1412,7 @@
         <v>2020</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D22" s="50" t="s">
         <v>34</v>
@@ -1403,14 +1421,12 @@
         <v>7</v>
       </c>
       <c r="F22" s="50" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="G22" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="H22" s="50" t="s">
-        <v>43</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="H22" s="50"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
@@ -1440,7 +1456,7 @@
         <v>2035</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D24" s="30" t="s">
         <v>28</v>
@@ -1542,7 +1558,7 @@
         <v>2035</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D29" s="22" t="s">
         <v>34</v>
@@ -1551,10 +1567,10 @@
         <v>7</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="G29" s="21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H29" s="22"/>
     </row>
@@ -1566,7 +1582,7 @@
         <v>2035</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>34</v>
@@ -1575,10 +1591,10 @@
         <v>7</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="G30" s="21" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H30" s="22"/>
     </row>
@@ -1590,7 +1606,7 @@
         <v>2035</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D31" s="22" t="s">
         <v>34</v>
@@ -1599,10 +1615,10 @@
         <v>7</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="G31" s="21" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H31" s="22"/>
     </row>
@@ -1614,19 +1630,19 @@
         <v>2035</v>
       </c>
       <c r="C32" s="54" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D32" s="54" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E32" s="54" t="s">
         <v>7</v>
       </c>
       <c r="F32" s="54" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="G32" s="53" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H32" s="54"/>
     </row>
@@ -1637,84 +1653,90 @@
       <c r="B33" s="18">
         <v>2035</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="D33" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="E33" s="25" t="s">
+      <c r="G33" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="H33" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E34" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="G33" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="H33" s="25" t="s">
+      <c r="F34" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="G34" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="H34" s="25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="39">
-        <v>2035</v>
-      </c>
-      <c r="C34" s="40" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C35" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="40" t="s">
+      <c r="D35" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F34" s="40"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="40"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="36">
-        <v>2035</v>
-      </c>
-      <c r="C35" s="37" t="s">
+      <c r="F35" s="40"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="40"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="36">
+        <v>2035</v>
+      </c>
+      <c r="C36" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" s="37" t="s">
+      <c r="D36" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="F35" s="37"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="37"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C36" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F36" s="22"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="22"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="37"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
@@ -1724,7 +1746,7 @@
         <v>2035</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D37" s="22" t="s">
         <v>34</v>
@@ -1744,7 +1766,7 @@
         <v>2035</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D38" s="22" t="s">
         <v>34</v>
@@ -1752,12 +1774,8 @@
       <c r="E38" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F38" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="G38" s="21" t="s">
-        <v>64</v>
-      </c>
+      <c r="F38" s="22"/>
+      <c r="G38" s="21"/>
       <c r="H38" s="22"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -1768,7 +1786,7 @@
         <v>2035</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D39" s="22" t="s">
         <v>34</v>
@@ -1780,7 +1798,7 @@
         <v>67</v>
       </c>
       <c r="G39" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H39" s="22"/>
     </row>
@@ -1792,7 +1810,7 @@
         <v>2035</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="D40" s="22" t="s">
         <v>34</v>
@@ -1801,10 +1819,10 @@
         <v>38</v>
       </c>
       <c r="F40" s="22" t="s">
-        <v>71</v>
+        <v>119</v>
       </c>
       <c r="G40" s="21" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H40" s="22"/>
     </row>
@@ -1816,7 +1834,7 @@
         <v>2035</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>34</v>
@@ -1825,10 +1843,10 @@
         <v>38</v>
       </c>
       <c r="F41" s="22" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="G41" s="21" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H41" s="22"/>
     </row>
@@ -1840,7 +1858,7 @@
         <v>2035</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D42" s="22" t="s">
         <v>34</v>
@@ -1849,10 +1867,10 @@
         <v>38</v>
       </c>
       <c r="F42" s="22" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
       <c r="G42" s="21" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H42" s="22"/>
     </row>
@@ -1864,7 +1882,7 @@
         <v>2035</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="D43" s="22" t="s">
         <v>34</v>
@@ -1873,38 +1891,38 @@
         <v>38</v>
       </c>
       <c r="F43" s="22" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="G43" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="H43" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="H43" s="22"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C44" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G44" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H44" s="22" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B44" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C44" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="D44" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E44" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="F44" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="G44" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="H44" s="30"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="51" t="s">
@@ -1914,7 +1932,7 @@
         <v>2035</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D45" s="30" t="s">
         <v>34</v>
@@ -1923,36 +1941,36 @@
         <v>38</v>
       </c>
       <c r="F45" s="22" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="G45" s="29" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H45" s="30"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B46" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C46" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="D46" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E46" s="22" t="s">
+      <c r="A46" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C46" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E46" s="30" t="s">
         <v>38</v>
       </c>
       <c r="F46" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="G46" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="H46" s="22"/>
+        <v>116</v>
+      </c>
+      <c r="G46" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="H46" s="30"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
@@ -1962,7 +1980,7 @@
         <v>2035</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D47" s="22" t="s">
         <v>34</v>
@@ -1971,10 +1989,10 @@
         <v>38</v>
       </c>
       <c r="F47" s="22" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="G47" s="21" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H47" s="22"/>
     </row>
@@ -1986,7 +2004,7 @@
         <v>2035</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D48" s="22" t="s">
         <v>34</v>
@@ -1995,10 +2013,10 @@
         <v>38</v>
       </c>
       <c r="F48" s="22" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="G48" s="21" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H48" s="22"/>
     </row>
@@ -2010,7 +2028,7 @@
         <v>2035</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D49" s="22" t="s">
         <v>34</v>
@@ -2019,60 +2037,60 @@
         <v>38</v>
       </c>
       <c r="F49" s="22" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="G49" s="21" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H49" s="22"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50" s="53">
-        <v>2035</v>
-      </c>
-      <c r="C50" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="D50" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="E50" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F50" s="54" t="s">
-        <v>86</v>
-      </c>
-      <c r="G50" s="53" t="s">
-        <v>87</v>
-      </c>
-      <c r="H50" s="54"/>
+      <c r="A50" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F50" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G50" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H50" s="22"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B51" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C51" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F51" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G51" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="H51" s="19"/>
+      <c r="A51" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="53">
+        <v>2035</v>
+      </c>
+      <c r="C51" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="D51" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E51" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F51" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="G51" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="H51" s="54"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
@@ -2082,19 +2100,19 @@
         <v>2035</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E52" s="19" t="s">
         <v>38</v>
       </c>
       <c r="F52" s="19" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="G52" s="18" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H52" s="19"/>
     </row>
@@ -2106,111 +2124,117 @@
         <v>2035</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E53" s="19" t="s">
         <v>38</v>
       </c>
       <c r="F53" s="19" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="G53" s="18" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H53" s="19"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B54" s="24">
-        <v>2035</v>
-      </c>
-      <c r="C54" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="D54" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="E54" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F54" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="G54" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="H54" s="25" t="s">
+      <c r="A54" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="G54" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="H54" s="19"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C55" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F55" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="G55" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="H55" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B55" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C55" s="43" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="24">
+        <v>2035</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="D56" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E56" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F56" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="G56" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="H56" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C57" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D55" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E55" s="43" t="s">
+      <c r="D57" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E57" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F55" s="43"/>
-      <c r="G55" s="42"/>
-      <c r="H55" s="43"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B56" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C56" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="D56" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E56" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F56" s="45"/>
-      <c r="G56" s="44"/>
-      <c r="H56" s="45"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B57" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C57" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="D57" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E57" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F57" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="G57" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="H57" s="45"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="42"/>
+      <c r="H57" s="43"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="31" t="s">
@@ -2220,7 +2244,7 @@
         <v>2050</v>
       </c>
       <c r="C58" s="45" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D58" s="45" t="s">
         <v>34</v>
@@ -2228,12 +2252,8 @@
       <c r="E58" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F58" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="G58" s="44" t="s">
-        <v>65</v>
-      </c>
+      <c r="F58" s="45"/>
+      <c r="G58" s="44"/>
       <c r="H58" s="45"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -2244,7 +2264,7 @@
         <v>2050</v>
       </c>
       <c r="C59" s="45" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="D59" s="45" t="s">
         <v>34</v>
@@ -2253,10 +2273,10 @@
         <v>7</v>
       </c>
       <c r="F59" s="45" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="G59" s="44" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="H59" s="45"/>
     </row>
@@ -2268,7 +2288,7 @@
         <v>2050</v>
       </c>
       <c r="C60" s="45" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="D60" s="45" t="s">
         <v>34</v>
@@ -2277,190 +2297,200 @@
         <v>7</v>
       </c>
       <c r="F60" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="G60" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="H60" s="45"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C61" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="G60" s="44" t="s">
+      <c r="D61" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E61" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F61" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="G61" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="H61" s="45"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C62" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="H60" s="45"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B61" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C61" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="D61" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E61" s="48" t="s">
+      <c r="D62" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E62" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F61" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="G61" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="H61" s="48"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B62" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C62" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="D62" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="E62" s="19" t="s">
+      <c r="F62" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="G62" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="H62" s="45"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C63" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D63" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E63" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F62" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="G62" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="H62" s="19"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B63" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C63" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="D63" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E63" s="19" t="s">
+      <c r="F63" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="G63" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="H63" s="48"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B64" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C64" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D64" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E64" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F63" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G63" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="H63" s="19" t="s">
+      <c r="F64" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="G64" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="H64" s="19"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B65" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C65" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D65" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F65" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="G65" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H65" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B64" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C64" s="43" t="s">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B66" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C66" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="D66" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E66" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F66" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="G66" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="H66" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C67" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D64" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E64" s="43" t="s">
+      <c r="D67" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E67" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="F64" s="43"/>
-      <c r="G64" s="42"/>
-      <c r="H64" s="43"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B65" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C65" s="48" t="s">
+      <c r="F67" s="43"/>
+      <c r="G67" s="42"/>
+      <c r="H67" s="43"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C68" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="D65" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E65" s="48" t="s">
+      <c r="D68" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E68" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F65" s="48"/>
-      <c r="G65" s="47"/>
-      <c r="H65" s="48"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B66" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C66" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D66" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E66" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F66" s="33"/>
-      <c r="G66" s="32"/>
-      <c r="H66" s="33"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B67" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C67" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D67" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E67" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F67" s="33"/>
-      <c r="G67" s="32"/>
-      <c r="H67" s="33"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B68" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C68" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="D68" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E68" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F68" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G68" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="H68" s="33"/>
+      <c r="F68" s="48"/>
+      <c r="G68" s="47"/>
+      <c r="H68" s="48"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="31" t="s">
@@ -2470,7 +2500,7 @@
         <v>2050</v>
       </c>
       <c r="C69" s="33" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D69" s="33" t="s">
         <v>34</v>
@@ -2478,12 +2508,8 @@
       <c r="E69" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F69" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G69" s="32" t="s">
-        <v>63</v>
-      </c>
+      <c r="F69" s="33"/>
+      <c r="G69" s="32"/>
       <c r="H69" s="33"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -2494,7 +2520,7 @@
         <v>2050</v>
       </c>
       <c r="C70" s="33" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="D70" s="33" t="s">
         <v>34</v>
@@ -2502,12 +2528,8 @@
       <c r="E70" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F70" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="G70" s="32" t="s">
-        <v>65</v>
-      </c>
+      <c r="F70" s="33"/>
+      <c r="G70" s="32"/>
       <c r="H70" s="33"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -2518,7 +2540,7 @@
         <v>2050</v>
       </c>
       <c r="C71" s="33" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D71" s="33" t="s">
         <v>34</v>
@@ -2527,10 +2549,10 @@
         <v>38</v>
       </c>
       <c r="F71" s="33" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G71" s="32" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H71" s="33"/>
     </row>
@@ -2542,7 +2564,7 @@
         <v>2050</v>
       </c>
       <c r="C72" s="33" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="D72" s="33" t="s">
         <v>34</v>
@@ -2551,10 +2573,10 @@
         <v>38</v>
       </c>
       <c r="F72" s="33" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="G72" s="32" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="H72" s="33"/>
     </row>
@@ -2566,7 +2588,7 @@
         <v>2050</v>
       </c>
       <c r="C73" s="33" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="D73" s="33" t="s">
         <v>34</v>
@@ -2575,10 +2597,10 @@
         <v>38</v>
       </c>
       <c r="F73" s="33" t="s">
-        <v>78</v>
+        <v>119</v>
       </c>
       <c r="G73" s="32" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="H73" s="33"/>
     </row>
@@ -2590,119 +2612,119 @@
         <v>2050</v>
       </c>
       <c r="C74" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D74" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E74" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F74" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="G74" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="H74" s="33"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B75" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C75" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D75" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E75" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F75" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="G75" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="H75" s="33"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B76" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C76" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D76" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E76" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F76" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="G76" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="H76" s="33"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B77" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C77" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D77" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E77" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F77" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="G77" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="H77" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B78" s="53">
+        <v>2050</v>
+      </c>
+      <c r="C78" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D78" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="D74" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E74" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F74" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="G74" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="H74" s="33" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B75" s="53">
-        <v>2050</v>
-      </c>
-      <c r="C75" s="54" t="s">
-        <v>97</v>
-      </c>
-      <c r="D75" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="E75" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F75" s="54" t="s">
-        <v>86</v>
-      </c>
-      <c r="G75" s="53" t="s">
-        <v>87</v>
-      </c>
-      <c r="H75" s="54"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B76" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C76" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="D76" s="55" t="s">
-        <v>96</v>
-      </c>
-      <c r="E76" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F76" s="55" t="s">
-        <v>86</v>
-      </c>
-      <c r="G76" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="H76" s="55"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B77" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C77" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="D77" s="55" t="s">
-        <v>96</v>
-      </c>
-      <c r="E77" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F77" s="55" t="s">
-        <v>86</v>
-      </c>
-      <c r="G77" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="H77" s="55"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B78" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C78" s="55" t="s">
-        <v>108</v>
-      </c>
-      <c r="D78" s="55" t="s">
-        <v>96</v>
-      </c>
-      <c r="E78" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F78" s="55" t="s">
-        <v>86</v>
-      </c>
-      <c r="G78" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="H78" s="55"/>
+      <c r="E78" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F78" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="G78" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="H78" s="54"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="55" t="s">
@@ -2712,19 +2734,19 @@
         <v>2050</v>
       </c>
       <c r="C79" s="55" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D79" s="55" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E79" s="55" t="s">
         <v>38</v>
       </c>
       <c r="F79" s="55" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="G79" s="56" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H79" s="55"/>
     </row>
@@ -2736,19 +2758,19 @@
         <v>2050</v>
       </c>
       <c r="C80" s="55" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D80" s="55" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E80" s="55" t="s">
         <v>38</v>
       </c>
       <c r="F80" s="55" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="G80" s="56" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H80" s="55"/>
     </row>
@@ -2760,19 +2782,19 @@
         <v>2050</v>
       </c>
       <c r="C81" s="55" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D81" s="55" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E81" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F81" s="19" t="s">
-        <v>78</v>
+      <c r="F81" s="55" t="s">
+        <v>116</v>
       </c>
       <c r="G81" s="56" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H81" s="55"/>
     </row>
@@ -2784,19 +2806,19 @@
         <v>2050</v>
       </c>
       <c r="C82" s="55" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D82" s="55" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E82" s="55" t="s">
         <v>38</v>
       </c>
       <c r="F82" s="55" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="G82" s="56" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H82" s="55"/>
     </row>
@@ -2808,19 +2830,19 @@
         <v>2050</v>
       </c>
       <c r="C83" s="55" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D83" s="55" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E83" s="55" t="s">
         <v>38</v>
       </c>
       <c r="F83" s="55" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="G83" s="56" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H83" s="55"/>
     </row>
@@ -2832,21 +2854,119 @@
         <v>2050</v>
       </c>
       <c r="C84" s="55" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D84" s="55" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E84" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F84" s="55" t="s">
-        <v>86</v>
+      <c r="F84" s="19" t="s">
+        <v>118</v>
       </c>
       <c r="G84" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="H84" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="H84" s="55"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B85" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C85" s="55" t="s">
+        <v>107</v>
+      </c>
+      <c r="D85" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E85" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F85" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G85" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H85" s="55"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B86" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C86" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="D86" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E86" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F86" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G86" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H86" s="55"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B87" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C87" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="D87" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E87" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F87" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G87" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H87" s="55" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B88" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C88" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="D88" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E88" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F88" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="G88" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="H88" s="25" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add v12 FBP Runs
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB897648-A177-40E7-B4D5-D2880A60FA2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44928A12-00D5-49B1-A2BA-A13C88807A61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="1710" windowWidth="22230" windowHeight="16890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20400" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="130">
   <si>
     <t>EEJ</t>
   </si>
@@ -403,6 +403,18 @@
   </si>
   <si>
     <t>2050_TM152_FBP_PlusCrossing_11</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_Plus_12</t>
+  </si>
+  <si>
+    <t>"Final Blueprint runs\Final Blueprint (s24)\BAUS v2.19"</t>
+  </si>
+  <si>
+    <t>run262</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_PlusCrossing_12</t>
   </si>
 </sst>
 </file>
@@ -958,11 +970,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H88"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A78" sqref="A78"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2191,70 +2203,74 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B56" s="24">
-        <v>2035</v>
-      </c>
-      <c r="C56" s="25" t="s">
+      <c r="A56" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C56" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="D56" s="25" t="s">
+      <c r="D56" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="E56" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F56" s="25" t="s">
+      <c r="E56" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F56" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="G56" s="24" t="s">
+      <c r="G56" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="H56" s="25" t="s">
+      <c r="H56" s="19"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" s="24">
+        <v>2035</v>
+      </c>
+      <c r="C57" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D57" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E57" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F57" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="G57" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="H57" s="25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B57" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C57" s="43" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C58" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D57" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E57" s="43" t="s">
+      <c r="D58" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E58" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F57" s="43"/>
-      <c r="G57" s="42"/>
-      <c r="H57" s="43"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B58" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C58" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="D58" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E58" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F58" s="45"/>
-      <c r="G58" s="44"/>
-      <c r="H58" s="45"/>
+      <c r="F58" s="43"/>
+      <c r="G58" s="42"/>
+      <c r="H58" s="43"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="31" t="s">
@@ -2264,7 +2280,7 @@
         <v>2050</v>
       </c>
       <c r="C59" s="45" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D59" s="45" t="s">
         <v>34</v>
@@ -2272,12 +2288,8 @@
       <c r="E59" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F59" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G59" s="44" t="s">
-        <v>65</v>
-      </c>
+      <c r="F59" s="45"/>
+      <c r="G59" s="44"/>
       <c r="H59" s="45"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -2288,7 +2300,7 @@
         <v>2050</v>
       </c>
       <c r="C60" s="45" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D60" s="45" t="s">
         <v>34</v>
@@ -2312,7 +2324,7 @@
         <v>2050</v>
       </c>
       <c r="C61" s="45" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D61" s="45" t="s">
         <v>34</v>
@@ -2321,10 +2333,10 @@
         <v>7</v>
       </c>
       <c r="F61" s="45" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G61" s="44" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H61" s="45"/>
     </row>
@@ -2336,7 +2348,7 @@
         <v>2050</v>
       </c>
       <c r="C62" s="45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D62" s="45" t="s">
         <v>34</v>
@@ -2345,60 +2357,60 @@
         <v>7</v>
       </c>
       <c r="F62" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="G62" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="H62" s="45"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C63" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="D63" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E63" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F63" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="G62" s="44" t="s">
+      <c r="G63" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="H62" s="45"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B63" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C63" s="48" t="s">
+      <c r="H63" s="45"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B64" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C64" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="D63" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E63" s="48" t="s">
+      <c r="D64" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E64" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F63" s="48" t="s">
+      <c r="F64" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="G63" s="47" t="s">
+      <c r="G64" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="H63" s="48"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B64" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C64" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D64" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E64" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F64" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="G64" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="H64" s="19"/>
+      <c r="H64" s="48"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="17" t="s">
@@ -2408,23 +2420,21 @@
         <v>2050</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="D65" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D65" s="54" t="s">
         <v>91</v>
       </c>
       <c r="E65" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F65" s="19" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G65" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H65" s="19" t="s">
-        <v>43</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="H65" s="19"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="17" t="s">
@@ -2434,7 +2444,7 @@
         <v>2050</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="D66" s="19" t="s">
         <v>91</v>
@@ -2442,75 +2452,81 @@
       <c r="E66" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F66" s="25" t="s">
+      <c r="F66" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="G66" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H66" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="D67" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F67" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="G66" s="24" t="s">
+      <c r="G67" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="H66" s="25" t="s">
+      <c r="H67" s="25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B67" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C67" s="43" t="s">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C68" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D67" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E67" s="43" t="s">
+      <c r="D68" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E68" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="F67" s="43"/>
-      <c r="G67" s="42"/>
-      <c r="H67" s="43"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B68" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C68" s="48" t="s">
+      <c r="F68" s="43"/>
+      <c r="G68" s="42"/>
+      <c r="H68" s="43"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B69" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C69" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="D68" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E68" s="48" t="s">
+      <c r="D69" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E69" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F68" s="48"/>
-      <c r="G68" s="47"/>
-      <c r="H68" s="48"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B69" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C69" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D69" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E69" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F69" s="33"/>
-      <c r="G69" s="32"/>
-      <c r="H69" s="33"/>
+      <c r="F69" s="48"/>
+      <c r="G69" s="47"/>
+      <c r="H69" s="48"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="31" t="s">
@@ -2520,7 +2536,7 @@
         <v>2050</v>
       </c>
       <c r="C70" s="33" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D70" s="33" t="s">
         <v>34</v>
@@ -2540,7 +2556,7 @@
         <v>2050</v>
       </c>
       <c r="C71" s="33" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D71" s="33" t="s">
         <v>34</v>
@@ -2548,12 +2564,8 @@
       <c r="E71" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F71" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G71" s="32" t="s">
-        <v>63</v>
-      </c>
+      <c r="F71" s="33"/>
+      <c r="G71" s="32"/>
       <c r="H71" s="33"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -2564,7 +2576,7 @@
         <v>2050</v>
       </c>
       <c r="C72" s="33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D72" s="33" t="s">
         <v>34</v>
@@ -2588,7 +2600,7 @@
         <v>2050</v>
       </c>
       <c r="C73" s="33" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D73" s="33" t="s">
         <v>34</v>
@@ -2597,10 +2609,10 @@
         <v>38</v>
       </c>
       <c r="F73" s="33" t="s">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="G73" s="32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H73" s="33"/>
     </row>
@@ -2612,7 +2624,7 @@
         <v>2050</v>
       </c>
       <c r="C74" s="33" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D74" s="33" t="s">
         <v>34</v>
@@ -2621,10 +2633,10 @@
         <v>38</v>
       </c>
       <c r="F74" s="33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G74" s="32" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H74" s="33"/>
     </row>
@@ -2636,7 +2648,7 @@
         <v>2050</v>
       </c>
       <c r="C75" s="33" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D75" s="33" t="s">
         <v>34</v>
@@ -2645,10 +2657,10 @@
         <v>38</v>
       </c>
       <c r="F75" s="33" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G75" s="32" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H75" s="33"/>
     </row>
@@ -2660,7 +2672,7 @@
         <v>2050</v>
       </c>
       <c r="C76" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D76" s="33" t="s">
         <v>34</v>
@@ -2669,10 +2681,10 @@
         <v>38</v>
       </c>
       <c r="F76" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G76" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H76" s="33"/>
     </row>
@@ -2684,71 +2696,71 @@
         <v>2050</v>
       </c>
       <c r="C77" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D77" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E77" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F77" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="G77" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="H77" s="33"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B78" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C78" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="D77" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E77" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F77" s="33" t="s">
+      <c r="D78" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E78" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F78" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="G77" s="32" t="s">
+      <c r="G78" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="H77" s="33" t="s">
+      <c r="H78" s="33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B78" s="53">
-        <v>2050</v>
-      </c>
-      <c r="C78" s="54" t="s">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B79" s="53">
+        <v>2050</v>
+      </c>
+      <c r="C79" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="D78" s="54" t="s">
+      <c r="D79" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="E78" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F78" s="54" t="s">
+      <c r="E79" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F79" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G78" s="53" t="s">
+      <c r="G79" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H78" s="54"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B79" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C79" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="D79" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E79" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F79" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G79" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H79" s="55"/>
+      <c r="H79" s="54"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="55" t="s">
@@ -2758,7 +2770,7 @@
         <v>2050</v>
       </c>
       <c r="C80" s="55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D80" s="55" t="s">
         <v>91</v>
@@ -2782,7 +2794,7 @@
         <v>2050</v>
       </c>
       <c r="C81" s="55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D81" s="55" t="s">
         <v>91</v>
@@ -2806,7 +2818,7 @@
         <v>2050</v>
       </c>
       <c r="C82" s="55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D82" s="55" t="s">
         <v>91</v>
@@ -2830,7 +2842,7 @@
         <v>2050</v>
       </c>
       <c r="C83" s="55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D83" s="55" t="s">
         <v>91</v>
@@ -2854,7 +2866,7 @@
         <v>2050</v>
       </c>
       <c r="C84" s="55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D84" s="55" t="s">
         <v>91</v>
@@ -2862,11 +2874,11 @@
       <c r="E84" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F84" s="19" t="s">
-        <v>118</v>
+      <c r="F84" s="55" t="s">
+        <v>116</v>
       </c>
       <c r="G84" s="56" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H84" s="55"/>
     </row>
@@ -2878,7 +2890,7 @@
         <v>2050</v>
       </c>
       <c r="C85" s="55" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D85" s="55" t="s">
         <v>91</v>
@@ -2886,11 +2898,11 @@
       <c r="E85" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F85" s="55" t="s">
-        <v>116</v>
+      <c r="F85" s="19" t="s">
+        <v>118</v>
       </c>
       <c r="G85" s="56" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H85" s="55"/>
     </row>
@@ -2902,7 +2914,7 @@
         <v>2050</v>
       </c>
       <c r="C86" s="55" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D86" s="55" t="s">
         <v>91</v>
@@ -2926,7 +2938,7 @@
         <v>2050</v>
       </c>
       <c r="C87" s="55" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D87" s="55" t="s">
         <v>91</v>
@@ -2940,9 +2952,7 @@
       <c r="G87" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="H87" s="55" t="s">
-        <v>43</v>
-      </c>
+      <c r="H87" s="55"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="55" t="s">
@@ -2952,7 +2962,7 @@
         <v>2050</v>
       </c>
       <c r="C88" s="55" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D88" s="55" t="s">
         <v>91</v>
@@ -2960,13 +2970,63 @@
       <c r="E88" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F88" s="25" t="s">
+      <c r="F88" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G88" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H88" s="55" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B89" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C89" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="D89" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E89" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F89" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="G88" s="24" t="s">
+      <c r="G89" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="H88" s="25" t="s">
+      <c r="H89" s="55"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B90" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C90" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="D90" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E90" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F90" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="G90" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="H90" s="19" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add NoProject 14 and 2005_TM152_IPA_03_en7check
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688DB295-4B62-48E3-B441-75DE25A81EB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5595" yWindow="3060" windowWidth="32130" windowHeight="15705"/>
+    <workbookView xWindow="0" yWindow="630" windowWidth="21600" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="140">
   <si>
     <t>EEJ</t>
   </si>
@@ -429,12 +430,27 @@
   </si>
   <si>
     <t>2035_TM152_FBP_Plus_13_EN7v2_01</t>
+  </si>
+  <si>
+    <t>2005_TM152_IPA_03_en7check</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_NoProject_14</t>
+  </si>
+  <si>
+    <t>"Final Blueprint runs\Final Blueprint (s24)\BAUS v2.25"</t>
+  </si>
+  <si>
+    <t>run182</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_NoProject_14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -665,7 +681,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -983,15 +999,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H93"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H58" sqref="H58"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
@@ -1000,7 +1016,7 @@
     <col min="7" max="7" width="15" style="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1026,7 +1042,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
@@ -1046,7 +1062,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
@@ -1066,7 +1082,7 @@
       <c r="G3" s="11"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>25</v>
       </c>
@@ -1086,7 +1102,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>25</v>
       </c>
@@ -1106,7 +1122,7 @@
       <c r="G5" s="15"/>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>25</v>
       </c>
@@ -1126,7 +1142,7 @@
       <c r="G6" s="15"/>
       <c r="H6" s="16"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>25</v>
       </c>
@@ -1146,7 +1162,7 @@
       <c r="G7" s="15"/>
       <c r="H7" s="16"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>25</v>
       </c>
@@ -1166,7 +1182,7 @@
       <c r="G8" s="15"/>
       <c r="H8" s="16"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>25</v>
       </c>
@@ -1186,7 +1202,7 @@
       <c r="G9" s="15"/>
       <c r="H9" s="16"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>25</v>
       </c>
@@ -1206,7 +1222,7 @@
       <c r="G10" s="21"/>
       <c r="H10" s="22"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>25</v>
       </c>
@@ -1226,7 +1242,7 @@
       <c r="G11" s="21"/>
       <c r="H11" s="22"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>25</v>
       </c>
@@ -1246,7 +1262,7 @@
       <c r="G12" s="21"/>
       <c r="H12" s="22"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>25</v>
       </c>
@@ -1266,7 +1282,7 @@
       <c r="G13" s="21"/>
       <c r="H13" s="22"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>25</v>
       </c>
@@ -1286,7 +1302,7 @@
       <c r="G14" s="21"/>
       <c r="H14" s="22"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>25</v>
       </c>
@@ -1306,7 +1322,7 @@
       <c r="G15" s="18"/>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>25</v>
       </c>
@@ -1326,7 +1342,7 @@
       <c r="G16" s="18"/>
       <c r="H16" s="19"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>25</v>
       </c>
@@ -1346,7 +1362,7 @@
       <c r="G17" s="18"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>25</v>
       </c>
@@ -1366,7 +1382,7 @@
       <c r="G18" s="18"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>25</v>
       </c>
@@ -1386,7 +1402,7 @@
       <c r="G19" s="24"/>
       <c r="H19" s="25"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
         <v>26</v>
       </c>
@@ -1408,81 +1424,83 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A21" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="27">
+        <v>2005</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="28"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="2">
         <v>2015</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="1" t="s">
+      <c r="F22" s="1"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A22" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="49">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="49">
         <v>2020</v>
       </c>
-      <c r="C22" s="50" t="s">
+      <c r="C23" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="50" t="s">
+      <c r="D23" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="50" t="s">
+      <c r="F23" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="G22" s="49" t="s">
+      <c r="G23" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="H22" s="50"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A23" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C23" s="30" t="s">
+      <c r="H23" s="50"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C24" s="30" t="s">
         <v>32</v>
-      </c>
-      <c r="D23" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="F23" s="30"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A24" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>93</v>
       </c>
       <c r="D24" s="30" t="s">
         <v>28</v>
@@ -1492,39 +1510,39 @@
       </c>
       <c r="F24" s="30"/>
       <c r="G24" s="29"/>
-      <c r="H24" s="30" t="s">
+      <c r="H24" s="29"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="30"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A25" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C25" s="20" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C26" s="20" t="s">
         <v>41</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="22"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="22"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A26" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>44</v>
       </c>
       <c r="D26" s="22" t="s">
         <v>34</v>
@@ -1536,7 +1554,7 @@
       <c r="G26" s="21"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
         <v>26</v>
       </c>
@@ -1544,7 +1562,7 @@
         <v>2035</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27" s="22" t="s">
         <v>34</v>
@@ -1556,7 +1574,7 @@
       <c r="G27" s="21"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
         <v>26</v>
       </c>
@@ -1564,7 +1582,7 @@
         <v>2035</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>34</v>
@@ -1576,7 +1594,7 @@
       <c r="G28" s="21"/>
       <c r="H28" s="22"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
         <v>26</v>
       </c>
@@ -1584,7 +1602,7 @@
         <v>2035</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="D29" s="22" t="s">
         <v>34</v>
@@ -1592,15 +1610,11 @@
       <c r="E29" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F29" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="G29" s="21" t="s">
-        <v>74</v>
-      </c>
+      <c r="F29" s="22"/>
+      <c r="G29" s="21"/>
       <c r="H29" s="22"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
         <v>26</v>
       </c>
@@ -1608,7 +1622,7 @@
         <v>2035</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>34</v>
@@ -1617,14 +1631,14 @@
         <v>7</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G30" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H30" s="22"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
         <v>26</v>
       </c>
@@ -1632,7 +1646,7 @@
         <v>2035</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D31" s="22" t="s">
         <v>34</v>
@@ -1641,412 +1655,414 @@
         <v>7</v>
       </c>
       <c r="F31" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="G31" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H31" s="22"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G31" s="21" t="s">
+      <c r="G32" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="H31" s="22"/>
-    </row>
-    <row r="32" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="53">
-        <v>2035</v>
-      </c>
-      <c r="C32" s="54" t="s">
+      <c r="H32" s="22"/>
+    </row>
+    <row r="33" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="53">
+        <v>2035</v>
+      </c>
+      <c r="C33" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="D32" s="54" t="s">
+      <c r="D33" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="E32" s="54" t="s">
+      <c r="E33" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="54" t="s">
+      <c r="F33" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G32" s="53" t="s">
+      <c r="G33" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H32" s="54"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A33" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C33" s="19" t="s">
+      <c r="H33" s="54"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C34" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D34" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="E34" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="19" t="s">
+      <c r="F34" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="G33" s="18" t="s">
+      <c r="G34" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="H33" s="19" t="s">
+      <c r="H34" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A34" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C34" s="25" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C35" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="D34" s="25" t="s">
+      <c r="D35" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="E34" s="25" t="s">
+      <c r="E35" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="25" t="s">
+      <c r="F35" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="G34" s="24" t="s">
+      <c r="G35" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="H34" s="25" t="s">
+      <c r="H35" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A35" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="39">
-        <v>2035</v>
-      </c>
-      <c r="C35" s="40" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="G36" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H36" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C37" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D35" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" s="40" t="s">
+      <c r="D37" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F35" s="40"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="40"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A36" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="36">
-        <v>2035</v>
-      </c>
-      <c r="C36" s="37" t="s">
+      <c r="F37" s="40"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="40"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="36">
+        <v>2035</v>
+      </c>
+      <c r="C38" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="37" t="s">
+      <c r="D38" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="F36" s="37"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="37"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A37" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C37" s="22" t="s">
+      <c r="F38" s="37"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="37"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C39" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="D37" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F37" s="22"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="22"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A38" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C38" s="22" t="s">
+      <c r="D39" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F39" s="22"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="22"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C40" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F38" s="22"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="22"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A39" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C39" s="22" t="s">
+      <c r="D40" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40" s="22"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="22"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C41" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D39" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F39" s="22" t="s">
+      <c r="D41" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F41" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="G39" s="21" t="s">
+      <c r="G41" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="H39" s="22"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A40" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C40" s="22" t="s">
+      <c r="H41" s="22"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C42" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E40" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F40" s="22" t="s">
+      <c r="D42" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F42" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="G40" s="21" t="s">
+      <c r="G42" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="H40" s="22"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A41" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B41" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C41" s="22" t="s">
+      <c r="H42" s="22"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C43" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D41" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E41" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F41" s="22" t="s">
+      <c r="D43" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="G41" s="21" t="s">
+      <c r="G43" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="H41" s="22"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A42" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C42" s="22" t="s">
+      <c r="H43" s="22"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C44" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="D42" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E42" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F42" s="22" t="s">
+      <c r="D44" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="G42" s="21" t="s">
+      <c r="G44" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="H42" s="22"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A43" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C43" s="22" t="s">
+      <c r="H44" s="22"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C45" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="D43" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E43" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F43" s="22" t="s">
+      <c r="D45" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F45" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="G43" s="21" t="s">
+      <c r="G45" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="H43" s="22"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A44" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B44" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C44" s="22" t="s">
+      <c r="H45" s="22"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C46" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E44" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F44" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="G44" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="H44" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A45" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C45" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="D45" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E45" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="F45" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="G45" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="H45" s="30"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A46" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B46" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C46" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D46" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E46" s="30" t="s">
+      <c r="D46" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E46" s="22" t="s">
         <v>38</v>
       </c>
       <c r="F46" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G46" s="29" t="s">
+      <c r="G46" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="H46" s="30"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A47" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C47" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D47" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E47" s="22" t="s">
+      <c r="H46" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C47" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D47" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E47" s="30" t="s">
         <v>38</v>
       </c>
       <c r="F47" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G47" s="21" t="s">
+      <c r="G47" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H47" s="22"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A48" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B48" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C48" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="D48" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E48" s="22" t="s">
+      <c r="H47" s="30"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E48" s="30" t="s">
         <v>38</v>
       </c>
       <c r="F48" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G48" s="21" t="s">
+      <c r="G48" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H48" s="22"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H48" s="30"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
         <v>26</v>
       </c>
@@ -2054,7 +2070,7 @@
         <v>2035</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D49" s="22" t="s">
         <v>34</v>
@@ -2070,7 +2086,7 @@
       </c>
       <c r="H49" s="22"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
         <v>26</v>
       </c>
@@ -2078,7 +2094,7 @@
         <v>2035</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D50" s="22" t="s">
         <v>34</v>
@@ -2094,87 +2110,87 @@
       </c>
       <c r="H50" s="22"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A51" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B51" s="53">
-        <v>2035</v>
-      </c>
-      <c r="C51" s="54" t="s">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F51" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G51" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H51" s="22"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D52" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F52" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G52" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H52" s="22"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="53">
+        <v>2035</v>
+      </c>
+      <c r="C53" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="D51" s="54" t="s">
+      <c r="D53" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="E51" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F51" s="54" t="s">
+      <c r="E53" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F53" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G51" s="53" t="s">
+      <c r="G53" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H51" s="54"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A52" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B52" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C52" s="19" t="s">
+      <c r="H53" s="54"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C54" s="19" t="s">
         <v>98</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E52" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F52" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G52" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="H52" s="19"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A53" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B53" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C53" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="D53" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E53" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F53" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G53" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="H53" s="19"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A54" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B54" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C54" s="19" t="s">
-        <v>113</v>
       </c>
       <c r="D54" s="19" t="s">
         <v>91</v>
@@ -2190,7 +2206,7 @@
       </c>
       <c r="H54" s="19"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
         <v>26</v>
       </c>
@@ -2198,7 +2214,7 @@
         <v>2035</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D55" s="19" t="s">
         <v>91</v>
@@ -2212,11 +2228,9 @@
       <c r="G55" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="H55" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H55" s="19"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="17" t="s">
         <v>26</v>
       </c>
@@ -2224,7 +2238,7 @@
         <v>2035</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D56" s="19" t="s">
         <v>91</v>
@@ -2233,14 +2247,14 @@
         <v>38</v>
       </c>
       <c r="F56" s="19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G56" s="18" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H56" s="19"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="17" t="s">
         <v>26</v>
       </c>
@@ -2248,7 +2262,7 @@
         <v>2035</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D57" s="19" t="s">
         <v>91</v>
@@ -2257,16 +2271,16 @@
         <v>38</v>
       </c>
       <c r="F57" s="19" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="G57" s="18" t="s">
-        <v>128</v>
+        <v>82</v>
       </c>
       <c r="H57" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="17" t="s">
         <v>26</v>
       </c>
@@ -2274,7 +2288,7 @@
         <v>2035</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="D58" s="19" t="s">
         <v>91</v>
@@ -2283,114 +2297,120 @@
         <v>38</v>
       </c>
       <c r="F58" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="G58" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="H58" s="19"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C59" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="D59" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F59" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="G59" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="H59" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B60" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D60" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E60" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F60" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="G58" s="18" t="s">
+      <c r="G60" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="H58" s="19" t="s">
+      <c r="H60" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A59" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B59" s="24">
-        <v>2035</v>
-      </c>
-      <c r="C59" s="25" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" s="24">
+        <v>2035</v>
+      </c>
+      <c r="C61" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="D59" s="25" t="s">
+      <c r="D61" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="E59" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F59" s="25" t="s">
+      <c r="E61" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F61" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="G59" s="24" t="s">
+      <c r="G61" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="H59" s="25" t="s">
+      <c r="H61" s="25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A60" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B60" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C60" s="43" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C62" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D60" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E60" s="43" t="s">
+      <c r="D62" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E62" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F60" s="43"/>
-      <c r="G60" s="42"/>
-      <c r="H60" s="43"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A61" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B61" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C61" s="45" t="s">
+      <c r="F62" s="43"/>
+      <c r="G62" s="42"/>
+      <c r="H62" s="43"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C63" s="45" t="s">
         <v>53</v>
-      </c>
-      <c r="D61" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E61" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F61" s="45"/>
-      <c r="G61" s="44"/>
-      <c r="H61" s="45"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A62" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B62" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C62" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="D62" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E62" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F62" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G62" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="H62" s="45"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A63" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B63" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C63" s="45" t="s">
-        <v>68</v>
       </c>
       <c r="D63" s="45" t="s">
         <v>34</v>
@@ -2398,15 +2418,11 @@
       <c r="E63" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F63" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G63" s="44" t="s">
-        <v>65</v>
-      </c>
+      <c r="F63" s="45"/>
+      <c r="G63" s="44"/>
       <c r="H63" s="45"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="31" t="s">
         <v>26</v>
       </c>
@@ -2414,7 +2430,7 @@
         <v>2050</v>
       </c>
       <c r="C64" s="45" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D64" s="45" t="s">
         <v>34</v>
@@ -2423,14 +2439,14 @@
         <v>7</v>
       </c>
       <c r="F64" s="45" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G64" s="44" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H64" s="45"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="31" t="s">
         <v>26</v>
       </c>
@@ -2438,7 +2454,7 @@
         <v>2050</v>
       </c>
       <c r="C65" s="45" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D65" s="45" t="s">
         <v>34</v>
@@ -2447,468 +2463,470 @@
         <v>7</v>
       </c>
       <c r="F65" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="G65" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="H65" s="45"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B66" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C66" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="D66" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E66" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F66" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="G66" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="H66" s="45"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C67" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="D67" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E67" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F67" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="G65" s="44" t="s">
+      <c r="G67" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="H65" s="45"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A66" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B66" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C66" s="48" t="s">
+      <c r="H67" s="45"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C68" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="D66" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E66" s="48" t="s">
+      <c r="D68" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E68" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F66" s="48" t="s">
+      <c r="F68" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="G66" s="47" t="s">
+      <c r="G68" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="H66" s="48"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A67" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B67" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C67" s="19" t="s">
+      <c r="H68" s="48"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B69" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C69" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="D67" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E67" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F67" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="G67" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="H67" s="19"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A68" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B68" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C68" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="D68" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E68" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F68" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G68" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H68" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A69" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B69" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C69" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="D69" s="19" t="s">
+      <c r="D69" s="54" t="s">
         <v>91</v>
       </c>
       <c r="E69" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F69" s="25" t="s">
+      <c r="F69" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="G69" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="H69" s="19"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B70" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C70" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D70" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F70" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="G70" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H70" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C71" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="D71" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E71" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F71" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="G69" s="24" t="s">
+      <c r="G71" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="H69" s="25" t="s">
+      <c r="H71" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A70" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B70" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C70" s="43" t="s">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B72" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C72" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D72" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F72" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="G72" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H72" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B73" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C73" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D70" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E70" s="43" t="s">
+      <c r="D73" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E73" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="F70" s="43"/>
-      <c r="G70" s="42"/>
-      <c r="H70" s="43"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A71" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B71" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C71" s="48" t="s">
+      <c r="F73" s="43"/>
+      <c r="G73" s="42"/>
+      <c r="H73" s="43"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C74" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="D71" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E71" s="48" t="s">
+      <c r="D74" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E74" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F71" s="48"/>
-      <c r="G71" s="47"/>
-      <c r="H71" s="48"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A72" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B72" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C72" s="33" t="s">
+      <c r="F74" s="48"/>
+      <c r="G74" s="47"/>
+      <c r="H74" s="48"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B75" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C75" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="D72" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E72" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F72" s="33"/>
-      <c r="G72" s="32"/>
-      <c r="H72" s="33"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A73" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B73" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C73" s="33" t="s">
+      <c r="D75" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E75" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F75" s="33"/>
+      <c r="G75" s="32"/>
+      <c r="H75" s="33"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B76" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C76" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="D73" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E73" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F73" s="33"/>
-      <c r="G73" s="32"/>
-      <c r="H73" s="33"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A74" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B74" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C74" s="33" t="s">
+      <c r="D76" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E76" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F76" s="33"/>
+      <c r="G76" s="32"/>
+      <c r="H76" s="33"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B77" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C77" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="D74" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E74" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F74" s="33" t="s">
+      <c r="D77" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E77" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F77" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="G74" s="32" t="s">
+      <c r="G77" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="H74" s="33"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A75" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B75" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C75" s="33" t="s">
+      <c r="H77" s="33"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B78" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C78" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="D75" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E75" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F75" s="33" t="s">
+      <c r="D78" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E78" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F78" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="G75" s="32" t="s">
+      <c r="G78" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="H75" s="33"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A76" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B76" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C76" s="33" t="s">
+      <c r="H78" s="33"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B79" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C79" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="D76" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E76" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F76" s="33" t="s">
+      <c r="D79" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E79" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F79" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="G76" s="32" t="s">
+      <c r="G79" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="H76" s="33"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A77" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B77" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C77" s="33" t="s">
+      <c r="H79" s="33"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B80" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C80" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="D77" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E77" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F77" s="33" t="s">
+      <c r="D80" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E80" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F80" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="G77" s="32" t="s">
+      <c r="G80" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="H77" s="33"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A78" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B78" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C78" s="33" t="s">
+      <c r="H80" s="33"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B81" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C81" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="D78" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E78" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F78" s="33" t="s">
+      <c r="D81" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E81" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F81" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="G78" s="32" t="s">
+      <c r="G81" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="H78" s="33"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A79" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B79" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C79" s="33" t="s">
+      <c r="H81" s="33"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B82" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C82" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="D79" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E79" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F79" s="33" t="s">
+      <c r="D82" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E82" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F82" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="G79" s="32" t="s">
+      <c r="G82" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="H79" s="33"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A80" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B80" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C80" s="33" t="s">
+      <c r="H82" s="33"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B83" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C83" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="D80" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E80" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F80" s="33" t="s">
+      <c r="D83" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E83" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F83" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="G80" s="32" t="s">
+      <c r="G83" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="H80" s="33" t="s">
+      <c r="H83" s="33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A81" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B81" s="53">
-        <v>2050</v>
-      </c>
-      <c r="C81" s="54" t="s">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B84" s="53">
+        <v>2050</v>
+      </c>
+      <c r="C84" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="D81" s="54" t="s">
+      <c r="D84" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="E81" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F81" s="54" t="s">
+      <c r="E84" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F84" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G81" s="53" t="s">
+      <c r="G84" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H81" s="54"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A82" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B82" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C82" s="55" t="s">
+      <c r="H84" s="54"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B85" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C85" s="55" t="s">
         <v>101</v>
-      </c>
-      <c r="D82" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E82" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F82" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G82" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H82" s="55"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A83" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B83" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C83" s="55" t="s">
-        <v>102</v>
-      </c>
-      <c r="D83" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E83" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F83" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G83" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H83" s="55"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A84" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B84" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C84" s="55" t="s">
-        <v>103</v>
-      </c>
-      <c r="D84" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E84" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F84" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G84" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H84" s="55"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A85" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B85" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C85" s="55" t="s">
-        <v>104</v>
       </c>
       <c r="D85" s="55" t="s">
         <v>91</v>
@@ -2924,7 +2942,7 @@
       </c>
       <c r="H85" s="55"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="55" t="s">
         <v>26</v>
       </c>
@@ -2932,7 +2950,7 @@
         <v>2050</v>
       </c>
       <c r="C86" s="55" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D86" s="55" t="s">
         <v>91</v>
@@ -2948,7 +2966,7 @@
       </c>
       <c r="H86" s="55"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="55" t="s">
         <v>26</v>
       </c>
@@ -2956,7 +2974,7 @@
         <v>2050</v>
       </c>
       <c r="C87" s="55" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D87" s="55" t="s">
         <v>91</v>
@@ -2964,15 +2982,15 @@
       <c r="E87" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F87" s="19" t="s">
-        <v>118</v>
+      <c r="F87" s="55" t="s">
+        <v>116</v>
       </c>
       <c r="G87" s="56" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H87" s="55"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="55" t="s">
         <v>26</v>
       </c>
@@ -2980,7 +2998,7 @@
         <v>2050</v>
       </c>
       <c r="C88" s="55" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D88" s="55" t="s">
         <v>91</v>
@@ -2996,7 +3014,7 @@
       </c>
       <c r="H88" s="55"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="55" t="s">
         <v>26</v>
       </c>
@@ -3004,7 +3022,7 @@
         <v>2050</v>
       </c>
       <c r="C89" s="55" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D89" s="55" t="s">
         <v>91</v>
@@ -3020,7 +3038,7 @@
       </c>
       <c r="H89" s="55"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="55" t="s">
         <v>26</v>
       </c>
@@ -3028,7 +3046,7 @@
         <v>2050</v>
       </c>
       <c r="C90" s="55" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D90" s="55" t="s">
         <v>91</v>
@@ -3036,17 +3054,15 @@
       <c r="E90" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F90" s="55" t="s">
-        <v>116</v>
+      <c r="F90" s="19" t="s">
+        <v>118</v>
       </c>
       <c r="G90" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H90" s="55" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.4">
+        <v>75</v>
+      </c>
+      <c r="H90" s="55"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="55" t="s">
         <v>26</v>
       </c>
@@ -3054,7 +3070,7 @@
         <v>2050</v>
       </c>
       <c r="C91" s="55" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="D91" s="55" t="s">
         <v>91</v>
@@ -3063,14 +3079,14 @@
         <v>38</v>
       </c>
       <c r="F91" s="55" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G91" s="56" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H91" s="55"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="55" t="s">
         <v>26</v>
       </c>
@@ -3078,7 +3094,7 @@
         <v>2050</v>
       </c>
       <c r="C92" s="55" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="D92" s="55" t="s">
         <v>91</v>
@@ -3086,17 +3102,15 @@
       <c r="E92" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F92" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="G92" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="H92" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F92" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G92" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H92" s="55"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="55" t="s">
         <v>26</v>
       </c>
@@ -3104,7 +3118,7 @@
         <v>2050</v>
       </c>
       <c r="C93" s="55" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="D93" s="55" t="s">
         <v>91</v>
@@ -3112,13 +3126,89 @@
       <c r="E93" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F93" s="19" t="s">
+      <c r="F93" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G93" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H93" s="55" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B94" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C94" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="D94" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E94" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F94" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="G94" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="H94" s="55"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B95" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C95" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="D95" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E95" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F95" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="G95" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="H95" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B96" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C96" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="D96" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E96" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F96" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="G93" s="18" t="s">
+      <c r="G96" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="H93" s="19" t="s">
+      <c r="H96" s="19" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 14 series Project
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688DB295-4B62-48E3-B441-75DE25A81EB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BC11B5-A56B-45EF-A1C1-0057D188353B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="630" windowWidth="21600" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="375" yWindow="375" windowWidth="20325" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="142">
   <si>
     <t>EEJ</t>
   </si>
@@ -445,6 +445,12 @@
   </si>
   <si>
     <t>2050_TM152_FBP_NoProject_14</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_Plus_14</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_PlusCrossing_14</t>
   </si>
 </sst>
 </file>
@@ -1000,11 +1006,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H96"/>
+  <dimension ref="A1:H98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2357,70 +2363,76 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B61" s="24">
-        <v>2035</v>
-      </c>
-      <c r="C61" s="25" t="s">
+      <c r="A61" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C61" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="D61" s="25" t="s">
+      <c r="D61" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="E61" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F61" s="25" t="s">
+      <c r="E61" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F61" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="G61" s="24" t="s">
+      <c r="G61" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="H61" s="25" t="s">
+      <c r="H61" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B62" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C62" s="43" t="s">
+      <c r="A62" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="24">
+        <v>2035</v>
+      </c>
+      <c r="C62" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="D62" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E62" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F62" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="G62" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H62" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C63" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D62" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E62" s="43" t="s">
+      <c r="D63" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E63" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F62" s="43"/>
-      <c r="G62" s="42"/>
-      <c r="H62" s="43"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B63" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C63" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="D63" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E63" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F63" s="45"/>
-      <c r="G63" s="44"/>
-      <c r="H63" s="45"/>
+      <c r="F63" s="43"/>
+      <c r="G63" s="42"/>
+      <c r="H63" s="43"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="31" t="s">
@@ -2430,7 +2442,7 @@
         <v>2050</v>
       </c>
       <c r="C64" s="45" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D64" s="45" t="s">
         <v>34</v>
@@ -2438,12 +2450,8 @@
       <c r="E64" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F64" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G64" s="44" t="s">
-        <v>65</v>
-      </c>
+      <c r="F64" s="45"/>
+      <c r="G64" s="44"/>
       <c r="H64" s="45"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -2454,7 +2462,7 @@
         <v>2050</v>
       </c>
       <c r="C65" s="45" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D65" s="45" t="s">
         <v>34</v>
@@ -2478,7 +2486,7 @@
         <v>2050</v>
       </c>
       <c r="C66" s="45" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D66" s="45" t="s">
         <v>34</v>
@@ -2487,10 +2495,10 @@
         <v>7</v>
       </c>
       <c r="F66" s="45" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G66" s="44" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H66" s="45"/>
     </row>
@@ -2502,7 +2510,7 @@
         <v>2050</v>
       </c>
       <c r="C67" s="45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D67" s="45" t="s">
         <v>34</v>
@@ -2511,60 +2519,60 @@
         <v>7</v>
       </c>
       <c r="F67" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="G67" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="H67" s="45"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C68" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="D68" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E68" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F68" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="G67" s="44" t="s">
+      <c r="G68" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="H67" s="45"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B68" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C68" s="48" t="s">
+      <c r="H68" s="45"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B69" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C69" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="D68" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E68" s="48" t="s">
+      <c r="D69" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E69" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F68" s="48" t="s">
+      <c r="F69" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="G68" s="47" t="s">
+      <c r="G69" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="H68" s="48"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B69" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C69" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D69" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E69" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F69" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="G69" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="H69" s="19"/>
+      <c r="H69" s="48"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="17" t="s">
@@ -2574,23 +2582,21 @@
         <v>2050</v>
       </c>
       <c r="C70" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="D70" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D70" s="54" t="s">
         <v>91</v>
       </c>
       <c r="E70" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F70" s="19" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G70" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H70" s="19" t="s">
-        <v>43</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="H70" s="19"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="17" t="s">
@@ -2600,7 +2606,7 @@
         <v>2050</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="D71" s="19" t="s">
         <v>91</v>
@@ -2609,10 +2615,10 @@
         <v>7</v>
       </c>
       <c r="F71" s="19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G71" s="56" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H71" s="19" t="s">
         <v>43</v>
@@ -2626,7 +2632,7 @@
         <v>2050</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="D72" s="19" t="s">
         <v>91</v>
@@ -2634,75 +2640,81 @@
       <c r="E72" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F72" s="25" t="s">
+      <c r="F72" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="G72" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="H72" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B73" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C73" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D73" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E73" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F73" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="G72" s="24" t="s">
+      <c r="G73" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="H72" s="25" t="s">
+      <c r="H73" s="25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B73" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C73" s="43" t="s">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C74" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D73" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E73" s="43" t="s">
+      <c r="D74" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E74" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="F73" s="43"/>
-      <c r="G73" s="42"/>
-      <c r="H73" s="43"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B74" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C74" s="48" t="s">
+      <c r="F74" s="43"/>
+      <c r="G74" s="42"/>
+      <c r="H74" s="43"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B75" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C75" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="D74" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E74" s="48" t="s">
+      <c r="D75" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E75" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F74" s="48"/>
-      <c r="G74" s="47"/>
-      <c r="H74" s="48"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B75" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C75" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D75" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E75" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F75" s="33"/>
-      <c r="G75" s="32"/>
-      <c r="H75" s="33"/>
+      <c r="F75" s="48"/>
+      <c r="G75" s="47"/>
+      <c r="H75" s="48"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="31" t="s">
@@ -2712,7 +2724,7 @@
         <v>2050</v>
       </c>
       <c r="C76" s="33" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D76" s="33" t="s">
         <v>34</v>
@@ -2732,7 +2744,7 @@
         <v>2050</v>
       </c>
       <c r="C77" s="33" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D77" s="33" t="s">
         <v>34</v>
@@ -2740,12 +2752,8 @@
       <c r="E77" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F77" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G77" s="32" t="s">
-        <v>63</v>
-      </c>
+      <c r="F77" s="33"/>
+      <c r="G77" s="32"/>
       <c r="H77" s="33"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -2756,7 +2764,7 @@
         <v>2050</v>
       </c>
       <c r="C78" s="33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D78" s="33" t="s">
         <v>34</v>
@@ -2780,7 +2788,7 @@
         <v>2050</v>
       </c>
       <c r="C79" s="33" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D79" s="33" t="s">
         <v>34</v>
@@ -2789,10 +2797,10 @@
         <v>38</v>
       </c>
       <c r="F79" s="33" t="s">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="G79" s="32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H79" s="33"/>
     </row>
@@ -2804,7 +2812,7 @@
         <v>2050</v>
       </c>
       <c r="C80" s="33" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D80" s="33" t="s">
         <v>34</v>
@@ -2813,10 +2821,10 @@
         <v>38</v>
       </c>
       <c r="F80" s="33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G80" s="32" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H80" s="33"/>
     </row>
@@ -2828,7 +2836,7 @@
         <v>2050</v>
       </c>
       <c r="C81" s="33" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D81" s="33" t="s">
         <v>34</v>
@@ -2837,10 +2845,10 @@
         <v>38</v>
       </c>
       <c r="F81" s="33" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G81" s="32" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H81" s="33"/>
     </row>
@@ -2852,7 +2860,7 @@
         <v>2050</v>
       </c>
       <c r="C82" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D82" s="33" t="s">
         <v>34</v>
@@ -2861,10 +2869,10 @@
         <v>38</v>
       </c>
       <c r="F82" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G82" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H82" s="33"/>
     </row>
@@ -2876,71 +2884,71 @@
         <v>2050</v>
       </c>
       <c r="C83" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D83" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E83" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F83" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="G83" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="H83" s="33"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B84" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C84" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="D83" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E83" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F83" s="33" t="s">
+      <c r="D84" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E84" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F84" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="G83" s="32" t="s">
+      <c r="G84" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="H83" s="33" t="s">
+      <c r="H84" s="33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B84" s="53">
-        <v>2050</v>
-      </c>
-      <c r="C84" s="54" t="s">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B85" s="53">
+        <v>2050</v>
+      </c>
+      <c r="C85" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="D84" s="54" t="s">
+      <c r="D85" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="E84" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F84" s="54" t="s">
+      <c r="E85" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F85" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G84" s="53" t="s">
+      <c r="G85" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H84" s="54"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B85" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C85" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="D85" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E85" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F85" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G85" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H85" s="55"/>
+      <c r="H85" s="54"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="55" t="s">
@@ -2950,7 +2958,7 @@
         <v>2050</v>
       </c>
       <c r="C86" s="55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D86" s="55" t="s">
         <v>91</v>
@@ -2974,7 +2982,7 @@
         <v>2050</v>
       </c>
       <c r="C87" s="55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D87" s="55" t="s">
         <v>91</v>
@@ -2998,7 +3006,7 @@
         <v>2050</v>
       </c>
       <c r="C88" s="55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D88" s="55" t="s">
         <v>91</v>
@@ -3022,7 +3030,7 @@
         <v>2050</v>
       </c>
       <c r="C89" s="55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D89" s="55" t="s">
         <v>91</v>
@@ -3046,7 +3054,7 @@
         <v>2050</v>
       </c>
       <c r="C90" s="55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D90" s="55" t="s">
         <v>91</v>
@@ -3054,11 +3062,11 @@
       <c r="E90" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F90" s="19" t="s">
-        <v>118</v>
+      <c r="F90" s="55" t="s">
+        <v>116</v>
       </c>
       <c r="G90" s="56" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H90" s="55"/>
     </row>
@@ -3070,7 +3078,7 @@
         <v>2050</v>
       </c>
       <c r="C91" s="55" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D91" s="55" t="s">
         <v>91</v>
@@ -3078,11 +3086,11 @@
       <c r="E91" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F91" s="55" t="s">
-        <v>116</v>
+      <c r="F91" s="19" t="s">
+        <v>118</v>
       </c>
       <c r="G91" s="56" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H91" s="55"/>
     </row>
@@ -3094,7 +3102,7 @@
         <v>2050</v>
       </c>
       <c r="C92" s="55" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D92" s="55" t="s">
         <v>91</v>
@@ -3118,7 +3126,7 @@
         <v>2050</v>
       </c>
       <c r="C93" s="55" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D93" s="55" t="s">
         <v>91</v>
@@ -3132,9 +3140,7 @@
       <c r="G93" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="H93" s="55" t="s">
-        <v>43</v>
-      </c>
+      <c r="H93" s="55"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="55" t="s">
@@ -3144,7 +3150,7 @@
         <v>2050</v>
       </c>
       <c r="C94" s="55" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D94" s="55" t="s">
         <v>91</v>
@@ -3153,12 +3159,14 @@
         <v>38</v>
       </c>
       <c r="F94" s="55" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G94" s="56" t="s">
-        <v>122</v>
-      </c>
-      <c r="H94" s="55"/>
+        <v>82</v>
+      </c>
+      <c r="H94" s="55" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="55" t="s">
@@ -3168,7 +3176,7 @@
         <v>2050</v>
       </c>
       <c r="C95" s="55" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D95" s="55" t="s">
         <v>91</v>
@@ -3176,15 +3184,13 @@
       <c r="E95" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F95" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="G95" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="H95" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="F95" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="G95" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="H95" s="55"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="55" t="s">
@@ -3194,7 +3200,7 @@
         <v>2050</v>
       </c>
       <c r="C96" s="55" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D96" s="55" t="s">
         <v>91</v>
@@ -3203,12 +3209,64 @@
         <v>38</v>
       </c>
       <c r="F96" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="G96" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="H96" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B97" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C97" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="D97" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E97" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F97" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="G96" s="18" t="s">
+      <c r="G97" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="H96" s="19" t="s">
+      <c r="H97" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B98" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C98" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="D98" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E98" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F98" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="G98" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H98" s="19" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add v15 run series
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BC11B5-A56B-45EF-A1C1-0057D188353B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C8787E-3DFF-4C64-A488-49AEDAD21BCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="375" windowWidth="20325" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7275" yWindow="4335" windowWidth="21570" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="146">
   <si>
     <t>EEJ</t>
   </si>
@@ -451,6 +451,18 @@
   </si>
   <si>
     <t>2050_TM152_FBP_PlusCrossing_14</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_NoProject_15</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_Plus_15</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_NoProject_15</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_PlusCrossing_15</t>
   </si>
 </sst>
 </file>
@@ -1006,11 +1018,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H98"/>
+  <dimension ref="A1:H102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A98" sqref="A98"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1775,84 +1787,90 @@
       <c r="B36" s="18">
         <v>2035</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="D36" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E36" s="25" t="s">
+      <c r="D36" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="25" t="s">
+      <c r="F36" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="G36" s="24" t="s">
+      <c r="G36" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="H36" s="25" t="s">
+      <c r="H36" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="39">
-        <v>2035</v>
-      </c>
-      <c r="C37" s="40" t="s">
+      <c r="A37" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="G37" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H37" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C38" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D37" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="E37" s="40" t="s">
+      <c r="D38" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F37" s="40"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="40"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="36">
-        <v>2035</v>
-      </c>
-      <c r="C38" s="37" t="s">
+      <c r="F38" s="40"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="40"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="36">
+        <v>2035</v>
+      </c>
+      <c r="C39" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="D38" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" s="37" t="s">
+      <c r="D39" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="F38" s="37"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="37"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C39" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D39" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F39" s="22"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="22"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="37"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
@@ -1862,7 +1880,7 @@
         <v>2035</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D40" s="22" t="s">
         <v>34</v>
@@ -1882,7 +1900,7 @@
         <v>2035</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>34</v>
@@ -1890,12 +1908,8 @@
       <c r="E41" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F41" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="G41" s="21" t="s">
-        <v>64</v>
-      </c>
+      <c r="F41" s="22"/>
+      <c r="G41" s="21"/>
       <c r="H41" s="22"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1906,7 +1920,7 @@
         <v>2035</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D42" s="22" t="s">
         <v>34</v>
@@ -1915,10 +1929,10 @@
         <v>38</v>
       </c>
       <c r="F42" s="22" t="s">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="G42" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H42" s="22"/>
     </row>
@@ -1930,7 +1944,7 @@
         <v>2035</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D43" s="22" t="s">
         <v>34</v>
@@ -1939,10 +1953,10 @@
         <v>38</v>
       </c>
       <c r="F43" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G43" s="21" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H43" s="22"/>
     </row>
@@ -1954,7 +1968,7 @@
         <v>2035</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D44" s="22" t="s">
         <v>34</v>
@@ -1963,10 +1977,10 @@
         <v>38</v>
       </c>
       <c r="F44" s="22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G44" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H44" s="22"/>
     </row>
@@ -1978,7 +1992,7 @@
         <v>2035</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D45" s="22" t="s">
         <v>34</v>
@@ -1987,10 +2001,10 @@
         <v>38</v>
       </c>
       <c r="F45" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G45" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H45" s="22"/>
     </row>
@@ -2002,47 +2016,47 @@
         <v>2035</v>
       </c>
       <c r="C46" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F46" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="G46" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H46" s="22"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C47" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="D46" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E46" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F46" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="G46" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="H46" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C47" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="D47" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E47" s="30" t="s">
+      <c r="D47" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E47" s="22" t="s">
         <v>38</v>
       </c>
       <c r="F47" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G47" s="29" t="s">
+      <c r="G47" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="H47" s="30"/>
+      <c r="H47" s="22" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="51" t="s">
@@ -2052,7 +2066,7 @@
         <v>2035</v>
       </c>
       <c r="C48" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D48" s="30" t="s">
         <v>34</v>
@@ -2069,28 +2083,28 @@
       <c r="H48" s="30"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B49" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C49" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E49" s="22" t="s">
+      <c r="A49" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C49" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" s="30" t="s">
         <v>38</v>
       </c>
       <c r="F49" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G49" s="21" t="s">
+      <c r="G49" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H49" s="22"/>
+      <c r="H49" s="30"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
@@ -2100,7 +2114,7 @@
         <v>2035</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D50" s="22" t="s">
         <v>34</v>
@@ -2124,7 +2138,7 @@
         <v>2035</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D51" s="22" t="s">
         <v>34</v>
@@ -2148,7 +2162,7 @@
         <v>2035</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D52" s="22" t="s">
         <v>34</v>
@@ -2165,52 +2179,52 @@
       <c r="H52" s="22"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B53" s="53">
-        <v>2035</v>
-      </c>
-      <c r="C53" s="54" t="s">
+      <c r="A53" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D53" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E53" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F53" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G53" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H53" s="22"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="53">
+        <v>2035</v>
+      </c>
+      <c r="C54" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E53" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F53" s="54" t="s">
+      <c r="D54" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E54" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F54" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G53" s="53" t="s">
+      <c r="G54" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H53" s="54"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B54" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C54" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D54" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E54" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F54" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G54" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="H54" s="19"/>
+      <c r="H54" s="54"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
@@ -2220,7 +2234,7 @@
         <v>2035</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D55" s="19" t="s">
         <v>91</v>
@@ -2244,7 +2258,7 @@
         <v>2035</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D56" s="19" t="s">
         <v>91</v>
@@ -2268,7 +2282,7 @@
         <v>2035</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D57" s="19" t="s">
         <v>91</v>
@@ -2282,9 +2296,7 @@
       <c r="G57" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="H57" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H57" s="19"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="17" t="s">
@@ -2294,7 +2306,7 @@
         <v>2035</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D58" s="19" t="s">
         <v>91</v>
@@ -2303,12 +2315,14 @@
         <v>38</v>
       </c>
       <c r="F58" s="19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G58" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="H58" s="19"/>
+        <v>82</v>
+      </c>
+      <c r="H58" s="19" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="17" t="s">
@@ -2318,7 +2332,7 @@
         <v>2035</v>
       </c>
       <c r="C59" s="19" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D59" s="19" t="s">
         <v>91</v>
@@ -2327,14 +2341,12 @@
         <v>38</v>
       </c>
       <c r="F59" s="19" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="G59" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="H59" s="19" t="s">
-        <v>43</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="H59" s="19"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="17" t="s">
@@ -2344,7 +2356,7 @@
         <v>2035</v>
       </c>
       <c r="C60" s="19" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D60" s="19" t="s">
         <v>91</v>
@@ -2353,10 +2365,10 @@
         <v>38</v>
       </c>
       <c r="F60" s="19" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G60" s="18" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H60" s="19" t="s">
         <v>43</v>
@@ -2370,7 +2382,7 @@
         <v>2035</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D61" s="19" t="s">
         <v>91</v>
@@ -2389,94 +2401,102 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B62" s="24">
-        <v>2035</v>
-      </c>
-      <c r="C62" s="25" t="s">
+      <c r="A62" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C62" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F62" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="G62" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="H62" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C63" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="D62" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E62" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F62" s="25" t="s">
+      <c r="D63" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F63" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="G62" s="24" t="s">
+      <c r="G63" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="H62" s="25" t="s">
+      <c r="H63" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B63" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C63" s="43" t="s">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B64" s="24">
+        <v>2035</v>
+      </c>
+      <c r="C64" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="D64" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E64" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F64" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="G64" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H64" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B65" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C65" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D63" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E63" s="43" t="s">
+      <c r="D65" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E65" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F63" s="43"/>
-      <c r="G63" s="42"/>
-      <c r="H63" s="43"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B64" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C64" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="D64" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E64" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F64" s="45"/>
-      <c r="G64" s="44"/>
-      <c r="H64" s="45"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B65" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C65" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="D65" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E65" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F65" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G65" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="H65" s="45"/>
+      <c r="F65" s="43"/>
+      <c r="G65" s="42"/>
+      <c r="H65" s="43"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="31" t="s">
@@ -2486,7 +2506,7 @@
         <v>2050</v>
       </c>
       <c r="C66" s="45" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="D66" s="45" t="s">
         <v>34</v>
@@ -2494,12 +2514,8 @@
       <c r="E66" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F66" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G66" s="44" t="s">
-        <v>65</v>
-      </c>
+      <c r="F66" s="45"/>
+      <c r="G66" s="44"/>
       <c r="H66" s="45"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -2510,7 +2526,7 @@
         <v>2050</v>
       </c>
       <c r="C67" s="45" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D67" s="45" t="s">
         <v>34</v>
@@ -2519,10 +2535,10 @@
         <v>7</v>
       </c>
       <c r="F67" s="45" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G67" s="44" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H67" s="45"/>
     </row>
@@ -2534,7 +2550,7 @@
         <v>2050</v>
       </c>
       <c r="C68" s="45" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D68" s="45" t="s">
         <v>34</v>
@@ -2543,86 +2559,84 @@
         <v>7</v>
       </c>
       <c r="F68" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="G68" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="H68" s="45"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B69" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C69" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="D69" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E69" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F69" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="G69" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="H69" s="45"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B70" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C70" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="D70" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E70" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F70" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="G68" s="44" t="s">
+      <c r="G70" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="H68" s="45"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B69" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C69" s="48" t="s">
+      <c r="H70" s="45"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C71" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="D69" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E69" s="48" t="s">
+      <c r="D71" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E71" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F69" s="48" t="s">
+      <c r="F71" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="G69" s="47" t="s">
+      <c r="G71" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="H69" s="48"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B70" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C70" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D70" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E70" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F70" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="G70" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="H70" s="19"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B71" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C71" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="D71" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E71" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F71" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G71" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H71" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H71" s="48"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="17" t="s">
@@ -2632,23 +2646,21 @@
         <v>2050</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="D72" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D72" s="54" t="s">
         <v>91</v>
       </c>
       <c r="E72" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F72" s="19" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G72" s="56" t="s">
-        <v>122</v>
-      </c>
-      <c r="H72" s="19" t="s">
-        <v>43</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="H72" s="19"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="17" t="s">
@@ -2658,7 +2670,7 @@
         <v>2050</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>139</v>
+        <v>100</v>
       </c>
       <c r="D73" s="19" t="s">
         <v>91</v>
@@ -2666,119 +2678,133 @@
       <c r="E73" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F73" s="25" t="s">
+      <c r="F73" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="G73" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H73" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C74" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="D74" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E74" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F74" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="G74" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="H74" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B75" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C75" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D75" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E75" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F75" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="G73" s="24" t="s">
+      <c r="G75" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="H73" s="25" t="s">
+      <c r="H75" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B74" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C74" s="43" t="s">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B76" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C76" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="D76" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E76" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F76" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="G76" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H76" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B77" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C77" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D74" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E74" s="43" t="s">
+      <c r="D77" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E77" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="F74" s="43"/>
-      <c r="G74" s="42"/>
-      <c r="H74" s="43"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B75" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C75" s="48" t="s">
+      <c r="F77" s="43"/>
+      <c r="G77" s="42"/>
+      <c r="H77" s="43"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B78" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C78" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="D75" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E75" s="48" t="s">
+      <c r="D78" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E78" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F75" s="48"/>
-      <c r="G75" s="47"/>
-      <c r="H75" s="48"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B76" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C76" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D76" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E76" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F76" s="33"/>
-      <c r="G76" s="32"/>
-      <c r="H76" s="33"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B77" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C77" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D77" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E77" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F77" s="33"/>
-      <c r="G77" s="32"/>
-      <c r="H77" s="33"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B78" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C78" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="D78" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E78" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F78" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G78" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="H78" s="33"/>
+      <c r="F78" s="48"/>
+      <c r="G78" s="47"/>
+      <c r="H78" s="48"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="31" t="s">
@@ -2788,7 +2814,7 @@
         <v>2050</v>
       </c>
       <c r="C79" s="33" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D79" s="33" t="s">
         <v>34</v>
@@ -2796,12 +2822,8 @@
       <c r="E79" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F79" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G79" s="32" t="s">
-        <v>63</v>
-      </c>
+      <c r="F79" s="33"/>
+      <c r="G79" s="32"/>
       <c r="H79" s="33"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -2812,7 +2834,7 @@
         <v>2050</v>
       </c>
       <c r="C80" s="33" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="D80" s="33" t="s">
         <v>34</v>
@@ -2820,12 +2842,8 @@
       <c r="E80" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F80" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="G80" s="32" t="s">
-        <v>65</v>
-      </c>
+      <c r="F80" s="33"/>
+      <c r="G80" s="32"/>
       <c r="H80" s="33"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -2836,7 +2854,7 @@
         <v>2050</v>
       </c>
       <c r="C81" s="33" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D81" s="33" t="s">
         <v>34</v>
@@ -2845,10 +2863,10 @@
         <v>38</v>
       </c>
       <c r="F81" s="33" t="s">
-        <v>120</v>
+        <v>66</v>
       </c>
       <c r="G81" s="32" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H81" s="33"/>
     </row>
@@ -2860,7 +2878,7 @@
         <v>2050</v>
       </c>
       <c r="C82" s="33" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="D82" s="33" t="s">
         <v>34</v>
@@ -2869,10 +2887,10 @@
         <v>38</v>
       </c>
       <c r="F82" s="33" t="s">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="G82" s="32" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="H82" s="33"/>
     </row>
@@ -2884,7 +2902,7 @@
         <v>2050</v>
       </c>
       <c r="C83" s="33" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="D83" s="33" t="s">
         <v>34</v>
@@ -2893,10 +2911,10 @@
         <v>38</v>
       </c>
       <c r="F83" s="33" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G83" s="32" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="H83" s="33"/>
     </row>
@@ -2908,119 +2926,119 @@
         <v>2050</v>
       </c>
       <c r="C84" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D84" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E84" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F84" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="G84" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="H84" s="33"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B85" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C85" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D85" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E85" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F85" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="G85" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="H85" s="33"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B86" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C86" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D86" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E86" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F86" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="G86" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="H86" s="33"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B87" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C87" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="D84" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E84" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F84" s="33" t="s">
+      <c r="D87" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E87" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F87" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="G84" s="32" t="s">
+      <c r="G87" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="H84" s="33" t="s">
+      <c r="H87" s="33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B85" s="53">
-        <v>2050</v>
-      </c>
-      <c r="C85" s="54" t="s">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B88" s="53">
+        <v>2050</v>
+      </c>
+      <c r="C88" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="D85" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E85" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F85" s="54" t="s">
+      <c r="D88" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E88" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F88" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G85" s="53" t="s">
+      <c r="G88" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H85" s="54"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B86" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C86" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="D86" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E86" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F86" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G86" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H86" s="55"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B87" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C87" s="55" t="s">
-        <v>102</v>
-      </c>
-      <c r="D87" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E87" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F87" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G87" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H87" s="55"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B88" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C88" s="55" t="s">
-        <v>103</v>
-      </c>
-      <c r="D88" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E88" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F88" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G88" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H88" s="55"/>
+      <c r="H88" s="54"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="55" t="s">
@@ -3030,7 +3048,7 @@
         <v>2050</v>
       </c>
       <c r="C89" s="55" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D89" s="55" t="s">
         <v>91</v>
@@ -3054,7 +3072,7 @@
         <v>2050</v>
       </c>
       <c r="C90" s="55" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D90" s="55" t="s">
         <v>91</v>
@@ -3078,7 +3096,7 @@
         <v>2050</v>
       </c>
       <c r="C91" s="55" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D91" s="55" t="s">
         <v>91</v>
@@ -3086,11 +3104,11 @@
       <c r="E91" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F91" s="19" t="s">
-        <v>118</v>
+      <c r="F91" s="55" t="s">
+        <v>116</v>
       </c>
       <c r="G91" s="56" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H91" s="55"/>
     </row>
@@ -3102,7 +3120,7 @@
         <v>2050</v>
       </c>
       <c r="C92" s="55" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D92" s="55" t="s">
         <v>91</v>
@@ -3126,7 +3144,7 @@
         <v>2050</v>
       </c>
       <c r="C93" s="55" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D93" s="55" t="s">
         <v>91</v>
@@ -3150,7 +3168,7 @@
         <v>2050</v>
       </c>
       <c r="C94" s="55" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D94" s="55" t="s">
         <v>91</v>
@@ -3158,15 +3176,13 @@
       <c r="E94" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F94" s="55" t="s">
-        <v>116</v>
+      <c r="F94" s="19" t="s">
+        <v>118</v>
       </c>
       <c r="G94" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H94" s="55" t="s">
-        <v>43</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="H94" s="55"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="55" t="s">
@@ -3176,7 +3192,7 @@
         <v>2050</v>
       </c>
       <c r="C95" s="55" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="D95" s="55" t="s">
         <v>91</v>
@@ -3185,10 +3201,10 @@
         <v>38</v>
       </c>
       <c r="F95" s="55" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G95" s="56" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H95" s="55"/>
     </row>
@@ -3200,7 +3216,7 @@
         <v>2050</v>
       </c>
       <c r="C96" s="55" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="D96" s="55" t="s">
         <v>91</v>
@@ -3208,15 +3224,13 @@
       <c r="E96" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F96" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="G96" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="H96" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="F96" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G96" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H96" s="55"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="55" t="s">
@@ -3226,7 +3240,7 @@
         <v>2050</v>
       </c>
       <c r="C97" s="55" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="D97" s="55" t="s">
         <v>91</v>
@@ -3234,13 +3248,13 @@
       <c r="E97" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F97" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="G97" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="H97" s="19" t="s">
+      <c r="F97" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G97" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H97" s="55" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3252,21 +3266,123 @@
         <v>2050</v>
       </c>
       <c r="C98" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="D98" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E98" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F98" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="G98" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="H98" s="55"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B99" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C99" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="D99" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E99" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F99" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="G99" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="H99" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B100" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C100" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="D100" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E100" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F100" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="G100" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="H100" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B101" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C101" s="55" t="s">
         <v>141</v>
       </c>
-      <c r="D98" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E98" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F98" s="19" t="s">
+      <c r="D101" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E101" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F101" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="G98" s="24" t="s">
+      <c r="G101" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="H98" s="19" t="s">
+      <c r="H101" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B102" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C102" s="55" t="s">
+        <v>145</v>
+      </c>
+      <c r="D102" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E102" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F102" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="G102" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="H102" s="19" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove pre-15 series from current, anticipate 2050_TM152_FBP_PlusCrossing_15b
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C8787E-3DFF-4C64-A488-49AEDAD21BCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735DF67A-16D4-4FA7-A732-4E7AD7313FED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7275" yWindow="4335" windowWidth="21570" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="630" windowWidth="21570" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="147">
   <si>
     <t>EEJ</t>
   </si>
@@ -463,6 +463,9 @@
   </si>
   <si>
     <t>2050_TM152_FBP_PlusCrossing_15</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_PlusCrossing_15b</t>
   </si>
 </sst>
 </file>
@@ -1018,11 +1021,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H102"/>
+  <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C100" sqref="C100"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1750,9 +1753,7 @@
       <c r="G34" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="H34" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H34" s="19"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
@@ -1776,9 +1777,7 @@
       <c r="G35" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="H35" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H35" s="19"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
@@ -1802,9 +1801,7 @@
       <c r="G36" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="H36" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H36" s="19"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
@@ -2320,9 +2317,7 @@
       <c r="G58" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="H58" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H58" s="19"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="17" t="s">
@@ -2370,9 +2365,7 @@
       <c r="G60" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="H60" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H60" s="19"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="17" t="s">
@@ -2396,9 +2389,7 @@
       <c r="G61" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="H61" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H61" s="19"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="17" t="s">
@@ -2422,9 +2413,7 @@
       <c r="G62" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="H62" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H62" s="19"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="17" t="s">
@@ -2448,9 +2437,7 @@
       <c r="G63" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="H63" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H63" s="19"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="s">
@@ -2684,9 +2671,7 @@
       <c r="G73" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="H73" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H73" s="19"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="17" t="s">
@@ -2710,9 +2695,7 @@
       <c r="G74" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="H74" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H74" s="19"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="17" t="s">
@@ -2736,9 +2719,7 @@
       <c r="G75" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="H75" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H75" s="19"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="17" t="s">
@@ -3254,9 +3235,7 @@
       <c r="G97" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="H97" s="55" t="s">
-        <v>43</v>
-      </c>
+      <c r="H97" s="55"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="55" t="s">
@@ -3304,9 +3283,7 @@
       <c r="G99" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="H99" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H99" s="19"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="55" t="s">
@@ -3330,9 +3307,7 @@
       <c r="G100" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="H100" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H100" s="19"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="55" t="s">
@@ -3356,9 +3331,7 @@
       <c r="G101" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="H101" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H101" s="19"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="55" t="s">
@@ -3383,6 +3356,32 @@
         <v>138</v>
       </c>
       <c r="H102" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B103" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C103" s="55" t="s">
+        <v>146</v>
+      </c>
+      <c r="D103" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E103" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F103" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="G103" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="H103" s="19" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove current tag from 2005_TM152_IPA_03_en7check
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735DF67A-16D4-4FA7-A732-4E7AD7313FED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8B34C9-308F-4389-A607-27A8A4111603}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="630" windowWidth="21570" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9585" yWindow="4425" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="147">
   <si>
     <t>EEJ</t>
   </si>
@@ -1024,8 +1024,8 @@
   <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C97" sqref="C97"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1463,9 +1463,7 @@
       </c>
       <c r="F21" s="28"/>
       <c r="G21" s="27"/>
-      <c r="H21" s="28" t="s">
-        <v>43</v>
-      </c>
+      <c r="H21" s="28"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">

</xml_diff>

<commit_message>
Add v16 series runs
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8B34C9-308F-4389-A607-27A8A4111603}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700F468F-C25E-403A-BCF6-442A6E6ED572}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9585" yWindow="4425" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="152">
   <si>
     <t>EEJ</t>
   </si>
@@ -438,9 +438,6 @@
     <t>2035_TM152_FBP_NoProject_14</t>
   </si>
   <si>
-    <t>"Final Blueprint runs\Final Blueprint (s24)\BAUS v2.25"</t>
-  </si>
-  <si>
     <t>run182</t>
   </si>
   <si>
@@ -466,6 +463,24 @@
   </si>
   <si>
     <t>2050_TM152_FBP_PlusCrossing_15b</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_NoTransportProject_16</t>
+  </si>
+  <si>
+    <t>"Final Blueprint runs\Final Blueprint (s24)\BAUS v2.25 - FINAL VERSION"</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_Plus_16</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_NoTransportProject_16</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_PlusCrossing_16</t>
+  </si>
+  <si>
+    <t>2020_TM152_FBP_NoProject_16</t>
   </si>
 </sst>
 </file>
@@ -1021,11 +1036,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H103"/>
+  <dimension ref="A1:H108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1512,46 +1527,50 @@
       <c r="H23" s="50"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C24" s="30" t="s">
+      <c r="A24" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="18">
+        <v>2020</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C25" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D25" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="30" t="s">
+      <c r="E25" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="30"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="D25" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="F25" s="30"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="30" t="s">
-        <v>43</v>
-      </c>
+      <c r="F25" s="40"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
@@ -1560,18 +1579,20 @@
       <c r="B26" s="21">
         <v>2035</v>
       </c>
-      <c r="C26" s="20" t="s">
-        <v>41</v>
+      <c r="C26" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="F26" s="22"/>
       <c r="G26" s="21"/>
-      <c r="H26" s="22"/>
+      <c r="H26" s="22" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
@@ -1581,7 +1602,7 @@
         <v>2035</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D27" s="22" t="s">
         <v>34</v>
@@ -1601,7 +1622,7 @@
         <v>2035</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>34</v>
@@ -1621,7 +1642,7 @@
         <v>2035</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D29" s="22" t="s">
         <v>34</v>
@@ -1641,7 +1662,7 @@
         <v>2035</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>34</v>
@@ -1649,12 +1670,8 @@
       <c r="E30" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="G30" s="21" t="s">
-        <v>74</v>
-      </c>
+      <c r="F30" s="22"/>
+      <c r="G30" s="21"/>
       <c r="H30" s="22"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1665,7 +1682,7 @@
         <v>2035</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D31" s="22" t="s">
         <v>34</v>
@@ -1674,10 +1691,10 @@
         <v>7</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G31" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H31" s="22"/>
     </row>
@@ -1689,7 +1706,7 @@
         <v>2035</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D32" s="22" t="s">
         <v>34</v>
@@ -1698,60 +1715,60 @@
         <v>7</v>
       </c>
       <c r="F32" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="G32" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H32" s="22"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="36">
+        <v>2035</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="G32" s="21" t="s">
+      <c r="G33" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="H32" s="22"/>
-    </row>
-    <row r="33" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="53">
-        <v>2035</v>
-      </c>
-      <c r="C33" s="54" t="s">
+      <c r="H33" s="37"/>
+    </row>
+    <row r="34" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="53">
+        <v>2035</v>
+      </c>
+      <c r="C34" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E33" s="54" t="s">
+      <c r="D34" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E34" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="54" t="s">
+      <c r="F34" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G33" s="53" t="s">
+      <c r="G34" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H33" s="54"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G34" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="H34" s="19"/>
+      <c r="H34" s="54"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
@@ -1761,7 +1778,7 @@
         <v>2035</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>91</v>
@@ -1770,10 +1787,10 @@
         <v>7</v>
       </c>
       <c r="F35" s="19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H35" s="19"/>
     </row>
@@ -1785,7 +1802,7 @@
         <v>2035</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>91</v>
@@ -1794,10 +1811,10 @@
         <v>7</v>
       </c>
       <c r="F36" s="19" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="H36" s="19"/>
     </row>
@@ -1808,104 +1825,114 @@
       <c r="B37" s="18">
         <v>2035</v>
       </c>
-      <c r="C37" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="D37" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E37" s="25" t="s">
+      <c r="C37" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F37" s="25" t="s">
+      <c r="F37" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G37" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G37" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="H37" s="25" t="s">
+      <c r="H37" s="19"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H38" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="39">
-        <v>2035</v>
-      </c>
-      <c r="C38" s="40" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C39" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E39" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G39" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="H39" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C40" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D38" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" s="40" t="s">
+      <c r="D40" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F38" s="40"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="40"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="36">
-        <v>2035</v>
-      </c>
-      <c r="C39" s="37" t="s">
+      <c r="F40" s="40"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="40"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="36">
+        <v>2035</v>
+      </c>
+      <c r="C41" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E39" s="37" t="s">
+      <c r="D41" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="F39" s="37"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="37"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E40" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F40" s="22"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="22"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B41" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C41" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D41" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E41" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F41" s="22"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="22"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="37"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
@@ -1915,7 +1942,7 @@
         <v>2035</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D42" s="22" t="s">
         <v>34</v>
@@ -1923,12 +1950,8 @@
       <c r="E42" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="G42" s="21" t="s">
-        <v>64</v>
-      </c>
+      <c r="F42" s="22"/>
+      <c r="G42" s="21"/>
       <c r="H42" s="22"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1939,7 +1962,7 @@
         <v>2035</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D43" s="22" t="s">
         <v>34</v>
@@ -1947,12 +1970,8 @@
       <c r="E43" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F43" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="G43" s="21" t="s">
-        <v>65</v>
-      </c>
+      <c r="F43" s="22"/>
+      <c r="G43" s="21"/>
       <c r="H43" s="22"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1963,7 +1982,7 @@
         <v>2035</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D44" s="22" t="s">
         <v>34</v>
@@ -1972,10 +1991,10 @@
         <v>38</v>
       </c>
       <c r="F44" s="22" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="G44" s="21" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H44" s="22"/>
     </row>
@@ -1987,7 +2006,7 @@
         <v>2035</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="D45" s="22" t="s">
         <v>34</v>
@@ -1996,10 +2015,10 @@
         <v>38</v>
       </c>
       <c r="F45" s="22" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G45" s="21" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H45" s="22"/>
     </row>
@@ -2011,7 +2030,7 @@
         <v>2035</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D46" s="22" t="s">
         <v>34</v>
@@ -2020,10 +2039,10 @@
         <v>38</v>
       </c>
       <c r="F46" s="22" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G46" s="21" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H46" s="22"/>
     </row>
@@ -2035,119 +2054,119 @@
         <v>2035</v>
       </c>
       <c r="C47" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F47" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="G47" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H47" s="22"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D48" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F48" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="G48" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H48" s="22"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C49" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="D47" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E47" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F47" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="G47" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="H47" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B48" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C48" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="D48" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E48" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="F48" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="G48" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="H48" s="30"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B49" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C49" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D49" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E49" s="30" t="s">
+      <c r="D49" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" s="22" t="s">
         <v>38</v>
       </c>
       <c r="F49" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G49" s="29" t="s">
+      <c r="G49" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="H49" s="30"/>
+      <c r="H49" s="22" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D50" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E50" s="22" t="s">
+      <c r="A50" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C50" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D50" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" s="30" t="s">
         <v>38</v>
       </c>
       <c r="F50" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G50" s="21" t="s">
+      <c r="G50" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H50" s="22"/>
+      <c r="H50" s="30"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B51" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C51" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="D51" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E51" s="22" t="s">
+      <c r="A51" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C51" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D51" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" s="30" t="s">
         <v>38</v>
       </c>
       <c r="F51" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G51" s="21" t="s">
+      <c r="G51" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H51" s="22"/>
+      <c r="H51" s="30"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="s">
@@ -2157,7 +2176,7 @@
         <v>2035</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D52" s="22" t="s">
         <v>34</v>
@@ -2181,7 +2200,7 @@
         <v>2035</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D53" s="22" t="s">
         <v>34</v>
@@ -2198,76 +2217,76 @@
       <c r="H53" s="22"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B54" s="53">
-        <v>2035</v>
-      </c>
-      <c r="C54" s="54" t="s">
+      <c r="A54" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E54" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F54" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G54" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H54" s="22"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D55" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F55" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G55" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H55" s="22"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="53">
+        <v>2035</v>
+      </c>
+      <c r="C56" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="D54" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E54" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F54" s="54" t="s">
+      <c r="D56" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E56" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F56" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G54" s="53" t="s">
+      <c r="G56" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H54" s="54"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B55" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C55" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D55" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E55" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F55" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G55" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="H55" s="19"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B56" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C56" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="D56" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E56" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F56" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G56" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="H56" s="19"/>
+      <c r="H56" s="54"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="17" t="s">
@@ -2277,7 +2296,7 @@
         <v>2035</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="D57" s="19" t="s">
         <v>91</v>
@@ -2301,7 +2320,7 @@
         <v>2035</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D58" s="19" t="s">
         <v>91</v>
@@ -2325,7 +2344,7 @@
         <v>2035</v>
       </c>
       <c r="C59" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D59" s="19" t="s">
         <v>91</v>
@@ -2334,10 +2353,10 @@
         <v>38</v>
       </c>
       <c r="F59" s="19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G59" s="18" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H59" s="19"/>
     </row>
@@ -2349,7 +2368,7 @@
         <v>2035</v>
       </c>
       <c r="C60" s="19" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D60" s="19" t="s">
         <v>91</v>
@@ -2358,10 +2377,10 @@
         <v>38</v>
       </c>
       <c r="F60" s="19" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="G60" s="18" t="s">
-        <v>128</v>
+        <v>82</v>
       </c>
       <c r="H60" s="19"/>
     </row>
@@ -2373,7 +2392,7 @@
         <v>2035</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="D61" s="19" t="s">
         <v>91</v>
@@ -2382,10 +2401,10 @@
         <v>38</v>
       </c>
       <c r="F61" s="19" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="G61" s="18" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="H61" s="19"/>
     </row>
@@ -2397,7 +2416,7 @@
         <v>2035</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D62" s="19" t="s">
         <v>91</v>
@@ -2406,10 +2425,10 @@
         <v>38</v>
       </c>
       <c r="F62" s="19" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G62" s="18" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H62" s="19"/>
     </row>
@@ -2421,7 +2440,7 @@
         <v>2035</v>
       </c>
       <c r="C63" s="19" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D63" s="19" t="s">
         <v>91</v>
@@ -2430,126 +2449,132 @@
         <v>38</v>
       </c>
       <c r="F63" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="G63" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="H63" s="19"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B64" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C64" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D64" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F64" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="G64" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="H64" s="19"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B65" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C65" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D65" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F65" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G65" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G63" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="H63" s="19"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B64" s="24">
-        <v>2035</v>
-      </c>
-      <c r="C64" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="D64" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E64" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F64" s="25" t="s">
+      <c r="H65" s="19"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B66" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C66" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="D66" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E66" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F66" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G66" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G64" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="H64" s="25" t="s">
+      <c r="H66" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B65" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C65" s="43" t="s">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" s="24">
+        <v>2035</v>
+      </c>
+      <c r="C67" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="D67" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E67" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F67" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="G67" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="H67" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C68" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D65" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E65" s="43" t="s">
+      <c r="D68" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E68" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F65" s="43"/>
-      <c r="G65" s="42"/>
-      <c r="H65" s="43"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B66" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C66" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="D66" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E66" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F66" s="45"/>
-      <c r="G66" s="44"/>
-      <c r="H66" s="45"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B67" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C67" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="D67" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E67" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F67" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G67" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="H67" s="45"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B68" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C68" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="D68" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E68" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F68" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G68" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="H68" s="45"/>
+      <c r="F68" s="43"/>
+      <c r="G68" s="42"/>
+      <c r="H68" s="43"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="31" t="s">
@@ -2559,7 +2584,7 @@
         <v>2050</v>
       </c>
       <c r="C69" s="45" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="D69" s="45" t="s">
         <v>34</v>
@@ -2567,12 +2592,8 @@
       <c r="E69" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F69" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="G69" s="44" t="s">
-        <v>74</v>
-      </c>
+      <c r="F69" s="45"/>
+      <c r="G69" s="44"/>
       <c r="H69" s="45"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -2583,7 +2604,7 @@
         <v>2050</v>
       </c>
       <c r="C70" s="45" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="D70" s="45" t="s">
         <v>34</v>
@@ -2592,108 +2613,108 @@
         <v>7</v>
       </c>
       <c r="F70" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="G70" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="H70" s="45"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C71" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D71" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E71" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F71" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="G71" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="H71" s="45"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B72" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C72" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="D72" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E72" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F72" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="G72" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="H72" s="45"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B73" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C73" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="D73" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E73" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F73" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="G70" s="44" t="s">
+      <c r="G73" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="H70" s="45"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B71" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C71" s="48" t="s">
+      <c r="H73" s="45"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C74" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="D71" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E71" s="48" t="s">
+      <c r="D74" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E74" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F71" s="48" t="s">
+      <c r="F74" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="G71" s="47" t="s">
+      <c r="G74" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="H71" s="48"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B72" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C72" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D72" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E72" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F72" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="G72" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="H72" s="19"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B73" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C73" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="D73" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E73" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F73" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G73" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H73" s="19"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B74" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C74" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="D74" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E74" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F74" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="G74" s="56" t="s">
-        <v>122</v>
-      </c>
-      <c r="H74" s="19"/>
+      <c r="H74" s="48"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="17" t="s">
@@ -2703,19 +2724,19 @@
         <v>2050</v>
       </c>
       <c r="C75" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="D75" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D75" s="54" t="s">
         <v>91</v>
       </c>
       <c r="E75" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F75" s="19" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="G75" s="56" t="s">
-        <v>138</v>
+        <v>75</v>
       </c>
       <c r="H75" s="19"/>
     </row>
@@ -2727,7 +2748,7 @@
         <v>2050</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
       <c r="D76" s="19" t="s">
         <v>91</v>
@@ -2735,143 +2756,153 @@
       <c r="E76" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F76" s="25" t="s">
+      <c r="F76" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="G76" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H76" s="19"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B77" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C77" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="D77" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E77" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F77" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="G77" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="H77" s="19"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B78" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C78" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="D78" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E78" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F78" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G78" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="G76" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="H76" s="25" t="s">
+      <c r="H78" s="19"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B79" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C79" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="D79" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E79" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F79" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G79" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H79" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B77" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C77" s="43" t="s">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B80" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C80" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D80" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E80" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F80" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G80" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="H80" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B81" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C81" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D77" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E77" s="43" t="s">
+      <c r="D81" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E81" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="F77" s="43"/>
-      <c r="G77" s="42"/>
-      <c r="H77" s="43"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B78" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C78" s="48" t="s">
+      <c r="F81" s="43"/>
+      <c r="G81" s="42"/>
+      <c r="H81" s="43"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B82" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C82" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="D78" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E78" s="48" t="s">
+      <c r="D82" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E82" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F78" s="48"/>
-      <c r="G78" s="47"/>
-      <c r="H78" s="48"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B79" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C79" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D79" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E79" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F79" s="33"/>
-      <c r="G79" s="32"/>
-      <c r="H79" s="33"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B80" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C80" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D80" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E80" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F80" s="33"/>
-      <c r="G80" s="32"/>
-      <c r="H80" s="33"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B81" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C81" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="D81" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E81" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F81" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G81" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="H81" s="33"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B82" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C82" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D82" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E82" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F82" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G82" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="H82" s="33"/>
+      <c r="F82" s="48"/>
+      <c r="G82" s="47"/>
+      <c r="H82" s="48"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="31" t="s">
@@ -2881,7 +2912,7 @@
         <v>2050</v>
       </c>
       <c r="C83" s="33" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D83" s="33" t="s">
         <v>34</v>
@@ -2889,12 +2920,8 @@
       <c r="E83" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F83" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="G83" s="32" t="s">
-        <v>65</v>
-      </c>
+      <c r="F83" s="33"/>
+      <c r="G83" s="32"/>
       <c r="H83" s="33"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -2905,7 +2932,7 @@
         <v>2050</v>
       </c>
       <c r="C84" s="33" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="D84" s="33" t="s">
         <v>34</v>
@@ -2913,12 +2940,8 @@
       <c r="E84" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F84" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="G84" s="32" t="s">
-        <v>70</v>
-      </c>
+      <c r="F84" s="33"/>
+      <c r="G84" s="32"/>
       <c r="H84" s="33"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -2929,7 +2952,7 @@
         <v>2050</v>
       </c>
       <c r="C85" s="33" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="D85" s="33" t="s">
         <v>34</v>
@@ -2938,10 +2961,10 @@
         <v>38</v>
       </c>
       <c r="F85" s="33" t="s">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="G85" s="32" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="H85" s="33"/>
     </row>
@@ -2953,7 +2976,7 @@
         <v>2050</v>
       </c>
       <c r="C86" s="33" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="D86" s="33" t="s">
         <v>34</v>
@@ -2962,10 +2985,10 @@
         <v>38</v>
       </c>
       <c r="F86" s="33" t="s">
-        <v>118</v>
+        <v>66</v>
       </c>
       <c r="G86" s="32" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="H86" s="33"/>
     </row>
@@ -2977,143 +3000,143 @@
         <v>2050</v>
       </c>
       <c r="C87" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D87" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E87" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F87" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="G87" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="H87" s="33"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B88" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C88" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D88" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E88" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F88" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="G88" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="H88" s="33"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B89" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C89" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D89" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E89" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F89" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="G89" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="H89" s="33"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B90" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C90" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D90" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E90" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F90" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="G90" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="H90" s="33"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B91" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C91" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="D87" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E87" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F87" s="33" t="s">
+      <c r="D91" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E91" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F91" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="G87" s="32" t="s">
+      <c r="G91" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="H87" s="33" t="s">
+      <c r="H91" s="33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B88" s="53">
-        <v>2050</v>
-      </c>
-      <c r="C88" s="54" t="s">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B92" s="53">
+        <v>2050</v>
+      </c>
+      <c r="C92" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="D88" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E88" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F88" s="54" t="s">
+      <c r="D92" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E92" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F92" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G88" s="53" t="s">
+      <c r="G92" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H88" s="54"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B89" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C89" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="D89" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E89" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F89" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G89" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H89" s="55"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A90" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B90" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C90" s="55" t="s">
-        <v>102</v>
-      </c>
-      <c r="D90" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E90" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F90" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G90" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H90" s="55"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B91" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C91" s="55" t="s">
-        <v>103</v>
-      </c>
-      <c r="D91" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E91" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F91" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G91" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H91" s="55"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B92" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C92" s="55" t="s">
-        <v>104</v>
-      </c>
-      <c r="D92" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E92" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F92" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G92" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H92" s="55"/>
+      <c r="H92" s="54"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="55" t="s">
@@ -3123,7 +3146,7 @@
         <v>2050</v>
       </c>
       <c r="C93" s="55" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D93" s="55" t="s">
         <v>91</v>
@@ -3147,7 +3170,7 @@
         <v>2050</v>
       </c>
       <c r="C94" s="55" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D94" s="55" t="s">
         <v>91</v>
@@ -3155,11 +3178,11 @@
       <c r="E94" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F94" s="19" t="s">
-        <v>118</v>
+      <c r="F94" s="55" t="s">
+        <v>116</v>
       </c>
       <c r="G94" s="56" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H94" s="55"/>
     </row>
@@ -3171,7 +3194,7 @@
         <v>2050</v>
       </c>
       <c r="C95" s="55" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D95" s="55" t="s">
         <v>91</v>
@@ -3195,7 +3218,7 @@
         <v>2050</v>
       </c>
       <c r="C96" s="55" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D96" s="55" t="s">
         <v>91</v>
@@ -3219,7 +3242,7 @@
         <v>2050</v>
       </c>
       <c r="C97" s="55" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D97" s="55" t="s">
         <v>91</v>
@@ -3243,7 +3266,7 @@
         <v>2050</v>
       </c>
       <c r="C98" s="55" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="D98" s="55" t="s">
         <v>91</v>
@@ -3251,11 +3274,11 @@
       <c r="E98" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F98" s="55" t="s">
-        <v>121</v>
+      <c r="F98" s="19" t="s">
+        <v>118</v>
       </c>
       <c r="G98" s="56" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="H98" s="55"/>
     </row>
@@ -3267,7 +3290,7 @@
         <v>2050</v>
       </c>
       <c r="C99" s="55" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="D99" s="55" t="s">
         <v>91</v>
@@ -3275,13 +3298,13 @@
       <c r="E99" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F99" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="G99" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="H99" s="19"/>
+      <c r="F99" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G99" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H99" s="55"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="55" t="s">
@@ -3291,7 +3314,7 @@
         <v>2050</v>
       </c>
       <c r="C100" s="55" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="D100" s="55" t="s">
         <v>91</v>
@@ -3299,13 +3322,13 @@
       <c r="E100" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F100" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="G100" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="H100" s="19"/>
+      <c r="F100" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G100" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H100" s="55"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="55" t="s">
@@ -3315,7 +3338,7 @@
         <v>2050</v>
       </c>
       <c r="C101" s="55" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="D101" s="55" t="s">
         <v>91</v>
@@ -3323,13 +3346,13 @@
       <c r="E101" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F101" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="G101" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="H101" s="19"/>
+      <c r="F101" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G101" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H101" s="55"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="55" t="s">
@@ -3339,7 +3362,7 @@
         <v>2050</v>
       </c>
       <c r="C102" s="55" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="D102" s="55" t="s">
         <v>91</v>
@@ -3347,15 +3370,13 @@
       <c r="E102" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F102" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="G102" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="H102" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="F102" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="G102" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="H102" s="55"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="55" t="s">
@@ -3365,7 +3386,7 @@
         <v>2050</v>
       </c>
       <c r="C103" s="55" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="D103" s="55" t="s">
         <v>91</v>
@@ -3374,12 +3395,134 @@
         <v>38</v>
       </c>
       <c r="F103" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="G103" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="H103" s="19"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B104" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C104" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="D104" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E104" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F104" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="G104" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="H104" s="19"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B105" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C105" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="D105" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E105" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F105" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G105" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G103" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="H103" s="19" t="s">
+      <c r="H105" s="19"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B106" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C106" s="55" t="s">
+        <v>144</v>
+      </c>
+      <c r="D106" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E106" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F106" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G106" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H106" s="19"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B107" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C107" s="55" t="s">
+        <v>145</v>
+      </c>
+      <c r="D107" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E107" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F107" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G107" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H107" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B108" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C108" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="D108" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E108" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F108" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G108" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H108" s="19" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add NP17 and FBP18 runs
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700F468F-C25E-403A-BCF6-442A6E6ED572}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF3215B-4BF9-42AD-942E-758C63F55872}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9615" yWindow="345" windowWidth="26550" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="158">
   <si>
     <t>EEJ</t>
   </si>
@@ -481,6 +481,24 @@
   </si>
   <si>
     <t>2020_TM152_FBP_NoProject_16</t>
+  </si>
+  <si>
+    <t>2035_TM152_IPA_02</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_PlusCrossing_18</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_NoProject_17</t>
+  </si>
+  <si>
+    <t>"EIR runs\Baseline Large (s25) runs\NP_v3"</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_Plus_18</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_NoProject_17</t>
   </si>
 </sst>
 </file>
@@ -1036,11 +1054,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H108"/>
+  <dimension ref="A1:H113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1590,9 +1608,7 @@
       </c>
       <c r="F26" s="22"/>
       <c r="G26" s="21"/>
-      <c r="H26" s="22" t="s">
-        <v>43</v>
-      </c>
+      <c r="H26" s="22"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
@@ -1601,18 +1617,20 @@
       <c r="B27" s="21">
         <v>2035</v>
       </c>
-      <c r="C27" s="20" t="s">
-        <v>41</v>
+      <c r="C27" s="22" t="s">
+        <v>152</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="F27" s="22"/>
       <c r="G27" s="21"/>
-      <c r="H27" s="22"/>
+      <c r="H27" s="22" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
@@ -1622,7 +1640,7 @@
         <v>2035</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>34</v>
@@ -1642,7 +1660,7 @@
         <v>2035</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D29" s="22" t="s">
         <v>34</v>
@@ -1662,7 +1680,7 @@
         <v>2035</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>34</v>
@@ -1682,7 +1700,7 @@
         <v>2035</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="D31" s="22" t="s">
         <v>34</v>
@@ -1690,12 +1708,8 @@
       <c r="E31" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="G31" s="21" t="s">
-        <v>74</v>
-      </c>
+      <c r="F31" s="22"/>
+      <c r="G31" s="21"/>
       <c r="H31" s="22"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1706,7 +1720,7 @@
         <v>2035</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D32" s="22" t="s">
         <v>34</v>
@@ -1715,84 +1729,84 @@
         <v>7</v>
       </c>
       <c r="F32" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="G32" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H32" s="22"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="G32" s="21" t="s">
+      <c r="G33" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="H32" s="22"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="36">
-        <v>2035</v>
-      </c>
-      <c r="C33" s="35" t="s">
+      <c r="H33" s="22"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="36">
+        <v>2035</v>
+      </c>
+      <c r="C34" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D33" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="37" t="s">
+      <c r="D34" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="37" t="s">
+      <c r="F34" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="G33" s="36" t="s">
+      <c r="G34" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="H33" s="37"/>
-    </row>
-    <row r="34" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="53">
-        <v>2035</v>
-      </c>
-      <c r="C34" s="54" t="s">
+      <c r="H34" s="37"/>
+    </row>
+    <row r="35" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="53">
+        <v>2035</v>
+      </c>
+      <c r="C35" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="D34" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E34" s="54" t="s">
+      <c r="D35" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="54" t="s">
+      <c r="F35" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G34" s="53" t="s">
+      <c r="G35" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H34" s="54"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E35" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G35" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="H35" s="19"/>
+      <c r="H35" s="54"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
@@ -1802,7 +1816,7 @@
         <v>2035</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>91</v>
@@ -1811,10 +1825,10 @@
         <v>7</v>
       </c>
       <c r="F36" s="19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H36" s="19"/>
     </row>
@@ -1826,7 +1840,7 @@
         <v>2035</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>91</v>
@@ -1835,10 +1849,10 @@
         <v>7</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="H37" s="19"/>
     </row>
@@ -1850,7 +1864,7 @@
         <v>2035</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>91</v>
@@ -1864,9 +1878,7 @@
       <c r="G38" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H38" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H38" s="19"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
@@ -1875,104 +1887,114 @@
       <c r="B39" s="18">
         <v>2035</v>
       </c>
-      <c r="C39" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="D39" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E39" s="25" t="s">
+      <c r="C39" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E39" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F39" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="G39" s="24" t="s">
+      <c r="G39" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H39" s="25" t="s">
+      <c r="H39" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="39">
-        <v>2035</v>
-      </c>
-      <c r="C40" s="40" t="s">
+      <c r="A40" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H40" s="19"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E41" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="G41" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="H41" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C42" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="E40" s="40" t="s">
+      <c r="D42" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F40" s="40"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="40"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B41" s="36">
-        <v>2035</v>
-      </c>
-      <c r="C41" s="37" t="s">
+      <c r="F42" s="40"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="40"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" s="36">
+        <v>2035</v>
+      </c>
+      <c r="C43" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="D41" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E41" s="37" t="s">
+      <c r="D43" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="F41" s="37"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="37"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C42" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D42" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E42" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F42" s="22"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="22"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C43" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D43" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E43" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F43" s="22"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="22"/>
+      <c r="F43" s="37"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="37"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
@@ -1982,7 +2004,7 @@
         <v>2035</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D44" s="22" t="s">
         <v>34</v>
@@ -1990,12 +2012,8 @@
       <c r="E44" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F44" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="G44" s="21" t="s">
-        <v>64</v>
-      </c>
+      <c r="F44" s="22"/>
+      <c r="G44" s="21"/>
       <c r="H44" s="22"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -2006,7 +2024,7 @@
         <v>2035</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D45" s="22" t="s">
         <v>34</v>
@@ -2014,12 +2032,8 @@
       <c r="E45" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F45" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="G45" s="21" t="s">
-        <v>65</v>
-      </c>
+      <c r="F45" s="22"/>
+      <c r="G45" s="21"/>
       <c r="H45" s="22"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -2030,7 +2044,7 @@
         <v>2035</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D46" s="22" t="s">
         <v>34</v>
@@ -2039,10 +2053,10 @@
         <v>38</v>
       </c>
       <c r="F46" s="22" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="G46" s="21" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H46" s="22"/>
     </row>
@@ -2054,7 +2068,7 @@
         <v>2035</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="D47" s="22" t="s">
         <v>34</v>
@@ -2063,10 +2077,10 @@
         <v>38</v>
       </c>
       <c r="F47" s="22" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G47" s="21" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H47" s="22"/>
     </row>
@@ -2078,7 +2092,7 @@
         <v>2035</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D48" s="22" t="s">
         <v>34</v>
@@ -2087,10 +2101,10 @@
         <v>38</v>
       </c>
       <c r="F48" s="22" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G48" s="21" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H48" s="22"/>
     </row>
@@ -2102,119 +2116,119 @@
         <v>2035</v>
       </c>
       <c r="C49" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F49" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="G49" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H49" s="22"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F50" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="G50" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H50" s="22"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C51" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="D49" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E49" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F49" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="G49" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="H49" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C50" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="D50" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E50" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="F50" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="G50" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="H50" s="30"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B51" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C51" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D51" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E51" s="30" t="s">
+      <c r="D51" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" s="22" t="s">
         <v>38</v>
       </c>
       <c r="F51" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G51" s="29" t="s">
+      <c r="G51" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="H51" s="30"/>
+      <c r="H51" s="22" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B52" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C52" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D52" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E52" s="22" t="s">
+      <c r="A52" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C52" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D52" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" s="30" t="s">
         <v>38</v>
       </c>
       <c r="F52" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G52" s="21" t="s">
+      <c r="G52" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H52" s="22"/>
+      <c r="H52" s="30"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B53" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C53" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="D53" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E53" s="22" t="s">
+      <c r="A53" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C53" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D53" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E53" s="30" t="s">
         <v>38</v>
       </c>
       <c r="F53" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G53" s="21" t="s">
+      <c r="G53" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H53" s="22"/>
+      <c r="H53" s="30"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="s">
@@ -2224,7 +2238,7 @@
         <v>2035</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D54" s="22" t="s">
         <v>34</v>
@@ -2248,7 +2262,7 @@
         <v>2035</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D55" s="22" t="s">
         <v>34</v>
@@ -2265,76 +2279,76 @@
       <c r="H55" s="22"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B56" s="53">
-        <v>2035</v>
-      </c>
-      <c r="C56" s="54" t="s">
+      <c r="A56" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D56" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F56" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G56" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H56" s="22"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D57" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E57" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F57" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G57" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H57" s="22"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" s="53">
+        <v>2035</v>
+      </c>
+      <c r="C58" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="D56" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E56" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F56" s="54" t="s">
+      <c r="D58" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E58" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F58" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G56" s="53" t="s">
+      <c r="G58" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H56" s="54"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B57" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C57" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D57" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E57" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F57" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G57" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="H57" s="19"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B58" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C58" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="D58" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E58" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F58" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G58" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="H58" s="19"/>
+      <c r="H58" s="54"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="17" t="s">
@@ -2344,7 +2358,7 @@
         <v>2035</v>
       </c>
       <c r="C59" s="19" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="D59" s="19" t="s">
         <v>91</v>
@@ -2368,7 +2382,7 @@
         <v>2035</v>
       </c>
       <c r="C60" s="19" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D60" s="19" t="s">
         <v>91</v>
@@ -2392,7 +2406,7 @@
         <v>2035</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D61" s="19" t="s">
         <v>91</v>
@@ -2401,10 +2415,10 @@
         <v>38</v>
       </c>
       <c r="F61" s="19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G61" s="18" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H61" s="19"/>
     </row>
@@ -2416,7 +2430,7 @@
         <v>2035</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D62" s="19" t="s">
         <v>91</v>
@@ -2425,10 +2439,10 @@
         <v>38</v>
       </c>
       <c r="F62" s="19" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="G62" s="18" t="s">
-        <v>128</v>
+        <v>82</v>
       </c>
       <c r="H62" s="19"/>
     </row>
@@ -2440,7 +2454,7 @@
         <v>2035</v>
       </c>
       <c r="C63" s="19" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="D63" s="19" t="s">
         <v>91</v>
@@ -2449,10 +2463,10 @@
         <v>38</v>
       </c>
       <c r="F63" s="19" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="G63" s="18" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="H63" s="19"/>
     </row>
@@ -2464,7 +2478,7 @@
         <v>2035</v>
       </c>
       <c r="C64" s="19" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D64" s="19" t="s">
         <v>91</v>
@@ -2473,10 +2487,10 @@
         <v>38</v>
       </c>
       <c r="F64" s="19" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G64" s="18" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H64" s="19"/>
     </row>
@@ -2488,7 +2502,7 @@
         <v>2035</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D65" s="19" t="s">
         <v>91</v>
@@ -2497,10 +2511,10 @@
         <v>38</v>
       </c>
       <c r="F65" s="19" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G65" s="18" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H65" s="19"/>
     </row>
@@ -2512,137 +2526,141 @@
         <v>2035</v>
       </c>
       <c r="C66" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D66" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E66" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F66" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="G66" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="H66" s="19"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D67" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F67" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G67" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H67" s="19"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C68" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="D66" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E66" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F66" s="19" t="s">
+      <c r="D68" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E68" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F68" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="G66" s="18" t="s">
+      <c r="G68" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H66" s="19" t="s">
+      <c r="H68" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B67" s="24">
-        <v>2035</v>
-      </c>
-      <c r="C67" s="25" t="s">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B69" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C69" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="D67" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E67" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F67" s="25" t="s">
+      <c r="D69" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E69" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F69" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="G67" s="24" t="s">
+      <c r="G69" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H67" s="25" t="s">
+      <c r="H69" s="19"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B70" s="24">
+        <v>2035</v>
+      </c>
+      <c r="C70" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="D70" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E70" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F70" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="G70" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="H70" s="25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B68" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C68" s="43" t="s">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C71" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D68" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E68" s="43" t="s">
+      <c r="D71" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E71" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F68" s="43"/>
-      <c r="G68" s="42"/>
-      <c r="H68" s="43"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B69" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C69" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="D69" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E69" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F69" s="45"/>
-      <c r="G69" s="44"/>
-      <c r="H69" s="45"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B70" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C70" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="D70" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E70" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F70" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G70" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="H70" s="45"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B71" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C71" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="D71" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E71" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F71" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G71" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="H71" s="45"/>
+      <c r="F71" s="43"/>
+      <c r="G71" s="42"/>
+      <c r="H71" s="43"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="31" t="s">
@@ -2652,7 +2670,7 @@
         <v>2050</v>
       </c>
       <c r="C72" s="45" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="D72" s="45" t="s">
         <v>34</v>
@@ -2660,12 +2678,8 @@
       <c r="E72" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F72" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="G72" s="44" t="s">
-        <v>74</v>
-      </c>
+      <c r="F72" s="45"/>
+      <c r="G72" s="44"/>
       <c r="H72" s="45"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -2676,7 +2690,7 @@
         <v>2050</v>
       </c>
       <c r="C73" s="45" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="D73" s="45" t="s">
         <v>34</v>
@@ -2685,108 +2699,108 @@
         <v>7</v>
       </c>
       <c r="F73" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="G73" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="H73" s="45"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C74" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D74" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E74" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F74" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="G74" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="H74" s="45"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B75" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C75" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="D75" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E75" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F75" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="G75" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="H75" s="45"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B76" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C76" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="D76" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E76" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F76" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="G73" s="44" t="s">
+      <c r="G76" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="H73" s="45"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B74" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C74" s="48" t="s">
+      <c r="H76" s="45"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B77" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C77" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="D74" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E74" s="48" t="s">
+      <c r="D77" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E77" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F74" s="48" t="s">
+      <c r="F77" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="G74" s="47" t="s">
+      <c r="G77" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="H74" s="48"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B75" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C75" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D75" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E75" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F75" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="G75" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="H75" s="19"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B76" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C76" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="D76" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E76" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F76" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G76" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H76" s="19"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B77" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C77" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="D77" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E77" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F77" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="G77" s="56" t="s">
-        <v>122</v>
-      </c>
-      <c r="H77" s="19"/>
+      <c r="H77" s="48"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="17" t="s">
@@ -2796,19 +2810,19 @@
         <v>2050</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="D78" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D78" s="54" t="s">
         <v>91</v>
       </c>
       <c r="E78" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F78" s="19" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="G78" s="56" t="s">
-        <v>137</v>
+        <v>75</v>
       </c>
       <c r="H78" s="19"/>
     </row>
@@ -2820,7 +2834,7 @@
         <v>2050</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>143</v>
+        <v>100</v>
       </c>
       <c r="D79" s="19" t="s">
         <v>91</v>
@@ -2829,14 +2843,12 @@
         <v>7</v>
       </c>
       <c r="F79" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="G79" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="H79" s="19" t="s">
-        <v>43</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="G79" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H79" s="19"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="17" t="s">
@@ -2846,7 +2858,7 @@
         <v>2050</v>
       </c>
       <c r="C80" s="19" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="D80" s="19" t="s">
         <v>91</v>
@@ -2855,142 +2867,152 @@
         <v>7</v>
       </c>
       <c r="F80" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="G80" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="H80" s="19"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B81" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C81" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="D81" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E81" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F81" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="G80" s="24" t="s">
+      <c r="G81" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="H80" s="25" t="s">
+      <c r="H81" s="19"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B82" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C82" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="D82" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E82" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F82" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G82" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H82" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B81" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C81" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="D81" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E81" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="F81" s="43"/>
-      <c r="G81" s="42"/>
-      <c r="H81" s="43"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B82" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C82" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="D82" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E82" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="F82" s="48"/>
-      <c r="G82" s="47"/>
-      <c r="H82" s="48"/>
-    </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B83" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C83" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D83" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E83" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F83" s="33"/>
-      <c r="G83" s="32"/>
-      <c r="H83" s="33"/>
+      <c r="A83" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B83" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C83" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D83" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E83" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F83" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G83" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H83" s="19"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B84" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C84" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D84" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E84" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F84" s="33"/>
-      <c r="G84" s="32"/>
-      <c r="H84" s="33"/>
+      <c r="A84" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B84" s="24">
+        <v>2050</v>
+      </c>
+      <c r="C84" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="D84" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E84" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F84" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="G84" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="H84" s="25" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B85" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C85" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="D85" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E85" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F85" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G85" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="H85" s="33"/>
+      <c r="B85" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C85" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="D85" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E85" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="F85" s="45"/>
+      <c r="G85" s="44"/>
+      <c r="H85" s="45"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B86" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C86" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D86" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E86" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F86" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G86" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="H86" s="33"/>
+      <c r="A86" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B86" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C86" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="D86" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E86" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="F86" s="48"/>
+      <c r="G86" s="47"/>
+      <c r="H86" s="48"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="31" t="s">
@@ -3000,7 +3022,7 @@
         <v>2050</v>
       </c>
       <c r="C87" s="33" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D87" s="33" t="s">
         <v>34</v>
@@ -3008,12 +3030,8 @@
       <c r="E87" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F87" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="G87" s="32" t="s">
-        <v>65</v>
-      </c>
+      <c r="F87" s="33"/>
+      <c r="G87" s="32"/>
       <c r="H87" s="33"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -3024,7 +3042,7 @@
         <v>2050</v>
       </c>
       <c r="C88" s="33" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="D88" s="33" t="s">
         <v>34</v>
@@ -3032,12 +3050,8 @@
       <c r="E88" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F88" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="G88" s="32" t="s">
-        <v>70</v>
-      </c>
+      <c r="F88" s="33"/>
+      <c r="G88" s="32"/>
       <c r="H88" s="33"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -3048,7 +3062,7 @@
         <v>2050</v>
       </c>
       <c r="C89" s="33" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="D89" s="33" t="s">
         <v>34</v>
@@ -3057,10 +3071,10 @@
         <v>38</v>
       </c>
       <c r="F89" s="33" t="s">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="G89" s="32" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="H89" s="33"/>
     </row>
@@ -3072,7 +3086,7 @@
         <v>2050</v>
       </c>
       <c r="C90" s="33" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="D90" s="33" t="s">
         <v>34</v>
@@ -3081,10 +3095,10 @@
         <v>38</v>
       </c>
       <c r="F90" s="33" t="s">
-        <v>118</v>
+        <v>66</v>
       </c>
       <c r="G90" s="32" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="H90" s="33"/>
     </row>
@@ -3096,143 +3110,143 @@
         <v>2050</v>
       </c>
       <c r="C91" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D91" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E91" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F91" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="G91" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="H91" s="33"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B92" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C92" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D92" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E92" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F92" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="G92" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="H92" s="33"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B93" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C93" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D93" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E93" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F93" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="G93" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="H93" s="33"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B94" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C94" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D94" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E94" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F94" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="G94" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="H94" s="33"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B95" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C95" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="D91" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E91" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F91" s="33" t="s">
+      <c r="D95" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E95" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F95" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="G91" s="32" t="s">
+      <c r="G95" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="H91" s="33" t="s">
+      <c r="H95" s="33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B92" s="53">
-        <v>2050</v>
-      </c>
-      <c r="C92" s="54" t="s">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B96" s="53">
+        <v>2050</v>
+      </c>
+      <c r="C96" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="D92" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E92" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F92" s="54" t="s">
+      <c r="D96" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E96" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F96" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G92" s="53" t="s">
+      <c r="G96" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H92" s="54"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B93" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C93" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="D93" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E93" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F93" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G93" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H93" s="55"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B94" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C94" s="55" t="s">
-        <v>102</v>
-      </c>
-      <c r="D94" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E94" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F94" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G94" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H94" s="55"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B95" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C95" s="55" t="s">
-        <v>103</v>
-      </c>
-      <c r="D95" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E95" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F95" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G95" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H95" s="55"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B96" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C96" s="55" t="s">
-        <v>104</v>
-      </c>
-      <c r="D96" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E96" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F96" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G96" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H96" s="55"/>
+      <c r="H96" s="54"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="55" t="s">
@@ -3242,7 +3256,7 @@
         <v>2050</v>
       </c>
       <c r="C97" s="55" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D97" s="55" t="s">
         <v>91</v>
@@ -3266,7 +3280,7 @@
         <v>2050</v>
       </c>
       <c r="C98" s="55" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D98" s="55" t="s">
         <v>91</v>
@@ -3274,11 +3288,11 @@
       <c r="E98" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F98" s="19" t="s">
-        <v>118</v>
+      <c r="F98" s="55" t="s">
+        <v>116</v>
       </c>
       <c r="G98" s="56" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H98" s="55"/>
     </row>
@@ -3290,7 +3304,7 @@
         <v>2050</v>
       </c>
       <c r="C99" s="55" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D99" s="55" t="s">
         <v>91</v>
@@ -3314,7 +3328,7 @@
         <v>2050</v>
       </c>
       <c r="C100" s="55" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D100" s="55" t="s">
         <v>91</v>
@@ -3338,7 +3352,7 @@
         <v>2050</v>
       </c>
       <c r="C101" s="55" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D101" s="55" t="s">
         <v>91</v>
@@ -3362,7 +3376,7 @@
         <v>2050</v>
       </c>
       <c r="C102" s="55" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="D102" s="55" t="s">
         <v>91</v>
@@ -3370,11 +3384,11 @@
       <c r="E102" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F102" s="55" t="s">
-        <v>121</v>
+      <c r="F102" s="19" t="s">
+        <v>118</v>
       </c>
       <c r="G102" s="56" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="H102" s="55"/>
     </row>
@@ -3386,7 +3400,7 @@
         <v>2050</v>
       </c>
       <c r="C103" s="55" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="D103" s="55" t="s">
         <v>91</v>
@@ -3394,13 +3408,13 @@
       <c r="E103" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F103" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="G103" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="H103" s="19"/>
+      <c r="F103" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G103" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H103" s="55"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="55" t="s">
@@ -3410,7 +3424,7 @@
         <v>2050</v>
       </c>
       <c r="C104" s="55" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="D104" s="55" t="s">
         <v>91</v>
@@ -3418,13 +3432,13 @@
       <c r="E104" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F104" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="G104" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="H104" s="19"/>
+      <c r="F104" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G104" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H104" s="55"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="55" t="s">
@@ -3434,7 +3448,7 @@
         <v>2050</v>
       </c>
       <c r="C105" s="55" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="D105" s="55" t="s">
         <v>91</v>
@@ -3442,13 +3456,13 @@
       <c r="E105" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F105" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="G105" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="H105" s="19"/>
+      <c r="F105" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G105" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H105" s="55"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="55" t="s">
@@ -3458,7 +3472,7 @@
         <v>2050</v>
       </c>
       <c r="C106" s="55" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="D106" s="55" t="s">
         <v>91</v>
@@ -3466,13 +3480,13 @@
       <c r="E106" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F106" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="G106" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="H106" s="19"/>
+      <c r="F106" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="G106" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="H106" s="55"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="55" t="s">
@@ -3482,7 +3496,7 @@
         <v>2050</v>
       </c>
       <c r="C107" s="55" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="D107" s="55" t="s">
         <v>91</v>
@@ -3491,14 +3505,12 @@
         <v>38</v>
       </c>
       <c r="F107" s="19" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="G107" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="H107" s="19" t="s">
-        <v>43</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="H107" s="19"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="55" t="s">
@@ -3508,21 +3520,143 @@
         <v>2050</v>
       </c>
       <c r="C108" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="D108" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E108" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F108" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="G108" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="H108" s="19"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B109" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C109" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="D109" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E109" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F109" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G109" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H109" s="19"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B110" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C110" s="55" t="s">
+        <v>144</v>
+      </c>
+      <c r="D110" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E110" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F110" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G110" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H110" s="19"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B111" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C111" s="55" t="s">
+        <v>145</v>
+      </c>
+      <c r="D111" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E111" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F111" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G111" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H111" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B112" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C112" s="55" t="s">
         <v>150</v>
       </c>
-      <c r="D108" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E108" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F108" s="19" t="s">
+      <c r="D112" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E112" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F112" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="G108" s="18" t="s">
+      <c r="G112" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H108" s="19" t="s">
+      <c r="H112" s="19"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B113" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C113" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="D113" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E113" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F113" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G113" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H113" s="19" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add FBP19, NoProject20, IPA3
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF3215B-4BF9-42AD-942E-758C63F55872}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11047A85-0E23-4553-A2E6-0DE02E2844AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9615" yWindow="345" windowWidth="26550" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6090" yWindow="1455" windowWidth="20595" windowHeight="15645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="165">
   <si>
     <t>EEJ</t>
   </si>
@@ -499,6 +499,27 @@
   </si>
   <si>
     <t>2035_TM152_FBP_NoProject_17</t>
+  </si>
+  <si>
+    <t>2035_TM152_IPA_03</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_NoProject_20</t>
+  </si>
+  <si>
+    <t>"EIR runs\Baseline Large (s25) runs\NP_v7"</t>
+  </si>
+  <si>
+    <t>run310</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_NoProject_20</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_Plus_19</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_PlusCrossing_19</t>
   </si>
 </sst>
 </file>
@@ -1054,11 +1075,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H113"/>
+  <dimension ref="A1:H118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1639,38 +1660,40 @@
       <c r="B28" s="21">
         <v>2035</v>
       </c>
-      <c r="C28" s="20" t="s">
-        <v>41</v>
+      <c r="C28" s="22" t="s">
+        <v>158</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="F28" s="22"/>
       <c r="G28" s="21"/>
-      <c r="H28" s="22"/>
+      <c r="H28" s="22" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" s="22" t="s">
+      <c r="A29" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C29" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F29" s="22"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="22"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="40"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
@@ -1680,7 +1703,7 @@
         <v>2035</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>34</v>
@@ -1700,7 +1723,7 @@
         <v>2035</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D31" s="22" t="s">
         <v>34</v>
@@ -1720,7 +1743,7 @@
         <v>2035</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="D32" s="22" t="s">
         <v>34</v>
@@ -1728,12 +1751,8 @@
       <c r="E32" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="G32" s="21" t="s">
-        <v>74</v>
-      </c>
+      <c r="F32" s="22"/>
+      <c r="G32" s="21"/>
       <c r="H32" s="22"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1744,7 +1763,7 @@
         <v>2035</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D33" s="22" t="s">
         <v>34</v>
@@ -1753,84 +1772,84 @@
         <v>7</v>
       </c>
       <c r="F33" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="G33" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H33" s="22"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="G33" s="21" t="s">
+      <c r="G34" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="H33" s="22"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="36">
-        <v>2035</v>
-      </c>
-      <c r="C34" s="35" t="s">
+      <c r="H34" s="22"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="36">
+        <v>2035</v>
+      </c>
+      <c r="C35" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D34" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="37" t="s">
+      <c r="D35" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="37" t="s">
+      <c r="F35" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="G34" s="36" t="s">
+      <c r="G35" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="H34" s="37"/>
-    </row>
-    <row r="35" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="53">
-        <v>2035</v>
-      </c>
-      <c r="C35" s="54" t="s">
+      <c r="H35" s="37"/>
+    </row>
+    <row r="36" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="53">
+        <v>2035</v>
+      </c>
+      <c r="C36" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="D35" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E35" s="54" t="s">
+      <c r="D36" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="54" t="s">
+      <c r="F36" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G35" s="53" t="s">
+      <c r="G36" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="54"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G36" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="H36" s="19"/>
+      <c r="H36" s="54"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
@@ -1840,7 +1859,7 @@
         <v>2035</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>91</v>
@@ -1849,10 +1868,10 @@
         <v>7</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H37" s="19"/>
     </row>
@@ -1864,7 +1883,7 @@
         <v>2035</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>91</v>
@@ -1873,10 +1892,10 @@
         <v>7</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="H38" s="19"/>
     </row>
@@ -1888,7 +1907,7 @@
         <v>2035</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>91</v>
@@ -1902,9 +1921,7 @@
       <c r="G39" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H39" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H39" s="19"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
@@ -1914,7 +1931,7 @@
         <v>2035</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>91</v>
@@ -1928,7 +1945,9 @@
       <c r="G40" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H40" s="19"/>
+      <c r="H40" s="19" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
@@ -1937,104 +1956,114 @@
       <c r="B41" s="18">
         <v>2035</v>
       </c>
-      <c r="C41" s="25" t="s">
+      <c r="C41" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H41" s="19"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C42" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="D41" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E41" s="25" t="s">
+      <c r="D42" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F41" s="25" t="s">
+      <c r="F42" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="G41" s="24" t="s">
+      <c r="G42" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H41" s="25" t="s">
+      <c r="H42" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42" s="39">
-        <v>2035</v>
-      </c>
-      <c r="C42" s="40" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="D43" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="G43" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="H43" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C44" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="E42" s="40" t="s">
+      <c r="D44" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="E44" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F42" s="40"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="40"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" s="36">
-        <v>2035</v>
-      </c>
-      <c r="C43" s="37" t="s">
+      <c r="F44" s="40"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="40"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="36">
+        <v>2035</v>
+      </c>
+      <c r="C45" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="D43" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E43" s="37" t="s">
+      <c r="D45" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E45" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="F43" s="37"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="37"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B44" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C44" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D44" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E44" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F44" s="22"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="22"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C45" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E45" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F45" s="22"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="22"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="37"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
@@ -2044,7 +2073,7 @@
         <v>2035</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D46" s="22" t="s">
         <v>34</v>
@@ -2052,12 +2081,8 @@
       <c r="E46" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F46" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="G46" s="21" t="s">
-        <v>64</v>
-      </c>
+      <c r="F46" s="22"/>
+      <c r="G46" s="21"/>
       <c r="H46" s="22"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -2068,7 +2093,7 @@
         <v>2035</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D47" s="22" t="s">
         <v>34</v>
@@ -2076,12 +2101,8 @@
       <c r="E47" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F47" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="G47" s="21" t="s">
-        <v>65</v>
-      </c>
+      <c r="F47" s="22"/>
+      <c r="G47" s="21"/>
       <c r="H47" s="22"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -2092,7 +2113,7 @@
         <v>2035</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D48" s="22" t="s">
         <v>34</v>
@@ -2101,10 +2122,10 @@
         <v>38</v>
       </c>
       <c r="F48" s="22" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="G48" s="21" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H48" s="22"/>
     </row>
@@ -2116,7 +2137,7 @@
         <v>2035</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="D49" s="22" t="s">
         <v>34</v>
@@ -2125,10 +2146,10 @@
         <v>38</v>
       </c>
       <c r="F49" s="22" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G49" s="21" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H49" s="22"/>
     </row>
@@ -2140,7 +2161,7 @@
         <v>2035</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D50" s="22" t="s">
         <v>34</v>
@@ -2149,10 +2170,10 @@
         <v>38</v>
       </c>
       <c r="F50" s="22" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G50" s="21" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H50" s="22"/>
     </row>
@@ -2164,119 +2185,119 @@
         <v>2035</v>
       </c>
       <c r="C51" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F51" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="G51" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H51" s="22"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D52" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F52" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="G52" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H52" s="22"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C53" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="D51" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E51" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F51" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="G51" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="H51" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B52" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C52" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="D52" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E52" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="F52" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="G52" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="H52" s="30"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B53" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C53" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D53" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E53" s="30" t="s">
+      <c r="D53" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E53" s="22" t="s">
         <v>38</v>
       </c>
       <c r="F53" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G53" s="29" t="s">
+      <c r="G53" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="H53" s="30"/>
+      <c r="H53" s="22" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B54" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C54" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D54" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E54" s="22" t="s">
+      <c r="A54" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E54" s="30" t="s">
         <v>38</v>
       </c>
       <c r="F54" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G54" s="21" t="s">
+      <c r="G54" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H54" s="22"/>
+      <c r="H54" s="30"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B55" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C55" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="D55" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E55" s="22" t="s">
+      <c r="A55" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C55" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D55" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E55" s="30" t="s">
         <v>38</v>
       </c>
       <c r="F55" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G55" s="21" t="s">
+      <c r="G55" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H55" s="22"/>
+      <c r="H55" s="30"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="20" t="s">
@@ -2286,7 +2307,7 @@
         <v>2035</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D56" s="22" t="s">
         <v>34</v>
@@ -2310,7 +2331,7 @@
         <v>2035</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D57" s="22" t="s">
         <v>34</v>
@@ -2327,76 +2348,76 @@
       <c r="H57" s="22"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B58" s="53">
-        <v>2035</v>
-      </c>
-      <c r="C58" s="54" t="s">
+      <c r="A58" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D58" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E58" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F58" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G58" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H58" s="22"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E59" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F59" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G59" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H59" s="22"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B60" s="53">
+        <v>2035</v>
+      </c>
+      <c r="C60" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="D58" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E58" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F58" s="54" t="s">
+      <c r="D60" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E60" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F60" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G58" s="53" t="s">
+      <c r="G60" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H58" s="54"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B59" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C59" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D59" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E59" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F59" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G59" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="H59" s="19"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B60" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C60" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="D60" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E60" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F60" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G60" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="H60" s="19"/>
+      <c r="H60" s="54"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="17" t="s">
@@ -2406,7 +2427,7 @@
         <v>2035</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="D61" s="19" t="s">
         <v>91</v>
@@ -2430,7 +2451,7 @@
         <v>2035</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D62" s="19" t="s">
         <v>91</v>
@@ -2454,7 +2475,7 @@
         <v>2035</v>
       </c>
       <c r="C63" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D63" s="19" t="s">
         <v>91</v>
@@ -2463,10 +2484,10 @@
         <v>38</v>
       </c>
       <c r="F63" s="19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G63" s="18" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H63" s="19"/>
     </row>
@@ -2478,7 +2499,7 @@
         <v>2035</v>
       </c>
       <c r="C64" s="19" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D64" s="19" t="s">
         <v>91</v>
@@ -2487,10 +2508,10 @@
         <v>38</v>
       </c>
       <c r="F64" s="19" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="G64" s="18" t="s">
-        <v>128</v>
+        <v>82</v>
       </c>
       <c r="H64" s="19"/>
     </row>
@@ -2502,7 +2523,7 @@
         <v>2035</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="D65" s="19" t="s">
         <v>91</v>
@@ -2511,10 +2532,10 @@
         <v>38</v>
       </c>
       <c r="F65" s="19" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="G65" s="18" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="H65" s="19"/>
     </row>
@@ -2526,7 +2547,7 @@
         <v>2035</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D66" s="19" t="s">
         <v>91</v>
@@ -2535,10 +2556,10 @@
         <v>38</v>
       </c>
       <c r="F66" s="19" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G66" s="18" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H66" s="19"/>
     </row>
@@ -2550,7 +2571,7 @@
         <v>2035</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D67" s="19" t="s">
         <v>91</v>
@@ -2559,10 +2580,10 @@
         <v>38</v>
       </c>
       <c r="F67" s="19" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G67" s="18" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H67" s="19"/>
     </row>
@@ -2574,7 +2595,7 @@
         <v>2035</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D68" s="19" t="s">
         <v>91</v>
@@ -2583,14 +2604,12 @@
         <v>38</v>
       </c>
       <c r="F68" s="19" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G68" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="H68" s="19" t="s">
-        <v>43</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="H68" s="19"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="17" t="s">
@@ -2600,7 +2619,7 @@
         <v>2035</v>
       </c>
       <c r="C69" s="19" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D69" s="19" t="s">
         <v>91</v>
@@ -2617,118 +2636,124 @@
       <c r="H69" s="19"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B70" s="24">
-        <v>2035</v>
-      </c>
-      <c r="C70" s="25" t="s">
+      <c r="A70" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B70" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C70" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="D70" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F70" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G70" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H70" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C71" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="D71" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E71" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F71" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G71" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H71" s="19"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B72" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C72" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="D70" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E70" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F70" s="25" t="s">
+      <c r="D72" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F72" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="G70" s="24" t="s">
+      <c r="G72" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H70" s="25" t="s">
+      <c r="H72" s="19"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B73" s="24">
+        <v>2035</v>
+      </c>
+      <c r="C73" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="D73" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E73" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F73" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="G73" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="H73" s="25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B71" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C71" s="43" t="s">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C74" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D71" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E71" s="43" t="s">
+      <c r="D74" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E74" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F71" s="43"/>
-      <c r="G71" s="42"/>
-      <c r="H71" s="43"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B72" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C72" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="D72" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E72" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F72" s="45"/>
-      <c r="G72" s="44"/>
-      <c r="H72" s="45"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B73" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C73" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="D73" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E73" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F73" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G73" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="H73" s="45"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B74" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C74" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="D74" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E74" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F74" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G74" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="H74" s="45"/>
+      <c r="F74" s="43"/>
+      <c r="G74" s="42"/>
+      <c r="H74" s="43"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="31" t="s">
@@ -2738,7 +2763,7 @@
         <v>2050</v>
       </c>
       <c r="C75" s="45" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="D75" s="45" t="s">
         <v>34</v>
@@ -2746,12 +2771,8 @@
       <c r="E75" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F75" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="G75" s="44" t="s">
-        <v>74</v>
-      </c>
+      <c r="F75" s="45"/>
+      <c r="G75" s="44"/>
       <c r="H75" s="45"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -2762,7 +2783,7 @@
         <v>2050</v>
       </c>
       <c r="C76" s="45" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="D76" s="45" t="s">
         <v>34</v>
@@ -2771,108 +2792,108 @@
         <v>7</v>
       </c>
       <c r="F76" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="G76" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="H76" s="45"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B77" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C77" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D77" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E77" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F77" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="G77" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="H77" s="45"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B78" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C78" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="D78" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E78" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F78" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="G78" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="H78" s="45"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B79" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C79" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="D79" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E79" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F79" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="G76" s="44" t="s">
+      <c r="G79" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="H76" s="45"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B77" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C77" s="48" t="s">
+      <c r="H79" s="45"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B80" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C80" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="D77" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E77" s="48" t="s">
+      <c r="D80" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E80" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F77" s="48" t="s">
+      <c r="F80" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="G77" s="47" t="s">
+      <c r="G80" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="H77" s="48"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B78" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C78" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D78" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E78" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F78" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="G78" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="H78" s="19"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B79" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C79" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="D79" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E79" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F79" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G79" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H79" s="19"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B80" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C80" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="D80" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E80" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F80" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="G80" s="56" t="s">
-        <v>122</v>
-      </c>
-      <c r="H80" s="19"/>
+      <c r="H80" s="48"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="17" t="s">
@@ -2882,19 +2903,19 @@
         <v>2050</v>
       </c>
       <c r="C81" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="D81" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D81" s="54" t="s">
         <v>91</v>
       </c>
       <c r="E81" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F81" s="19" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="G81" s="56" t="s">
-        <v>137</v>
+        <v>75</v>
       </c>
       <c r="H81" s="19"/>
     </row>
@@ -2906,7 +2927,7 @@
         <v>2050</v>
       </c>
       <c r="C82" s="19" t="s">
-        <v>143</v>
+        <v>100</v>
       </c>
       <c r="D82" s="19" t="s">
         <v>91</v>
@@ -2915,14 +2936,12 @@
         <v>7</v>
       </c>
       <c r="F82" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="G82" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="H82" s="19" t="s">
-        <v>43</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="G82" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H82" s="19"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="17" t="s">
@@ -2932,7 +2951,7 @@
         <v>2050</v>
       </c>
       <c r="C83" s="19" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="D83" s="19" t="s">
         <v>91</v>
@@ -2941,166 +2960,178 @@
         <v>7</v>
       </c>
       <c r="F83" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="G83" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="H83" s="19"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B84" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C84" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="D84" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E84" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F84" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="G83" s="18" t="s">
+      <c r="G84" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="H83" s="19"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B84" s="24">
-        <v>2050</v>
-      </c>
-      <c r="C84" s="25" t="s">
+      <c r="H84" s="19"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B85" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C85" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="D85" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E85" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F85" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G85" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H85" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B86" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C86" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D86" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E86" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F86" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G86" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H86" s="19"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B87" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C87" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="D84" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E84" s="25" t="s">
+      <c r="D87" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E87" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F84" s="25" t="s">
+      <c r="F87" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="G84" s="24" t="s">
+      <c r="G87" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H84" s="25" t="s">
+      <c r="H87" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B85" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C85" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="D85" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E85" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="F85" s="45"/>
-      <c r="G85" s="44"/>
-      <c r="H85" s="45"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B86" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C86" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="D86" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E86" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="F86" s="48"/>
-      <c r="G86" s="47"/>
-      <c r="H86" s="48"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B87" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C87" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D87" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E87" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F87" s="33"/>
-      <c r="G87" s="32"/>
-      <c r="H87" s="33"/>
-    </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B88" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C88" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D88" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E88" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F88" s="33"/>
-      <c r="G88" s="32"/>
-      <c r="H88" s="33"/>
+      <c r="A88" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B88" s="24">
+        <v>2050</v>
+      </c>
+      <c r="C88" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="D88" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E88" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F88" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="G88" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="H88" s="25" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B89" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C89" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="D89" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E89" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F89" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G89" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="H89" s="33"/>
+      <c r="B89" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C89" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="D89" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E89" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="F89" s="45"/>
+      <c r="G89" s="44"/>
+      <c r="H89" s="45"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A90" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B90" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C90" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D90" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E90" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F90" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G90" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="H90" s="33"/>
+      <c r="A90" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B90" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C90" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="D90" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E90" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="F90" s="48"/>
+      <c r="G90" s="47"/>
+      <c r="H90" s="48"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="31" t="s">
@@ -3110,7 +3141,7 @@
         <v>2050</v>
       </c>
       <c r="C91" s="33" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D91" s="33" t="s">
         <v>34</v>
@@ -3118,12 +3149,8 @@
       <c r="E91" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F91" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="G91" s="32" t="s">
-        <v>65</v>
-      </c>
+      <c r="F91" s="33"/>
+      <c r="G91" s="32"/>
       <c r="H91" s="33"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -3134,7 +3161,7 @@
         <v>2050</v>
       </c>
       <c r="C92" s="33" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="D92" s="33" t="s">
         <v>34</v>
@@ -3142,12 +3169,8 @@
       <c r="E92" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F92" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="G92" s="32" t="s">
-        <v>70</v>
-      </c>
+      <c r="F92" s="33"/>
+      <c r="G92" s="32"/>
       <c r="H92" s="33"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -3158,7 +3181,7 @@
         <v>2050</v>
       </c>
       <c r="C93" s="33" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="D93" s="33" t="s">
         <v>34</v>
@@ -3167,10 +3190,10 @@
         <v>38</v>
       </c>
       <c r="F93" s="33" t="s">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="G93" s="32" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="H93" s="33"/>
     </row>
@@ -3182,7 +3205,7 @@
         <v>2050</v>
       </c>
       <c r="C94" s="33" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="D94" s="33" t="s">
         <v>34</v>
@@ -3191,10 +3214,10 @@
         <v>38</v>
       </c>
       <c r="F94" s="33" t="s">
-        <v>118</v>
+        <v>66</v>
       </c>
       <c r="G94" s="32" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="H94" s="33"/>
     </row>
@@ -3206,143 +3229,143 @@
         <v>2050</v>
       </c>
       <c r="C95" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D95" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E95" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F95" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="G95" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="H95" s="33"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B96" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C96" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D96" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E96" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F96" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="G96" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="H96" s="33"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B97" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C97" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D97" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E97" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F97" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="G97" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="H97" s="33"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B98" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C98" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D98" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E98" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F98" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="G98" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="H98" s="33"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B99" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C99" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="D95" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E95" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F95" s="33" t="s">
+      <c r="D99" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E99" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F99" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="G95" s="32" t="s">
+      <c r="G99" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="H95" s="33" t="s">
+      <c r="H99" s="33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B96" s="53">
-        <v>2050</v>
-      </c>
-      <c r="C96" s="54" t="s">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B100" s="53">
+        <v>2050</v>
+      </c>
+      <c r="C100" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="D96" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E96" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F96" s="54" t="s">
+      <c r="D100" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E100" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F100" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G96" s="53" t="s">
+      <c r="G100" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H96" s="54"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B97" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C97" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="D97" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E97" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F97" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G97" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H97" s="55"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B98" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C98" s="55" t="s">
-        <v>102</v>
-      </c>
-      <c r="D98" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E98" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F98" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G98" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H98" s="55"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B99" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C99" s="55" t="s">
-        <v>103</v>
-      </c>
-      <c r="D99" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E99" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F99" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G99" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H99" s="55"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B100" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C100" s="55" t="s">
-        <v>104</v>
-      </c>
-      <c r="D100" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E100" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F100" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G100" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H100" s="55"/>
+      <c r="H100" s="54"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="55" t="s">
@@ -3352,7 +3375,7 @@
         <v>2050</v>
       </c>
       <c r="C101" s="55" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D101" s="55" t="s">
         <v>91</v>
@@ -3376,7 +3399,7 @@
         <v>2050</v>
       </c>
       <c r="C102" s="55" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D102" s="55" t="s">
         <v>91</v>
@@ -3384,11 +3407,11 @@
       <c r="E102" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F102" s="19" t="s">
-        <v>118</v>
+      <c r="F102" s="55" t="s">
+        <v>116</v>
       </c>
       <c r="G102" s="56" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H102" s="55"/>
     </row>
@@ -3400,7 +3423,7 @@
         <v>2050</v>
       </c>
       <c r="C103" s="55" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D103" s="55" t="s">
         <v>91</v>
@@ -3424,7 +3447,7 @@
         <v>2050</v>
       </c>
       <c r="C104" s="55" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D104" s="55" t="s">
         <v>91</v>
@@ -3448,7 +3471,7 @@
         <v>2050</v>
       </c>
       <c r="C105" s="55" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D105" s="55" t="s">
         <v>91</v>
@@ -3472,7 +3495,7 @@
         <v>2050</v>
       </c>
       <c r="C106" s="55" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="D106" s="55" t="s">
         <v>91</v>
@@ -3480,11 +3503,11 @@
       <c r="E106" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F106" s="55" t="s">
-        <v>121</v>
+      <c r="F106" s="19" t="s">
+        <v>118</v>
       </c>
       <c r="G106" s="56" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="H106" s="55"/>
     </row>
@@ -3496,7 +3519,7 @@
         <v>2050</v>
       </c>
       <c r="C107" s="55" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="D107" s="55" t="s">
         <v>91</v>
@@ -3504,13 +3527,13 @@
       <c r="E107" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F107" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="G107" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="H107" s="19"/>
+      <c r="F107" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G107" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H107" s="55"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="55" t="s">
@@ -3520,7 +3543,7 @@
         <v>2050</v>
       </c>
       <c r="C108" s="55" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="D108" s="55" t="s">
         <v>91</v>
@@ -3528,13 +3551,13 @@
       <c r="E108" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F108" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="G108" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="H108" s="19"/>
+      <c r="F108" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G108" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H108" s="55"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="55" t="s">
@@ -3544,7 +3567,7 @@
         <v>2050</v>
       </c>
       <c r="C109" s="55" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="D109" s="55" t="s">
         <v>91</v>
@@ -3552,13 +3575,13 @@
       <c r="E109" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F109" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="G109" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="H109" s="19"/>
+      <c r="F109" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G109" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H109" s="55"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="55" t="s">
@@ -3568,7 +3591,7 @@
         <v>2050</v>
       </c>
       <c r="C110" s="55" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="D110" s="55" t="s">
         <v>91</v>
@@ -3576,13 +3599,13 @@
       <c r="E110" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F110" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="G110" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="H110" s="19"/>
+      <c r="F110" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="G110" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="H110" s="55"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="55" t="s">
@@ -3592,7 +3615,7 @@
         <v>2050</v>
       </c>
       <c r="C111" s="55" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="D111" s="55" t="s">
         <v>91</v>
@@ -3601,14 +3624,12 @@
         <v>38</v>
       </c>
       <c r="F111" s="19" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="G111" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="H111" s="19" t="s">
-        <v>43</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="H111" s="19"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="55" t="s">
@@ -3618,7 +3639,7 @@
         <v>2050</v>
       </c>
       <c r="C112" s="55" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D112" s="55" t="s">
         <v>91</v>
@@ -3627,10 +3648,10 @@
         <v>38</v>
       </c>
       <c r="F112" s="19" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G112" s="18" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H112" s="19"/>
     </row>
@@ -3642,7 +3663,7 @@
         <v>2050</v>
       </c>
       <c r="C113" s="55" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="D113" s="55" t="s">
         <v>91</v>
@@ -3656,7 +3677,129 @@
       <c r="G113" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H113" s="19" t="s">
+      <c r="H113" s="19"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B114" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C114" s="55" t="s">
+        <v>144</v>
+      </c>
+      <c r="D114" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E114" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F114" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G114" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H114" s="19"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B115" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C115" s="55" t="s">
+        <v>145</v>
+      </c>
+      <c r="D115" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E115" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F115" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G115" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H115" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B116" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C116" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="D116" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E116" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F116" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G116" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H116" s="19"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B117" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C117" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="D117" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E117" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F117" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G117" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H117" s="19"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B118" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C118" s="55" t="s">
+        <v>164</v>
+      </c>
+      <c r="D118" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E118" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F118" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G118" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H118" s="19" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update with latest runs
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bespin\Documents\GitHub\travel-model-one\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11047A85-0E23-4553-A2E6-0DE02E2844AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6090" yWindow="1455" windowWidth="20595" windowHeight="15645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6090" yWindow="1455" windowWidth="20595" windowHeight="15645"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="171">
   <si>
     <t>EEJ</t>
   </si>
@@ -520,12 +519,30 @@
   </si>
   <si>
     <t>2050_TM152_FBP_PlusCrossing_19</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_PlusCrossing_20</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_NoProject_21</t>
+  </si>
+  <si>
+    <t>"EIR runs\Baseline Large (s25) runs\NP_v8"</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_Plus_20</t>
+  </si>
+  <si>
+    <t>run314</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_NoProject_22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -756,15 +773,15 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFFFCCFF"/>
       <color rgb="FFE4C9FF"/>
-      <color rgb="FFFFCCFF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1074,12 +1091,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H118"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A118" sqref="A118"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2006,84 +2023,90 @@
       <c r="B43" s="18">
         <v>2035</v>
       </c>
-      <c r="C43" s="25" t="s">
+      <c r="C43" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="D43" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E43" s="25" t="s">
+      <c r="D43" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F43" s="25" t="s">
+      <c r="F43" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="G43" s="24" t="s">
+      <c r="G43" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="H43" s="25" t="s">
+      <c r="H43" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B44" s="39">
-        <v>2035</v>
-      </c>
-      <c r="C44" s="40" t="s">
+      <c r="A44" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="24">
+        <v>2035</v>
+      </c>
+      <c r="C44" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="D44" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="G44" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="H44" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C45" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D44" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="E44" s="40" t="s">
+      <c r="D45" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="E45" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F44" s="40"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="40"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" s="36">
-        <v>2035</v>
-      </c>
-      <c r="C45" s="37" t="s">
+      <c r="F45" s="40"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="40"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="36">
+        <v>2035</v>
+      </c>
+      <c r="C46" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="D45" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E45" s="37" t="s">
+      <c r="D46" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E46" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="F45" s="37"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="37"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B46" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C46" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D46" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E46" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F46" s="22"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="22"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="37"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
@@ -2093,7 +2116,7 @@
         <v>2035</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D47" s="22" t="s">
         <v>34</v>
@@ -2113,7 +2136,7 @@
         <v>2035</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D48" s="22" t="s">
         <v>34</v>
@@ -2121,12 +2144,8 @@
       <c r="E48" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F48" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="G48" s="21" t="s">
-        <v>64</v>
-      </c>
+      <c r="F48" s="22"/>
+      <c r="G48" s="21"/>
       <c r="H48" s="22"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -2137,7 +2156,7 @@
         <v>2035</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D49" s="22" t="s">
         <v>34</v>
@@ -2146,10 +2165,10 @@
         <v>38</v>
       </c>
       <c r="F49" s="22" t="s">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="G49" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H49" s="22"/>
     </row>
@@ -2161,7 +2180,7 @@
         <v>2035</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D50" s="22" t="s">
         <v>34</v>
@@ -2170,10 +2189,10 @@
         <v>38</v>
       </c>
       <c r="F50" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G50" s="21" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H50" s="22"/>
     </row>
@@ -2185,7 +2204,7 @@
         <v>2035</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D51" s="22" t="s">
         <v>34</v>
@@ -2194,10 +2213,10 @@
         <v>38</v>
       </c>
       <c r="F51" s="22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G51" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H51" s="22"/>
     </row>
@@ -2209,7 +2228,7 @@
         <v>2035</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D52" s="22" t="s">
         <v>34</v>
@@ -2218,10 +2237,10 @@
         <v>38</v>
       </c>
       <c r="F52" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G52" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H52" s="22"/>
     </row>
@@ -2233,47 +2252,47 @@
         <v>2035</v>
       </c>
       <c r="C53" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D53" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E53" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F53" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="G53" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H53" s="22"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C54" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="D53" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E53" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F53" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="G53" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="H53" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B54" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C54" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="D54" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E54" s="30" t="s">
+      <c r="D54" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E54" s="22" t="s">
         <v>38</v>
       </c>
       <c r="F54" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G54" s="29" t="s">
+      <c r="G54" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="H54" s="30"/>
+      <c r="H54" s="22" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="51" t="s">
@@ -2283,7 +2302,7 @@
         <v>2035</v>
       </c>
       <c r="C55" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D55" s="30" t="s">
         <v>34</v>
@@ -2300,28 +2319,28 @@
       <c r="H55" s="30"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B56" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C56" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D56" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E56" s="22" t="s">
+      <c r="A56" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C56" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D56" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E56" s="30" t="s">
         <v>38</v>
       </c>
       <c r="F56" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G56" s="21" t="s">
+      <c r="G56" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H56" s="22"/>
+      <c r="H56" s="30"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="20" t="s">
@@ -2331,7 +2350,7 @@
         <v>2035</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D57" s="22" t="s">
         <v>34</v>
@@ -2355,7 +2374,7 @@
         <v>2035</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D58" s="22" t="s">
         <v>34</v>
@@ -2379,7 +2398,7 @@
         <v>2035</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D59" s="22" t="s">
         <v>34</v>
@@ -2396,52 +2415,52 @@
       <c r="H59" s="22"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B60" s="53">
-        <v>2035</v>
-      </c>
-      <c r="C60" s="54" t="s">
+      <c r="A60" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B60" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C60" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E60" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F60" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G60" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H60" s="22"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" s="53">
+        <v>2035</v>
+      </c>
+      <c r="C61" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="D60" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E60" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F60" s="54" t="s">
+      <c r="D61" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E61" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F61" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G60" s="53" t="s">
+      <c r="G61" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H60" s="54"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B61" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C61" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D61" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E61" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F61" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G61" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="H61" s="19"/>
+      <c r="H61" s="54"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="17" t="s">
@@ -2451,7 +2470,7 @@
         <v>2035</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D62" s="19" t="s">
         <v>91</v>
@@ -2475,7 +2494,7 @@
         <v>2035</v>
       </c>
       <c r="C63" s="19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D63" s="19" t="s">
         <v>91</v>
@@ -2499,7 +2518,7 @@
         <v>2035</v>
       </c>
       <c r="C64" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D64" s="19" t="s">
         <v>91</v>
@@ -2523,7 +2542,7 @@
         <v>2035</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D65" s="19" t="s">
         <v>91</v>
@@ -2532,10 +2551,10 @@
         <v>38</v>
       </c>
       <c r="F65" s="19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G65" s="18" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H65" s="19"/>
     </row>
@@ -2547,7 +2566,7 @@
         <v>2035</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D66" s="19" t="s">
         <v>91</v>
@@ -2556,10 +2575,10 @@
         <v>38</v>
       </c>
       <c r="F66" s="19" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="G66" s="18" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H66" s="19"/>
     </row>
@@ -2571,7 +2590,7 @@
         <v>2035</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D67" s="19" t="s">
         <v>91</v>
@@ -2580,10 +2599,10 @@
         <v>38</v>
       </c>
       <c r="F67" s="19" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G67" s="18" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H67" s="19"/>
     </row>
@@ -2595,7 +2614,7 @@
         <v>2035</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D68" s="19" t="s">
         <v>91</v>
@@ -2619,7 +2638,7 @@
         <v>2035</v>
       </c>
       <c r="C69" s="19" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D69" s="19" t="s">
         <v>91</v>
@@ -2628,10 +2647,10 @@
         <v>38</v>
       </c>
       <c r="F69" s="19" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G69" s="18" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H69" s="19"/>
     </row>
@@ -2643,7 +2662,7 @@
         <v>2035</v>
       </c>
       <c r="C70" s="19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D70" s="19" t="s">
         <v>91</v>
@@ -2657,9 +2676,7 @@
       <c r="G70" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H70" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H70" s="19"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="17" t="s">
@@ -2669,7 +2686,7 @@
         <v>2035</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D71" s="19" t="s">
         <v>91</v>
@@ -2683,7 +2700,9 @@
       <c r="G71" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H71" s="19"/>
+      <c r="H71" s="19" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="17" t="s">
@@ -2693,7 +2712,7 @@
         <v>2035</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D72" s="19" t="s">
         <v>91</v>
@@ -2710,94 +2729,100 @@
       <c r="H72" s="19"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B73" s="24">
-        <v>2035</v>
-      </c>
-      <c r="C73" s="25" t="s">
+      <c r="A73" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B73" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C73" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="D73" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E73" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F73" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G73" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H73" s="19"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C74" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="D73" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E73" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F73" s="25" t="s">
+      <c r="D74" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E74" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F74" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="G73" s="24" t="s">
+      <c r="G74" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H73" s="25" t="s">
+      <c r="H74" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B74" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C74" s="43" t="s">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B75" s="24">
+        <v>2035</v>
+      </c>
+      <c r="C75" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="D75" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E75" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F75" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="G75" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="H75" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B76" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C76" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D74" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E74" s="43" t="s">
+      <c r="D76" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E76" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F74" s="43"/>
-      <c r="G74" s="42"/>
-      <c r="H74" s="43"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B75" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C75" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="D75" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E75" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F75" s="45"/>
-      <c r="G75" s="44"/>
-      <c r="H75" s="45"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B76" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C76" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="D76" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E76" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F76" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G76" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="H76" s="45"/>
+      <c r="F76" s="43"/>
+      <c r="G76" s="42"/>
+      <c r="H76" s="43"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="31" t="s">
@@ -2807,7 +2832,7 @@
         <v>2050</v>
       </c>
       <c r="C77" s="45" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="D77" s="45" t="s">
         <v>34</v>
@@ -2815,12 +2840,8 @@
       <c r="E77" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F77" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G77" s="44" t="s">
-        <v>65</v>
-      </c>
+      <c r="F77" s="45"/>
+      <c r="G77" s="44"/>
       <c r="H77" s="45"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -2831,7 +2852,7 @@
         <v>2050</v>
       </c>
       <c r="C78" s="45" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D78" s="45" t="s">
         <v>34</v>
@@ -2840,10 +2861,10 @@
         <v>7</v>
       </c>
       <c r="F78" s="45" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G78" s="44" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H78" s="45"/>
     </row>
@@ -2855,7 +2876,7 @@
         <v>2050</v>
       </c>
       <c r="C79" s="45" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D79" s="45" t="s">
         <v>34</v>
@@ -2864,84 +2885,84 @@
         <v>7</v>
       </c>
       <c r="F79" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="G79" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="H79" s="45"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B80" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C80" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="D80" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E80" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F80" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="G80" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="H80" s="45"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B81" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C81" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="D81" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E81" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F81" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="G79" s="44" t="s">
+      <c r="G81" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="H79" s="45"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B80" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C80" s="48" t="s">
+      <c r="H81" s="45"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B82" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C82" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="D80" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E80" s="48" t="s">
+      <c r="D82" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E82" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F80" s="48" t="s">
+      <c r="F82" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="G80" s="47" t="s">
+      <c r="G82" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="H80" s="48"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B81" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C81" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D81" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E81" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F81" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="G81" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="H81" s="19"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B82" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C82" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="D82" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E82" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F82" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G82" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H82" s="19"/>
+      <c r="H82" s="48"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="17" t="s">
@@ -2951,19 +2972,19 @@
         <v>2050</v>
       </c>
       <c r="C83" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="D83" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D83" s="54" t="s">
         <v>91</v>
       </c>
       <c r="E83" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F83" s="19" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G83" s="56" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="H83" s="19"/>
     </row>
@@ -2975,7 +2996,7 @@
         <v>2050</v>
       </c>
       <c r="C84" s="19" t="s">
-        <v>138</v>
+        <v>100</v>
       </c>
       <c r="D84" s="19" t="s">
         <v>91</v>
@@ -2984,10 +3005,10 @@
         <v>7</v>
       </c>
       <c r="F84" s="19" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="G84" s="56" t="s">
-        <v>137</v>
+        <v>82</v>
       </c>
       <c r="H84" s="19"/>
     </row>
@@ -2999,7 +3020,7 @@
         <v>2050</v>
       </c>
       <c r="C85" s="19" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="D85" s="19" t="s">
         <v>91</v>
@@ -3008,14 +3029,12 @@
         <v>7</v>
       </c>
       <c r="F85" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="G85" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="H85" s="19" t="s">
-        <v>43</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="G85" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="H85" s="19"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="17" t="s">
@@ -3025,7 +3044,7 @@
         <v>2050</v>
       </c>
       <c r="C86" s="19" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="D86" s="19" t="s">
         <v>91</v>
@@ -3036,7 +3055,7 @@
       <c r="F86" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="G86" s="18" t="s">
+      <c r="G86" s="56" t="s">
         <v>137</v>
       </c>
       <c r="H86" s="19"/>
@@ -3049,7 +3068,7 @@
         <v>2050</v>
       </c>
       <c r="C87" s="19" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D87" s="19" t="s">
         <v>91</v>
@@ -3058,7 +3077,7 @@
         <v>7</v>
       </c>
       <c r="F87" s="19" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="G87" s="18" t="s">
         <v>137</v>
@@ -3068,134 +3087,146 @@
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B88" s="24">
-        <v>2050</v>
-      </c>
-      <c r="C88" s="25" t="s">
+      <c r="A88" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B88" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C88" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D88" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E88" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F88" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G88" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H88" s="19"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B89" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C89" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="D89" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E89" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F89" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="G89" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H89" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B90" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C90" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="D88" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E88" s="25" t="s">
+      <c r="D90" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E90" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F88" s="25" t="s">
+      <c r="F90" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="G88" s="24" t="s">
+      <c r="G90" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="H88" s="25" t="s">
+      <c r="H90" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B89" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C89" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="D89" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E89" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="F89" s="45"/>
-      <c r="G89" s="44"/>
-      <c r="H89" s="45"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A90" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B90" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C90" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="D90" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E90" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="F90" s="48"/>
-      <c r="G90" s="47"/>
-      <c r="H90" s="48"/>
-    </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B91" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C91" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D91" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E91" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F91" s="33"/>
-      <c r="G91" s="32"/>
-      <c r="H91" s="33"/>
+      <c r="A91" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B91" s="24">
+        <v>2050</v>
+      </c>
+      <c r="C91" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D91" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E91" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F91" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="G91" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="H91" s="25" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B92" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C92" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D92" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E92" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F92" s="33"/>
-      <c r="G92" s="32"/>
-      <c r="H92" s="33"/>
+      <c r="B92" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C92" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="D92" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E92" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="F92" s="45"/>
+      <c r="G92" s="44"/>
+      <c r="H92" s="45"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B93" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C93" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="D93" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E93" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F93" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G93" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="H93" s="33"/>
+      <c r="A93" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B93" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C93" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="D93" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E93" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="F93" s="48"/>
+      <c r="G93" s="47"/>
+      <c r="H93" s="48"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="31" t="s">
@@ -3205,7 +3236,7 @@
         <v>2050</v>
       </c>
       <c r="C94" s="33" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D94" s="33" t="s">
         <v>34</v>
@@ -3213,12 +3244,8 @@
       <c r="E94" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F94" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G94" s="32" t="s">
-        <v>63</v>
-      </c>
+      <c r="F94" s="33"/>
+      <c r="G94" s="32"/>
       <c r="H94" s="33"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
@@ -3229,7 +3256,7 @@
         <v>2050</v>
       </c>
       <c r="C95" s="33" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="D95" s="33" t="s">
         <v>34</v>
@@ -3237,12 +3264,8 @@
       <c r="E95" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F95" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="G95" s="32" t="s">
-        <v>65</v>
-      </c>
+      <c r="F95" s="33"/>
+      <c r="G95" s="32"/>
       <c r="H95" s="33"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
@@ -3253,7 +3276,7 @@
         <v>2050</v>
       </c>
       <c r="C96" s="33" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D96" s="33" t="s">
         <v>34</v>
@@ -3262,10 +3285,10 @@
         <v>38</v>
       </c>
       <c r="F96" s="33" t="s">
-        <v>120</v>
+        <v>66</v>
       </c>
       <c r="G96" s="32" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H96" s="33"/>
     </row>
@@ -3277,7 +3300,7 @@
         <v>2050</v>
       </c>
       <c r="C97" s="33" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="D97" s="33" t="s">
         <v>34</v>
@@ -3286,10 +3309,10 @@
         <v>38</v>
       </c>
       <c r="F97" s="33" t="s">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="G97" s="32" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="H97" s="33"/>
     </row>
@@ -3301,7 +3324,7 @@
         <v>2050</v>
       </c>
       <c r="C98" s="33" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="D98" s="33" t="s">
         <v>34</v>
@@ -3310,10 +3333,10 @@
         <v>38</v>
       </c>
       <c r="F98" s="33" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G98" s="32" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="H98" s="33"/>
     </row>
@@ -3325,119 +3348,119 @@
         <v>2050</v>
       </c>
       <c r="C99" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D99" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E99" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F99" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="G99" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="H99" s="33"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B100" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C100" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D100" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E100" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F100" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="G100" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="H100" s="33"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B101" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C101" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D101" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E101" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F101" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="G101" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="H101" s="33"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B102" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C102" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="D99" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E99" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F99" s="33" t="s">
+      <c r="D102" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E102" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F102" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="G99" s="32" t="s">
+      <c r="G102" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="H99" s="33" t="s">
+      <c r="H102" s="33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B100" s="53">
-        <v>2050</v>
-      </c>
-      <c r="C100" s="54" t="s">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B103" s="53">
+        <v>2050</v>
+      </c>
+      <c r="C103" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="D100" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E100" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F100" s="54" t="s">
+      <c r="D103" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E103" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F103" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G100" s="53" t="s">
+      <c r="G103" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H100" s="54"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B101" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C101" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="D101" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E101" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F101" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G101" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H101" s="55"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B102" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C102" s="55" t="s">
-        <v>102</v>
-      </c>
-      <c r="D102" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E102" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F102" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G102" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H102" s="55"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B103" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C103" s="55" t="s">
-        <v>103</v>
-      </c>
-      <c r="D103" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E103" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F103" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G103" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H103" s="55"/>
+      <c r="H103" s="54"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="55" t="s">
@@ -3447,7 +3470,7 @@
         <v>2050</v>
       </c>
       <c r="C104" s="55" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D104" s="55" t="s">
         <v>91</v>
@@ -3471,7 +3494,7 @@
         <v>2050</v>
       </c>
       <c r="C105" s="55" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D105" s="55" t="s">
         <v>91</v>
@@ -3495,7 +3518,7 @@
         <v>2050</v>
       </c>
       <c r="C106" s="55" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D106" s="55" t="s">
         <v>91</v>
@@ -3503,11 +3526,11 @@
       <c r="E106" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F106" s="19" t="s">
-        <v>118</v>
+      <c r="F106" s="55" t="s">
+        <v>116</v>
       </c>
       <c r="G106" s="56" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H106" s="55"/>
     </row>
@@ -3519,7 +3542,7 @@
         <v>2050</v>
       </c>
       <c r="C107" s="55" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D107" s="55" t="s">
         <v>91</v>
@@ -3543,7 +3566,7 @@
         <v>2050</v>
       </c>
       <c r="C108" s="55" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D108" s="55" t="s">
         <v>91</v>
@@ -3567,7 +3590,7 @@
         <v>2050</v>
       </c>
       <c r="C109" s="55" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D109" s="55" t="s">
         <v>91</v>
@@ -3575,11 +3598,11 @@
       <c r="E109" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F109" s="55" t="s">
-        <v>116</v>
+      <c r="F109" s="19" t="s">
+        <v>118</v>
       </c>
       <c r="G109" s="56" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H109" s="55"/>
     </row>
@@ -3591,7 +3614,7 @@
         <v>2050</v>
       </c>
       <c r="C110" s="55" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="D110" s="55" t="s">
         <v>91</v>
@@ -3600,10 +3623,10 @@
         <v>38</v>
       </c>
       <c r="F110" s="55" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G110" s="56" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H110" s="55"/>
     </row>
@@ -3615,7 +3638,7 @@
         <v>2050</v>
       </c>
       <c r="C111" s="55" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="D111" s="55" t="s">
         <v>91</v>
@@ -3623,13 +3646,13 @@
       <c r="E111" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F111" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="G111" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="H111" s="19"/>
+      <c r="F111" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G111" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H111" s="55"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="55" t="s">
@@ -3639,7 +3662,7 @@
         <v>2050</v>
       </c>
       <c r="C112" s="55" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="D112" s="55" t="s">
         <v>91</v>
@@ -3647,13 +3670,13 @@
       <c r="E112" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F112" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="G112" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="H112" s="19"/>
+      <c r="F112" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G112" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H112" s="55"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="55" t="s">
@@ -3663,7 +3686,7 @@
         <v>2050</v>
       </c>
       <c r="C113" s="55" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="D113" s="55" t="s">
         <v>91</v>
@@ -3671,13 +3694,13 @@
       <c r="E113" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F113" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="G113" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="H113" s="19"/>
+      <c r="F113" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="G113" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="H113" s="55"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="55" t="s">
@@ -3687,7 +3710,7 @@
         <v>2050</v>
       </c>
       <c r="C114" s="55" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="D114" s="55" t="s">
         <v>91</v>
@@ -3696,10 +3719,10 @@
         <v>38</v>
       </c>
       <c r="F114" s="19" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="G114" s="18" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="H114" s="19"/>
     </row>
@@ -3711,7 +3734,7 @@
         <v>2050</v>
       </c>
       <c r="C115" s="55" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="D115" s="55" t="s">
         <v>91</v>
@@ -3720,14 +3743,12 @@
         <v>38</v>
       </c>
       <c r="F115" s="19" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G115" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="H115" s="19" t="s">
-        <v>43</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="H115" s="19"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="55" t="s">
@@ -3737,7 +3758,7 @@
         <v>2050</v>
       </c>
       <c r="C116" s="55" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D116" s="55" t="s">
         <v>91</v>
@@ -3761,7 +3782,7 @@
         <v>2050</v>
       </c>
       <c r="C117" s="55" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D117" s="55" t="s">
         <v>91</v>
@@ -3785,7 +3806,7 @@
         <v>2050</v>
       </c>
       <c r="C118" s="55" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="D118" s="55" t="s">
         <v>91</v>
@@ -3800,6 +3821,106 @@
         <v>137</v>
       </c>
       <c r="H118" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B119" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C119" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="D119" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E119" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F119" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G119" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H119" s="19"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A120" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B120" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C120" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="D120" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E120" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F120" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G120" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H120" s="19"/>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A121" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B121" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C121" s="55" t="s">
+        <v>164</v>
+      </c>
+      <c r="D121" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E121" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F121" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G121" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H121" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A122" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B122" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C122" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="D122" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E122" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F122" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G122" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H122" s="19" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 2025, 2030 FBP No Project runs
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bespin\Documents\GitHub\travel-model-one\utilities\RTP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A02ABE7-377C-4F2D-A3EE-F9DBF87AB392}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6090" yWindow="1455" windowWidth="20595" windowHeight="15645"/>
+    <workbookView xWindow="11220" yWindow="3900" windowWidth="20595" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="173">
   <si>
     <t>EEJ</t>
   </si>
@@ -537,12 +538,18 @@
   </si>
   <si>
     <t>2035_TM152_FBP_NoProject_22</t>
+  </si>
+  <si>
+    <t>2025_TM152_FBP_NoProject_21</t>
+  </si>
+  <si>
+    <t>2030_TM152_FBP_NoProject_21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -773,7 +780,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1091,12 +1098,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H122"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F53" sqref="F53"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1609,66 +1616,76 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="39">
-        <v>2035</v>
-      </c>
-      <c r="C25" s="40" t="s">
+      <c r="A25" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="18">
+        <v>2025</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="18">
+        <v>2030</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="G26" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C27" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D27" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="40" t="s">
+      <c r="E27" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="40"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="F26" s="22"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="22"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="F27" s="22"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="22" t="s">
-        <v>43</v>
-      </c>
+      <c r="F27" s="40"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
@@ -1678,7 +1695,7 @@
         <v>2035</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>158</v>
+        <v>93</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>28</v>
@@ -1688,29 +1705,29 @@
       </c>
       <c r="F28" s="22"/>
       <c r="G28" s="21"/>
-      <c r="H28" s="22" t="s">
+      <c r="H28" s="22"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="22"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="22" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="39">
-        <v>2035</v>
-      </c>
-      <c r="C29" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="40"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="40"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
@@ -1719,38 +1736,40 @@
       <c r="B30" s="21">
         <v>2035</v>
       </c>
-      <c r="C30" s="20" t="s">
-        <v>44</v>
+      <c r="C30" s="22" t="s">
+        <v>158</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="F30" s="22"/>
       <c r="G30" s="21"/>
-      <c r="H30" s="22"/>
+      <c r="H30" s="22" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="22" t="s">
+      <c r="A31" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="22"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="22"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="40"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
@@ -1760,7 +1779,7 @@
         <v>2035</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D32" s="22" t="s">
         <v>34</v>
@@ -1780,7 +1799,7 @@
         <v>2035</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="D33" s="22" t="s">
         <v>34</v>
@@ -1788,12 +1807,8 @@
       <c r="E33" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="G33" s="21" t="s">
-        <v>74</v>
-      </c>
+      <c r="F33" s="22"/>
+      <c r="G33" s="21"/>
       <c r="H33" s="22"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1804,7 +1819,7 @@
         <v>2035</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D34" s="22" t="s">
         <v>34</v>
@@ -1812,109 +1827,105 @@
       <c r="E34" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="22" t="s">
+      <c r="F34" s="22"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="22"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H35" s="22"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="G34" s="21" t="s">
+      <c r="G36" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="H34" s="22"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="36">
-        <v>2035</v>
-      </c>
-      <c r="C35" s="35" t="s">
+      <c r="H36" s="22"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="36">
+        <v>2035</v>
+      </c>
+      <c r="C37" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D35" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" s="37" t="s">
+      <c r="D37" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="37" t="s">
+      <c r="F37" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="G35" s="36" t="s">
+      <c r="G37" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="37"/>
-    </row>
-    <row r="36" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="53">
-        <v>2035</v>
-      </c>
-      <c r="C36" s="54" t="s">
+      <c r="H37" s="37"/>
+    </row>
+    <row r="38" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="53">
+        <v>2035</v>
+      </c>
+      <c r="C38" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="D36" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E36" s="54" t="s">
+      <c r="D38" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E38" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="54" t="s">
+      <c r="F38" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G36" s="53" t="s">
+      <c r="G38" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H36" s="54"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G37" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="H37" s="19"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="G38" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="H38" s="19"/>
+      <c r="H38" s="54"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
@@ -1924,7 +1935,7 @@
         <v>2035</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>91</v>
@@ -1933,10 +1944,10 @@
         <v>7</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="G39" s="18" t="s">
-        <v>137</v>
+        <v>82</v>
       </c>
       <c r="H39" s="19"/>
     </row>
@@ -1948,7 +1959,7 @@
         <v>2035</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>91</v>
@@ -1957,14 +1968,12 @@
         <v>7</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="G40" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="H40" s="19" t="s">
-        <v>43</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="H40" s="19"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
@@ -1974,7 +1983,7 @@
         <v>2035</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="D41" s="19" t="s">
         <v>91</v>
@@ -1998,7 +2007,7 @@
         <v>2035</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="D42" s="19" t="s">
         <v>91</v>
@@ -2007,7 +2016,7 @@
         <v>7</v>
       </c>
       <c r="F42" s="19" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="G42" s="18" t="s">
         <v>137</v>
@@ -2024,7 +2033,7 @@
         <v>2035</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="D43" s="19" t="s">
         <v>91</v>
@@ -2033,120 +2042,130 @@
         <v>7</v>
       </c>
       <c r="F43" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H43" s="19"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="G44" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H44" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="G43" s="18" t="s">
+      <c r="G45" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="H43" s="19" t="s">
+      <c r="H45" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B44" s="24">
-        <v>2035</v>
-      </c>
-      <c r="C44" s="25" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="24">
+        <v>2035</v>
+      </c>
+      <c r="C46" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="D44" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E44" s="25" t="s">
+      <c r="D46" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E46" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="F44" s="25" t="s">
+      <c r="F46" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="G44" s="24" t="s">
+      <c r="G46" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="H44" s="25" t="s">
+      <c r="H46" s="25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" s="39">
-        <v>2035</v>
-      </c>
-      <c r="C45" s="40" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="39">
+        <v>2035</v>
+      </c>
+      <c r="C47" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D45" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="E45" s="40" t="s">
+      <c r="D47" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="E47" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F45" s="40"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="40"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B46" s="36">
-        <v>2035</v>
-      </c>
-      <c r="C46" s="37" t="s">
+      <c r="F47" s="40"/>
+      <c r="G47" s="39"/>
+      <c r="H47" s="40"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="36">
+        <v>2035</v>
+      </c>
+      <c r="C48" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="D46" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E46" s="37" t="s">
+      <c r="D48" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E48" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="F46" s="37"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="37"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C47" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D47" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E47" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F47" s="22"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="22"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B48" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C48" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D48" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E48" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F48" s="22"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="22"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="37"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
@@ -2156,7 +2175,7 @@
         <v>2035</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D49" s="22" t="s">
         <v>34</v>
@@ -2164,12 +2183,8 @@
       <c r="E49" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F49" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="G49" s="21" t="s">
-        <v>64</v>
-      </c>
+      <c r="F49" s="22"/>
+      <c r="G49" s="21"/>
       <c r="H49" s="22"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -2180,7 +2195,7 @@
         <v>2035</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D50" s="22" t="s">
         <v>34</v>
@@ -2188,12 +2203,8 @@
       <c r="E50" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F50" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="G50" s="21" t="s">
-        <v>65</v>
-      </c>
+      <c r="F50" s="22"/>
+      <c r="G50" s="21"/>
       <c r="H50" s="22"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -2204,7 +2215,7 @@
         <v>2035</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D51" s="22" t="s">
         <v>34</v>
@@ -2213,10 +2224,10 @@
         <v>38</v>
       </c>
       <c r="F51" s="22" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="G51" s="21" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H51" s="22"/>
     </row>
@@ -2228,7 +2239,7 @@
         <v>2035</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="D52" s="22" t="s">
         <v>34</v>
@@ -2237,10 +2248,10 @@
         <v>38</v>
       </c>
       <c r="F52" s="22" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G52" s="21" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H52" s="22"/>
     </row>
@@ -2252,7 +2263,7 @@
         <v>2035</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D53" s="22" t="s">
         <v>34</v>
@@ -2261,10 +2272,10 @@
         <v>38</v>
       </c>
       <c r="F53" s="22" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G53" s="21" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H53" s="22"/>
     </row>
@@ -2276,119 +2287,119 @@
         <v>2035</v>
       </c>
       <c r="C54" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E54" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F54" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="G54" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H54" s="22"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D55" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F55" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="G55" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H55" s="22"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C56" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="D54" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E54" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F54" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="G54" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="H54" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B55" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C55" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="D55" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E55" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="F55" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="G55" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="H55" s="30"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B56" s="29">
-        <v>2035</v>
-      </c>
-      <c r="C56" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D56" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E56" s="30" t="s">
+      <c r="D56" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E56" s="22" t="s">
         <v>38</v>
       </c>
       <c r="F56" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G56" s="29" t="s">
+      <c r="G56" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="H56" s="30"/>
+      <c r="H56" s="22" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B57" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C57" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D57" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E57" s="22" t="s">
+      <c r="A57" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C57" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D57" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E57" s="30" t="s">
         <v>38</v>
       </c>
       <c r="F57" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G57" s="21" t="s">
+      <c r="G57" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H57" s="22"/>
+      <c r="H57" s="30"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B58" s="21">
-        <v>2035</v>
-      </c>
-      <c r="C58" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E58" s="22" t="s">
+      <c r="A58" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" s="29">
+        <v>2035</v>
+      </c>
+      <c r="C58" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D58" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E58" s="30" t="s">
         <v>38</v>
       </c>
       <c r="F58" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G58" s="21" t="s">
+      <c r="G58" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="H58" s="22"/>
+      <c r="H58" s="30"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
@@ -2398,7 +2409,7 @@
         <v>2035</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D59" s="22" t="s">
         <v>34</v>
@@ -2422,7 +2433,7 @@
         <v>2035</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D60" s="22" t="s">
         <v>34</v>
@@ -2439,76 +2450,76 @@
       <c r="H60" s="22"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B61" s="53">
-        <v>2035</v>
-      </c>
-      <c r="C61" s="54" t="s">
+      <c r="A61" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C61" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D61" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E61" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F61" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G61" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H61" s="22"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="21">
+        <v>2035</v>
+      </c>
+      <c r="C62" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D62" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E62" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F62" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G62" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="H62" s="22"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" s="53">
+        <v>2035</v>
+      </c>
+      <c r="C63" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="D61" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E61" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F61" s="54" t="s">
+      <c r="D63" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E63" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F63" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G61" s="53" t="s">
+      <c r="G63" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H61" s="54"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B62" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C62" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D62" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E62" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F62" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G62" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="H62" s="19"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B63" s="18">
-        <v>2035</v>
-      </c>
-      <c r="C63" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="D63" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E63" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F63" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G63" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="H63" s="19"/>
+      <c r="H63" s="54"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="17" t="s">
@@ -2518,7 +2529,7 @@
         <v>2035</v>
       </c>
       <c r="C64" s="19" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="D64" s="19" t="s">
         <v>91</v>
@@ -2542,7 +2553,7 @@
         <v>2035</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D65" s="19" t="s">
         <v>91</v>
@@ -2566,7 +2577,7 @@
         <v>2035</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D66" s="19" t="s">
         <v>91</v>
@@ -2575,10 +2586,10 @@
         <v>38</v>
       </c>
       <c r="F66" s="19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G66" s="18" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H66" s="19"/>
     </row>
@@ -2590,7 +2601,7 @@
         <v>2035</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D67" s="19" t="s">
         <v>91</v>
@@ -2599,10 +2610,10 @@
         <v>38</v>
       </c>
       <c r="F67" s="19" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="G67" s="18" t="s">
-        <v>128</v>
+        <v>82</v>
       </c>
       <c r="H67" s="19"/>
     </row>
@@ -2614,7 +2625,7 @@
         <v>2035</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="D68" s="19" t="s">
         <v>91</v>
@@ -2623,10 +2634,10 @@
         <v>38</v>
       </c>
       <c r="F68" s="19" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="G68" s="18" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="H68" s="19"/>
     </row>
@@ -2638,7 +2649,7 @@
         <v>2035</v>
       </c>
       <c r="C69" s="19" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D69" s="19" t="s">
         <v>91</v>
@@ -2647,10 +2658,10 @@
         <v>38</v>
       </c>
       <c r="F69" s="19" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G69" s="18" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H69" s="19"/>
     </row>
@@ -2662,7 +2673,7 @@
         <v>2035</v>
       </c>
       <c r="C70" s="19" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D70" s="19" t="s">
         <v>91</v>
@@ -2671,10 +2682,10 @@
         <v>38</v>
       </c>
       <c r="F70" s="19" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G70" s="18" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H70" s="19"/>
     </row>
@@ -2686,7 +2697,7 @@
         <v>2035</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D71" s="19" t="s">
         <v>91</v>
@@ -2695,14 +2706,12 @@
         <v>38</v>
       </c>
       <c r="F71" s="19" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G71" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="H71" s="19" t="s">
-        <v>43</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="H71" s="19"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="17" t="s">
@@ -2712,7 +2721,7 @@
         <v>2035</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D72" s="19" t="s">
         <v>91</v>
@@ -2736,7 +2745,7 @@
         <v>2035</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="D73" s="19" t="s">
         <v>91</v>
@@ -2750,7 +2759,9 @@
       <c r="G73" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H73" s="19"/>
+      <c r="H73" s="19" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="17" t="s">
@@ -2760,7 +2771,7 @@
         <v>2035</v>
       </c>
       <c r="C74" s="19" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D74" s="19" t="s">
         <v>91</v>
@@ -2774,99 +2785,103 @@
       <c r="G74" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H74" s="19" t="s">
+      <c r="H74" s="19"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B75" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C75" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="D75" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E75" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F75" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G75" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H75" s="19"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B76" s="18">
+        <v>2035</v>
+      </c>
+      <c r="C76" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D76" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E76" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F76" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G76" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H76" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B75" s="24">
-        <v>2035</v>
-      </c>
-      <c r="C75" s="25" t="s">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B77" s="24">
+        <v>2035</v>
+      </c>
+      <c r="C77" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D75" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E75" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F75" s="25" t="s">
+      <c r="D77" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E77" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F77" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="G75" s="24" t="s">
+      <c r="G77" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="H75" s="25" t="s">
+      <c r="H77" s="25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B76" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C76" s="43" t="s">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B78" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C78" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D76" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E76" s="43" t="s">
+      <c r="D78" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E78" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F76" s="43"/>
-      <c r="G76" s="42"/>
-      <c r="H76" s="43"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B77" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C77" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="D77" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E77" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F77" s="45"/>
-      <c r="G77" s="44"/>
-      <c r="H77" s="45"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B78" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C78" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="D78" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E78" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F78" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G78" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="H78" s="45"/>
+      <c r="F78" s="43"/>
+      <c r="G78" s="42"/>
+      <c r="H78" s="43"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="31" t="s">
@@ -2876,7 +2891,7 @@
         <v>2050</v>
       </c>
       <c r="C79" s="45" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="D79" s="45" t="s">
         <v>34</v>
@@ -2884,12 +2899,8 @@
       <c r="E79" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="F79" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G79" s="44" t="s">
-        <v>65</v>
-      </c>
+      <c r="F79" s="45"/>
+      <c r="G79" s="44"/>
       <c r="H79" s="45"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -2900,7 +2911,7 @@
         <v>2050</v>
       </c>
       <c r="C80" s="45" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D80" s="45" t="s">
         <v>34</v>
@@ -2909,10 +2920,10 @@
         <v>7</v>
       </c>
       <c r="F80" s="45" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G80" s="44" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H80" s="45"/>
     </row>
@@ -2924,7 +2935,7 @@
         <v>2050</v>
       </c>
       <c r="C81" s="45" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D81" s="45" t="s">
         <v>34</v>
@@ -2933,84 +2944,84 @@
         <v>7</v>
       </c>
       <c r="F81" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="G81" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="H81" s="45"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B82" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C82" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="D82" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E82" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F82" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="G82" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="H82" s="45"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B83" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C83" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="D83" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E83" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F83" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="G81" s="44" t="s">
+      <c r="G83" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="H81" s="45"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B82" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C82" s="48" t="s">
+      <c r="H83" s="45"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B84" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C84" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="D82" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E82" s="48" t="s">
+      <c r="D84" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E84" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F82" s="48" t="s">
+      <c r="F84" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="G82" s="47" t="s">
+      <c r="G84" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="H82" s="48"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B83" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C83" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D83" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E83" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F83" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="G83" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="H83" s="19"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B84" s="18">
-        <v>2050</v>
-      </c>
-      <c r="C84" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="D84" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E84" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F84" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G84" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H84" s="19"/>
+      <c r="H84" s="48"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="17" t="s">
@@ -3020,19 +3031,19 @@
         <v>2050</v>
       </c>
       <c r="C85" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="D85" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D85" s="54" t="s">
         <v>91</v>
       </c>
       <c r="E85" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F85" s="19" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G85" s="56" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="H85" s="19"/>
     </row>
@@ -3044,7 +3055,7 @@
         <v>2050</v>
       </c>
       <c r="C86" s="19" t="s">
-        <v>138</v>
+        <v>100</v>
       </c>
       <c r="D86" s="19" t="s">
         <v>91</v>
@@ -3053,10 +3064,10 @@
         <v>7</v>
       </c>
       <c r="F86" s="19" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="G86" s="56" t="s">
-        <v>137</v>
+        <v>82</v>
       </c>
       <c r="H86" s="19"/>
     </row>
@@ -3068,7 +3079,7 @@
         <v>2050</v>
       </c>
       <c r="C87" s="19" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="D87" s="19" t="s">
         <v>91</v>
@@ -3077,14 +3088,12 @@
         <v>7</v>
       </c>
       <c r="F87" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="G87" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="H87" s="19" t="s">
-        <v>43</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="G87" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="H87" s="19"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="17" t="s">
@@ -3094,7 +3103,7 @@
         <v>2050</v>
       </c>
       <c r="C88" s="19" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="D88" s="19" t="s">
         <v>91</v>
@@ -3105,7 +3114,7 @@
       <c r="F88" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="G88" s="18" t="s">
+      <c r="G88" s="56" t="s">
         <v>137</v>
       </c>
       <c r="H88" s="19"/>
@@ -3118,7 +3127,7 @@
         <v>2050</v>
       </c>
       <c r="C89" s="19" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D89" s="19" t="s">
         <v>91</v>
@@ -3127,7 +3136,7 @@
         <v>7</v>
       </c>
       <c r="F89" s="19" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="G89" s="18" t="s">
         <v>137</v>
@@ -3144,7 +3153,7 @@
         <v>2050</v>
       </c>
       <c r="C90" s="19" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D90" s="19" t="s">
         <v>91</v>
@@ -3153,120 +3162,130 @@
         <v>7</v>
       </c>
       <c r="F90" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G90" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H90" s="19"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B91" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C91" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="D91" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E91" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F91" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="G91" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H91" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B92" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C92" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="D92" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E92" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F92" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="G90" s="18" t="s">
+      <c r="G92" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="H90" s="19" t="s">
+      <c r="H92" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B91" s="24">
-        <v>2050</v>
-      </c>
-      <c r="C91" s="25" t="s">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B93" s="24">
+        <v>2050</v>
+      </c>
+      <c r="C93" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="D91" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E91" s="25" t="s">
+      <c r="D93" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E93" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="F91" s="25" t="s">
+      <c r="F93" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="G91" s="24" t="s">
+      <c r="G93" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="H91" s="25" t="s">
+      <c r="H93" s="25" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B92" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C92" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="D92" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E92" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="F92" s="45"/>
-      <c r="G92" s="44"/>
-      <c r="H92" s="45"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B93" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C93" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="D93" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E93" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="F93" s="48"/>
-      <c r="G93" s="47"/>
-      <c r="H93" s="48"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B94" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C94" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D94" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E94" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F94" s="33"/>
-      <c r="G94" s="32"/>
-      <c r="H94" s="33"/>
+      <c r="B94" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C94" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="D94" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E94" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="F94" s="45"/>
+      <c r="G94" s="44"/>
+      <c r="H94" s="45"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B95" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C95" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D95" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E95" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F95" s="33"/>
-      <c r="G95" s="32"/>
-      <c r="H95" s="33"/>
+      <c r="A95" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B95" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C95" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="D95" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E95" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="F95" s="48"/>
+      <c r="G95" s="47"/>
+      <c r="H95" s="48"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="31" t="s">
@@ -3276,7 +3295,7 @@
         <v>2050</v>
       </c>
       <c r="C96" s="33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D96" s="33" t="s">
         <v>34</v>
@@ -3284,12 +3303,8 @@
       <c r="E96" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F96" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G96" s="32" t="s">
-        <v>63</v>
-      </c>
+      <c r="F96" s="33"/>
+      <c r="G96" s="32"/>
       <c r="H96" s="33"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
@@ -3300,7 +3315,7 @@
         <v>2050</v>
       </c>
       <c r="C97" s="33" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D97" s="33" t="s">
         <v>34</v>
@@ -3308,12 +3323,8 @@
       <c r="E97" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F97" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G97" s="32" t="s">
-        <v>63</v>
-      </c>
+      <c r="F97" s="33"/>
+      <c r="G97" s="32"/>
       <c r="H97" s="33"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
@@ -3324,7 +3335,7 @@
         <v>2050</v>
       </c>
       <c r="C98" s="33" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D98" s="33" t="s">
         <v>34</v>
@@ -3333,10 +3344,10 @@
         <v>38</v>
       </c>
       <c r="F98" s="33" t="s">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="G98" s="32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H98" s="33"/>
     </row>
@@ -3348,7 +3359,7 @@
         <v>2050</v>
       </c>
       <c r="C99" s="33" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="D99" s="33" t="s">
         <v>34</v>
@@ -3357,10 +3368,10 @@
         <v>38</v>
       </c>
       <c r="F99" s="33" t="s">
-        <v>120</v>
+        <v>66</v>
       </c>
       <c r="G99" s="32" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H99" s="33"/>
     </row>
@@ -3372,7 +3383,7 @@
         <v>2050</v>
       </c>
       <c r="C100" s="33" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="D100" s="33" t="s">
         <v>34</v>
@@ -3381,10 +3392,10 @@
         <v>38</v>
       </c>
       <c r="F100" s="33" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G100" s="32" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H100" s="33"/>
     </row>
@@ -3396,7 +3407,7 @@
         <v>2050</v>
       </c>
       <c r="C101" s="33" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D101" s="33" t="s">
         <v>34</v>
@@ -3405,10 +3416,10 @@
         <v>38</v>
       </c>
       <c r="F101" s="33" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G101" s="32" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H101" s="33"/>
     </row>
@@ -3420,95 +3431,95 @@
         <v>2050</v>
       </c>
       <c r="C102" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D102" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E102" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F102" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="G102" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="H102" s="33"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B103" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C103" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D103" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E103" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F103" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="G103" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="H103" s="33"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B104" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C104" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="D102" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E102" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F102" s="33" t="s">
+      <c r="D104" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E104" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F104" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="G102" s="32" t="s">
+      <c r="G104" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="H102" s="33" t="s">
+      <c r="H104" s="33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B103" s="53">
-        <v>2050</v>
-      </c>
-      <c r="C103" s="54" t="s">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B105" s="53">
+        <v>2050</v>
+      </c>
+      <c r="C105" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="D103" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E103" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F103" s="54" t="s">
+      <c r="D105" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E105" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F105" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G103" s="53" t="s">
+      <c r="G105" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H103" s="54"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B104" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C104" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="D104" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E104" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F104" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G104" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H104" s="55"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B105" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C105" s="55" t="s">
-        <v>102</v>
-      </c>
-      <c r="D105" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E105" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F105" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G105" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H105" s="55"/>
+      <c r="H105" s="54"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="55" t="s">
@@ -3518,7 +3529,7 @@
         <v>2050</v>
       </c>
       <c r="C106" s="55" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D106" s="55" t="s">
         <v>91</v>
@@ -3542,7 +3553,7 @@
         <v>2050</v>
       </c>
       <c r="C107" s="55" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D107" s="55" t="s">
         <v>91</v>
@@ -3566,7 +3577,7 @@
         <v>2050</v>
       </c>
       <c r="C108" s="55" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D108" s="55" t="s">
         <v>91</v>
@@ -3590,7 +3601,7 @@
         <v>2050</v>
       </c>
       <c r="C109" s="55" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D109" s="55" t="s">
         <v>91</v>
@@ -3598,11 +3609,11 @@
       <c r="E109" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F109" s="19" t="s">
-        <v>118</v>
+      <c r="F109" s="55" t="s">
+        <v>116</v>
       </c>
       <c r="G109" s="56" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H109" s="55"/>
     </row>
@@ -3614,7 +3625,7 @@
         <v>2050</v>
       </c>
       <c r="C110" s="55" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D110" s="55" t="s">
         <v>91</v>
@@ -3638,7 +3649,7 @@
         <v>2050</v>
       </c>
       <c r="C111" s="55" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D111" s="55" t="s">
         <v>91</v>
@@ -3646,11 +3657,11 @@
       <c r="E111" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F111" s="55" t="s">
-        <v>116</v>
+      <c r="F111" s="19" t="s">
+        <v>118</v>
       </c>
       <c r="G111" s="56" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H111" s="55"/>
     </row>
@@ -3662,7 +3673,7 @@
         <v>2050</v>
       </c>
       <c r="C112" s="55" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D112" s="55" t="s">
         <v>91</v>
@@ -3686,7 +3697,7 @@
         <v>2050</v>
       </c>
       <c r="C113" s="55" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D113" s="55" t="s">
         <v>91</v>
@@ -3695,10 +3706,10 @@
         <v>38</v>
       </c>
       <c r="F113" s="55" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G113" s="56" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H113" s="55"/>
     </row>
@@ -3710,7 +3721,7 @@
         <v>2050</v>
       </c>
       <c r="C114" s="55" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="D114" s="55" t="s">
         <v>91</v>
@@ -3718,13 +3729,13 @@
       <c r="E114" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F114" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="G114" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="H114" s="19"/>
+      <c r="F114" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G114" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="H114" s="55"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="55" t="s">
@@ -3734,7 +3745,7 @@
         <v>2050</v>
       </c>
       <c r="C115" s="55" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D115" s="55" t="s">
         <v>91</v>
@@ -3742,13 +3753,13 @@
       <c r="E115" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F115" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="G115" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="H115" s="19"/>
+      <c r="F115" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="G115" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="H115" s="55"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="55" t="s">
@@ -3758,7 +3769,7 @@
         <v>2050</v>
       </c>
       <c r="C116" s="55" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="D116" s="55" t="s">
         <v>91</v>
@@ -3767,10 +3778,10 @@
         <v>38</v>
       </c>
       <c r="F116" s="19" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="G116" s="18" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="H116" s="19"/>
     </row>
@@ -3782,7 +3793,7 @@
         <v>2050</v>
       </c>
       <c r="C117" s="55" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="D117" s="55" t="s">
         <v>91</v>
@@ -3791,10 +3802,10 @@
         <v>38</v>
       </c>
       <c r="F117" s="19" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G117" s="18" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H117" s="19"/>
     </row>
@@ -3806,7 +3817,7 @@
         <v>2050</v>
       </c>
       <c r="C118" s="55" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D118" s="55" t="s">
         <v>91</v>
@@ -3820,9 +3831,7 @@
       <c r="G118" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H118" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H118" s="19"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="55" t="s">
@@ -3832,7 +3841,7 @@
         <v>2050</v>
       </c>
       <c r="C119" s="55" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D119" s="55" t="s">
         <v>91</v>
@@ -3856,7 +3865,7 @@
         <v>2050</v>
       </c>
       <c r="C120" s="55" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D120" s="55" t="s">
         <v>91</v>
@@ -3870,7 +3879,9 @@
       <c r="G120" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H120" s="19"/>
+      <c r="H120" s="19" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="55" t="s">
@@ -3880,7 +3891,7 @@
         <v>2050</v>
       </c>
       <c r="C121" s="55" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="D121" s="55" t="s">
         <v>91</v>
@@ -3894,9 +3905,7 @@
       <c r="G121" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H121" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H121" s="19"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="55" t="s">
@@ -3906,7 +3915,7 @@
         <v>2050</v>
       </c>
       <c r="C122" s="55" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="D122" s="55" t="s">
         <v>91</v>
@@ -3920,7 +3929,57 @@
       <c r="G122" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H122" s="19" t="s">
+      <c r="H122" s="19"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A123" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B123" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C123" s="55" t="s">
+        <v>164</v>
+      </c>
+      <c r="D123" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E123" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F123" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G123" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H123" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A124" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B124" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C124" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="D124" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E124" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F124" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G124" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H124" s="19" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 2050 FBP Plus Crossing V21 and 2050 FBP NP V22
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bespin\Documents\GitHub\travel-model-one\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A02ABE7-377C-4F2D-A3EE-F9DBF87AB392}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11220" yWindow="3900" windowWidth="20595" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11220" yWindow="3900" windowWidth="20595" windowHeight="12900"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="175">
   <si>
     <t>EEJ</t>
   </si>
@@ -544,12 +543,18 @@
   </si>
   <si>
     <t>2030_TM152_FBP_NoProject_21</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_PlusCrossing_21</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_NoProject_22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -780,7 +785,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1098,12 +1103,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H124"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F93" sqref="F93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3222,90 +3227,96 @@
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B93" s="24">
-        <v>2050</v>
-      </c>
-      <c r="C93" s="25" t="s">
+      <c r="A93" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B93" s="18">
+        <v>2050</v>
+      </c>
+      <c r="C93" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="D93" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E93" s="25" t="s">
+      <c r="D93" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E93" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F93" s="25" t="s">
+      <c r="F93" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="G93" s="24" t="s">
+      <c r="G93" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="H93" s="25" t="s">
+      <c r="H93" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B94" s="44">
-        <v>2050</v>
-      </c>
-      <c r="C94" s="45" t="s">
+      <c r="A94" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B94" s="24">
+        <v>2050</v>
+      </c>
+      <c r="C94" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="D94" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E94" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F94" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="G94" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="H94" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B95" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C95" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="D94" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E94" s="45" t="s">
+      <c r="D95" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E95" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="F94" s="45"/>
-      <c r="G94" s="44"/>
-      <c r="H94" s="45"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B95" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C95" s="48" t="s">
+      <c r="F95" s="45"/>
+      <c r="G95" s="44"/>
+      <c r="H95" s="45"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B96" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C96" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="D95" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E95" s="48" t="s">
+      <c r="D96" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E96" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F95" s="48"/>
-      <c r="G95" s="47"/>
-      <c r="H95" s="48"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B96" s="32">
-        <v>2050</v>
-      </c>
-      <c r="C96" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D96" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E96" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F96" s="33"/>
-      <c r="G96" s="32"/>
-      <c r="H96" s="33"/>
+      <c r="F96" s="48"/>
+      <c r="G96" s="47"/>
+      <c r="H96" s="48"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="31" t="s">
@@ -3315,7 +3326,7 @@
         <v>2050</v>
       </c>
       <c r="C97" s="33" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D97" s="33" t="s">
         <v>34</v>
@@ -3335,7 +3346,7 @@
         <v>2050</v>
       </c>
       <c r="C98" s="33" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D98" s="33" t="s">
         <v>34</v>
@@ -3343,12 +3354,8 @@
       <c r="E98" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F98" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G98" s="32" t="s">
-        <v>63</v>
-      </c>
+      <c r="F98" s="33"/>
+      <c r="G98" s="32"/>
       <c r="H98" s="33"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
@@ -3359,7 +3366,7 @@
         <v>2050</v>
       </c>
       <c r="C99" s="33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D99" s="33" t="s">
         <v>34</v>
@@ -3383,7 +3390,7 @@
         <v>2050</v>
       </c>
       <c r="C100" s="33" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D100" s="33" t="s">
         <v>34</v>
@@ -3392,10 +3399,10 @@
         <v>38</v>
       </c>
       <c r="F100" s="33" t="s">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="G100" s="32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H100" s="33"/>
     </row>
@@ -3407,7 +3414,7 @@
         <v>2050</v>
       </c>
       <c r="C101" s="33" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D101" s="33" t="s">
         <v>34</v>
@@ -3416,10 +3423,10 @@
         <v>38</v>
       </c>
       <c r="F101" s="33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G101" s="32" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H101" s="33"/>
     </row>
@@ -3431,7 +3438,7 @@
         <v>2050</v>
       </c>
       <c r="C102" s="33" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D102" s="33" t="s">
         <v>34</v>
@@ -3440,10 +3447,10 @@
         <v>38</v>
       </c>
       <c r="F102" s="33" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G102" s="32" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H102" s="33"/>
     </row>
@@ -3455,7 +3462,7 @@
         <v>2050</v>
       </c>
       <c r="C103" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D103" s="33" t="s">
         <v>34</v>
@@ -3464,10 +3471,10 @@
         <v>38</v>
       </c>
       <c r="F103" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G103" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H103" s="33"/>
     </row>
@@ -3479,71 +3486,71 @@
         <v>2050</v>
       </c>
       <c r="C104" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D104" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E104" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F104" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="G104" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="H104" s="33"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B105" s="32">
+        <v>2050</v>
+      </c>
+      <c r="C105" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="D104" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E104" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F104" s="33" t="s">
+      <c r="D105" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E105" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F105" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="G104" s="32" t="s">
+      <c r="G105" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="H104" s="33" t="s">
+      <c r="H105" s="33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B105" s="53">
-        <v>2050</v>
-      </c>
-      <c r="C105" s="54" t="s">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B106" s="53">
+        <v>2050</v>
+      </c>
+      <c r="C106" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="D105" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="E105" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="F105" s="54" t="s">
+      <c r="D106" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E106" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F106" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G105" s="53" t="s">
+      <c r="G106" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="H105" s="54"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B106" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C106" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="D106" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E106" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F106" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G106" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H106" s="55"/>
+      <c r="H106" s="54"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="55" t="s">
@@ -3553,7 +3560,7 @@
         <v>2050</v>
       </c>
       <c r="C107" s="55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D107" s="55" t="s">
         <v>91</v>
@@ -3577,7 +3584,7 @@
         <v>2050</v>
       </c>
       <c r="C108" s="55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D108" s="55" t="s">
         <v>91</v>
@@ -3601,7 +3608,7 @@
         <v>2050</v>
       </c>
       <c r="C109" s="55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D109" s="55" t="s">
         <v>91</v>
@@ -3625,7 +3632,7 @@
         <v>2050</v>
       </c>
       <c r="C110" s="55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D110" s="55" t="s">
         <v>91</v>
@@ -3649,7 +3656,7 @@
         <v>2050</v>
       </c>
       <c r="C111" s="55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D111" s="55" t="s">
         <v>91</v>
@@ -3657,11 +3664,11 @@
       <c r="E111" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F111" s="19" t="s">
-        <v>118</v>
+      <c r="F111" s="55" t="s">
+        <v>116</v>
       </c>
       <c r="G111" s="56" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H111" s="55"/>
     </row>
@@ -3673,7 +3680,7 @@
         <v>2050</v>
       </c>
       <c r="C112" s="55" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D112" s="55" t="s">
         <v>91</v>
@@ -3681,11 +3688,11 @@
       <c r="E112" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F112" s="55" t="s">
-        <v>116</v>
+      <c r="F112" s="19" t="s">
+        <v>118</v>
       </c>
       <c r="G112" s="56" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H112" s="55"/>
     </row>
@@ -3697,7 +3704,7 @@
         <v>2050</v>
       </c>
       <c r="C113" s="55" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D113" s="55" t="s">
         <v>91</v>
@@ -3721,7 +3728,7 @@
         <v>2050</v>
       </c>
       <c r="C114" s="55" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D114" s="55" t="s">
         <v>91</v>
@@ -3745,7 +3752,7 @@
         <v>2050</v>
       </c>
       <c r="C115" s="55" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D115" s="55" t="s">
         <v>91</v>
@@ -3754,10 +3761,10 @@
         <v>38</v>
       </c>
       <c r="F115" s="55" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G115" s="56" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H115" s="55"/>
     </row>
@@ -3769,7 +3776,7 @@
         <v>2050</v>
       </c>
       <c r="C116" s="55" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D116" s="55" t="s">
         <v>91</v>
@@ -3777,13 +3784,13 @@
       <c r="E116" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F116" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="G116" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="H116" s="19"/>
+      <c r="F116" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="G116" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="H116" s="55"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="55" t="s">
@@ -3793,7 +3800,7 @@
         <v>2050</v>
       </c>
       <c r="C117" s="55" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D117" s="55" t="s">
         <v>91</v>
@@ -3802,10 +3809,10 @@
         <v>38</v>
       </c>
       <c r="F117" s="19" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G117" s="18" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H117" s="19"/>
     </row>
@@ -3817,7 +3824,7 @@
         <v>2050</v>
       </c>
       <c r="C118" s="55" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D118" s="55" t="s">
         <v>91</v>
@@ -3826,10 +3833,10 @@
         <v>38</v>
       </c>
       <c r="F118" s="19" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G118" s="18" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H118" s="19"/>
     </row>
@@ -3841,7 +3848,7 @@
         <v>2050</v>
       </c>
       <c r="C119" s="55" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D119" s="55" t="s">
         <v>91</v>
@@ -3865,7 +3872,7 @@
         <v>2050</v>
       </c>
       <c r="C120" s="55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D120" s="55" t="s">
         <v>91</v>
@@ -3879,9 +3886,7 @@
       <c r="G120" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H120" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H120" s="19"/>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="55" t="s">
@@ -3891,7 +3896,7 @@
         <v>2050</v>
       </c>
       <c r="C121" s="55" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D121" s="55" t="s">
         <v>91</v>
@@ -3905,7 +3910,9 @@
       <c r="G121" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H121" s="19"/>
+      <c r="H121" s="19" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="55" t="s">
@@ -3915,7 +3922,7 @@
         <v>2050</v>
       </c>
       <c r="C122" s="55" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D122" s="55" t="s">
         <v>91</v>
@@ -3939,7 +3946,7 @@
         <v>2050</v>
       </c>
       <c r="C123" s="55" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D123" s="55" t="s">
         <v>91</v>
@@ -3953,9 +3960,7 @@
       <c r="G123" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H123" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="H123" s="19"/>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="55" t="s">
@@ -3965,7 +3970,7 @@
         <v>2050</v>
       </c>
       <c r="C124" s="55" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D124" s="55" t="s">
         <v>91</v>
@@ -3980,6 +3985,58 @@
         <v>137</v>
       </c>
       <c r="H124" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A125" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B125" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C125" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="D125" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E125" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F125" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G125" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H125" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A126" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B126" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C126" s="55" t="s">
+        <v>173</v>
+      </c>
+      <c r="D126" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E126" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F126" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G126" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H126" s="19" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove post-v15 and pre-final runs from "current"
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bespin\Documents\GitHub\travel-model-one\utilities\RTP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40B0DC6-6127-4661-89B1-B9E3E792AB8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11220" yWindow="3900" windowWidth="20595" windowHeight="12900"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="175">
   <si>
     <t>EEJ</t>
   </si>
@@ -554,7 +555,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -785,7 +786,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1103,24 +1104,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F93" sqref="F93"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.296875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="70.85546875" customWidth="1"/>
+    <col min="6" max="6" width="70.8984375" customWidth="1"/>
     <col min="7" max="7" width="15" style="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1146,7 +1147,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
@@ -1166,7 +1167,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
@@ -1186,7 +1187,7 @@
       <c r="G3" s="11"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>25</v>
       </c>
@@ -1206,7 +1207,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>25</v>
       </c>
@@ -1226,7 +1227,7 @@
       <c r="G5" s="15"/>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>25</v>
       </c>
@@ -1246,7 +1247,7 @@
       <c r="G6" s="15"/>
       <c r="H6" s="16"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>25</v>
       </c>
@@ -1266,7 +1267,7 @@
       <c r="G7" s="15"/>
       <c r="H7" s="16"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>25</v>
       </c>
@@ -1286,7 +1287,7 @@
       <c r="G8" s="15"/>
       <c r="H8" s="16"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>25</v>
       </c>
@@ -1306,7 +1307,7 @@
       <c r="G9" s="15"/>
       <c r="H9" s="16"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>25</v>
       </c>
@@ -1326,7 +1327,7 @@
       <c r="G10" s="21"/>
       <c r="H10" s="22"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>25</v>
       </c>
@@ -1346,7 +1347,7 @@
       <c r="G11" s="21"/>
       <c r="H11" s="22"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>25</v>
       </c>
@@ -1366,7 +1367,7 @@
       <c r="G12" s="21"/>
       <c r="H12" s="22"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>25</v>
       </c>
@@ -1386,7 +1387,7 @@
       <c r="G13" s="21"/>
       <c r="H13" s="22"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>25</v>
       </c>
@@ -1406,7 +1407,7 @@
       <c r="G14" s="21"/>
       <c r="H14" s="22"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>25</v>
       </c>
@@ -1426,7 +1427,7 @@
       <c r="G15" s="18"/>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>25</v>
       </c>
@@ -1446,7 +1447,7 @@
       <c r="G16" s="18"/>
       <c r="H16" s="19"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>25</v>
       </c>
@@ -1466,7 +1467,7 @@
       <c r="G17" s="18"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>25</v>
       </c>
@@ -1486,7 +1487,7 @@
       <c r="G18" s="18"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="23" t="s">
         <v>25</v>
       </c>
@@ -1506,7 +1507,7 @@
       <c r="G19" s="24"/>
       <c r="H19" s="25"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="26" t="s">
         <v>26</v>
       </c>
@@ -1528,7 +1529,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="26" t="s">
         <v>26</v>
       </c>
@@ -1548,7 +1549,7 @@
       <c r="G21" s="27"/>
       <c r="H21" s="28"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
         <v>26</v>
       </c>
@@ -1570,7 +1571,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>26</v>
       </c>
@@ -1594,7 +1595,7 @@
       </c>
       <c r="H23" s="50"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>26</v>
       </c>
@@ -1620,7 +1621,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
         <v>26</v>
       </c>
@@ -1646,7 +1647,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
         <v>26</v>
       </c>
@@ -1672,7 +1673,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="38" t="s">
         <v>26</v>
       </c>
@@ -1692,7 +1693,7 @@
       <c r="G27" s="39"/>
       <c r="H27" s="39"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="20" t="s">
         <v>26</v>
       </c>
@@ -1712,7 +1713,7 @@
       <c r="G28" s="21"/>
       <c r="H28" s="22"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>26</v>
       </c>
@@ -1734,7 +1735,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
         <v>26</v>
       </c>
@@ -1756,7 +1757,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="38" t="s">
         <v>26</v>
       </c>
@@ -1776,7 +1777,7 @@
       <c r="G31" s="39"/>
       <c r="H31" s="40"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="20" t="s">
         <v>26</v>
       </c>
@@ -1796,7 +1797,7 @@
       <c r="G32" s="21"/>
       <c r="H32" s="22"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>26</v>
       </c>
@@ -1816,7 +1817,7 @@
       <c r="G33" s="21"/>
       <c r="H33" s="22"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="20" t="s">
         <v>26</v>
       </c>
@@ -1836,7 +1837,7 @@
       <c r="G34" s="21"/>
       <c r="H34" s="22"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>26</v>
       </c>
@@ -1860,7 +1861,7 @@
       </c>
       <c r="H35" s="22"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="20" t="s">
         <v>26</v>
       </c>
@@ -1884,7 +1885,7 @@
       </c>
       <c r="H36" s="22"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="35" t="s">
         <v>26</v>
       </c>
@@ -1908,7 +1909,7 @@
       </c>
       <c r="H37" s="37"/>
     </row>
-    <row r="38" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="52" t="s">
         <v>26</v>
       </c>
@@ -1932,7 +1933,7 @@
       </c>
       <c r="H38" s="54"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
         <v>26</v>
       </c>
@@ -1956,7 +1957,7 @@
       </c>
       <c r="H39" s="19"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
         <v>26</v>
       </c>
@@ -1980,7 +1981,7 @@
       </c>
       <c r="H40" s="19"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
         <v>26</v>
       </c>
@@ -2004,7 +2005,7 @@
       </c>
       <c r="H41" s="19"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
         <v>26</v>
       </c>
@@ -2030,7 +2031,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
         <v>26</v>
       </c>
@@ -2054,7 +2055,7 @@
       </c>
       <c r="H43" s="19"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
         <v>26</v>
       </c>
@@ -2076,11 +2077,9 @@
       <c r="G44" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H44" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H44" s="19"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="17" t="s">
         <v>26</v>
       </c>
@@ -2102,11 +2101,9 @@
       <c r="G45" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="H45" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H45" s="19"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="23" t="s">
         <v>26</v>
       </c>
@@ -2132,7 +2129,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="38" t="s">
         <v>26</v>
       </c>
@@ -2152,7 +2149,7 @@
       <c r="G47" s="39"/>
       <c r="H47" s="40"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="35" t="s">
         <v>26</v>
       </c>
@@ -2172,7 +2169,7 @@
       <c r="G48" s="36"/>
       <c r="H48" s="37"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
         <v>26</v>
       </c>
@@ -2192,7 +2189,7 @@
       <c r="G49" s="21"/>
       <c r="H49" s="22"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="20" t="s">
         <v>26</v>
       </c>
@@ -2212,7 +2209,7 @@
       <c r="G50" s="21"/>
       <c r="H50" s="22"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="s">
         <v>26</v>
       </c>
@@ -2236,7 +2233,7 @@
       </c>
       <c r="H51" s="22"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="20" t="s">
         <v>26</v>
       </c>
@@ -2260,7 +2257,7 @@
       </c>
       <c r="H52" s="22"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="20" t="s">
         <v>26</v>
       </c>
@@ -2284,7 +2281,7 @@
       </c>
       <c r="H53" s="22"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="20" t="s">
         <v>26</v>
       </c>
@@ -2308,7 +2305,7 @@
       </c>
       <c r="H54" s="22"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="20" t="s">
         <v>26</v>
       </c>
@@ -2332,7 +2329,7 @@
       </c>
       <c r="H55" s="22"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="20" t="s">
         <v>26</v>
       </c>
@@ -2358,7 +2355,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="51" t="s">
         <v>26</v>
       </c>
@@ -2382,7 +2379,7 @@
       </c>
       <c r="H57" s="30"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="51" t="s">
         <v>26</v>
       </c>
@@ -2406,7 +2403,7 @@
       </c>
       <c r="H58" s="30"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="20" t="s">
         <v>26</v>
       </c>
@@ -2430,7 +2427,7 @@
       </c>
       <c r="H59" s="22"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="20" t="s">
         <v>26</v>
       </c>
@@ -2454,7 +2451,7 @@
       </c>
       <c r="H60" s="22"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="s">
         <v>26</v>
       </c>
@@ -2478,7 +2475,7 @@
       </c>
       <c r="H61" s="22"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="20" t="s">
         <v>26</v>
       </c>
@@ -2502,7 +2499,7 @@
       </c>
       <c r="H62" s="22"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="52" t="s">
         <v>26</v>
       </c>
@@ -2526,7 +2523,7 @@
       </c>
       <c r="H63" s="54"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="17" t="s">
         <v>26</v>
       </c>
@@ -2550,7 +2547,7 @@
       </c>
       <c r="H64" s="19"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="17" t="s">
         <v>26</v>
       </c>
@@ -2574,7 +2571,7 @@
       </c>
       <c r="H65" s="19"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="17" t="s">
         <v>26</v>
       </c>
@@ -2598,7 +2595,7 @@
       </c>
       <c r="H66" s="19"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="17" t="s">
         <v>26</v>
       </c>
@@ -2622,7 +2619,7 @@
       </c>
       <c r="H67" s="19"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="17" t="s">
         <v>26</v>
       </c>
@@ -2646,7 +2643,7 @@
       </c>
       <c r="H68" s="19"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="17" t="s">
         <v>26</v>
       </c>
@@ -2670,7 +2667,7 @@
       </c>
       <c r="H69" s="19"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="17" t="s">
         <v>26</v>
       </c>
@@ -2694,7 +2691,7 @@
       </c>
       <c r="H70" s="19"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="17" t="s">
         <v>26</v>
       </c>
@@ -2718,7 +2715,7 @@
       </c>
       <c r="H71" s="19"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="17" t="s">
         <v>26</v>
       </c>
@@ -2742,7 +2739,7 @@
       </c>
       <c r="H72" s="19"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="17" t="s">
         <v>26</v>
       </c>
@@ -2768,7 +2765,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="17" t="s">
         <v>26</v>
       </c>
@@ -2792,7 +2789,7 @@
       </c>
       <c r="H74" s="19"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="17" t="s">
         <v>26</v>
       </c>
@@ -2816,7 +2813,7 @@
       </c>
       <c r="H75" s="19"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="17" t="s">
         <v>26</v>
       </c>
@@ -2838,11 +2835,9 @@
       <c r="G76" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H76" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H76" s="19"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="23" t="s">
         <v>26</v>
       </c>
@@ -2868,7 +2863,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="41" t="s">
         <v>26</v>
       </c>
@@ -2888,7 +2883,7 @@
       <c r="G78" s="42"/>
       <c r="H78" s="43"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="31" t="s">
         <v>26</v>
       </c>
@@ -2908,7 +2903,7 @@
       <c r="G79" s="44"/>
       <c r="H79" s="45"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="31" t="s">
         <v>26</v>
       </c>
@@ -2932,7 +2927,7 @@
       </c>
       <c r="H80" s="45"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="31" t="s">
         <v>26</v>
       </c>
@@ -2956,7 +2951,7 @@
       </c>
       <c r="H81" s="45"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="31" t="s">
         <v>26</v>
       </c>
@@ -2980,7 +2975,7 @@
       </c>
       <c r="H82" s="45"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="31" t="s">
         <v>26</v>
       </c>
@@ -3004,7 +2999,7 @@
       </c>
       <c r="H83" s="45"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="46" t="s">
         <v>26</v>
       </c>
@@ -3028,7 +3023,7 @@
       </c>
       <c r="H84" s="48"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="17" t="s">
         <v>26</v>
       </c>
@@ -3052,7 +3047,7 @@
       </c>
       <c r="H85" s="19"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="17" t="s">
         <v>26</v>
       </c>
@@ -3076,7 +3071,7 @@
       </c>
       <c r="H86" s="19"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="17" t="s">
         <v>26</v>
       </c>
@@ -3100,7 +3095,7 @@
       </c>
       <c r="H87" s="19"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="17" t="s">
         <v>26</v>
       </c>
@@ -3124,7 +3119,7 @@
       </c>
       <c r="H88" s="19"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="17" t="s">
         <v>26</v>
       </c>
@@ -3150,7 +3145,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="17" t="s">
         <v>26</v>
       </c>
@@ -3174,7 +3169,7 @@
       </c>
       <c r="H90" s="19"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="17" t="s">
         <v>26</v>
       </c>
@@ -3196,11 +3191,9 @@
       <c r="G91" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H91" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H91" s="19"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="17" t="s">
         <v>26</v>
       </c>
@@ -3222,11 +3215,9 @@
       <c r="G92" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="H92" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H92" s="19"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="17" t="s">
         <v>26</v>
       </c>
@@ -3248,11 +3239,9 @@
       <c r="G93" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="H93" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H93" s="19"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="23" t="s">
         <v>26</v>
       </c>
@@ -3278,7 +3267,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="31" t="s">
         <v>26</v>
       </c>
@@ -3298,7 +3287,7 @@
       <c r="G95" s="44"/>
       <c r="H95" s="45"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="46" t="s">
         <v>26</v>
       </c>
@@ -3318,7 +3307,7 @@
       <c r="G96" s="47"/>
       <c r="H96" s="48"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="31" t="s">
         <v>26</v>
       </c>
@@ -3338,7 +3327,7 @@
       <c r="G97" s="32"/>
       <c r="H97" s="33"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="31" t="s">
         <v>26</v>
       </c>
@@ -3358,7 +3347,7 @@
       <c r="G98" s="32"/>
       <c r="H98" s="33"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="31" t="s">
         <v>26</v>
       </c>
@@ -3382,7 +3371,7 @@
       </c>
       <c r="H99" s="33"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="31" t="s">
         <v>26</v>
       </c>
@@ -3406,7 +3395,7 @@
       </c>
       <c r="H100" s="33"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="31" t="s">
         <v>26</v>
       </c>
@@ -3430,7 +3419,7 @@
       </c>
       <c r="H101" s="33"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="31" t="s">
         <v>26</v>
       </c>
@@ -3454,7 +3443,7 @@
       </c>
       <c r="H102" s="33"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="31" t="s">
         <v>26</v>
       </c>
@@ -3478,7 +3467,7 @@
       </c>
       <c r="H103" s="33"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="31" t="s">
         <v>26</v>
       </c>
@@ -3502,7 +3491,7 @@
       </c>
       <c r="H104" s="33"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="31" t="s">
         <v>26</v>
       </c>
@@ -3528,7 +3517,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="52" t="s">
         <v>26</v>
       </c>
@@ -3552,7 +3541,7 @@
       </c>
       <c r="H106" s="54"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="55" t="s">
         <v>26</v>
       </c>
@@ -3576,7 +3565,7 @@
       </c>
       <c r="H107" s="55"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="55" t="s">
         <v>26</v>
       </c>
@@ -3600,7 +3589,7 @@
       </c>
       <c r="H108" s="55"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="55" t="s">
         <v>26</v>
       </c>
@@ -3624,7 +3613,7 @@
       </c>
       <c r="H109" s="55"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="55" t="s">
         <v>26</v>
       </c>
@@ -3648,7 +3637,7 @@
       </c>
       <c r="H110" s="55"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="55" t="s">
         <v>26</v>
       </c>
@@ -3672,7 +3661,7 @@
       </c>
       <c r="H111" s="55"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="55" t="s">
         <v>26</v>
       </c>
@@ -3696,7 +3685,7 @@
       </c>
       <c r="H112" s="55"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="55" t="s">
         <v>26</v>
       </c>
@@ -3720,7 +3709,7 @@
       </c>
       <c r="H113" s="55"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="55" t="s">
         <v>26</v>
       </c>
@@ -3744,7 +3733,7 @@
       </c>
       <c r="H114" s="55"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="55" t="s">
         <v>26</v>
       </c>
@@ -3768,7 +3757,7 @@
       </c>
       <c r="H115" s="55"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="55" t="s">
         <v>26</v>
       </c>
@@ -3792,7 +3781,7 @@
       </c>
       <c r="H116" s="55"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="55" t="s">
         <v>26</v>
       </c>
@@ -3816,7 +3805,7 @@
       </c>
       <c r="H117" s="19"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="55" t="s">
         <v>26</v>
       </c>
@@ -3840,7 +3829,7 @@
       </c>
       <c r="H118" s="19"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="55" t="s">
         <v>26</v>
       </c>
@@ -3864,7 +3853,7 @@
       </c>
       <c r="H119" s="19"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="55" t="s">
         <v>26</v>
       </c>
@@ -3888,7 +3877,7 @@
       </c>
       <c r="H120" s="19"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="55" t="s">
         <v>26</v>
       </c>
@@ -3914,7 +3903,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="55" t="s">
         <v>26</v>
       </c>
@@ -3938,7 +3927,7 @@
       </c>
       <c r="H122" s="19"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="55" t="s">
         <v>26</v>
       </c>
@@ -3962,7 +3951,7 @@
       </c>
       <c r="H123" s="19"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="55" t="s">
         <v>26</v>
       </c>
@@ -3984,11 +3973,9 @@
       <c r="G124" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H124" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H124" s="19"/>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="55" t="s">
         <v>26</v>
       </c>
@@ -4010,11 +3997,9 @@
       <c r="G125" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H125" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H125" s="19"/>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="55" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Added 2025/2030 FBP v21 runs
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2EA11F-EDA0-4D84-B941-B98F30294E2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C0415B-9ACE-4859-A002-D9EF75742809}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="2880" windowWidth="21075" windowHeight="15645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="22830" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="180">
   <si>
     <t>EEJ</t>
   </si>
@@ -559,6 +559,12 @@
   </si>
   <si>
     <t>2040_TM152_FBP_Plus_20</t>
+  </si>
+  <si>
+    <t>2025_TM152_FBP_Plus_21</t>
+  </si>
+  <si>
+    <t>2030_TM152_FBP_Plus_21</t>
   </si>
 </sst>
 </file>
@@ -1130,11 +1136,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H129"/>
+  <dimension ref="A1:H131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1673,142 +1679,150 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="34">
+      <c r="A26" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="19">
         <v>2025</v>
       </c>
-      <c r="C26" s="35" t="s">
+      <c r="C26" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="D26" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" s="35" t="s">
+      <c r="D26" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="G26" s="34" t="s">
+      <c r="G26" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="H26" s="35" t="s">
+      <c r="H26" s="20"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="34">
+        <v>2025</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="G27" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="H27" s="35" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="16">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="16">
         <v>2030</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C28" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="D27" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E27" s="17" t="s">
+      <c r="D28" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="F28" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="G28" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="H27" s="17" t="s">
+      <c r="H28" s="17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="19">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="19">
         <v>2030</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C29" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="D28" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F28" s="35" t="s">
+      <c r="D29" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="G28" s="34" t="s">
+      <c r="G29" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="H28" s="35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="37">
-        <v>2035</v>
-      </c>
-      <c r="C29" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="E29" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="F29" s="38"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
+      <c r="H29" s="20"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B30" s="19">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>93</v>
+        <v>179</v>
       </c>
       <c r="D30" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="G30" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="H30" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="37">
+        <v>2035</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="E31" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="20"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="20"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F31" s="20"/>
+      <c r="F31" s="38"/>
       <c r="G31" s="19"/>
-      <c r="H31" s="20"/>
+      <c r="H31" s="19"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
@@ -1818,7 +1832,7 @@
         <v>2035</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>158</v>
+        <v>93</v>
       </c>
       <c r="D32" s="20" t="s">
         <v>28</v>
@@ -1828,29 +1842,27 @@
       </c>
       <c r="F32" s="20"/>
       <c r="G32" s="19"/>
-      <c r="H32" s="20" t="s">
-        <v>43</v>
-      </c>
+      <c r="H32" s="20"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="37">
-        <v>2035</v>
-      </c>
-      <c r="C33" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="D33" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33" s="38"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="38"/>
+      <c r="A33" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" s="20"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="20"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
@@ -1859,38 +1871,40 @@
       <c r="B34" s="19">
         <v>2035</v>
       </c>
-      <c r="C34" s="18" t="s">
-        <v>44</v>
+      <c r="C34" s="20" t="s">
+        <v>158</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="F34" s="20"/>
       <c r="G34" s="19"/>
-      <c r="H34" s="20"/>
+      <c r="H34" s="20" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D35" s="20" t="s">
+      <c r="A35" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="37">
+        <v>2035</v>
+      </c>
+      <c r="C35" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="E35" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="20"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="20"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="38"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
@@ -1900,7 +1914,7 @@
         <v>2035</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D36" s="20" t="s">
         <v>34</v>
@@ -1920,7 +1934,7 @@
         <v>2035</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="D37" s="20" t="s">
         <v>34</v>
@@ -1928,12 +1942,8 @@
       <c r="E37" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="F37" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="G37" s="19" t="s">
-        <v>74</v>
-      </c>
+      <c r="F37" s="20"/>
+      <c r="G37" s="19"/>
       <c r="H37" s="20"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1944,7 +1954,7 @@
         <v>2035</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D38" s="20" t="s">
         <v>34</v>
@@ -1952,109 +1962,105 @@
       <c r="E38" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="F38" s="20" t="s">
+      <c r="F38" s="20"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="20"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="H39" s="20"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="G38" s="19" t="s">
+      <c r="G40" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="H38" s="20"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="34">
-        <v>2035</v>
-      </c>
-      <c r="C39" s="33" t="s">
+      <c r="H40" s="20"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C41" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="D39" s="35" t="s">
+      <c r="D41" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="E39" s="35" t="s">
+      <c r="E41" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F39" s="35" t="s">
+      <c r="F41" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="G39" s="34" t="s">
+      <c r="G41" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="H39" s="35"/>
-    </row>
-    <row r="40" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="51">
-        <v>2035</v>
-      </c>
-      <c r="C40" s="52" t="s">
+      <c r="H41" s="35"/>
+    </row>
+    <row r="42" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="51">
+        <v>2035</v>
+      </c>
+      <c r="C42" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="D40" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="E40" s="52" t="s">
+      <c r="D42" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="F40" s="52" t="s">
+      <c r="F42" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="G40" s="51" t="s">
+      <c r="G42" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="H40" s="52"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B41" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="G41" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="H41" s="17"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E42" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="G42" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="H42" s="17"/>
+      <c r="H42" s="52"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
@@ -2064,7 +2070,7 @@
         <v>2035</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="D43" s="17" t="s">
         <v>91</v>
@@ -2073,10 +2079,10 @@
         <v>7</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="G43" s="16" t="s">
-        <v>137</v>
+        <v>82</v>
       </c>
       <c r="H43" s="17"/>
     </row>
@@ -2088,7 +2094,7 @@
         <v>2035</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="D44" s="17" t="s">
         <v>91</v>
@@ -2097,14 +2103,12 @@
         <v>7</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="G44" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="H44" s="17" t="s">
-        <v>43</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="H44" s="17"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
@@ -2114,7 +2118,7 @@
         <v>2035</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="D45" s="17" t="s">
         <v>91</v>
@@ -2138,7 +2142,7 @@
         <v>2035</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="D46" s="17" t="s">
         <v>91</v>
@@ -2147,12 +2151,14 @@
         <v>7</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="G46" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H46" s="17"/>
+      <c r="H46" s="17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
@@ -2162,7 +2168,7 @@
         <v>2035</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="D47" s="17" t="s">
         <v>91</v>
@@ -2171,118 +2177,126 @@
         <v>7</v>
       </c>
       <c r="F47" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="G47" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H47" s="17"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="G48" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H48" s="17"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="G47" s="16" t="s">
+      <c r="G49" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="H47" s="17"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B48" s="22">
-        <v>2035</v>
-      </c>
-      <c r="C48" s="23" t="s">
+      <c r="H49" s="17"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="22">
+        <v>2035</v>
+      </c>
+      <c r="C50" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="D48" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E48" s="23" t="s">
+      <c r="D50" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="E50" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F48" s="23" t="s">
+      <c r="F50" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="G48" s="22" t="s">
+      <c r="G50" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="H48" s="23" t="s">
+      <c r="H50" s="23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="B49" s="37">
-        <v>2035</v>
-      </c>
-      <c r="C49" s="38" t="s">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="37">
+        <v>2035</v>
+      </c>
+      <c r="C51" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D49" s="38" t="s">
+      <c r="D51" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="E49" s="38" t="s">
+      <c r="E51" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="F49" s="38"/>
-      <c r="G49" s="37"/>
-      <c r="H49" s="38"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50" s="34">
-        <v>2035</v>
-      </c>
-      <c r="C50" s="35" t="s">
+      <c r="F51" s="38"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="38"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C52" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="D50" s="35" t="s">
+      <c r="D52" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="E50" s="35" t="s">
+      <c r="E52" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="F50" s="35"/>
-      <c r="G50" s="34"/>
-      <c r="H50" s="35"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B51" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C51" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D51" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E51" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F51" s="20"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="20"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B52" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C52" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D52" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E52" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F52" s="20"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="20"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="34"/>
+      <c r="H52" s="35"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="18" t="s">
@@ -2292,7 +2306,7 @@
         <v>2035</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D53" s="20" t="s">
         <v>34</v>
@@ -2300,12 +2314,8 @@
       <c r="E53" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F53" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="G53" s="19" t="s">
-        <v>64</v>
-      </c>
+      <c r="F53" s="20"/>
+      <c r="G53" s="19"/>
       <c r="H53" s="20"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -2316,7 +2326,7 @@
         <v>2035</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D54" s="20" t="s">
         <v>34</v>
@@ -2324,12 +2334,8 @@
       <c r="E54" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F54" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="G54" s="19" t="s">
-        <v>65</v>
-      </c>
+      <c r="F54" s="20"/>
+      <c r="G54" s="19"/>
       <c r="H54" s="20"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -2340,7 +2346,7 @@
         <v>2035</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D55" s="20" t="s">
         <v>34</v>
@@ -2349,10 +2355,10 @@
         <v>38</v>
       </c>
       <c r="F55" s="20" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="G55" s="19" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H55" s="20"/>
     </row>
@@ -2364,7 +2370,7 @@
         <v>2035</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="D56" s="20" t="s">
         <v>34</v>
@@ -2373,10 +2379,10 @@
         <v>38</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G56" s="19" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H56" s="20"/>
     </row>
@@ -2388,7 +2394,7 @@
         <v>2035</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D57" s="20" t="s">
         <v>34</v>
@@ -2397,10 +2403,10 @@
         <v>38</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H57" s="20"/>
     </row>
@@ -2412,7 +2418,7 @@
         <v>2035</v>
       </c>
       <c r="C58" s="20" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D58" s="20" t="s">
         <v>34</v>
@@ -2421,110 +2427,110 @@
         <v>38</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G58" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="H58" s="20" t="s">
-        <v>43</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="H58" s="20"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B59" s="27">
-        <v>2035</v>
-      </c>
-      <c r="C59" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D59" s="28" t="s">
+      <c r="A59" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D59" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E59" s="28" t="s">
+      <c r="E59" s="20" t="s">
         <v>38</v>
       </c>
       <c r="F59" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="G59" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="H59" s="28"/>
+        <v>118</v>
+      </c>
+      <c r="G59" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="H59" s="20"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B60" s="27">
-        <v>2035</v>
-      </c>
-      <c r="C60" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="D60" s="28" t="s">
+      <c r="A60" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B60" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D60" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E60" s="28" t="s">
+      <c r="E60" s="20" t="s">
         <v>38</v>
       </c>
       <c r="F60" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="G60" s="27" t="s">
+      <c r="G60" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="H60" s="28"/>
+      <c r="H60" s="20" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B61" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C61" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="D61" s="20" t="s">
+      <c r="A61" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" s="27">
+        <v>2035</v>
+      </c>
+      <c r="C61" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="D61" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E61" s="20" t="s">
+      <c r="E61" s="28" t="s">
         <v>38</v>
       </c>
       <c r="F61" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="G61" s="19" t="s">
+      <c r="G61" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="H61" s="20"/>
+      <c r="H61" s="28"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B62" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C62" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D62" s="20" t="s">
+      <c r="A62" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="27">
+        <v>2035</v>
+      </c>
+      <c r="C62" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D62" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E62" s="20" t="s">
+      <c r="E62" s="28" t="s">
         <v>38</v>
       </c>
       <c r="F62" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="G62" s="19" t="s">
+      <c r="G62" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="H62" s="20"/>
+      <c r="H62" s="28"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="18" t="s">
@@ -2534,7 +2540,7 @@
         <v>2035</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D63" s="20" t="s">
         <v>34</v>
@@ -2558,7 +2564,7 @@
         <v>2035</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D64" s="20" t="s">
         <v>34</v>
@@ -2575,76 +2581,76 @@
       <c r="H64" s="20"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B65" s="51">
-        <v>2035</v>
-      </c>
-      <c r="C65" s="52" t="s">
+      <c r="A65" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B65" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D65" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E65" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F65" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="G65" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="H65" s="20"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B66" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C66" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D66" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E66" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F66" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="G66" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="H66" s="20"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" s="51">
+        <v>2035</v>
+      </c>
+      <c r="C67" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="D65" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="E65" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="F65" s="52" t="s">
+      <c r="D67" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="E67" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="F67" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="G65" s="51" t="s">
+      <c r="G67" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="H65" s="52"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B66" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C66" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="D66" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E66" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F66" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="G66" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="H66" s="17"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B67" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C67" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="D67" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E67" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F67" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="G67" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="H67" s="17"/>
+      <c r="H67" s="52"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="15" t="s">
@@ -2654,7 +2660,7 @@
         <v>2035</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="D68" s="17" t="s">
         <v>91</v>
@@ -2678,7 +2684,7 @@
         <v>2035</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D69" s="17" t="s">
         <v>91</v>
@@ -2702,7 +2708,7 @@
         <v>2035</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D70" s="17" t="s">
         <v>91</v>
@@ -2711,10 +2717,10 @@
         <v>38</v>
       </c>
       <c r="F70" s="17" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G70" s="16" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H70" s="17"/>
     </row>
@@ -2726,7 +2732,7 @@
         <v>2035</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D71" s="17" t="s">
         <v>91</v>
@@ -2735,10 +2741,10 @@
         <v>38</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="G71" s="16" t="s">
-        <v>128</v>
+        <v>82</v>
       </c>
       <c r="H71" s="17"/>
     </row>
@@ -2750,7 +2756,7 @@
         <v>2035</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="D72" s="17" t="s">
         <v>91</v>
@@ -2759,10 +2765,10 @@
         <v>38</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="G72" s="16" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="H72" s="17"/>
     </row>
@@ -2774,7 +2780,7 @@
         <v>2035</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D73" s="17" t="s">
         <v>91</v>
@@ -2783,10 +2789,10 @@
         <v>38</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G73" s="16" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H73" s="17"/>
     </row>
@@ -2798,7 +2804,7 @@
         <v>2035</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D74" s="17" t="s">
         <v>91</v>
@@ -2807,10 +2813,10 @@
         <v>38</v>
       </c>
       <c r="F74" s="17" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G74" s="16" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H74" s="17"/>
     </row>
@@ -2822,7 +2828,7 @@
         <v>2035</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D75" s="17" t="s">
         <v>91</v>
@@ -2831,14 +2837,12 @@
         <v>38</v>
       </c>
       <c r="F75" s="17" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G75" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="H75" s="17" t="s">
-        <v>43</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="H75" s="17"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="15" t="s">
@@ -2848,7 +2852,7 @@
         <v>2035</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D76" s="17" t="s">
         <v>91</v>
@@ -2872,7 +2876,7 @@
         <v>2035</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="D77" s="17" t="s">
         <v>91</v>
@@ -2886,7 +2890,9 @@
       <c r="G77" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H77" s="17"/>
+      <c r="H77" s="17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
@@ -2896,7 +2902,7 @@
         <v>2035</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D78" s="17" t="s">
         <v>91</v>
@@ -2913,120 +2919,124 @@
       <c r="H78" s="17"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B79" s="22">
-        <v>2035</v>
-      </c>
-      <c r="C79" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="D79" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E79" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F79" s="23" t="s">
+      <c r="A79" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B79" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C79" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D79" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E79" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F79" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="G79" s="22" t="s">
+      <c r="G79" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H79" s="23" t="s">
-        <v>43</v>
-      </c>
+      <c r="H79" s="17"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B80" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C80" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D80" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E80" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F80" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="G80" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H80" s="17"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B81" s="22">
+        <v>2035</v>
+      </c>
+      <c r="C81" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="D81" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="E81" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F81" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="G81" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="H81" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B82" s="16">
         <v>2040</v>
       </c>
-      <c r="C80" s="17" t="s">
+      <c r="C82" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="D80" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E80" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F80" s="23" t="s">
+      <c r="D82" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E82" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F82" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="G80" s="22" t="s">
+      <c r="G82" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="H80" s="23" t="s">
+      <c r="H82" s="23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="B81" s="40">
-        <v>2050</v>
-      </c>
-      <c r="C81" s="41" t="s">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B83" s="40">
+        <v>2050</v>
+      </c>
+      <c r="C83" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D81" s="41" t="s">
+      <c r="D83" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="E81" s="41" t="s">
+      <c r="E83" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F81" s="41"/>
-      <c r="G81" s="40"/>
-      <c r="H81" s="41"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B82" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C82" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="D82" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E82" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="F82" s="43"/>
-      <c r="G82" s="42"/>
-      <c r="H82" s="43"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B83" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C83" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="D83" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E83" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="F83" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="G83" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="H83" s="43"/>
+      <c r="F83" s="41"/>
+      <c r="G83" s="40"/>
+      <c r="H83" s="41"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="29" t="s">
@@ -3036,7 +3046,7 @@
         <v>2050</v>
       </c>
       <c r="C84" s="43" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="D84" s="43" t="s">
         <v>34</v>
@@ -3044,12 +3054,8 @@
       <c r="E84" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F84" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="G84" s="42" t="s">
-        <v>65</v>
-      </c>
+      <c r="F84" s="43"/>
+      <c r="G84" s="42"/>
       <c r="H84" s="43"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -3060,7 +3066,7 @@
         <v>2050</v>
       </c>
       <c r="C85" s="43" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D85" s="43" t="s">
         <v>34</v>
@@ -3069,10 +3075,10 @@
         <v>7</v>
       </c>
       <c r="F85" s="43" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G85" s="42" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H85" s="43"/>
     </row>
@@ -3084,7 +3090,7 @@
         <v>2050</v>
       </c>
       <c r="C86" s="43" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D86" s="43" t="s">
         <v>34</v>
@@ -3093,84 +3099,84 @@
         <v>7</v>
       </c>
       <c r="F86" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="G86" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="H86" s="43"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B87" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C87" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D87" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E87" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F87" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="G87" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="H87" s="43"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B88" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C88" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="D88" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E88" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F88" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="G86" s="42" t="s">
+      <c r="G88" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="H86" s="43"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B87" s="45">
-        <v>2050</v>
-      </c>
-      <c r="C87" s="46" t="s">
+      <c r="H88" s="43"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="B89" s="45">
+        <v>2050</v>
+      </c>
+      <c r="C89" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="D87" s="46" t="s">
+      <c r="D89" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="E87" s="46" t="s">
+      <c r="E89" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="F87" s="46" t="s">
+      <c r="F89" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="G87" s="45" t="s">
+      <c r="G89" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="H87" s="46"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B88" s="16">
-        <v>2050</v>
-      </c>
-      <c r="C88" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="D88" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="E88" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F88" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="G88" s="54" t="s">
-        <v>75</v>
-      </c>
-      <c r="H88" s="17"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B89" s="16">
-        <v>2050</v>
-      </c>
-      <c r="C89" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D89" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E89" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F89" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="G89" s="54" t="s">
-        <v>82</v>
-      </c>
-      <c r="H89" s="17"/>
+      <c r="H89" s="46"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="15" t="s">
@@ -3180,19 +3186,19 @@
         <v>2050</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="D90" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D90" s="52" t="s">
         <v>91</v>
       </c>
       <c r="E90" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F90" s="17" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G90" s="54" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="H90" s="17"/>
     </row>
@@ -3204,7 +3210,7 @@
         <v>2050</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>138</v>
+        <v>100</v>
       </c>
       <c r="D91" s="17" t="s">
         <v>91</v>
@@ -3213,10 +3219,10 @@
         <v>7</v>
       </c>
       <c r="F91" s="17" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="G91" s="54" t="s">
-        <v>137</v>
+        <v>82</v>
       </c>
       <c r="H91" s="17"/>
     </row>
@@ -3228,7 +3234,7 @@
         <v>2050</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="D92" s="17" t="s">
         <v>91</v>
@@ -3237,14 +3243,12 @@
         <v>7</v>
       </c>
       <c r="F92" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="G92" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="H92" s="17" t="s">
-        <v>43</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="G92" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="H92" s="17"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="15" t="s">
@@ -3254,7 +3258,7 @@
         <v>2050</v>
       </c>
       <c r="C93" s="17" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="D93" s="17" t="s">
         <v>91</v>
@@ -3265,7 +3269,7 @@
       <c r="F93" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="G93" s="16" t="s">
+      <c r="G93" s="54" t="s">
         <v>137</v>
       </c>
       <c r="H93" s="17"/>
@@ -3278,7 +3282,7 @@
         <v>2050</v>
       </c>
       <c r="C94" s="17" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D94" s="17" t="s">
         <v>91</v>
@@ -3287,12 +3291,14 @@
         <v>7</v>
       </c>
       <c r="F94" s="17" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="G94" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H94" s="17"/>
+      <c r="H94" s="17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="15" t="s">
@@ -3302,7 +3308,7 @@
         <v>2050</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D95" s="17" t="s">
         <v>91</v>
@@ -3311,10 +3317,10 @@
         <v>7</v>
       </c>
       <c r="F95" s="17" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="G95" s="16" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="H95" s="17"/>
     </row>
@@ -3326,7 +3332,7 @@
         <v>2050</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="D96" s="17" t="s">
         <v>91</v>
@@ -3335,118 +3341,126 @@
         <v>7</v>
       </c>
       <c r="F96" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="G96" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H96" s="17"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B97" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C97" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="D97" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E97" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F97" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="G97" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="H97" s="17"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B98" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C98" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D98" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E98" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F98" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="G96" s="16" t="s">
+      <c r="G98" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="H96" s="17"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B97" s="22">
-        <v>2050</v>
-      </c>
-      <c r="C97" s="23" t="s">
+      <c r="H98" s="17"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B99" s="22">
+        <v>2050</v>
+      </c>
+      <c r="C99" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="D97" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E97" s="23" t="s">
+      <c r="D99" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="E99" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F97" s="23" t="s">
+      <c r="F99" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="G97" s="22" t="s">
+      <c r="G99" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="H97" s="23" t="s">
+      <c r="H99" s="23" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B98" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C98" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="D98" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E98" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="F98" s="43"/>
-      <c r="G98" s="42"/>
-      <c r="H98" s="43"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B99" s="45">
-        <v>2050</v>
-      </c>
-      <c r="C99" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="D99" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="E99" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="F99" s="46"/>
-      <c r="G99" s="45"/>
-      <c r="H99" s="46"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B100" s="30">
-        <v>2050</v>
-      </c>
-      <c r="C100" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="D100" s="31" t="s">
+      <c r="B100" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C100" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="D100" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E100" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="F100" s="31"/>
-      <c r="G100" s="30"/>
-      <c r="H100" s="31"/>
+      <c r="E100" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="F100" s="43"/>
+      <c r="G100" s="42"/>
+      <c r="H100" s="43"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B101" s="30">
-        <v>2050</v>
-      </c>
-      <c r="C101" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="D101" s="31" t="s">
+      <c r="A101" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="B101" s="45">
+        <v>2050</v>
+      </c>
+      <c r="C101" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="D101" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="E101" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="F101" s="31"/>
-      <c r="G101" s="30"/>
-      <c r="H101" s="31"/>
+      <c r="E101" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="F101" s="46"/>
+      <c r="G101" s="45"/>
+      <c r="H101" s="46"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="29" t="s">
@@ -3456,7 +3470,7 @@
         <v>2050</v>
       </c>
       <c r="C102" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D102" s="31" t="s">
         <v>34</v>
@@ -3464,12 +3478,8 @@
       <c r="E102" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="F102" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="G102" s="30" t="s">
-        <v>63</v>
-      </c>
+      <c r="F102" s="31"/>
+      <c r="G102" s="30"/>
       <c r="H102" s="31"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
@@ -3480,7 +3490,7 @@
         <v>2050</v>
       </c>
       <c r="C103" s="31" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D103" s="31" t="s">
         <v>34</v>
@@ -3488,12 +3498,8 @@
       <c r="E103" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="F103" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="G103" s="30" t="s">
-        <v>63</v>
-      </c>
+      <c r="F103" s="31"/>
+      <c r="G103" s="30"/>
       <c r="H103" s="31"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
@@ -3504,7 +3510,7 @@
         <v>2050</v>
       </c>
       <c r="C104" s="31" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D104" s="31" t="s">
         <v>34</v>
@@ -3513,10 +3519,10 @@
         <v>38</v>
       </c>
       <c r="F104" s="31" t="s">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="G104" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H104" s="31"/>
     </row>
@@ -3528,7 +3534,7 @@
         <v>2050</v>
       </c>
       <c r="C105" s="31" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="D105" s="31" t="s">
         <v>34</v>
@@ -3537,10 +3543,10 @@
         <v>38</v>
       </c>
       <c r="F105" s="31" t="s">
-        <v>120</v>
+        <v>66</v>
       </c>
       <c r="G105" s="30" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H105" s="31"/>
     </row>
@@ -3552,7 +3558,7 @@
         <v>2050</v>
       </c>
       <c r="C106" s="31" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="D106" s="31" t="s">
         <v>34</v>
@@ -3561,10 +3567,10 @@
         <v>38</v>
       </c>
       <c r="F106" s="31" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G106" s="30" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H106" s="31"/>
     </row>
@@ -3576,7 +3582,7 @@
         <v>2050</v>
       </c>
       <c r="C107" s="31" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D107" s="31" t="s">
         <v>34</v>
@@ -3585,10 +3591,10 @@
         <v>38</v>
       </c>
       <c r="F107" s="31" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G107" s="30" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H107" s="31"/>
     </row>
@@ -3600,7 +3606,7 @@
         <v>2050</v>
       </c>
       <c r="C108" s="31" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D108" s="31" t="s">
         <v>34</v>
@@ -3609,86 +3615,86 @@
         <v>38</v>
       </c>
       <c r="F108" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="G108" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="H108" s="31"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B109" s="30">
+        <v>2050</v>
+      </c>
+      <c r="C109" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D109" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E109" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F109" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="G109" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H109" s="31"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B110" s="30">
+        <v>2050</v>
+      </c>
+      <c r="C110" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="D110" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E110" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F110" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="G108" s="30" t="s">
+      <c r="G110" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="H108" s="31" t="s">
+      <c r="H110" s="31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B109" s="51">
-        <v>2050</v>
-      </c>
-      <c r="C109" s="52" t="s">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B111" s="51">
+        <v>2050</v>
+      </c>
+      <c r="C111" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="D109" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="E109" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="F109" s="52" t="s">
+      <c r="D111" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="E111" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="F111" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="G109" s="51" t="s">
+      <c r="G111" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="H109" s="52"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="B110" s="54">
-        <v>2050</v>
-      </c>
-      <c r="C110" s="53" t="s">
-        <v>101</v>
-      </c>
-      <c r="D110" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="E110" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F110" s="53" t="s">
-        <v>116</v>
-      </c>
-      <c r="G110" s="54" t="s">
-        <v>82</v>
-      </c>
-      <c r="H110" s="53"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A111" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="B111" s="54">
-        <v>2050</v>
-      </c>
-      <c r="C111" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="D111" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="E111" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F111" s="53" t="s">
-        <v>116</v>
-      </c>
-      <c r="G111" s="54" t="s">
-        <v>82</v>
-      </c>
-      <c r="H111" s="53"/>
+      <c r="H111" s="52"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="53" t="s">
@@ -3698,7 +3704,7 @@
         <v>2050</v>
       </c>
       <c r="C112" s="53" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D112" s="53" t="s">
         <v>91</v>
@@ -3722,7 +3728,7 @@
         <v>2050</v>
       </c>
       <c r="C113" s="53" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D113" s="53" t="s">
         <v>91</v>
@@ -3746,7 +3752,7 @@
         <v>2050</v>
       </c>
       <c r="C114" s="53" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D114" s="53" t="s">
         <v>91</v>
@@ -3770,7 +3776,7 @@
         <v>2050</v>
       </c>
       <c r="C115" s="53" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D115" s="53" t="s">
         <v>91</v>
@@ -3778,11 +3784,11 @@
       <c r="E115" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="F115" s="17" t="s">
-        <v>118</v>
+      <c r="F115" s="53" t="s">
+        <v>116</v>
       </c>
       <c r="G115" s="54" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H115" s="53"/>
     </row>
@@ -3794,7 +3800,7 @@
         <v>2050</v>
       </c>
       <c r="C116" s="53" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D116" s="53" t="s">
         <v>91</v>
@@ -3818,7 +3824,7 @@
         <v>2050</v>
       </c>
       <c r="C117" s="53" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D117" s="53" t="s">
         <v>91</v>
@@ -3826,11 +3832,11 @@
       <c r="E117" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="F117" s="53" t="s">
-        <v>116</v>
+      <c r="F117" s="17" t="s">
+        <v>118</v>
       </c>
       <c r="G117" s="54" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H117" s="53"/>
     </row>
@@ -3842,7 +3848,7 @@
         <v>2050</v>
       </c>
       <c r="C118" s="53" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D118" s="53" t="s">
         <v>91</v>
@@ -3866,7 +3872,7 @@
         <v>2050</v>
       </c>
       <c r="C119" s="53" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D119" s="53" t="s">
         <v>91</v>
@@ -3875,10 +3881,10 @@
         <v>38</v>
       </c>
       <c r="F119" s="53" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G119" s="54" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H119" s="53"/>
     </row>
@@ -3890,7 +3896,7 @@
         <v>2050</v>
       </c>
       <c r="C120" s="53" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="D120" s="53" t="s">
         <v>91</v>
@@ -3898,13 +3904,13 @@
       <c r="E120" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="F120" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="G120" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="H120" s="17"/>
+      <c r="F120" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="G120" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="H120" s="53"/>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="53" t="s">
@@ -3914,7 +3920,7 @@
         <v>2050</v>
       </c>
       <c r="C121" s="53" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D121" s="53" t="s">
         <v>91</v>
@@ -3922,13 +3928,13 @@
       <c r="E121" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="F121" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="G121" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="H121" s="17"/>
+      <c r="F121" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="G121" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="H121" s="53"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="53" t="s">
@@ -3938,7 +3944,7 @@
         <v>2050</v>
       </c>
       <c r="C122" s="53" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="D122" s="53" t="s">
         <v>91</v>
@@ -3947,10 +3953,10 @@
         <v>38</v>
       </c>
       <c r="F122" s="17" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="G122" s="16" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="H122" s="17"/>
     </row>
@@ -3962,7 +3968,7 @@
         <v>2050</v>
       </c>
       <c r="C123" s="53" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="D123" s="53" t="s">
         <v>91</v>
@@ -3971,10 +3977,10 @@
         <v>38</v>
       </c>
       <c r="F123" s="17" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G123" s="16" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H123" s="17"/>
     </row>
@@ -3986,7 +3992,7 @@
         <v>2050</v>
       </c>
       <c r="C124" s="53" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D124" s="53" t="s">
         <v>91</v>
@@ -4000,9 +4006,7 @@
       <c r="G124" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H124" s="17" t="s">
-        <v>43</v>
-      </c>
+      <c r="H124" s="17"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="53" t="s">
@@ -4012,7 +4016,7 @@
         <v>2050</v>
       </c>
       <c r="C125" s="53" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D125" s="53" t="s">
         <v>91</v>
@@ -4036,7 +4040,7 @@
         <v>2050</v>
       </c>
       <c r="C126" s="53" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D126" s="53" t="s">
         <v>91</v>
@@ -4050,7 +4054,9 @@
       <c r="G126" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H126" s="17"/>
+      <c r="H126" s="17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="53" t="s">
@@ -4060,7 +4066,7 @@
         <v>2050</v>
       </c>
       <c r="C127" s="53" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="D127" s="53" t="s">
         <v>91</v>
@@ -4084,7 +4090,7 @@
         <v>2050</v>
       </c>
       <c r="C128" s="53" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="D128" s="53" t="s">
         <v>91</v>
@@ -4108,7 +4114,7 @@
         <v>2050</v>
       </c>
       <c r="C129" s="53" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D129" s="53" t="s">
         <v>91</v>
@@ -4122,7 +4128,55 @@
       <c r="G129" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H129" s="17" t="s">
+      <c r="H129" s="17"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A130" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B130" s="54">
+        <v>2050</v>
+      </c>
+      <c r="C130" s="53" t="s">
+        <v>165</v>
+      </c>
+      <c r="D130" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E130" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F130" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="G130" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H130" s="17"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A131" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B131" s="54">
+        <v>2050</v>
+      </c>
+      <c r="C131" s="53" t="s">
+        <v>173</v>
+      </c>
+      <c r="D131" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E131" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F131" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="G131" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H131" s="17" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 2040 NoProject and 2050 EIR Alt1
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C0415B-9ACE-4859-A002-D9EF75742809}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB1ABB4-9A62-4474-A3A1-D5EA167459A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="22830" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6525" yWindow="1800" windowWidth="22830" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="187">
   <si>
     <t>EEJ</t>
   </si>
@@ -565,6 +565,27 @@
   </si>
   <si>
     <t>2030_TM152_FBP_Plus_21</t>
+  </si>
+  <si>
+    <t>2050_TM152_EIR_Alt1_01</t>
+  </si>
+  <si>
+    <t>EIR</t>
+  </si>
+  <si>
+    <t>Alt1</t>
+  </si>
+  <si>
+    <t>2040_TM152_FBP_NoProject_20</t>
+  </si>
+  <si>
+    <t>NoProject</t>
+  </si>
+  <si>
+    <t>"EIR runs\Alt1 (s26) runs\Alt1_v1"</t>
+  </si>
+  <si>
+    <t>run208</t>
   </si>
 </sst>
 </file>
@@ -656,7 +677,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -682,11 +703,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -788,6 +820,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1136,11 +1177,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H131"/>
+  <dimension ref="A1:H133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F133" sqref="F133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2993,70 +3034,76 @@
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B82" s="16">
+      <c r="A82" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B82" s="62">
         <v>2040</v>
       </c>
-      <c r="C82" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="D82" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E82" s="23" t="s">
-        <v>38</v>
+      <c r="C82" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="D82" s="63" t="s">
+        <v>91</v>
+      </c>
+      <c r="E82" s="63" t="s">
+        <v>184</v>
       </c>
       <c r="F82" s="23" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="G82" s="22" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="H82" s="23" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="B83" s="40">
-        <v>2050</v>
-      </c>
-      <c r="C83" s="41" t="s">
+      <c r="A83" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B83" s="16">
+        <v>2040</v>
+      </c>
+      <c r="C83" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="D83" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E83" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F83" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="G83" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="H83" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B84" s="40">
+        <v>2050</v>
+      </c>
+      <c r="C84" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D83" s="41" t="s">
+      <c r="D84" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="E83" s="41" t="s">
+      <c r="E84" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F83" s="41"/>
-      <c r="G83" s="40"/>
-      <c r="H83" s="41"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B84" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C84" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="D84" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E84" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="F84" s="43"/>
-      <c r="G84" s="42"/>
-      <c r="H84" s="43"/>
+      <c r="F84" s="41"/>
+      <c r="G84" s="40"/>
+      <c r="H84" s="41"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="29" t="s">
@@ -3066,7 +3113,7 @@
         <v>2050</v>
       </c>
       <c r="C85" s="43" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D85" s="43" t="s">
         <v>34</v>
@@ -3074,12 +3121,8 @@
       <c r="E85" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F85" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="G85" s="42" t="s">
-        <v>65</v>
-      </c>
+      <c r="F85" s="43"/>
+      <c r="G85" s="42"/>
       <c r="H85" s="43"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -3090,7 +3133,7 @@
         <v>2050</v>
       </c>
       <c r="C86" s="43" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D86" s="43" t="s">
         <v>34</v>
@@ -3114,7 +3157,7 @@
         <v>2050</v>
       </c>
       <c r="C87" s="43" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D87" s="43" t="s">
         <v>34</v>
@@ -3123,10 +3166,10 @@
         <v>7</v>
       </c>
       <c r="F87" s="43" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G87" s="42" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H87" s="43"/>
     </row>
@@ -3138,7 +3181,7 @@
         <v>2050</v>
       </c>
       <c r="C88" s="43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D88" s="43" t="s">
         <v>34</v>
@@ -3147,60 +3190,60 @@
         <v>7</v>
       </c>
       <c r="F88" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="G88" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="H88" s="43"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B89" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C89" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="D89" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E89" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F89" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="G88" s="42" t="s">
+      <c r="G89" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="H88" s="43"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B89" s="45">
-        <v>2050</v>
-      </c>
-      <c r="C89" s="46" t="s">
+      <c r="H89" s="43"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="B90" s="45">
+        <v>2050</v>
+      </c>
+      <c r="C90" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="D89" s="46" t="s">
+      <c r="D90" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="E89" s="46" t="s">
+      <c r="E90" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="F89" s="46" t="s">
+      <c r="F90" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="G89" s="45" t="s">
+      <c r="G90" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="H89" s="46"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A90" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B90" s="16">
-        <v>2050</v>
-      </c>
-      <c r="C90" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="D90" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="E90" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F90" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="G90" s="54" t="s">
-        <v>75</v>
-      </c>
-      <c r="H90" s="17"/>
+      <c r="H90" s="46"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="15" t="s">
@@ -3210,19 +3253,19 @@
         <v>2050</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D91" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D91" s="52" t="s">
         <v>91</v>
       </c>
       <c r="E91" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F91" s="17" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G91" s="54" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H91" s="17"/>
     </row>
@@ -3234,7 +3277,7 @@
         <v>2050</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="D92" s="17" t="s">
         <v>91</v>
@@ -3243,10 +3286,10 @@
         <v>7</v>
       </c>
       <c r="F92" s="17" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G92" s="54" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H92" s="17"/>
     </row>
@@ -3258,7 +3301,7 @@
         <v>2050</v>
       </c>
       <c r="C93" s="17" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="D93" s="17" t="s">
         <v>91</v>
@@ -3267,10 +3310,10 @@
         <v>7</v>
       </c>
       <c r="F93" s="17" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="G93" s="54" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="H93" s="17"/>
     </row>
@@ -3282,7 +3325,7 @@
         <v>2050</v>
       </c>
       <c r="C94" s="17" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D94" s="17" t="s">
         <v>91</v>
@@ -3293,12 +3336,10 @@
       <c r="F94" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="G94" s="16" t="s">
+      <c r="G94" s="54" t="s">
         <v>137</v>
       </c>
-      <c r="H94" s="17" t="s">
-        <v>43</v>
-      </c>
+      <c r="H94" s="17"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="15" t="s">
@@ -3308,7 +3349,7 @@
         <v>2050</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D95" s="17" t="s">
         <v>91</v>
@@ -3322,7 +3363,9 @@
       <c r="G95" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H95" s="17"/>
+      <c r="H95" s="17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="15" t="s">
@@ -3332,7 +3375,7 @@
         <v>2050</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D96" s="17" t="s">
         <v>91</v>
@@ -3341,7 +3384,7 @@
         <v>7</v>
       </c>
       <c r="F96" s="17" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="G96" s="16" t="s">
         <v>137</v>
@@ -3356,7 +3399,7 @@
         <v>2050</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D97" s="17" t="s">
         <v>91</v>
@@ -3365,10 +3408,10 @@
         <v>7</v>
       </c>
       <c r="F97" s="17" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G97" s="16" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="H97" s="17"/>
     </row>
@@ -3380,7 +3423,7 @@
         <v>2050</v>
       </c>
       <c r="C98" s="17" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D98" s="17" t="s">
         <v>91</v>
@@ -3389,98 +3432,102 @@
         <v>7</v>
       </c>
       <c r="F98" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="G98" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="H98" s="17"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B99" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C99" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D99" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E99" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F99" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="G98" s="16" t="s">
+      <c r="G99" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="H98" s="17"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B99" s="22">
-        <v>2050</v>
-      </c>
-      <c r="C99" s="23" t="s">
+      <c r="H99" s="17"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B100" s="22">
+        <v>2050</v>
+      </c>
+      <c r="C100" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="D99" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E99" s="23" t="s">
+      <c r="D100" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="E100" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F99" s="23" t="s">
+      <c r="F100" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="G99" s="22" t="s">
+      <c r="G100" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="H99" s="23" t="s">
+      <c r="H100" s="23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B100" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C100" s="43" t="s">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B101" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C101" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D100" s="43" t="s">
+      <c r="D101" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E100" s="43" t="s">
+      <c r="E101" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="F100" s="43"/>
-      <c r="G100" s="42"/>
-      <c r="H100" s="43"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B101" s="45">
-        <v>2050</v>
-      </c>
-      <c r="C101" s="46" t="s">
+      <c r="F101" s="43"/>
+      <c r="G101" s="42"/>
+      <c r="H101" s="43"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="B102" s="45">
+        <v>2050</v>
+      </c>
+      <c r="C102" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="D101" s="46" t="s">
+      <c r="D102" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="E101" s="46" t="s">
+      <c r="E102" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="F101" s="46"/>
-      <c r="G101" s="45"/>
-      <c r="H101" s="46"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B102" s="30">
-        <v>2050</v>
-      </c>
-      <c r="C102" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="D102" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E102" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="F102" s="31"/>
-      <c r="G102" s="30"/>
-      <c r="H102" s="31"/>
+      <c r="F102" s="46"/>
+      <c r="G102" s="45"/>
+      <c r="H102" s="46"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="29" t="s">
@@ -3490,7 +3537,7 @@
         <v>2050</v>
       </c>
       <c r="C103" s="31" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D103" s="31" t="s">
         <v>34</v>
@@ -3510,7 +3557,7 @@
         <v>2050</v>
       </c>
       <c r="C104" s="31" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D104" s="31" t="s">
         <v>34</v>
@@ -3518,12 +3565,8 @@
       <c r="E104" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="F104" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="G104" s="30" t="s">
-        <v>63</v>
-      </c>
+      <c r="F104" s="31"/>
+      <c r="G104" s="30"/>
       <c r="H104" s="31"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
@@ -3534,7 +3577,7 @@
         <v>2050</v>
       </c>
       <c r="C105" s="31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D105" s="31" t="s">
         <v>34</v>
@@ -3558,7 +3601,7 @@
         <v>2050</v>
       </c>
       <c r="C106" s="31" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D106" s="31" t="s">
         <v>34</v>
@@ -3567,10 +3610,10 @@
         <v>38</v>
       </c>
       <c r="F106" s="31" t="s">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="G106" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H106" s="31"/>
     </row>
@@ -3582,7 +3625,7 @@
         <v>2050</v>
       </c>
       <c r="C107" s="31" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D107" s="31" t="s">
         <v>34</v>
@@ -3591,10 +3634,10 @@
         <v>38</v>
       </c>
       <c r="F107" s="31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G107" s="30" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H107" s="31"/>
     </row>
@@ -3606,7 +3649,7 @@
         <v>2050</v>
       </c>
       <c r="C108" s="31" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D108" s="31" t="s">
         <v>34</v>
@@ -3615,10 +3658,10 @@
         <v>38</v>
       </c>
       <c r="F108" s="31" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G108" s="30" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H108" s="31"/>
     </row>
@@ -3630,7 +3673,7 @@
         <v>2050</v>
       </c>
       <c r="C109" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D109" s="31" t="s">
         <v>34</v>
@@ -3639,10 +3682,10 @@
         <v>38</v>
       </c>
       <c r="F109" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G109" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H109" s="31"/>
     </row>
@@ -3654,7 +3697,7 @@
         <v>2050</v>
       </c>
       <c r="C110" s="31" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D110" s="31" t="s">
         <v>34</v>
@@ -3663,62 +3706,62 @@
         <v>38</v>
       </c>
       <c r="F110" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="G110" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H110" s="31"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B111" s="30">
+        <v>2050</v>
+      </c>
+      <c r="C111" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="D111" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E111" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F111" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="G110" s="30" t="s">
+      <c r="G111" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="H110" s="31" t="s">
+      <c r="H111" s="31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A111" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B111" s="51">
-        <v>2050</v>
-      </c>
-      <c r="C111" s="52" t="s">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B112" s="51">
+        <v>2050</v>
+      </c>
+      <c r="C112" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="D111" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="E111" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="F111" s="52" t="s">
+      <c r="D112" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="E112" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="F112" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="G111" s="51" t="s">
+      <c r="G112" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="H111" s="52"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A112" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="B112" s="54">
-        <v>2050</v>
-      </c>
-      <c r="C112" s="53" t="s">
-        <v>101</v>
-      </c>
-      <c r="D112" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="E112" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F112" s="53" t="s">
-        <v>116</v>
-      </c>
-      <c r="G112" s="54" t="s">
-        <v>82</v>
-      </c>
-      <c r="H112" s="53"/>
+      <c r="H112" s="52"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="53" t="s">
@@ -3728,7 +3771,7 @@
         <v>2050</v>
       </c>
       <c r="C113" s="53" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D113" s="53" t="s">
         <v>91</v>
@@ -3752,7 +3795,7 @@
         <v>2050</v>
       </c>
       <c r="C114" s="53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D114" s="53" t="s">
         <v>91</v>
@@ -3776,7 +3819,7 @@
         <v>2050</v>
       </c>
       <c r="C115" s="53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D115" s="53" t="s">
         <v>91</v>
@@ -3800,7 +3843,7 @@
         <v>2050</v>
       </c>
       <c r="C116" s="53" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D116" s="53" t="s">
         <v>91</v>
@@ -3824,7 +3867,7 @@
         <v>2050</v>
       </c>
       <c r="C117" s="53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D117" s="53" t="s">
         <v>91</v>
@@ -3832,11 +3875,11 @@
       <c r="E117" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="F117" s="17" t="s">
-        <v>118</v>
+      <c r="F117" s="53" t="s">
+        <v>116</v>
       </c>
       <c r="G117" s="54" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H117" s="53"/>
     </row>
@@ -3848,7 +3891,7 @@
         <v>2050</v>
       </c>
       <c r="C118" s="53" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D118" s="53" t="s">
         <v>91</v>
@@ -3856,11 +3899,11 @@
       <c r="E118" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="F118" s="53" t="s">
-        <v>116</v>
+      <c r="F118" s="17" t="s">
+        <v>118</v>
       </c>
       <c r="G118" s="54" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H118" s="53"/>
     </row>
@@ -3872,7 +3915,7 @@
         <v>2050</v>
       </c>
       <c r="C119" s="53" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D119" s="53" t="s">
         <v>91</v>
@@ -3896,7 +3939,7 @@
         <v>2050</v>
       </c>
       <c r="C120" s="53" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D120" s="53" t="s">
         <v>91</v>
@@ -3920,7 +3963,7 @@
         <v>2050</v>
       </c>
       <c r="C121" s="53" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D121" s="53" t="s">
         <v>91</v>
@@ -3929,10 +3972,10 @@
         <v>38</v>
       </c>
       <c r="F121" s="53" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G121" s="54" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H121" s="53"/>
     </row>
@@ -3944,7 +3987,7 @@
         <v>2050</v>
       </c>
       <c r="C122" s="53" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D122" s="53" t="s">
         <v>91</v>
@@ -3952,13 +3995,13 @@
       <c r="E122" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="F122" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="G122" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="H122" s="17"/>
+      <c r="F122" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="G122" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="H122" s="53"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="53" t="s">
@@ -3968,7 +4011,7 @@
         <v>2050</v>
       </c>
       <c r="C123" s="53" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D123" s="53" t="s">
         <v>91</v>
@@ -3977,10 +4020,10 @@
         <v>38</v>
       </c>
       <c r="F123" s="17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G123" s="16" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H123" s="17"/>
     </row>
@@ -3992,7 +4035,7 @@
         <v>2050</v>
       </c>
       <c r="C124" s="53" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D124" s="53" t="s">
         <v>91</v>
@@ -4001,10 +4044,10 @@
         <v>38</v>
       </c>
       <c r="F124" s="17" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G124" s="16" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H124" s="17"/>
     </row>
@@ -4016,7 +4059,7 @@
         <v>2050</v>
       </c>
       <c r="C125" s="53" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D125" s="53" t="s">
         <v>91</v>
@@ -4040,7 +4083,7 @@
         <v>2050</v>
       </c>
       <c r="C126" s="53" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D126" s="53" t="s">
         <v>91</v>
@@ -4054,9 +4097,7 @@
       <c r="G126" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H126" s="17" t="s">
-        <v>43</v>
-      </c>
+      <c r="H126" s="17"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="53" t="s">
@@ -4066,7 +4107,7 @@
         <v>2050</v>
       </c>
       <c r="C127" s="53" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D127" s="53" t="s">
         <v>91</v>
@@ -4080,7 +4121,9 @@
       <c r="G127" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H127" s="17"/>
+      <c r="H127" s="17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="53" t="s">
@@ -4090,7 +4133,7 @@
         <v>2050</v>
       </c>
       <c r="C128" s="53" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D128" s="53" t="s">
         <v>91</v>
@@ -4114,7 +4157,7 @@
         <v>2050</v>
       </c>
       <c r="C129" s="53" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D129" s="53" t="s">
         <v>91</v>
@@ -4138,7 +4181,7 @@
         <v>2050</v>
       </c>
       <c r="C130" s="53" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D130" s="53" t="s">
         <v>91</v>
@@ -4162,7 +4205,7 @@
         <v>2050</v>
       </c>
       <c r="C131" s="53" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D131" s="53" t="s">
         <v>91</v>
@@ -4176,7 +4219,57 @@
       <c r="G131" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H131" s="17" t="s">
+      <c r="H131" s="17"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A132" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B132" s="54">
+        <v>2050</v>
+      </c>
+      <c r="C132" s="53" t="s">
+        <v>173</v>
+      </c>
+      <c r="D132" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E132" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F132" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="G132" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H132" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A133" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B133" s="60">
+        <v>2050</v>
+      </c>
+      <c r="C133" s="59" t="s">
+        <v>180</v>
+      </c>
+      <c r="D133" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="E133" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="F133" s="59" t="s">
+        <v>185</v>
+      </c>
+      <c r="G133" s="60" t="s">
+        <v>186</v>
+      </c>
+      <c r="H133" s="59" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix last commit - No Project not NoProject
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB1ABB4-9A62-4474-A3A1-D5EA167459A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2ACAB26-859B-4335-9C72-02FB87BBAE27}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6525" yWindow="1800" windowWidth="22830" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="186">
   <si>
     <t>EEJ</t>
   </si>
@@ -577,9 +577,6 @@
   </si>
   <si>
     <t>2040_TM152_FBP_NoProject_20</t>
-  </si>
-  <si>
-    <t>NoProject</t>
   </si>
   <si>
     <t>"EIR runs\Alt1 (s26) runs\Alt1_v1"</t>
@@ -1180,8 +1177,8 @@
   <dimension ref="A1:H133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F133" sqref="F133"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3047,7 +3044,7 @@
         <v>91</v>
       </c>
       <c r="E82" s="63" t="s">
-        <v>184</v>
+        <v>7</v>
       </c>
       <c r="F82" s="23" t="s">
         <v>167</v>
@@ -4264,10 +4261,10 @@
         <v>182</v>
       </c>
       <c r="F133" s="59" t="s">
+        <v>184</v>
+      </c>
+      <c r="G133" s="60" t="s">
         <v>185</v>
-      </c>
-      <c r="G133" s="60" t="s">
-        <v>186</v>
       </c>
       <c r="H133" s="59" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
fixed typo in the last commit (2035 not 2030)
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD14EB38-C22B-4902-B472-29D56792879B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67426F18-45A1-421D-9CE3-8CCCC1130666}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -585,7 +585,7 @@
     <t>run208</t>
   </si>
   <si>
-    <t>2030_TM152_EIR_Alt1_01</t>
+    <t>2035_TM152_EIR_Alt1_01</t>
   </si>
 </sst>
 </file>
@@ -1181,7 +1181,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F133" sqref="F133"/>
+      <selection pane="bottomLeft" activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added dummy 2015_UrbanSim_FBP run
This isn't a real TM run so it's a placeholder for the taz data from UrbanSim
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67426F18-45A1-421D-9CE3-8CCCC1130666}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A067FE1-A955-4AF4-AF3B-D26BC9ADAE5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14535" yWindow="3930" windowWidth="22830" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="188">
   <si>
     <t>EEJ</t>
   </si>
@@ -586,6 +586,9 @@
   </si>
   <si>
     <t>2035_TM152_EIR_Alt1_01</t>
+  </si>
+  <si>
+    <t>2015_UrbanSim_FBP</t>
   </si>
 </sst>
 </file>
@@ -1177,23 +1180,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H134"/>
+  <dimension ref="A1:H135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C134" sqref="C134"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="36.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.296875" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="70.8984375" customWidth="1"/>
+    <col min="6" max="6" width="70.85546875" customWidth="1"/>
     <col min="7" max="7" width="15" style="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="56" t="s">
         <v>40</v>
       </c>
@@ -1219,7 +1222,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
@@ -1239,7 +1242,7 @@
       <c r="G2" s="6"/>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>25</v>
       </c>
@@ -1259,7 +1262,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="10"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>25</v>
       </c>
@@ -1279,7 +1282,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>25</v>
       </c>
@@ -1299,7 +1302,7 @@
       <c r="G5" s="13"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>25</v>
       </c>
@@ -1319,7 +1322,7 @@
       <c r="G6" s="13"/>
       <c r="H6" s="14"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>25</v>
       </c>
@@ -1339,7 +1342,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>25</v>
       </c>
@@ -1359,7 +1362,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="14"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>25</v>
       </c>
@@ -1379,7 +1382,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>25</v>
       </c>
@@ -1399,7 +1402,7 @@
       <c r="G10" s="19"/>
       <c r="H10" s="20"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
         <v>25</v>
       </c>
@@ -1419,7 +1422,7 @@
       <c r="G11" s="19"/>
       <c r="H11" s="20"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>25</v>
       </c>
@@ -1439,7 +1442,7 @@
       <c r="G12" s="19"/>
       <c r="H12" s="20"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>25</v>
       </c>
@@ -1459,7 +1462,7 @@
       <c r="G13" s="19"/>
       <c r="H13" s="20"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>25</v>
       </c>
@@ -1479,7 +1482,7 @@
       <c r="G14" s="19"/>
       <c r="H14" s="20"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>25</v>
       </c>
@@ -1499,7 +1502,7 @@
       <c r="G15" s="16"/>
       <c r="H15" s="17"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>25</v>
       </c>
@@ -1519,7 +1522,7 @@
       <c r="G16" s="16"/>
       <c r="H16" s="17"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>25</v>
       </c>
@@ -1539,7 +1542,7 @@
       <c r="G17" s="16"/>
       <c r="H17" s="17"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>25</v>
       </c>
@@ -1559,7 +1562,7 @@
       <c r="G18" s="16"/>
       <c r="H18" s="17"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
         <v>25</v>
       </c>
@@ -1579,7 +1582,7 @@
       <c r="G19" s="22"/>
       <c r="H19" s="23"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="24" t="s">
         <v>26</v>
       </c>
@@ -1601,7 +1604,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="24" t="s">
         <v>26</v>
       </c>
@@ -1621,7 +1624,7 @@
       <c r="G21" s="25"/>
       <c r="H21" s="26"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>26</v>
       </c>
@@ -1643,183 +1646,185 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="47">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2015</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="47">
         <v>2020</v>
       </c>
-      <c r="C23" s="48" t="s">
+      <c r="C24" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="D23" s="48" t="s">
+      <c r="D24" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="48" t="s">
+      <c r="E24" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="48" t="s">
+      <c r="F24" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="G23" s="47" t="s">
+      <c r="G24" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="H23" s="48"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="16">
+      <c r="H24" s="48"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="16">
         <v>2020</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C25" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E24" s="17" t="s">
+      <c r="D25" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F25" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="G24" s="16" t="s">
+      <c r="G25" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H24" s="17" t="s">
+      <c r="H25" s="17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="51">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="51">
         <v>2025</v>
       </c>
-      <c r="C25" s="52" t="s">
+      <c r="C26" s="52" t="s">
         <v>171</v>
       </c>
-      <c r="D25" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25" s="52" t="s">
+      <c r="D26" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="52" t="s">
+      <c r="F26" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="G25" s="51" t="s">
+      <c r="G26" s="51" t="s">
         <v>169</v>
       </c>
-      <c r="H25" s="52" t="s">
+      <c r="H26" s="52" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="19">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="19">
         <v>2025</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C27" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="D26" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" s="20" t="s">
+      <c r="D27" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="G26" s="19" t="s">
+      <c r="G27" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="H26" s="20"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="34">
+      <c r="H27" s="20"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="34">
         <v>2025</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C28" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="D27" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="E27" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="F27" s="35" t="s">
+      <c r="D28" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="G27" s="34" t="s">
+      <c r="G28" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="H27" s="35" t="s">
+      <c r="H28" s="35" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="16">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="16">
         <v>2030</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C29" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="D28" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E28" s="17" t="s">
+      <c r="D29" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="F29" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="G28" s="16" t="s">
+      <c r="G29" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="H28" s="17" t="s">
+      <c r="H29" s="17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="19">
-        <v>2030</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="G29" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="H29" s="20"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
         <v>26</v>
       </c>
@@ -1827,73 +1832,77 @@
         <v>2030</v>
       </c>
       <c r="C30" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="G30" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="H30" s="20"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="19">
+        <v>2030</v>
+      </c>
+      <c r="C31" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="D30" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F30" s="35" t="s">
+      <c r="D31" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="G30" s="34" t="s">
+      <c r="G31" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="H30" s="35" t="s">
+      <c r="H31" s="35" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="37">
-        <v>2035</v>
-      </c>
-      <c r="C31" s="38" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="37">
+        <v>2035</v>
+      </c>
+      <c r="C32" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="38" t="s">
+      <c r="D32" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="38" t="s">
+      <c r="E32" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="F31" s="38"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C32" s="20" t="s">
+      <c r="F32" s="38"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C33" s="20" t="s">
         <v>93</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E32" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F32" s="20"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="20"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>152</v>
       </c>
       <c r="D33" s="20" t="s">
         <v>28</v>
@@ -1905,7 +1914,7 @@
       <c r="G33" s="19"/>
       <c r="H33" s="20"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
         <v>26</v>
       </c>
@@ -1913,7 +1922,7 @@
         <v>2035</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D34" s="20" t="s">
         <v>28</v>
@@ -1923,59 +1932,59 @@
       </c>
       <c r="F34" s="20"/>
       <c r="G34" s="19"/>
-      <c r="H34" s="20" t="s">
+      <c r="H34" s="20"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F35" s="20"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="37">
-        <v>2035</v>
-      </c>
-      <c r="C35" s="36" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="37">
+        <v>2035</v>
+      </c>
+      <c r="C36" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="38" t="s">
+      <c r="D36" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="38" t="s">
+      <c r="E36" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="38"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="38"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C36" s="18" t="s">
+      <c r="F36" s="38"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="38"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C37" s="18" t="s">
         <v>44</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="20"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="20"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>45</v>
       </c>
       <c r="D37" s="20" t="s">
         <v>34</v>
@@ -1987,7 +1996,7 @@
       <c r="G37" s="19"/>
       <c r="H37" s="20"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="18" t="s">
         <v>26</v>
       </c>
@@ -1995,7 +2004,7 @@
         <v>2035</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D38" s="20" t="s">
         <v>34</v>
@@ -2007,7 +2016,7 @@
       <c r="G38" s="19"/>
       <c r="H38" s="20"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
         <v>26</v>
       </c>
@@ -2015,7 +2024,7 @@
         <v>2035</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="D39" s="20" t="s">
         <v>34</v>
@@ -2023,15 +2032,11 @@
       <c r="E39" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="F39" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="G39" s="19" t="s">
-        <v>74</v>
-      </c>
+      <c r="F39" s="20"/>
+      <c r="G39" s="19"/>
       <c r="H39" s="20"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="18" t="s">
         <v>26</v>
       </c>
@@ -2039,7 +2044,7 @@
         <v>2035</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D40" s="20" t="s">
         <v>34</v>
@@ -2048,94 +2053,94 @@
         <v>7</v>
       </c>
       <c r="F40" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="G40" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="H40" s="20"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="G40" s="19" t="s">
+      <c r="G41" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="H40" s="20"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="B41" s="34">
-        <v>2035</v>
-      </c>
-      <c r="C41" s="33" t="s">
+      <c r="H41" s="20"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C42" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="D41" s="35" t="s">
+      <c r="D42" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="E41" s="35" t="s">
+      <c r="E42" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F41" s="35" t="s">
+      <c r="F42" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="G41" s="34" t="s">
+      <c r="G42" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="H41" s="35"/>
-    </row>
-    <row r="42" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42" s="51">
-        <v>2035</v>
-      </c>
-      <c r="C42" s="52" t="s">
+      <c r="H42" s="35"/>
+    </row>
+    <row r="43" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" s="51">
+        <v>2035</v>
+      </c>
+      <c r="C43" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="D42" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="E42" s="52" t="s">
+      <c r="D43" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="F42" s="52" t="s">
+      <c r="F43" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="G42" s="51" t="s">
+      <c r="G43" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="H42" s="52"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C43" s="17" t="s">
+      <c r="H43" s="52"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C44" s="17" t="s">
         <v>111</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="G43" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="H43" s="17"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B44" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>123</v>
       </c>
       <c r="D44" s="17" t="s">
         <v>91</v>
@@ -2144,14 +2149,14 @@
         <v>7</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G44" s="16" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H44" s="17"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
         <v>26</v>
       </c>
@@ -2159,7 +2164,7 @@
         <v>2035</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="D45" s="17" t="s">
         <v>91</v>
@@ -2168,14 +2173,14 @@
         <v>7</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="G45" s="16" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="H45" s="17"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
         <v>26</v>
       </c>
@@ -2183,7 +2188,7 @@
         <v>2035</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D46" s="17" t="s">
         <v>91</v>
@@ -2197,11 +2202,9 @@
       <c r="G46" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H46" s="17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H46" s="17"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
         <v>26</v>
       </c>
@@ -2209,7 +2212,7 @@
         <v>2035</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D47" s="17" t="s">
         <v>91</v>
@@ -2223,9 +2226,11 @@
       <c r="G47" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H47" s="17"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H47" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
         <v>26</v>
       </c>
@@ -2233,7 +2238,7 @@
         <v>2035</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D48" s="17" t="s">
         <v>91</v>
@@ -2242,14 +2247,14 @@
         <v>7</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="G48" s="16" t="s">
         <v>137</v>
       </c>
       <c r="H48" s="17"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
         <v>26</v>
       </c>
@@ -2257,7 +2262,7 @@
         <v>2035</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D49" s="17" t="s">
         <v>91</v>
@@ -2266,108 +2271,112 @@
         <v>7</v>
       </c>
       <c r="F49" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="G49" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H49" s="17"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="G49" s="16" t="s">
+      <c r="G50" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="H49" s="17"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50" s="22">
-        <v>2035</v>
-      </c>
-      <c r="C50" s="23" t="s">
+      <c r="H50" s="17"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="22">
+        <v>2035</v>
+      </c>
+      <c r="C51" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="D50" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E50" s="23" t="s">
+      <c r="D51" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="E51" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F50" s="23" t="s">
+      <c r="F51" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="G50" s="22" t="s">
+      <c r="G51" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="H50" s="23" t="s">
+      <c r="H51" s="23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="B51" s="37">
-        <v>2035</v>
-      </c>
-      <c r="C51" s="38" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="37">
+        <v>2035</v>
+      </c>
+      <c r="C52" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D51" s="38" t="s">
+      <c r="D52" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="E51" s="38" t="s">
+      <c r="E52" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="F51" s="38"/>
-      <c r="G51" s="37"/>
-      <c r="H51" s="38"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="B52" s="34">
-        <v>2035</v>
-      </c>
-      <c r="C52" s="35" t="s">
+      <c r="F52" s="38"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="38"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="34">
+        <v>2035</v>
+      </c>
+      <c r="C53" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="D52" s="35" t="s">
+      <c r="D53" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="E52" s="35" t="s">
+      <c r="E53" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="F52" s="35"/>
-      <c r="G52" s="34"/>
-      <c r="H52" s="35"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B53" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C53" s="20" t="s">
+      <c r="F53" s="35"/>
+      <c r="G53" s="34"/>
+      <c r="H53" s="35"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C54" s="20" t="s">
         <v>47</v>
-      </c>
-      <c r="D53" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E53" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F53" s="20"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="20"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B54" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C54" s="20" t="s">
-        <v>37</v>
       </c>
       <c r="D54" s="20" t="s">
         <v>34</v>
@@ -2379,7 +2388,7 @@
       <c r="G54" s="19"/>
       <c r="H54" s="20"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="18" t="s">
         <v>26</v>
       </c>
@@ -2387,7 +2396,7 @@
         <v>2035</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D55" s="20" t="s">
         <v>34</v>
@@ -2395,15 +2404,11 @@
       <c r="E55" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F55" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="G55" s="19" t="s">
-        <v>64</v>
-      </c>
+      <c r="F55" s="20"/>
+      <c r="G55" s="19"/>
       <c r="H55" s="20"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="18" t="s">
         <v>26</v>
       </c>
@@ -2411,7 +2416,7 @@
         <v>2035</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D56" s="20" t="s">
         <v>34</v>
@@ -2420,14 +2425,14 @@
         <v>38</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="G56" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H56" s="20"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="18" t="s">
         <v>26</v>
       </c>
@@ -2435,7 +2440,7 @@
         <v>2035</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D57" s="20" t="s">
         <v>34</v>
@@ -2444,14 +2449,14 @@
         <v>38</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H57" s="20"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="18" t="s">
         <v>26</v>
       </c>
@@ -2459,7 +2464,7 @@
         <v>2035</v>
       </c>
       <c r="C58" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D58" s="20" t="s">
         <v>34</v>
@@ -2468,14 +2473,14 @@
         <v>38</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G58" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H58" s="20"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="18" t="s">
         <v>26</v>
       </c>
@@ -2483,7 +2488,7 @@
         <v>2035</v>
       </c>
       <c r="C59" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D59" s="20" t="s">
         <v>34</v>
@@ -2492,14 +2497,14 @@
         <v>38</v>
       </c>
       <c r="F59" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G59" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H59" s="20"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="18" t="s">
         <v>26</v>
       </c>
@@ -2507,7 +2512,7 @@
         <v>2035</v>
       </c>
       <c r="C60" s="20" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="D60" s="20" t="s">
         <v>34</v>
@@ -2516,40 +2521,40 @@
         <v>38</v>
       </c>
       <c r="F60" s="20" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G60" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="H60" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A61" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B61" s="27">
-        <v>2035</v>
-      </c>
-      <c r="C61" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D61" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="H60" s="20"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D61" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E61" s="28" t="s">
+      <c r="E61" s="20" t="s">
         <v>38</v>
       </c>
       <c r="F61" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="G61" s="27" t="s">
+      <c r="G61" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="H61" s="28"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H61" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="49" t="s">
         <v>26</v>
       </c>
@@ -2557,7 +2562,7 @@
         <v>2035</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D62" s="28" t="s">
         <v>34</v>
@@ -2573,31 +2578,31 @@
       </c>
       <c r="H62" s="28"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B63" s="19">
-        <v>2035</v>
-      </c>
-      <c r="C63" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="D63" s="20" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" s="27">
+        <v>2035</v>
+      </c>
+      <c r="C63" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D63" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E63" s="20" t="s">
+      <c r="E63" s="28" t="s">
         <v>38</v>
       </c>
       <c r="F63" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="G63" s="19" t="s">
+      <c r="G63" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="H63" s="20"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H63" s="28"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="18" t="s">
         <v>26</v>
       </c>
@@ -2605,7 +2610,7 @@
         <v>2035</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D64" s="20" t="s">
         <v>34</v>
@@ -2621,7 +2626,7 @@
       </c>
       <c r="H64" s="20"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="18" t="s">
         <v>26</v>
       </c>
@@ -2629,7 +2634,7 @@
         <v>2035</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D65" s="20" t="s">
         <v>34</v>
@@ -2645,7 +2650,7 @@
       </c>
       <c r="H65" s="20"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="18" t="s">
         <v>26</v>
       </c>
@@ -2653,7 +2658,7 @@
         <v>2035</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D66" s="20" t="s">
         <v>34</v>
@@ -2669,63 +2674,63 @@
       </c>
       <c r="H66" s="20"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A67" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B67" s="51">
-        <v>2035</v>
-      </c>
-      <c r="C67" s="52" t="s">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D67" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E67" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F67" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="G67" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="H67" s="20"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" s="51">
+        <v>2035</v>
+      </c>
+      <c r="C68" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="D67" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="E67" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="F67" s="52" t="s">
+      <c r="D68" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="E68" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="F68" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="G67" s="51" t="s">
+      <c r="G68" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="H67" s="52"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A68" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B68" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C68" s="17" t="s">
+      <c r="H68" s="52"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B69" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C69" s="17" t="s">
         <v>98</v>
-      </c>
-      <c r="D68" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E68" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F68" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="G68" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="H68" s="17"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A69" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B69" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C69" s="17" t="s">
-        <v>110</v>
       </c>
       <c r="D69" s="17" t="s">
         <v>91</v>
@@ -2741,7 +2746,7 @@
       </c>
       <c r="H69" s="17"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="15" t="s">
         <v>26</v>
       </c>
@@ -2749,7 +2754,7 @@
         <v>2035</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D70" s="17" t="s">
         <v>91</v>
@@ -2765,7 +2770,7 @@
       </c>
       <c r="H70" s="17"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="15" t="s">
         <v>26</v>
       </c>
@@ -2773,7 +2778,7 @@
         <v>2035</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D71" s="17" t="s">
         <v>91</v>
@@ -2789,7 +2794,7 @@
       </c>
       <c r="H71" s="17"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="15" t="s">
         <v>26</v>
       </c>
@@ -2797,79 +2802,79 @@
         <v>2035</v>
       </c>
       <c r="C72" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D72" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E72" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F72" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="G72" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="H72" s="17"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B73" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C73" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="D72" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E72" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F72" s="17" t="s">
+      <c r="D73" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E73" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F73" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="G72" s="16" t="s">
+      <c r="G73" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="H72" s="17"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A73" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B73" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C73" s="17" t="s">
+      <c r="H73" s="17"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C74" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="D73" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E73" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F73" s="17" t="s">
+      <c r="D74" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E74" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F74" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="G73" s="16" t="s">
+      <c r="G74" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="H73" s="17"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A74" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B74" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C74" s="17" t="s">
+      <c r="H74" s="17"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B75" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C75" s="17" t="s">
         <v>134</v>
-      </c>
-      <c r="D74" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E74" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F74" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="G74" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="H74" s="17"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A75" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B75" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C75" s="17" t="s">
-        <v>133</v>
       </c>
       <c r="D75" s="17" t="s">
         <v>91</v>
@@ -2885,7 +2890,7 @@
       </c>
       <c r="H75" s="17"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="15" t="s">
         <v>26</v>
       </c>
@@ -2893,31 +2898,31 @@
         <v>2035</v>
       </c>
       <c r="C76" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D76" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E76" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F76" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G76" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="H76" s="17"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B77" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C77" s="17" t="s">
         <v>139</v>
-      </c>
-      <c r="D76" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E76" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F76" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="G76" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="H76" s="17"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A77" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B77" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C77" s="17" t="s">
-        <v>142</v>
       </c>
       <c r="D77" s="17" t="s">
         <v>91</v>
@@ -2931,11 +2936,9 @@
       <c r="G77" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H77" s="17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H77" s="17"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
         <v>26</v>
       </c>
@@ -2943,7 +2946,7 @@
         <v>2035</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D78" s="17" t="s">
         <v>91</v>
@@ -2957,9 +2960,11 @@
       <c r="G78" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H78" s="17"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H78" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="15" t="s">
         <v>26</v>
       </c>
@@ -2967,7 +2972,7 @@
         <v>2035</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D79" s="17" t="s">
         <v>91</v>
@@ -2983,7 +2988,7 @@
       </c>
       <c r="H79" s="17"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="15" t="s">
         <v>26</v>
       </c>
@@ -2991,7 +2996,7 @@
         <v>2035</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D80" s="17" t="s">
         <v>91</v>
@@ -3007,133 +3012,137 @@
       </c>
       <c r="H80" s="17"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A81" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B81" s="22">
-        <v>2035</v>
-      </c>
-      <c r="C81" s="23" t="s">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B81" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C81" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D81" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E81" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F81" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="G81" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H81" s="17"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B82" s="22">
+        <v>2035</v>
+      </c>
+      <c r="C82" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="D81" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E81" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F81" s="23" t="s">
+      <c r="D82" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="E82" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F82" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="G81" s="22" t="s">
+      <c r="G82" s="22" t="s">
         <v>137</v>
-      </c>
-      <c r="H81" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A82" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="B82" s="62">
-        <v>2040</v>
-      </c>
-      <c r="C82" s="63" t="s">
-        <v>183</v>
-      </c>
-      <c r="D82" s="63" t="s">
-        <v>91</v>
-      </c>
-      <c r="E82" s="63" t="s">
-        <v>7</v>
-      </c>
-      <c r="F82" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="G82" s="22" t="s">
-        <v>169</v>
       </c>
       <c r="H82" s="23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A83" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B83" s="16">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B83" s="62">
         <v>2040</v>
       </c>
-      <c r="C83" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="D83" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E83" s="23" t="s">
-        <v>38</v>
+      <c r="C83" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="D83" s="63" t="s">
+        <v>91</v>
+      </c>
+      <c r="E83" s="63" t="s">
+        <v>7</v>
       </c>
       <c r="F83" s="23" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="G83" s="22" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="H83" s="23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A84" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="B84" s="40">
-        <v>2050</v>
-      </c>
-      <c r="C84" s="41" t="s">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B84" s="16">
+        <v>2040</v>
+      </c>
+      <c r="C84" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="D84" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E84" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F84" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="G84" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="H84" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B85" s="40">
+        <v>2050</v>
+      </c>
+      <c r="C85" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D84" s="41" t="s">
+      <c r="D85" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="E84" s="41" t="s">
+      <c r="E85" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F84" s="41"/>
-      <c r="G84" s="40"/>
-      <c r="H84" s="41"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A85" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B85" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C85" s="43" t="s">
+      <c r="F85" s="41"/>
+      <c r="G85" s="40"/>
+      <c r="H85" s="41"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B86" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C86" s="43" t="s">
         <v>53</v>
-      </c>
-      <c r="D85" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E85" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="F85" s="43"/>
-      <c r="G85" s="42"/>
-      <c r="H85" s="43"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A86" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B86" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C86" s="43" t="s">
-        <v>57</v>
       </c>
       <c r="D86" s="43" t="s">
         <v>34</v>
@@ -3141,15 +3150,11 @@
       <c r="E86" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F86" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="G86" s="42" t="s">
-        <v>65</v>
-      </c>
+      <c r="F86" s="43"/>
+      <c r="G86" s="42"/>
       <c r="H86" s="43"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="29" t="s">
         <v>26</v>
       </c>
@@ -3157,7 +3162,7 @@
         <v>2050</v>
       </c>
       <c r="C87" s="43" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D87" s="43" t="s">
         <v>34</v>
@@ -3173,7 +3178,7 @@
       </c>
       <c r="H87" s="43"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="29" t="s">
         <v>26</v>
       </c>
@@ -3181,7 +3186,7 @@
         <v>2050</v>
       </c>
       <c r="C88" s="43" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D88" s="43" t="s">
         <v>34</v>
@@ -3190,14 +3195,14 @@
         <v>7</v>
       </c>
       <c r="F88" s="43" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G88" s="42" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H88" s="43"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="29" t="s">
         <v>26</v>
       </c>
@@ -3205,7 +3210,7 @@
         <v>2050</v>
       </c>
       <c r="C89" s="43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D89" s="43" t="s">
         <v>34</v>
@@ -3214,86 +3219,86 @@
         <v>7</v>
       </c>
       <c r="F89" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="G89" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="H89" s="43"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B90" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C90" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="D90" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E90" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F90" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="G89" s="42" t="s">
+      <c r="G90" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="H89" s="43"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A90" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B90" s="45">
-        <v>2050</v>
-      </c>
-      <c r="C90" s="46" t="s">
+      <c r="H90" s="43"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="B91" s="45">
+        <v>2050</v>
+      </c>
+      <c r="C91" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="D90" s="46" t="s">
+      <c r="D91" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="E90" s="46" t="s">
+      <c r="E91" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="F90" s="46" t="s">
+      <c r="F91" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="G90" s="45" t="s">
+      <c r="G91" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="H90" s="46"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A91" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B91" s="16">
-        <v>2050</v>
-      </c>
-      <c r="C91" s="17" t="s">
+      <c r="H91" s="46"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B92" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C92" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="D91" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="E91" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F91" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="G91" s="54" t="s">
-        <v>75</v>
-      </c>
-      <c r="H91" s="17"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A92" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B92" s="16">
-        <v>2050</v>
-      </c>
-      <c r="C92" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D92" s="17" t="s">
+      <c r="D92" s="52" t="s">
         <v>91</v>
       </c>
       <c r="E92" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F92" s="17" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G92" s="54" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H92" s="17"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="15" t="s">
         <v>26</v>
       </c>
@@ -3301,7 +3306,7 @@
         <v>2050</v>
       </c>
       <c r="C93" s="17" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="D93" s="17" t="s">
         <v>91</v>
@@ -3310,14 +3315,14 @@
         <v>7</v>
       </c>
       <c r="F93" s="17" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G93" s="54" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H93" s="17"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="15" t="s">
         <v>26</v>
       </c>
@@ -3325,7 +3330,7 @@
         <v>2050</v>
       </c>
       <c r="C94" s="17" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="D94" s="17" t="s">
         <v>91</v>
@@ -3334,14 +3339,14 @@
         <v>7</v>
       </c>
       <c r="F94" s="17" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="G94" s="54" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="H94" s="17"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="15" t="s">
         <v>26</v>
       </c>
@@ -3349,7 +3354,7 @@
         <v>2050</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D95" s="17" t="s">
         <v>91</v>
@@ -3360,14 +3365,12 @@
       <c r="F95" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="G95" s="16" t="s">
+      <c r="G95" s="54" t="s">
         <v>137</v>
       </c>
-      <c r="H95" s="17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H95" s="17"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="15" t="s">
         <v>26</v>
       </c>
@@ -3375,7 +3378,7 @@
         <v>2050</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D96" s="17" t="s">
         <v>91</v>
@@ -3389,9 +3392,11 @@
       <c r="G96" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H96" s="17"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H96" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="15" t="s">
         <v>26</v>
       </c>
@@ -3399,7 +3404,7 @@
         <v>2050</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D97" s="17" t="s">
         <v>91</v>
@@ -3408,14 +3413,14 @@
         <v>7</v>
       </c>
       <c r="F97" s="17" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="G97" s="16" t="s">
         <v>137</v>
       </c>
       <c r="H97" s="17"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="15" t="s">
         <v>26</v>
       </c>
@@ -3423,7 +3428,7 @@
         <v>2050</v>
       </c>
       <c r="C98" s="17" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D98" s="17" t="s">
         <v>91</v>
@@ -3432,14 +3437,14 @@
         <v>7</v>
       </c>
       <c r="F98" s="17" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G98" s="16" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="H98" s="17"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="15" t="s">
         <v>26</v>
       </c>
@@ -3447,7 +3452,7 @@
         <v>2050</v>
       </c>
       <c r="C99" s="17" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D99" s="17" t="s">
         <v>91</v>
@@ -3456,108 +3461,112 @@
         <v>7</v>
       </c>
       <c r="F99" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="G99" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="H99" s="17"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B100" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C100" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D100" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E100" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F100" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="G99" s="16" t="s">
+      <c r="G100" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="H99" s="17"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A100" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B100" s="22">
-        <v>2050</v>
-      </c>
-      <c r="C100" s="23" t="s">
+      <c r="H100" s="17"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B101" s="22">
+        <v>2050</v>
+      </c>
+      <c r="C101" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="D100" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E100" s="23" t="s">
+      <c r="D101" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="E101" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F100" s="23" t="s">
+      <c r="F101" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="G100" s="22" t="s">
+      <c r="G101" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="H100" s="23" t="s">
+      <c r="H101" s="23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A101" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B101" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C101" s="43" t="s">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B102" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C102" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D101" s="43" t="s">
+      <c r="D102" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E101" s="43" t="s">
+      <c r="E102" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="F101" s="43"/>
-      <c r="G101" s="42"/>
-      <c r="H101" s="43"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A102" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B102" s="45">
-        <v>2050</v>
-      </c>
-      <c r="C102" s="46" t="s">
+      <c r="F102" s="43"/>
+      <c r="G102" s="42"/>
+      <c r="H102" s="43"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="B103" s="45">
+        <v>2050</v>
+      </c>
+      <c r="C103" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="D102" s="46" t="s">
+      <c r="D103" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="E102" s="46" t="s">
+      <c r="E103" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="F102" s="46"/>
-      <c r="G102" s="45"/>
-      <c r="H102" s="46"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A103" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B103" s="30">
-        <v>2050</v>
-      </c>
-      <c r="C103" s="31" t="s">
+      <c r="F103" s="46"/>
+      <c r="G103" s="45"/>
+      <c r="H103" s="46"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B104" s="30">
+        <v>2050</v>
+      </c>
+      <c r="C104" s="31" t="s">
         <v>51</v>
-      </c>
-      <c r="D103" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E103" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="F103" s="31"/>
-      <c r="G103" s="30"/>
-      <c r="H103" s="31"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A104" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B104" s="30">
-        <v>2050</v>
-      </c>
-      <c r="C104" s="31" t="s">
-        <v>39</v>
       </c>
       <c r="D104" s="31" t="s">
         <v>34</v>
@@ -3569,7 +3578,7 @@
       <c r="G104" s="30"/>
       <c r="H104" s="31"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="29" t="s">
         <v>26</v>
       </c>
@@ -3577,7 +3586,7 @@
         <v>2050</v>
       </c>
       <c r="C105" s="31" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D105" s="31" t="s">
         <v>34</v>
@@ -3585,15 +3594,11 @@
       <c r="E105" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="F105" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="G105" s="30" t="s">
-        <v>63</v>
-      </c>
+      <c r="F105" s="31"/>
+      <c r="G105" s="30"/>
       <c r="H105" s="31"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="29" t="s">
         <v>26</v>
       </c>
@@ -3601,7 +3606,7 @@
         <v>2050</v>
       </c>
       <c r="C106" s="31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D106" s="31" t="s">
         <v>34</v>
@@ -3617,7 +3622,7 @@
       </c>
       <c r="H106" s="31"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="29" t="s">
         <v>26</v>
       </c>
@@ -3625,7 +3630,7 @@
         <v>2050</v>
       </c>
       <c r="C107" s="31" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D107" s="31" t="s">
         <v>34</v>
@@ -3634,14 +3639,14 @@
         <v>38</v>
       </c>
       <c r="F107" s="31" t="s">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="G107" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H107" s="31"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="29" t="s">
         <v>26</v>
       </c>
@@ -3649,7 +3654,7 @@
         <v>2050</v>
       </c>
       <c r="C108" s="31" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D108" s="31" t="s">
         <v>34</v>
@@ -3658,14 +3663,14 @@
         <v>38</v>
       </c>
       <c r="F108" s="31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G108" s="30" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H108" s="31"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="29" t="s">
         <v>26</v>
       </c>
@@ -3673,7 +3678,7 @@
         <v>2050</v>
       </c>
       <c r="C109" s="31" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D109" s="31" t="s">
         <v>34</v>
@@ -3682,14 +3687,14 @@
         <v>38</v>
       </c>
       <c r="F109" s="31" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G109" s="30" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H109" s="31"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="29" t="s">
         <v>26</v>
       </c>
@@ -3697,7 +3702,7 @@
         <v>2050</v>
       </c>
       <c r="C110" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D110" s="31" t="s">
         <v>34</v>
@@ -3706,14 +3711,14 @@
         <v>38</v>
       </c>
       <c r="F110" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G110" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H110" s="31"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="29" t="s">
         <v>26</v>
       </c>
@@ -3721,7 +3726,7 @@
         <v>2050</v>
       </c>
       <c r="C111" s="31" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D111" s="31" t="s">
         <v>34</v>
@@ -3730,72 +3735,72 @@
         <v>38</v>
       </c>
       <c r="F111" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="G111" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H111" s="31"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B112" s="30">
+        <v>2050</v>
+      </c>
+      <c r="C112" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="D112" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E112" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F112" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="G111" s="30" t="s">
+      <c r="G112" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="H111" s="31" t="s">
+      <c r="H112" s="31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A112" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B112" s="51">
-        <v>2050</v>
-      </c>
-      <c r="C112" s="52" t="s">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B113" s="51">
+        <v>2050</v>
+      </c>
+      <c r="C113" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="D112" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="E112" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="F112" s="52" t="s">
+      <c r="D113" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="E113" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="F113" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="G112" s="51" t="s">
+      <c r="G113" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="H112" s="52"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A113" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="B113" s="54">
-        <v>2050</v>
-      </c>
-      <c r="C113" s="53" t="s">
+      <c r="H113" s="52"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B114" s="54">
+        <v>2050</v>
+      </c>
+      <c r="C114" s="53" t="s">
         <v>101</v>
-      </c>
-      <c r="D113" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="E113" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F113" s="53" t="s">
-        <v>116</v>
-      </c>
-      <c r="G113" s="54" t="s">
-        <v>82</v>
-      </c>
-      <c r="H113" s="53"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A114" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="B114" s="54">
-        <v>2050</v>
-      </c>
-      <c r="C114" s="53" t="s">
-        <v>102</v>
       </c>
       <c r="D114" s="53" t="s">
         <v>91</v>
@@ -3811,7 +3816,7 @@
       </c>
       <c r="H114" s="53"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="53" t="s">
         <v>26</v>
       </c>
@@ -3819,7 +3824,7 @@
         <v>2050</v>
       </c>
       <c r="C115" s="53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D115" s="53" t="s">
         <v>91</v>
@@ -3835,7 +3840,7 @@
       </c>
       <c r="H115" s="53"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="53" t="s">
         <v>26</v>
       </c>
@@ -3843,7 +3848,7 @@
         <v>2050</v>
       </c>
       <c r="C116" s="53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D116" s="53" t="s">
         <v>91</v>
@@ -3859,7 +3864,7 @@
       </c>
       <c r="H116" s="53"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="53" t="s">
         <v>26</v>
       </c>
@@ -3867,7 +3872,7 @@
         <v>2050</v>
       </c>
       <c r="C117" s="53" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D117" s="53" t="s">
         <v>91</v>
@@ -3883,7 +3888,7 @@
       </c>
       <c r="H117" s="53"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="53" t="s">
         <v>26</v>
       </c>
@@ -3891,55 +3896,55 @@
         <v>2050</v>
       </c>
       <c r="C118" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="D118" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E118" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F118" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="G118" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="H118" s="53"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B119" s="54">
+        <v>2050</v>
+      </c>
+      <c r="C119" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="D118" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="E118" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F118" s="17" t="s">
+      <c r="D119" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E119" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F119" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="G118" s="54" t="s">
+      <c r="G119" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="H118" s="53"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A119" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="B119" s="54">
-        <v>2050</v>
-      </c>
-      <c r="C119" s="53" t="s">
+      <c r="H119" s="53"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A120" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B120" s="54">
+        <v>2050</v>
+      </c>
+      <c r="C120" s="53" t="s">
         <v>107</v>
-      </c>
-      <c r="D119" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="E119" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F119" s="53" t="s">
-        <v>116</v>
-      </c>
-      <c r="G119" s="54" t="s">
-        <v>82</v>
-      </c>
-      <c r="H119" s="53"/>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A120" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="B120" s="54">
-        <v>2050</v>
-      </c>
-      <c r="C120" s="53" t="s">
-        <v>109</v>
       </c>
       <c r="D120" s="53" t="s">
         <v>91</v>
@@ -3955,7 +3960,7 @@
       </c>
       <c r="H120" s="53"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="53" t="s">
         <v>26</v>
       </c>
@@ -3963,7 +3968,7 @@
         <v>2050</v>
       </c>
       <c r="C121" s="53" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D121" s="53" t="s">
         <v>91</v>
@@ -3979,7 +3984,7 @@
       </c>
       <c r="H121" s="53"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="53" t="s">
         <v>26</v>
       </c>
@@ -3987,103 +3992,103 @@
         <v>2050</v>
       </c>
       <c r="C122" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="D122" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E122" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F122" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="G122" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="H122" s="53"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A123" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B123" s="54">
+        <v>2050</v>
+      </c>
+      <c r="C123" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="D122" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="E122" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F122" s="53" t="s">
+      <c r="D123" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E123" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F123" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="G122" s="54" t="s">
+      <c r="G123" s="54" t="s">
         <v>122</v>
       </c>
-      <c r="H122" s="53"/>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A123" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="B123" s="54">
-        <v>2050</v>
-      </c>
-      <c r="C123" s="53" t="s">
+      <c r="H123" s="53"/>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A124" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B124" s="54">
+        <v>2050</v>
+      </c>
+      <c r="C124" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="D123" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="E123" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F123" s="17" t="s">
+      <c r="D124" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E124" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F124" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="G123" s="16" t="s">
+      <c r="G124" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="H123" s="17"/>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A124" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="B124" s="54">
-        <v>2050</v>
-      </c>
-      <c r="C124" s="53" t="s">
+      <c r="H124" s="17"/>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A125" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B125" s="54">
+        <v>2050</v>
+      </c>
+      <c r="C125" s="53" t="s">
         <v>130</v>
       </c>
-      <c r="D124" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="E124" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F124" s="17" t="s">
+      <c r="D125" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E125" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F125" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="G124" s="16" t="s">
+      <c r="G125" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="H124" s="17"/>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A125" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="B125" s="54">
-        <v>2050</v>
-      </c>
-      <c r="C125" s="53" t="s">
+      <c r="H125" s="17"/>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A126" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B126" s="54">
+        <v>2050</v>
+      </c>
+      <c r="C126" s="53" t="s">
         <v>140</v>
-      </c>
-      <c r="D125" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="E125" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F125" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="G125" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="H125" s="17"/>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A126" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="B126" s="54">
-        <v>2050</v>
-      </c>
-      <c r="C126" s="53" t="s">
-        <v>144</v>
       </c>
       <c r="D126" s="53" t="s">
         <v>91</v>
@@ -4099,7 +4104,7 @@
       </c>
       <c r="H126" s="17"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="53" t="s">
         <v>26</v>
       </c>
@@ -4107,7 +4112,7 @@
         <v>2050</v>
       </c>
       <c r="C127" s="53" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D127" s="53" t="s">
         <v>91</v>
@@ -4121,11 +4126,9 @@
       <c r="G127" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H127" s="17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H127" s="17"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="53" t="s">
         <v>26</v>
       </c>
@@ -4133,7 +4136,7 @@
         <v>2050</v>
       </c>
       <c r="C128" s="53" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D128" s="53" t="s">
         <v>91</v>
@@ -4147,9 +4150,11 @@
       <c r="G128" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H128" s="17"/>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H128" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="53" t="s">
         <v>26</v>
       </c>
@@ -4157,7 +4162,7 @@
         <v>2050</v>
       </c>
       <c r="C129" s="53" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D129" s="53" t="s">
         <v>91</v>
@@ -4173,7 +4178,7 @@
       </c>
       <c r="H129" s="17"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="53" t="s">
         <v>26</v>
       </c>
@@ -4181,7 +4186,7 @@
         <v>2050</v>
       </c>
       <c r="C130" s="53" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D130" s="53" t="s">
         <v>91</v>
@@ -4197,7 +4202,7 @@
       </c>
       <c r="H130" s="17"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="53" t="s">
         <v>26</v>
       </c>
@@ -4205,7 +4210,7 @@
         <v>2050</v>
       </c>
       <c r="C131" s="53" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D131" s="53" t="s">
         <v>91</v>
@@ -4221,7 +4226,7 @@
       </c>
       <c r="H131" s="17"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="53" t="s">
         <v>26</v>
       </c>
@@ -4229,7 +4234,7 @@
         <v>2050</v>
       </c>
       <c r="C132" s="53" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D132" s="53" t="s">
         <v>91</v>
@@ -4243,45 +4248,43 @@
       <c r="G132" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H132" s="17" t="s">
+      <c r="H132" s="17"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A133" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B133" s="54">
+        <v>2050</v>
+      </c>
+      <c r="C133" s="53" t="s">
+        <v>173</v>
+      </c>
+      <c r="D133" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E133" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F133" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="G133" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H133" s="17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A133" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="B133" s="60">
-        <v>2035</v>
-      </c>
-      <c r="C133" s="59" t="s">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A134" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B134" s="60">
+        <v>2035</v>
+      </c>
+      <c r="C134" s="59" t="s">
         <v>186</v>
-      </c>
-      <c r="D133" s="59" t="s">
-        <v>181</v>
-      </c>
-      <c r="E133" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="F133" s="59" t="s">
-        <v>184</v>
-      </c>
-      <c r="G133" s="60" t="s">
-        <v>185</v>
-      </c>
-      <c r="H133" s="59" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A134" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="B134" s="60">
-        <v>2050</v>
-      </c>
-      <c r="C134" s="59" t="s">
-        <v>180</v>
       </c>
       <c r="D134" s="59" t="s">
         <v>181</v>
@@ -4296,6 +4299,32 @@
         <v>185</v>
       </c>
       <c r="H134" s="59" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A135" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B135" s="60">
+        <v>2050</v>
+      </c>
+      <c r="C135" s="59" t="s">
+        <v>180</v>
+      </c>
+      <c r="D135" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="E135" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="F135" s="59" t="s">
+        <v>184</v>
+      </c>
+      <c r="G135" s="60" t="s">
+        <v>185</v>
+      </c>
+      <c r="H135" s="59" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added EIR alt1_v2 and alt2_v1
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A067FE1-A955-4AF4-AF3B-D26BC9ADAE5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019CC91F-4A5B-4365-A3A6-A205A6D61475}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14535" yWindow="3930" windowWidth="22830" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="197">
   <si>
     <t>EEJ</t>
   </si>
@@ -589,6 +589,33 @@
   </si>
   <si>
     <t>2015_UrbanSim_FBP</t>
+  </si>
+  <si>
+    <t>2035_TM152_EIR_Alt1_02</t>
+  </si>
+  <si>
+    <t>"EIR runs\Alt1 (s26) runs\Alt1_v2"</t>
+  </si>
+  <si>
+    <t>run373</t>
+  </si>
+  <si>
+    <t>2050_TM152_EIR_Alt1_02</t>
+  </si>
+  <si>
+    <t>2035_TM152_EIR_Alt2_01</t>
+  </si>
+  <si>
+    <t>Alt2</t>
+  </si>
+  <si>
+    <t>"EIR runs\Alt2 (s28) runs\Alt2_v1"</t>
+  </si>
+  <si>
+    <t>run374</t>
+  </si>
+  <si>
+    <t>2050_TM152_EIR_Alt2_01</t>
   </si>
 </sst>
 </file>
@@ -1180,23 +1207,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H135"/>
+  <dimension ref="A1:H139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A136" sqref="A136:XFD139"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.296875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="70.85546875" customWidth="1"/>
+    <col min="6" max="6" width="70.8984375" customWidth="1"/>
     <col min="7" max="7" width="15" style="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="56" t="s">
         <v>40</v>
       </c>
@@ -1222,7 +1249,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
@@ -1242,7 +1269,7 @@
       <c r="G2" s="6"/>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>25</v>
       </c>
@@ -1262,7 +1289,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="10"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>25</v>
       </c>
@@ -1282,7 +1309,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>25</v>
       </c>
@@ -1302,7 +1329,7 @@
       <c r="G5" s="13"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>25</v>
       </c>
@@ -1322,7 +1349,7 @@
       <c r="G6" s="13"/>
       <c r="H6" s="14"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>25</v>
       </c>
@@ -1342,7 +1369,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>25</v>
       </c>
@@ -1362,7 +1389,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="14"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>25</v>
       </c>
@@ -1382,7 +1409,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>25</v>
       </c>
@@ -1402,7 +1429,7 @@
       <c r="G10" s="19"/>
       <c r="H10" s="20"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>25</v>
       </c>
@@ -1422,7 +1449,7 @@
       <c r="G11" s="19"/>
       <c r="H11" s="20"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>25</v>
       </c>
@@ -1442,7 +1469,7 @@
       <c r="G12" s="19"/>
       <c r="H12" s="20"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>25</v>
       </c>
@@ -1462,7 +1489,7 @@
       <c r="G13" s="19"/>
       <c r="H13" s="20"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>25</v>
       </c>
@@ -1482,7 +1509,7 @@
       <c r="G14" s="19"/>
       <c r="H14" s="20"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>25</v>
       </c>
@@ -1502,7 +1529,7 @@
       <c r="G15" s="16"/>
       <c r="H15" s="17"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>25</v>
       </c>
@@ -1522,7 +1549,7 @@
       <c r="G16" s="16"/>
       <c r="H16" s="17"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>25</v>
       </c>
@@ -1542,7 +1569,7 @@
       <c r="G17" s="16"/>
       <c r="H17" s="17"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>25</v>
       </c>
@@ -1562,7 +1589,7 @@
       <c r="G18" s="16"/>
       <c r="H18" s="17"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="21" t="s">
         <v>25</v>
       </c>
@@ -1582,7 +1609,7 @@
       <c r="G19" s="22"/>
       <c r="H19" s="23"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
         <v>26</v>
       </c>
@@ -1604,7 +1631,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
         <v>26</v>
       </c>
@@ -1624,7 +1651,7 @@
       <c r="G21" s="25"/>
       <c r="H21" s="26"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>26</v>
       </c>
@@ -1646,7 +1673,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>26</v>
       </c>
@@ -1672,7 +1699,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>26</v>
       </c>
@@ -1696,7 +1723,7 @@
       </c>
       <c r="H24" s="48"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>26</v>
       </c>
@@ -1722,7 +1749,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="50" t="s">
         <v>26</v>
       </c>
@@ -1748,7 +1775,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
         <v>26</v>
       </c>
@@ -1772,7 +1799,7 @@
       </c>
       <c r="H27" s="20"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="33" t="s">
         <v>26</v>
       </c>
@@ -1798,7 +1825,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>26</v>
       </c>
@@ -1824,7 +1851,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
         <v>26</v>
       </c>
@@ -1848,7 +1875,7 @@
       </c>
       <c r="H30" s="20"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
         <v>26</v>
       </c>
@@ -1874,7 +1901,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="36" t="s">
         <v>26</v>
       </c>
@@ -1894,7 +1921,7 @@
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>26</v>
       </c>
@@ -1914,7 +1941,7 @@
       <c r="G33" s="19"/>
       <c r="H33" s="20"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
         <v>26</v>
       </c>
@@ -1934,7 +1961,7 @@
       <c r="G34" s="19"/>
       <c r="H34" s="20"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
         <v>26</v>
       </c>
@@ -1956,7 +1983,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="36" t="s">
         <v>26</v>
       </c>
@@ -1976,7 +2003,7 @@
       <c r="G36" s="37"/>
       <c r="H36" s="38"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="18" t="s">
         <v>26</v>
       </c>
@@ -1996,7 +2023,7 @@
       <c r="G37" s="19"/>
       <c r="H37" s="20"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="18" t="s">
         <v>26</v>
       </c>
@@ -2016,7 +2043,7 @@
       <c r="G38" s="19"/>
       <c r="H38" s="20"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
         <v>26</v>
       </c>
@@ -2036,7 +2063,7 @@
       <c r="G39" s="19"/>
       <c r="H39" s="20"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="18" t="s">
         <v>26</v>
       </c>
@@ -2060,7 +2087,7 @@
       </c>
       <c r="H40" s="20"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="18" t="s">
         <v>26</v>
       </c>
@@ -2084,7 +2111,7 @@
       </c>
       <c r="H41" s="20"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="33" t="s">
         <v>26</v>
       </c>
@@ -2108,7 +2135,7 @@
       </c>
       <c r="H42" s="35"/>
     </row>
-    <row r="43" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="50" t="s">
         <v>26</v>
       </c>
@@ -2132,7 +2159,7 @@
       </c>
       <c r="H43" s="52"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="15" t="s">
         <v>26</v>
       </c>
@@ -2156,7 +2183,7 @@
       </c>
       <c r="H44" s="17"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
         <v>26</v>
       </c>
@@ -2180,7 +2207,7 @@
       </c>
       <c r="H45" s="17"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="15" t="s">
         <v>26</v>
       </c>
@@ -2204,7 +2231,7 @@
       </c>
       <c r="H46" s="17"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="15" t="s">
         <v>26</v>
       </c>
@@ -2230,7 +2257,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="15" t="s">
         <v>26</v>
       </c>
@@ -2254,7 +2281,7 @@
       </c>
       <c r="H48" s="17"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="15" t="s">
         <v>26</v>
       </c>
@@ -2278,7 +2305,7 @@
       </c>
       <c r="H49" s="17"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="15" t="s">
         <v>26</v>
       </c>
@@ -2302,7 +2329,7 @@
       </c>
       <c r="H50" s="17"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="21" t="s">
         <v>26</v>
       </c>
@@ -2328,7 +2355,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="36" t="s">
         <v>26</v>
       </c>
@@ -2348,7 +2375,7 @@
       <c r="G52" s="37"/>
       <c r="H52" s="38"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="33" t="s">
         <v>26</v>
       </c>
@@ -2368,7 +2395,7 @@
       <c r="G53" s="34"/>
       <c r="H53" s="35"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="18" t="s">
         <v>26</v>
       </c>
@@ -2388,7 +2415,7 @@
       <c r="G54" s="19"/>
       <c r="H54" s="20"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="18" t="s">
         <v>26</v>
       </c>
@@ -2408,7 +2435,7 @@
       <c r="G55" s="19"/>
       <c r="H55" s="20"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="18" t="s">
         <v>26</v>
       </c>
@@ -2432,7 +2459,7 @@
       </c>
       <c r="H56" s="20"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="18" t="s">
         <v>26</v>
       </c>
@@ -2456,7 +2483,7 @@
       </c>
       <c r="H57" s="20"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="18" t="s">
         <v>26</v>
       </c>
@@ -2480,7 +2507,7 @@
       </c>
       <c r="H58" s="20"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="18" t="s">
         <v>26</v>
       </c>
@@ -2504,7 +2531,7 @@
       </c>
       <c r="H59" s="20"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="18" t="s">
         <v>26</v>
       </c>
@@ -2528,7 +2555,7 @@
       </c>
       <c r="H60" s="20"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="18" t="s">
         <v>26</v>
       </c>
@@ -2554,7 +2581,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="49" t="s">
         <v>26</v>
       </c>
@@ -2578,7 +2605,7 @@
       </c>
       <c r="H62" s="28"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="49" t="s">
         <v>26</v>
       </c>
@@ -2602,7 +2629,7 @@
       </c>
       <c r="H63" s="28"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="18" t="s">
         <v>26</v>
       </c>
@@ -2626,7 +2653,7 @@
       </c>
       <c r="H64" s="20"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="18" t="s">
         <v>26</v>
       </c>
@@ -2650,7 +2677,7 @@
       </c>
       <c r="H65" s="20"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="18" t="s">
         <v>26</v>
       </c>
@@ -2674,7 +2701,7 @@
       </c>
       <c r="H66" s="20"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="18" t="s">
         <v>26</v>
       </c>
@@ -2698,7 +2725,7 @@
       </c>
       <c r="H67" s="20"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="50" t="s">
         <v>26</v>
       </c>
@@ -2722,7 +2749,7 @@
       </c>
       <c r="H68" s="52"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="15" t="s">
         <v>26</v>
       </c>
@@ -2746,7 +2773,7 @@
       </c>
       <c r="H69" s="17"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="15" t="s">
         <v>26</v>
       </c>
@@ -2770,7 +2797,7 @@
       </c>
       <c r="H70" s="17"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="15" t="s">
         <v>26</v>
       </c>
@@ -2794,7 +2821,7 @@
       </c>
       <c r="H71" s="17"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="15" t="s">
         <v>26</v>
       </c>
@@ -2818,7 +2845,7 @@
       </c>
       <c r="H72" s="17"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="15" t="s">
         <v>26</v>
       </c>
@@ -2842,7 +2869,7 @@
       </c>
       <c r="H73" s="17"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="15" t="s">
         <v>26</v>
       </c>
@@ -2866,7 +2893,7 @@
       </c>
       <c r="H74" s="17"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="15" t="s">
         <v>26</v>
       </c>
@@ -2890,7 +2917,7 @@
       </c>
       <c r="H75" s="17"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="15" t="s">
         <v>26</v>
       </c>
@@ -2914,7 +2941,7 @@
       </c>
       <c r="H76" s="17"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="15" t="s">
         <v>26</v>
       </c>
@@ -2938,7 +2965,7 @@
       </c>
       <c r="H77" s="17"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="15" t="s">
         <v>26</v>
       </c>
@@ -2964,7 +2991,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="15" t="s">
         <v>26</v>
       </c>
@@ -2988,7 +3015,7 @@
       </c>
       <c r="H79" s="17"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="15" t="s">
         <v>26</v>
       </c>
@@ -3012,7 +3039,7 @@
       </c>
       <c r="H80" s="17"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="15" t="s">
         <v>26</v>
       </c>
@@ -3036,7 +3063,7 @@
       </c>
       <c r="H81" s="17"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="21" t="s">
         <v>26</v>
       </c>
@@ -3062,7 +3089,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="61" t="s">
         <v>26</v>
       </c>
@@ -3088,7 +3115,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="15" t="s">
         <v>26</v>
       </c>
@@ -3114,7 +3141,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="39" t="s">
         <v>26</v>
       </c>
@@ -3134,7 +3161,7 @@
       <c r="G85" s="40"/>
       <c r="H85" s="41"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="29" t="s">
         <v>26</v>
       </c>
@@ -3154,7 +3181,7 @@
       <c r="G86" s="42"/>
       <c r="H86" s="43"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="29" t="s">
         <v>26</v>
       </c>
@@ -3178,7 +3205,7 @@
       </c>
       <c r="H87" s="43"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="29" t="s">
         <v>26</v>
       </c>
@@ -3202,7 +3229,7 @@
       </c>
       <c r="H88" s="43"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="29" t="s">
         <v>26</v>
       </c>
@@ -3226,7 +3253,7 @@
       </c>
       <c r="H89" s="43"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="29" t="s">
         <v>26</v>
       </c>
@@ -3250,7 +3277,7 @@
       </c>
       <c r="H90" s="43"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="44" t="s">
         <v>26</v>
       </c>
@@ -3274,7 +3301,7 @@
       </c>
       <c r="H91" s="46"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="15" t="s">
         <v>26</v>
       </c>
@@ -3298,7 +3325,7 @@
       </c>
       <c r="H92" s="17"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="15" t="s">
         <v>26</v>
       </c>
@@ -3322,7 +3349,7 @@
       </c>
       <c r="H93" s="17"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="15" t="s">
         <v>26</v>
       </c>
@@ -3346,7 +3373,7 @@
       </c>
       <c r="H94" s="17"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="15" t="s">
         <v>26</v>
       </c>
@@ -3370,7 +3397,7 @@
       </c>
       <c r="H95" s="17"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="15" t="s">
         <v>26</v>
       </c>
@@ -3396,7 +3423,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="15" t="s">
         <v>26</v>
       </c>
@@ -3420,7 +3447,7 @@
       </c>
       <c r="H97" s="17"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="15" t="s">
         <v>26</v>
       </c>
@@ -3444,7 +3471,7 @@
       </c>
       <c r="H98" s="17"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="15" t="s">
         <v>26</v>
       </c>
@@ -3468,7 +3495,7 @@
       </c>
       <c r="H99" s="17"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="15" t="s">
         <v>26</v>
       </c>
@@ -3492,7 +3519,7 @@
       </c>
       <c r="H100" s="17"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="21" t="s">
         <v>26</v>
       </c>
@@ -3518,7 +3545,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="29" t="s">
         <v>26</v>
       </c>
@@ -3538,7 +3565,7 @@
       <c r="G102" s="42"/>
       <c r="H102" s="43"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="44" t="s">
         <v>26</v>
       </c>
@@ -3558,7 +3585,7 @@
       <c r="G103" s="45"/>
       <c r="H103" s="46"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="29" t="s">
         <v>26</v>
       </c>
@@ -3578,7 +3605,7 @@
       <c r="G104" s="30"/>
       <c r="H104" s="31"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="29" t="s">
         <v>26</v>
       </c>
@@ -3598,7 +3625,7 @@
       <c r="G105" s="30"/>
       <c r="H105" s="31"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="29" t="s">
         <v>26</v>
       </c>
@@ -3622,7 +3649,7 @@
       </c>
       <c r="H106" s="31"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="29" t="s">
         <v>26</v>
       </c>
@@ -3646,7 +3673,7 @@
       </c>
       <c r="H107" s="31"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="29" t="s">
         <v>26</v>
       </c>
@@ -3670,7 +3697,7 @@
       </c>
       <c r="H108" s="31"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="29" t="s">
         <v>26</v>
       </c>
@@ -3694,7 +3721,7 @@
       </c>
       <c r="H109" s="31"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="29" t="s">
         <v>26</v>
       </c>
@@ -3718,7 +3745,7 @@
       </c>
       <c r="H110" s="31"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="29" t="s">
         <v>26</v>
       </c>
@@ -3742,7 +3769,7 @@
       </c>
       <c r="H111" s="31"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="29" t="s">
         <v>26</v>
       </c>
@@ -3768,7 +3795,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="50" t="s">
         <v>26</v>
       </c>
@@ -3792,7 +3819,7 @@
       </c>
       <c r="H113" s="52"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="53" t="s">
         <v>26</v>
       </c>
@@ -3816,7 +3843,7 @@
       </c>
       <c r="H114" s="53"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="53" t="s">
         <v>26</v>
       </c>
@@ -3840,7 +3867,7 @@
       </c>
       <c r="H115" s="53"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="53" t="s">
         <v>26</v>
       </c>
@@ -3864,7 +3891,7 @@
       </c>
       <c r="H116" s="53"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="53" t="s">
         <v>26</v>
       </c>
@@ -3888,7 +3915,7 @@
       </c>
       <c r="H117" s="53"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="53" t="s">
         <v>26</v>
       </c>
@@ -3912,7 +3939,7 @@
       </c>
       <c r="H118" s="53"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="53" t="s">
         <v>26</v>
       </c>
@@ -3936,7 +3963,7 @@
       </c>
       <c r="H119" s="53"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="53" t="s">
         <v>26</v>
       </c>
@@ -3960,7 +3987,7 @@
       </c>
       <c r="H120" s="53"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="53" t="s">
         <v>26</v>
       </c>
@@ -3984,7 +4011,7 @@
       </c>
       <c r="H121" s="53"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="53" t="s">
         <v>26</v>
       </c>
@@ -4008,7 +4035,7 @@
       </c>
       <c r="H122" s="53"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="53" t="s">
         <v>26</v>
       </c>
@@ -4032,7 +4059,7 @@
       </c>
       <c r="H123" s="53"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="53" t="s">
         <v>26</v>
       </c>
@@ -4056,7 +4083,7 @@
       </c>
       <c r="H124" s="17"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="53" t="s">
         <v>26</v>
       </c>
@@ -4080,7 +4107,7 @@
       </c>
       <c r="H125" s="17"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="53" t="s">
         <v>26</v>
       </c>
@@ -4104,7 +4131,7 @@
       </c>
       <c r="H126" s="17"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="53" t="s">
         <v>26</v>
       </c>
@@ -4128,7 +4155,7 @@
       </c>
       <c r="H127" s="17"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="53" t="s">
         <v>26</v>
       </c>
@@ -4154,7 +4181,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="53" t="s">
         <v>26</v>
       </c>
@@ -4178,7 +4205,7 @@
       </c>
       <c r="H129" s="17"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="53" t="s">
         <v>26</v>
       </c>
@@ -4202,7 +4229,7 @@
       </c>
       <c r="H130" s="17"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="53" t="s">
         <v>26</v>
       </c>
@@ -4226,7 +4253,7 @@
       </c>
       <c r="H131" s="17"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="53" t="s">
         <v>26</v>
       </c>
@@ -4250,7 +4277,7 @@
       </c>
       <c r="H132" s="17"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="53" t="s">
         <v>26</v>
       </c>
@@ -4276,7 +4303,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="59" t="s">
         <v>26</v>
       </c>
@@ -4302,7 +4329,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="59" t="s">
         <v>26</v>
       </c>
@@ -4325,6 +4352,110 @@
         <v>185</v>
       </c>
       <c r="H135" s="59" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A136" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B136" s="60">
+        <v>2035</v>
+      </c>
+      <c r="C136" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="D136" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="E136" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="F136" s="59" t="s">
+        <v>189</v>
+      </c>
+      <c r="G136" s="60" t="s">
+        <v>190</v>
+      </c>
+      <c r="H136" s="59" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A137" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B137" s="60">
+        <v>2050</v>
+      </c>
+      <c r="C137" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="D137" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="E137" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="F137" s="59" t="s">
+        <v>189</v>
+      </c>
+      <c r="G137" s="60" t="s">
+        <v>190</v>
+      </c>
+      <c r="H137" s="59" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A138" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B138" s="60">
+        <v>2035</v>
+      </c>
+      <c r="C138" s="59" t="s">
+        <v>192</v>
+      </c>
+      <c r="D138" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="E138" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="F138" s="59" t="s">
+        <v>194</v>
+      </c>
+      <c r="G138" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="H138" s="59" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A139" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B139" s="60">
+        <v>2050</v>
+      </c>
+      <c r="C139" s="59" t="s">
+        <v>196</v>
+      </c>
+      <c r="D139" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="E139" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="F139" s="59" t="s">
+        <v>194</v>
+      </c>
+      <c r="G139" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="H139" s="59" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
anticipating the completion of new EIR Alt1 and Alt2 runs
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019CC91F-4A5B-4365-A3A6-A205A6D61475}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCE57E1-85DF-4C80-8350-5BABF1D9FCDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="203">
   <si>
     <t>EEJ</t>
   </si>
@@ -616,6 +616,24 @@
   </si>
   <si>
     <t>2050_TM152_EIR_Alt2_01</t>
+  </si>
+  <si>
+    <t>run375</t>
+  </si>
+  <si>
+    <t>2035_TM152_EIR_Alt1_03</t>
+  </si>
+  <si>
+    <t>2050_TM152_EIR_Alt1_03</t>
+  </si>
+  <si>
+    <t>"EIR runs\Alt1 (s26) runs\Alt1_v3_test_far_tiers_FINAL_EIR_ALT"</t>
+  </si>
+  <si>
+    <t>2035_TM152_EIR_Alt2_02</t>
+  </si>
+  <si>
+    <t>2050_TM152_EIR_Alt2_02</t>
   </si>
 </sst>
 </file>
@@ -1207,11 +1225,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H139"/>
+  <dimension ref="A1:H143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A136" sqref="A136:XFD139"/>
+      <selection pane="bottomLeft" activeCell="C144" sqref="C144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -4325,9 +4343,7 @@
       <c r="G134" s="60" t="s">
         <v>185</v>
       </c>
-      <c r="H134" s="59" t="s">
-        <v>43</v>
-      </c>
+      <c r="H134" s="59"/>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="59" t="s">
@@ -4351,9 +4367,7 @@
       <c r="G135" s="60" t="s">
         <v>185</v>
       </c>
-      <c r="H135" s="59" t="s">
-        <v>43</v>
-      </c>
+      <c r="H135" s="59"/>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" s="59" t="s">
@@ -4377,9 +4391,7 @@
       <c r="G136" s="60" t="s">
         <v>190</v>
       </c>
-      <c r="H136" s="59" t="s">
-        <v>43</v>
-      </c>
+      <c r="H136" s="59"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="59" t="s">
@@ -4403,9 +4415,7 @@
       <c r="G137" s="60" t="s">
         <v>190</v>
       </c>
-      <c r="H137" s="59" t="s">
-        <v>43</v>
-      </c>
+      <c r="H137" s="59"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="59" t="s">
@@ -4415,19 +4425,19 @@
         <v>2035</v>
       </c>
       <c r="C138" s="59" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="D138" s="59" t="s">
         <v>181</v>
       </c>
       <c r="E138" s="59" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="F138" s="59" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="G138" s="60" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="H138" s="59" t="s">
         <v>43</v>
@@ -4441,21 +4451,121 @@
         <v>2050</v>
       </c>
       <c r="C139" s="59" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D139" s="59" t="s">
         <v>181</v>
       </c>
       <c r="E139" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="F139" s="59" t="s">
+        <v>200</v>
+      </c>
+      <c r="G139" s="60" t="s">
+        <v>197</v>
+      </c>
+      <c r="H139" s="59" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A140" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B140" s="60">
+        <v>2035</v>
+      </c>
+      <c r="C140" s="59" t="s">
+        <v>192</v>
+      </c>
+      <c r="D140" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="E140" s="59" t="s">
         <v>193</v>
       </c>
-      <c r="F139" s="59" t="s">
+      <c r="F140" s="59" t="s">
         <v>194</v>
       </c>
-      <c r="G139" s="60" t="s">
+      <c r="G140" s="60" t="s">
         <v>195</v>
       </c>
-      <c r="H139" s="59" t="s">
+      <c r="H140" s="59"/>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A141" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B141" s="60">
+        <v>2050</v>
+      </c>
+      <c r="C141" s="59" t="s">
+        <v>196</v>
+      </c>
+      <c r="D141" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="E141" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="F141" s="59" t="s">
+        <v>194</v>
+      </c>
+      <c r="G141" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="H141" s="59"/>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A142" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B142" s="60">
+        <v>2035</v>
+      </c>
+      <c r="C142" s="59" t="s">
+        <v>201</v>
+      </c>
+      <c r="D142" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="E142" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="F142" s="59" t="s">
+        <v>194</v>
+      </c>
+      <c r="G142" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="H142" s="59" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A143" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B143" s="60">
+        <v>2050</v>
+      </c>
+      <c r="C143" s="59" t="s">
+        <v>202</v>
+      </c>
+      <c r="D143" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="E143" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="F143" s="59" t="s">
+        <v>194</v>
+      </c>
+      <c r="G143" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="H143" s="59" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added the no Q2 fare discount test run for Alt2
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCE57E1-85DF-4C80-8350-5BABF1D9FCDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E0BE73-6A08-420C-B868-6838A620F313}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="204">
   <si>
     <t>EEJ</t>
   </si>
@@ -634,6 +634,9 @@
   </si>
   <si>
     <t>2050_TM152_EIR_Alt2_02</t>
+  </si>
+  <si>
+    <t>2035_TM152_EIR_Alt2_02_noQ2FareDiscount</t>
   </si>
 </sst>
 </file>
@@ -675,7 +678,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -724,6 +727,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -766,7 +775,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -877,6 +886,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1225,11 +1238,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H143"/>
+  <dimension ref="A1:H144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C144" sqref="C144"/>
+      <selection pane="bottomLeft" activeCell="F144" sqref="F144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -4569,6 +4582,32 @@
         <v>43</v>
       </c>
     </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A144" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="B144" s="65">
+        <v>2035</v>
+      </c>
+      <c r="C144" s="64" t="s">
+        <v>203</v>
+      </c>
+      <c r="D144" s="64" t="s">
+        <v>181</v>
+      </c>
+      <c r="E144" s="64" t="s">
+        <v>193</v>
+      </c>
+      <c r="F144" s="64" t="s">
+        <v>194</v>
+      </c>
+      <c r="G144" s="65" t="s">
+        <v>195</v>
+      </c>
+      <c r="H144" s="64" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added 2035_TM152_FBP_Plus_21 (the run with the SF congestion pricing fix)
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E0BE73-6A08-420C-B868-6838A620F313}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1220557-BFC9-4ADC-A6EE-41819389DC33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="205">
   <si>
     <t>EEJ</t>
   </si>
@@ -637,6 +637,9 @@
   </si>
   <si>
     <t>2035_TM152_EIR_Alt2_02_noQ2FareDiscount</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_Plus_21</t>
   </si>
 </sst>
 </file>
@@ -1238,11 +1241,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H144"/>
+  <dimension ref="A1:H145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F144" sqref="F144"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -3095,122 +3098,128 @@
       <c r="H81" s="17"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A82" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B82" s="22">
-        <v>2035</v>
-      </c>
-      <c r="C82" s="23" t="s">
+      <c r="A82" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B82" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C82" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="D82" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E82" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F82" s="23" t="s">
+      <c r="D82" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E82" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F82" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="G82" s="22" t="s">
+      <c r="G82" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H82" s="23" t="s">
+      <c r="H82" s="17" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A83" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="B83" s="62">
-        <v>2040</v>
-      </c>
-      <c r="C83" s="63" t="s">
-        <v>183</v>
-      </c>
-      <c r="D83" s="63" t="s">
-        <v>91</v>
-      </c>
-      <c r="E83" s="63" t="s">
-        <v>7</v>
+      <c r="A83" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B83" s="22">
+        <v>2035</v>
+      </c>
+      <c r="C83" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="D83" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="E83" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="F83" s="23" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="G83" s="22" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
       <c r="H83" s="23" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A84" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B84" s="16">
+      <c r="A84" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B84" s="62">
         <v>2040</v>
       </c>
-      <c r="C84" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="D84" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E84" s="23" t="s">
-        <v>38</v>
+      <c r="C84" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="D84" s="63" t="s">
+        <v>91</v>
+      </c>
+      <c r="E84" s="63" t="s">
+        <v>7</v>
       </c>
       <c r="F84" s="23" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="G84" s="22" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="H84" s="23" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A85" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="B85" s="40">
-        <v>2050</v>
-      </c>
-      <c r="C85" s="41" t="s">
+      <c r="A85" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B85" s="16">
+        <v>2040</v>
+      </c>
+      <c r="C85" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="D85" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E85" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F85" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="G85" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="H85" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A86" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B86" s="40">
+        <v>2050</v>
+      </c>
+      <c r="C86" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D85" s="41" t="s">
+      <c r="D86" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="E85" s="41" t="s">
+      <c r="E86" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F85" s="41"/>
-      <c r="G85" s="40"/>
-      <c r="H85" s="41"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A86" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B86" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C86" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="D86" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E86" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="F86" s="43"/>
-      <c r="G86" s="42"/>
-      <c r="H86" s="43"/>
+      <c r="F86" s="41"/>
+      <c r="G86" s="40"/>
+      <c r="H86" s="41"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="29" t="s">
@@ -3220,7 +3229,7 @@
         <v>2050</v>
       </c>
       <c r="C87" s="43" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D87" s="43" t="s">
         <v>34</v>
@@ -3228,12 +3237,8 @@
       <c r="E87" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F87" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="G87" s="42" t="s">
-        <v>65</v>
-      </c>
+      <c r="F87" s="43"/>
+      <c r="G87" s="42"/>
       <c r="H87" s="43"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
@@ -3244,7 +3249,7 @@
         <v>2050</v>
       </c>
       <c r="C88" s="43" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D88" s="43" t="s">
         <v>34</v>
@@ -3268,7 +3273,7 @@
         <v>2050</v>
       </c>
       <c r="C89" s="43" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D89" s="43" t="s">
         <v>34</v>
@@ -3277,10 +3282,10 @@
         <v>7</v>
       </c>
       <c r="F89" s="43" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G89" s="42" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H89" s="43"/>
     </row>
@@ -3292,7 +3297,7 @@
         <v>2050</v>
       </c>
       <c r="C90" s="43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D90" s="43" t="s">
         <v>34</v>
@@ -3301,60 +3306,60 @@
         <v>7</v>
       </c>
       <c r="F90" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="G90" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="H90" s="43"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A91" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B91" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C91" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="D91" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E91" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F91" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="G90" s="42" t="s">
+      <c r="G91" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="H90" s="43"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A91" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B91" s="45">
-        <v>2050</v>
-      </c>
-      <c r="C91" s="46" t="s">
+      <c r="H91" s="43"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A92" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="B92" s="45">
+        <v>2050</v>
+      </c>
+      <c r="C92" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="D91" s="46" t="s">
+      <c r="D92" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="E91" s="46" t="s">
+      <c r="E92" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="F91" s="46" t="s">
+      <c r="F92" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="G91" s="45" t="s">
+      <c r="G92" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="H91" s="46"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A92" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B92" s="16">
-        <v>2050</v>
-      </c>
-      <c r="C92" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="D92" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="E92" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F92" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="G92" s="54" t="s">
-        <v>75</v>
-      </c>
-      <c r="H92" s="17"/>
+      <c r="H92" s="46"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="15" t="s">
@@ -3364,19 +3369,19 @@
         <v>2050</v>
       </c>
       <c r="C93" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D93" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D93" s="52" t="s">
         <v>91</v>
       </c>
       <c r="E93" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F93" s="17" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G93" s="54" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H93" s="17"/>
     </row>
@@ -3388,7 +3393,7 @@
         <v>2050</v>
       </c>
       <c r="C94" s="17" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="D94" s="17" t="s">
         <v>91</v>
@@ -3397,10 +3402,10 @@
         <v>7</v>
       </c>
       <c r="F94" s="17" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G94" s="54" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H94" s="17"/>
     </row>
@@ -3412,7 +3417,7 @@
         <v>2050</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="D95" s="17" t="s">
         <v>91</v>
@@ -3421,10 +3426,10 @@
         <v>7</v>
       </c>
       <c r="F95" s="17" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="G95" s="54" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="H95" s="17"/>
     </row>
@@ -3436,7 +3441,7 @@
         <v>2050</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D96" s="17" t="s">
         <v>91</v>
@@ -3447,12 +3452,10 @@
       <c r="F96" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="G96" s="16" t="s">
+      <c r="G96" s="54" t="s">
         <v>137</v>
       </c>
-      <c r="H96" s="17" t="s">
-        <v>43</v>
-      </c>
+      <c r="H96" s="17"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="15" t="s">
@@ -3462,7 +3465,7 @@
         <v>2050</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D97" s="17" t="s">
         <v>91</v>
@@ -3476,7 +3479,9 @@
       <c r="G97" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H97" s="17"/>
+      <c r="H97" s="17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="15" t="s">
@@ -3486,7 +3491,7 @@
         <v>2050</v>
       </c>
       <c r="C98" s="17" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D98" s="17" t="s">
         <v>91</v>
@@ -3495,7 +3500,7 @@
         <v>7</v>
       </c>
       <c r="F98" s="17" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="G98" s="16" t="s">
         <v>137</v>
@@ -3510,7 +3515,7 @@
         <v>2050</v>
       </c>
       <c r="C99" s="17" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D99" s="17" t="s">
         <v>91</v>
@@ -3519,10 +3524,10 @@
         <v>7</v>
       </c>
       <c r="F99" s="17" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G99" s="16" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="H99" s="17"/>
     </row>
@@ -3534,7 +3539,7 @@
         <v>2050</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D100" s="17" t="s">
         <v>91</v>
@@ -3543,98 +3548,102 @@
         <v>7</v>
       </c>
       <c r="F100" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="G100" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="H100" s="17"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A101" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B101" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C101" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D101" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E101" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F101" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="G100" s="16" t="s">
+      <c r="G101" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="H100" s="17"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A101" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B101" s="22">
-        <v>2050</v>
-      </c>
-      <c r="C101" s="23" t="s">
+      <c r="H101" s="17"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A102" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B102" s="22">
+        <v>2050</v>
+      </c>
+      <c r="C102" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="D101" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E101" s="23" t="s">
+      <c r="D102" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="E102" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F101" s="23" t="s">
+      <c r="F102" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="G101" s="22" t="s">
+      <c r="G102" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="H101" s="23" t="s">
+      <c r="H102" s="23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A102" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B102" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C102" s="43" t="s">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A103" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B103" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C103" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D102" s="43" t="s">
+      <c r="D103" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E102" s="43" t="s">
+      <c r="E103" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="F102" s="43"/>
-      <c r="G102" s="42"/>
-      <c r="H102" s="43"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A103" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B103" s="45">
-        <v>2050</v>
-      </c>
-      <c r="C103" s="46" t="s">
+      <c r="F103" s="43"/>
+      <c r="G103" s="42"/>
+      <c r="H103" s="43"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A104" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="B104" s="45">
+        <v>2050</v>
+      </c>
+      <c r="C104" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="D103" s="46" t="s">
+      <c r="D104" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="E103" s="46" t="s">
+      <c r="E104" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="F103" s="46"/>
-      <c r="G103" s="45"/>
-      <c r="H103" s="46"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A104" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B104" s="30">
-        <v>2050</v>
-      </c>
-      <c r="C104" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="D104" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E104" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="F104" s="31"/>
-      <c r="G104" s="30"/>
-      <c r="H104" s="31"/>
+      <c r="F104" s="46"/>
+      <c r="G104" s="45"/>
+      <c r="H104" s="46"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="29" t="s">
@@ -3644,7 +3653,7 @@
         <v>2050</v>
       </c>
       <c r="C105" s="31" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D105" s="31" t="s">
         <v>34</v>
@@ -3664,7 +3673,7 @@
         <v>2050</v>
       </c>
       <c r="C106" s="31" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D106" s="31" t="s">
         <v>34</v>
@@ -3672,12 +3681,8 @@
       <c r="E106" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="F106" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="G106" s="30" t="s">
-        <v>63</v>
-      </c>
+      <c r="F106" s="31"/>
+      <c r="G106" s="30"/>
       <c r="H106" s="31"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
@@ -3688,7 +3693,7 @@
         <v>2050</v>
       </c>
       <c r="C107" s="31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D107" s="31" t="s">
         <v>34</v>
@@ -3712,7 +3717,7 @@
         <v>2050</v>
       </c>
       <c r="C108" s="31" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D108" s="31" t="s">
         <v>34</v>
@@ -3721,10 +3726,10 @@
         <v>38</v>
       </c>
       <c r="F108" s="31" t="s">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="G108" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H108" s="31"/>
     </row>
@@ -3736,7 +3741,7 @@
         <v>2050</v>
       </c>
       <c r="C109" s="31" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D109" s="31" t="s">
         <v>34</v>
@@ -3745,10 +3750,10 @@
         <v>38</v>
       </c>
       <c r="F109" s="31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G109" s="30" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H109" s="31"/>
     </row>
@@ -3760,7 +3765,7 @@
         <v>2050</v>
       </c>
       <c r="C110" s="31" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D110" s="31" t="s">
         <v>34</v>
@@ -3769,10 +3774,10 @@
         <v>38</v>
       </c>
       <c r="F110" s="31" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G110" s="30" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H110" s="31"/>
     </row>
@@ -3784,7 +3789,7 @@
         <v>2050</v>
       </c>
       <c r="C111" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D111" s="31" t="s">
         <v>34</v>
@@ -3793,10 +3798,10 @@
         <v>38</v>
       </c>
       <c r="F111" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G111" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H111" s="31"/>
     </row>
@@ -3808,7 +3813,7 @@
         <v>2050</v>
       </c>
       <c r="C112" s="31" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D112" s="31" t="s">
         <v>34</v>
@@ -3817,62 +3822,62 @@
         <v>38</v>
       </c>
       <c r="F112" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="G112" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H112" s="31"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A113" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B113" s="30">
+        <v>2050</v>
+      </c>
+      <c r="C113" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="D113" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E113" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F113" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="G112" s="30" t="s">
+      <c r="G113" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="H112" s="31" t="s">
+      <c r="H113" s="31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A113" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B113" s="51">
-        <v>2050</v>
-      </c>
-      <c r="C113" s="52" t="s">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A114" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B114" s="51">
+        <v>2050</v>
+      </c>
+      <c r="C114" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="D113" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="E113" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="F113" s="52" t="s">
+      <c r="D114" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="E114" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="F114" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="G113" s="51" t="s">
+      <c r="G114" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="H113" s="52"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A114" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="B114" s="54">
-        <v>2050</v>
-      </c>
-      <c r="C114" s="53" t="s">
-        <v>101</v>
-      </c>
-      <c r="D114" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="E114" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F114" s="53" t="s">
-        <v>116</v>
-      </c>
-      <c r="G114" s="54" t="s">
-        <v>82</v>
-      </c>
-      <c r="H114" s="53"/>
+      <c r="H114" s="52"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="53" t="s">
@@ -3882,7 +3887,7 @@
         <v>2050</v>
       </c>
       <c r="C115" s="53" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D115" s="53" t="s">
         <v>91</v>
@@ -3906,7 +3911,7 @@
         <v>2050</v>
       </c>
       <c r="C116" s="53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D116" s="53" t="s">
         <v>91</v>
@@ -3930,7 +3935,7 @@
         <v>2050</v>
       </c>
       <c r="C117" s="53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D117" s="53" t="s">
         <v>91</v>
@@ -3954,7 +3959,7 @@
         <v>2050</v>
       </c>
       <c r="C118" s="53" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D118" s="53" t="s">
         <v>91</v>
@@ -3978,7 +3983,7 @@
         <v>2050</v>
       </c>
       <c r="C119" s="53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D119" s="53" t="s">
         <v>91</v>
@@ -3986,11 +3991,11 @@
       <c r="E119" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="F119" s="17" t="s">
-        <v>118</v>
+      <c r="F119" s="53" t="s">
+        <v>116</v>
       </c>
       <c r="G119" s="54" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H119" s="53"/>
     </row>
@@ -4002,7 +4007,7 @@
         <v>2050</v>
       </c>
       <c r="C120" s="53" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D120" s="53" t="s">
         <v>91</v>
@@ -4010,11 +4015,11 @@
       <c r="E120" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="F120" s="53" t="s">
-        <v>116</v>
+      <c r="F120" s="17" t="s">
+        <v>118</v>
       </c>
       <c r="G120" s="54" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H120" s="53"/>
     </row>
@@ -4026,7 +4031,7 @@
         <v>2050</v>
       </c>
       <c r="C121" s="53" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D121" s="53" t="s">
         <v>91</v>
@@ -4050,7 +4055,7 @@
         <v>2050</v>
       </c>
       <c r="C122" s="53" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D122" s="53" t="s">
         <v>91</v>
@@ -4074,7 +4079,7 @@
         <v>2050</v>
       </c>
       <c r="C123" s="53" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D123" s="53" t="s">
         <v>91</v>
@@ -4083,10 +4088,10 @@
         <v>38</v>
       </c>
       <c r="F123" s="53" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G123" s="54" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H123" s="53"/>
     </row>
@@ -4098,7 +4103,7 @@
         <v>2050</v>
       </c>
       <c r="C124" s="53" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D124" s="53" t="s">
         <v>91</v>
@@ -4106,13 +4111,13 @@
       <c r="E124" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="F124" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="G124" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="H124" s="17"/>
+      <c r="F124" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="G124" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="H124" s="53"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="53" t="s">
@@ -4122,7 +4127,7 @@
         <v>2050</v>
       </c>
       <c r="C125" s="53" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D125" s="53" t="s">
         <v>91</v>
@@ -4131,10 +4136,10 @@
         <v>38</v>
       </c>
       <c r="F125" s="17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G125" s="16" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H125" s="17"/>
     </row>
@@ -4146,7 +4151,7 @@
         <v>2050</v>
       </c>
       <c r="C126" s="53" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D126" s="53" t="s">
         <v>91</v>
@@ -4155,10 +4160,10 @@
         <v>38</v>
       </c>
       <c r="F126" s="17" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G126" s="16" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H126" s="17"/>
     </row>
@@ -4170,7 +4175,7 @@
         <v>2050</v>
       </c>
       <c r="C127" s="53" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D127" s="53" t="s">
         <v>91</v>
@@ -4194,7 +4199,7 @@
         <v>2050</v>
       </c>
       <c r="C128" s="53" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D128" s="53" t="s">
         <v>91</v>
@@ -4208,9 +4213,7 @@
       <c r="G128" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H128" s="17" t="s">
-        <v>43</v>
-      </c>
+      <c r="H128" s="17"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="53" t="s">
@@ -4220,7 +4223,7 @@
         <v>2050</v>
       </c>
       <c r="C129" s="53" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D129" s="53" t="s">
         <v>91</v>
@@ -4234,7 +4237,9 @@
       <c r="G129" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H129" s="17"/>
+      <c r="H129" s="17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="53" t="s">
@@ -4244,7 +4249,7 @@
         <v>2050</v>
       </c>
       <c r="C130" s="53" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D130" s="53" t="s">
         <v>91</v>
@@ -4268,7 +4273,7 @@
         <v>2050</v>
       </c>
       <c r="C131" s="53" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D131" s="53" t="s">
         <v>91</v>
@@ -4292,7 +4297,7 @@
         <v>2050</v>
       </c>
       <c r="C132" s="53" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D132" s="53" t="s">
         <v>91</v>
@@ -4316,7 +4321,7 @@
         <v>2050</v>
       </c>
       <c r="C133" s="53" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D133" s="53" t="s">
         <v>91</v>
@@ -4330,43 +4335,43 @@
       <c r="G133" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H133" s="17" t="s">
+      <c r="H133" s="17"/>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A134" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B134" s="54">
+        <v>2050</v>
+      </c>
+      <c r="C134" s="53" t="s">
+        <v>173</v>
+      </c>
+      <c r="D134" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E134" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F134" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="G134" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H134" s="17" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A134" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="B134" s="60">
-        <v>2035</v>
-      </c>
-      <c r="C134" s="59" t="s">
-        <v>186</v>
-      </c>
-      <c r="D134" s="59" t="s">
-        <v>181</v>
-      </c>
-      <c r="E134" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="F134" s="59" t="s">
-        <v>184</v>
-      </c>
-      <c r="G134" s="60" t="s">
-        <v>185</v>
-      </c>
-      <c r="H134" s="59"/>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="59" t="s">
         <v>26</v>
       </c>
       <c r="B135" s="60">
-        <v>2050</v>
+        <v>2035</v>
       </c>
       <c r="C135" s="59" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="D135" s="59" t="s">
         <v>181</v>
@@ -4387,10 +4392,10 @@
         <v>26</v>
       </c>
       <c r="B136" s="60">
-        <v>2035</v>
+        <v>2050</v>
       </c>
       <c r="C136" s="59" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D136" s="59" t="s">
         <v>181</v>
@@ -4399,10 +4404,10 @@
         <v>182</v>
       </c>
       <c r="F136" s="59" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G136" s="60" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="H136" s="59"/>
     </row>
@@ -4411,10 +4416,10 @@
         <v>26</v>
       </c>
       <c r="B137" s="60">
-        <v>2050</v>
+        <v>2035</v>
       </c>
       <c r="C137" s="59" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D137" s="59" t="s">
         <v>181</v>
@@ -4435,10 +4440,10 @@
         <v>26</v>
       </c>
       <c r="B138" s="60">
-        <v>2035</v>
+        <v>2050</v>
       </c>
       <c r="C138" s="59" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D138" s="59" t="s">
         <v>181</v>
@@ -4447,24 +4452,22 @@
         <v>182</v>
       </c>
       <c r="F138" s="59" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="G138" s="60" t="s">
-        <v>197</v>
-      </c>
-      <c r="H138" s="59" t="s">
-        <v>43</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="H138" s="59"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="59" t="s">
         <v>26</v>
       </c>
       <c r="B139" s="60">
-        <v>2050</v>
+        <v>2035</v>
       </c>
       <c r="C139" s="59" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D139" s="59" t="s">
         <v>181</v>
@@ -4487,34 +4490,36 @@
         <v>26</v>
       </c>
       <c r="B140" s="60">
-        <v>2035</v>
+        <v>2050</v>
       </c>
       <c r="C140" s="59" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="D140" s="59" t="s">
         <v>181</v>
       </c>
       <c r="E140" s="59" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="F140" s="59" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="G140" s="60" t="s">
-        <v>195</v>
-      </c>
-      <c r="H140" s="59"/>
+        <v>197</v>
+      </c>
+      <c r="H140" s="59" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" s="59" t="s">
         <v>26</v>
       </c>
       <c r="B141" s="60">
-        <v>2050</v>
+        <v>2035</v>
       </c>
       <c r="C141" s="59" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D141" s="59" t="s">
         <v>181</v>
@@ -4535,10 +4540,10 @@
         <v>26</v>
       </c>
       <c r="B142" s="60">
-        <v>2035</v>
+        <v>2050</v>
       </c>
       <c r="C142" s="59" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D142" s="59" t="s">
         <v>181</v>
@@ -4552,19 +4557,17 @@
       <c r="G142" s="60" t="s">
         <v>195</v>
       </c>
-      <c r="H142" s="59" t="s">
-        <v>43</v>
-      </c>
+      <c r="H142" s="59"/>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" s="59" t="s">
         <v>26</v>
       </c>
       <c r="B143" s="60">
-        <v>2050</v>
+        <v>2035</v>
       </c>
       <c r="C143" s="59" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D143" s="59" t="s">
         <v>181</v>
@@ -4583,28 +4586,54 @@
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A144" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="B144" s="65">
-        <v>2035</v>
-      </c>
-      <c r="C144" s="64" t="s">
+      <c r="A144" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B144" s="60">
+        <v>2050</v>
+      </c>
+      <c r="C144" s="59" t="s">
+        <v>202</v>
+      </c>
+      <c r="D144" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="E144" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="F144" s="59" t="s">
+        <v>194</v>
+      </c>
+      <c r="G144" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="H144" s="59" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A145" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="B145" s="65">
+        <v>2035</v>
+      </c>
+      <c r="C145" s="64" t="s">
         <v>203</v>
       </c>
-      <c r="D144" s="64" t="s">
+      <c r="D145" s="64" t="s">
         <v>181</v>
       </c>
-      <c r="E144" s="64" t="s">
+      <c r="E145" s="64" t="s">
         <v>193</v>
       </c>
-      <c r="F144" s="64" t="s">
+      <c r="F145" s="64" t="s">
         <v>194</v>
       </c>
-      <c r="G144" s="65" t="s">
+      <c r="G145" s="65" t="s">
         <v>195</v>
       </c>
-      <c r="H144" s="64" t="s">
+      <c r="H145" s="64" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove 2035_TM152_FBP_Plus_21 from "current" as it's practically the same as v20
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1220557-BFC9-4ADC-A6EE-41819389DC33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0FA887-EF58-4935-8955-DFDA3CDA9B90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="205">
   <si>
     <t>EEJ</t>
   </si>
@@ -1245,7 +1245,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H83" sqref="H83"/>
+      <selection pane="bottomLeft" activeCell="I83" sqref="I83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -3145,9 +3145,7 @@
       <c r="G83" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="H83" s="23" t="s">
-        <v>43</v>
-      </c>
+      <c r="H83" s="23"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="61" t="s">

</xml_diff>

<commit_message>
clean up - drop the noQ2FareDiscount test run from current
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0FA887-EF58-4935-8955-DFDA3CDA9B90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A580921D-67E0-4D66-83E8-3FB94F9042FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="205">
   <si>
     <t>EEJ</t>
   </si>
@@ -1244,8 +1244,8 @@
   <dimension ref="A1:H145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I83" sqref="I83"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -4631,9 +4631,7 @@
       <c r="G145" s="65" t="s">
         <v>195</v>
       </c>
-      <c r="H145" s="64" t="s">
-        <v>43</v>
-      </c>
+      <c r="H145" s="64"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
added FBP v21 and v22 for 2040 (they incl only minor fixes). 2040_TM152_FBP_Plus_20 remains "current"
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A580921D-67E0-4D66-83E8-3FB94F9042FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F67A27-F381-4074-AE6D-D62ADE54EDC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="207">
   <si>
     <t>EEJ</t>
   </si>
@@ -640,6 +640,12 @@
   </si>
   <si>
     <t>2035_TM152_FBP_Plus_21</t>
+  </si>
+  <si>
+    <t>2040_TM152_FBP_Plus_21</t>
+  </si>
+  <si>
+    <t>2040_TM152_FBP_Plus_22</t>
   </si>
 </sst>
 </file>
@@ -1241,11 +1247,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H145"/>
+  <dimension ref="A1:H147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -3160,16 +3166,16 @@
       <c r="D84" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="E84" s="63" t="s">
+      <c r="E84" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="F84" s="23" t="s">
+      <c r="F84" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="G84" s="22" t="s">
+      <c r="G84" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="H84" s="23" t="s">
+      <c r="H84" s="17" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3186,81 +3192,85 @@
       <c r="D85" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="E85" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F85" s="23" t="s">
+      <c r="E85" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="F85" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="G85" s="22" t="s">
+      <c r="G85" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="H85" s="23" t="s">
+      <c r="H85" s="52" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A86" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="B86" s="40">
-        <v>2050</v>
-      </c>
-      <c r="C86" s="41" t="s">
+      <c r="A86" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B86" s="16">
+        <v>2040</v>
+      </c>
+      <c r="C86" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="D86" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E86" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F86" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="G86" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H86" s="17"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A87" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B87" s="16">
+        <v>2040</v>
+      </c>
+      <c r="C87" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="D87" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E87" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F87" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="G87" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="H87" s="23"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A88" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B88" s="40">
+        <v>2050</v>
+      </c>
+      <c r="C88" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D86" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="E86" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="F86" s="41"/>
-      <c r="G86" s="40"/>
-      <c r="H86" s="41"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A87" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B87" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C87" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="D87" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E87" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="F87" s="43"/>
-      <c r="G87" s="42"/>
-      <c r="H87" s="43"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A88" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B88" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C88" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="D88" s="43" t="s">
+      <c r="D88" s="41" t="s">
         <v>34</v>
       </c>
       <c r="E88" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F88" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="G88" s="42" t="s">
-        <v>65</v>
-      </c>
+      <c r="F88" s="43"/>
+      <c r="G88" s="42"/>
       <c r="H88" s="43"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
@@ -3271,7 +3281,7 @@
         <v>2050</v>
       </c>
       <c r="C89" s="43" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="D89" s="43" t="s">
         <v>34</v>
@@ -3279,12 +3289,8 @@
       <c r="E89" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F89" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="G89" s="42" t="s">
-        <v>65</v>
-      </c>
+      <c r="F89" s="43"/>
+      <c r="G89" s="42"/>
       <c r="H89" s="43"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
@@ -3295,7 +3301,7 @@
         <v>2050</v>
       </c>
       <c r="C90" s="43" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D90" s="43" t="s">
         <v>34</v>
@@ -3304,10 +3310,10 @@
         <v>7</v>
       </c>
       <c r="F90" s="43" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G90" s="42" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H90" s="43"/>
     </row>
@@ -3319,7 +3325,7 @@
         <v>2050</v>
       </c>
       <c r="C91" s="43" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D91" s="43" t="s">
         <v>34</v>
@@ -3328,84 +3334,84 @@
         <v>7</v>
       </c>
       <c r="F91" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="G91" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="H91" s="43"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A92" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B92" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C92" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D92" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E92" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F92" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="G92" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="H92" s="43"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A93" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B93" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C93" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="D93" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E93" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F93" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="G91" s="42" t="s">
+      <c r="G93" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="H91" s="43"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A92" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B92" s="45">
-        <v>2050</v>
-      </c>
-      <c r="C92" s="46" t="s">
+      <c r="H93" s="43"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A94" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="B94" s="45">
+        <v>2050</v>
+      </c>
+      <c r="C94" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="D92" s="46" t="s">
+      <c r="D94" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="E92" s="46" t="s">
+      <c r="E94" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="F92" s="46" t="s">
+      <c r="F94" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="G92" s="45" t="s">
+      <c r="G94" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="H92" s="46"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A93" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B93" s="16">
-        <v>2050</v>
-      </c>
-      <c r="C93" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="D93" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="E93" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F93" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="G93" s="54" t="s">
-        <v>75</v>
-      </c>
-      <c r="H93" s="17"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A94" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B94" s="16">
-        <v>2050</v>
-      </c>
-      <c r="C94" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D94" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E94" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F94" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="G94" s="54" t="s">
-        <v>82</v>
-      </c>
-      <c r="H94" s="17"/>
+      <c r="H94" s="46"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="15" t="s">
@@ -3415,19 +3421,19 @@
         <v>2050</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="D95" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D95" s="52" t="s">
         <v>91</v>
       </c>
       <c r="E95" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F95" s="17" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G95" s="54" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="H95" s="17"/>
     </row>
@@ -3439,7 +3445,7 @@
         <v>2050</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>138</v>
+        <v>100</v>
       </c>
       <c r="D96" s="17" t="s">
         <v>91</v>
@@ -3448,10 +3454,10 @@
         <v>7</v>
       </c>
       <c r="F96" s="17" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="G96" s="54" t="s">
-        <v>137</v>
+        <v>82</v>
       </c>
       <c r="H96" s="17"/>
     </row>
@@ -3463,7 +3469,7 @@
         <v>2050</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="D97" s="17" t="s">
         <v>91</v>
@@ -3472,14 +3478,12 @@
         <v>7</v>
       </c>
       <c r="F97" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="G97" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="H97" s="17" t="s">
-        <v>43</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="G97" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="H97" s="17"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="15" t="s">
@@ -3489,7 +3493,7 @@
         <v>2050</v>
       </c>
       <c r="C98" s="17" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="D98" s="17" t="s">
         <v>91</v>
@@ -3500,7 +3504,7 @@
       <c r="F98" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="G98" s="16" t="s">
+      <c r="G98" s="54" t="s">
         <v>137</v>
       </c>
       <c r="H98" s="17"/>
@@ -3513,7 +3517,7 @@
         <v>2050</v>
       </c>
       <c r="C99" s="17" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D99" s="17" t="s">
         <v>91</v>
@@ -3522,12 +3526,14 @@
         <v>7</v>
       </c>
       <c r="F99" s="17" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="G99" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H99" s="17"/>
+      <c r="H99" s="17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="15" t="s">
@@ -3537,7 +3543,7 @@
         <v>2050</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D100" s="17" t="s">
         <v>91</v>
@@ -3546,10 +3552,10 @@
         <v>7</v>
       </c>
       <c r="F100" s="17" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="G100" s="16" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="H100" s="17"/>
     </row>
@@ -3561,7 +3567,7 @@
         <v>2050</v>
       </c>
       <c r="C101" s="17" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="D101" s="17" t="s">
         <v>91</v>
@@ -3570,118 +3576,126 @@
         <v>7</v>
       </c>
       <c r="F101" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="G101" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H101" s="17"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A102" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B102" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C102" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="D102" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E102" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F102" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="G102" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="H102" s="17"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A103" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B103" s="16">
+        <v>2050</v>
+      </c>
+      <c r="C103" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D103" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E103" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F103" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="G101" s="16" t="s">
+      <c r="G103" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="H101" s="17"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A102" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B102" s="22">
-        <v>2050</v>
-      </c>
-      <c r="C102" s="23" t="s">
+      <c r="H103" s="17"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A104" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B104" s="22">
+        <v>2050</v>
+      </c>
+      <c r="C104" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="D102" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E102" s="23" t="s">
+      <c r="D104" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="E104" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F102" s="23" t="s">
+      <c r="F104" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="G102" s="22" t="s">
+      <c r="G104" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="H102" s="23" t="s">
+      <c r="H104" s="23" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A103" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B103" s="42">
-        <v>2050</v>
-      </c>
-      <c r="C103" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="D103" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E103" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="F103" s="43"/>
-      <c r="G103" s="42"/>
-      <c r="H103" s="43"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A104" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B104" s="45">
-        <v>2050</v>
-      </c>
-      <c r="C104" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="D104" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="E104" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="F104" s="46"/>
-      <c r="G104" s="45"/>
-      <c r="H104" s="46"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B105" s="30">
-        <v>2050</v>
-      </c>
-      <c r="C105" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="D105" s="31" t="s">
+      <c r="B105" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C105" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="D105" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E105" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="F105" s="31"/>
-      <c r="G105" s="30"/>
-      <c r="H105" s="31"/>
+      <c r="E105" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="F105" s="43"/>
+      <c r="G105" s="42"/>
+      <c r="H105" s="43"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A106" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B106" s="30">
-        <v>2050</v>
-      </c>
-      <c r="C106" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="D106" s="31" t="s">
+      <c r="A106" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="B106" s="45">
+        <v>2050</v>
+      </c>
+      <c r="C106" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="D106" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="E106" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="F106" s="31"/>
-      <c r="G106" s="30"/>
-      <c r="H106" s="31"/>
+      <c r="E106" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="F106" s="46"/>
+      <c r="G106" s="45"/>
+      <c r="H106" s="46"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="29" t="s">
@@ -3691,7 +3705,7 @@
         <v>2050</v>
       </c>
       <c r="C107" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D107" s="31" t="s">
         <v>34</v>
@@ -3699,12 +3713,8 @@
       <c r="E107" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="F107" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="G107" s="30" t="s">
-        <v>63</v>
-      </c>
+      <c r="F107" s="31"/>
+      <c r="G107" s="30"/>
       <c r="H107" s="31"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
@@ -3715,7 +3725,7 @@
         <v>2050</v>
       </c>
       <c r="C108" s="31" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D108" s="31" t="s">
         <v>34</v>
@@ -3723,12 +3733,8 @@
       <c r="E108" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="F108" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="G108" s="30" t="s">
-        <v>63</v>
-      </c>
+      <c r="F108" s="31"/>
+      <c r="G108" s="30"/>
       <c r="H108" s="31"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
@@ -3739,7 +3745,7 @@
         <v>2050</v>
       </c>
       <c r="C109" s="31" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D109" s="31" t="s">
         <v>34</v>
@@ -3748,10 +3754,10 @@
         <v>38</v>
       </c>
       <c r="F109" s="31" t="s">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="G109" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H109" s="31"/>
     </row>
@@ -3763,7 +3769,7 @@
         <v>2050</v>
       </c>
       <c r="C110" s="31" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="D110" s="31" t="s">
         <v>34</v>
@@ -3772,10 +3778,10 @@
         <v>38</v>
       </c>
       <c r="F110" s="31" t="s">
-        <v>120</v>
+        <v>66</v>
       </c>
       <c r="G110" s="30" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H110" s="31"/>
     </row>
@@ -3787,7 +3793,7 @@
         <v>2050</v>
       </c>
       <c r="C111" s="31" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="D111" s="31" t="s">
         <v>34</v>
@@ -3796,10 +3802,10 @@
         <v>38</v>
       </c>
       <c r="F111" s="31" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G111" s="30" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H111" s="31"/>
     </row>
@@ -3811,7 +3817,7 @@
         <v>2050</v>
       </c>
       <c r="C112" s="31" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D112" s="31" t="s">
         <v>34</v>
@@ -3820,10 +3826,10 @@
         <v>38</v>
       </c>
       <c r="F112" s="31" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G112" s="30" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H112" s="31"/>
     </row>
@@ -3835,7 +3841,7 @@
         <v>2050</v>
       </c>
       <c r="C113" s="31" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D113" s="31" t="s">
         <v>34</v>
@@ -3844,86 +3850,86 @@
         <v>38</v>
       </c>
       <c r="F113" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="G113" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="H113" s="31"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A114" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B114" s="30">
+        <v>2050</v>
+      </c>
+      <c r="C114" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D114" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E114" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F114" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="G114" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H114" s="31"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A115" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B115" s="30">
+        <v>2050</v>
+      </c>
+      <c r="C115" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="D115" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E115" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F115" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="G113" s="30" t="s">
+      <c r="G115" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="H113" s="31" t="s">
+      <c r="H115" s="31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A114" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B114" s="51">
-        <v>2050</v>
-      </c>
-      <c r="C114" s="52" t="s">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A116" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B116" s="51">
+        <v>2050</v>
+      </c>
+      <c r="C116" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="D114" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="E114" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="F114" s="52" t="s">
+      <c r="D116" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="E116" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="F116" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="G114" s="51" t="s">
+      <c r="G116" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="H114" s="52"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A115" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="B115" s="54">
-        <v>2050</v>
-      </c>
-      <c r="C115" s="53" t="s">
-        <v>101</v>
-      </c>
-      <c r="D115" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="E115" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F115" s="53" t="s">
-        <v>116</v>
-      </c>
-      <c r="G115" s="54" t="s">
-        <v>82</v>
-      </c>
-      <c r="H115" s="53"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A116" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="B116" s="54">
-        <v>2050</v>
-      </c>
-      <c r="C116" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="D116" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="E116" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F116" s="53" t="s">
-        <v>116</v>
-      </c>
-      <c r="G116" s="54" t="s">
-        <v>82</v>
-      </c>
-      <c r="H116" s="53"/>
+      <c r="H116" s="52"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="53" t="s">
@@ -3933,7 +3939,7 @@
         <v>2050</v>
       </c>
       <c r="C117" s="53" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D117" s="53" t="s">
         <v>91</v>
@@ -3957,7 +3963,7 @@
         <v>2050</v>
       </c>
       <c r="C118" s="53" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D118" s="53" t="s">
         <v>91</v>
@@ -3981,7 +3987,7 @@
         <v>2050</v>
       </c>
       <c r="C119" s="53" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D119" s="53" t="s">
         <v>91</v>
@@ -4005,7 +4011,7 @@
         <v>2050</v>
       </c>
       <c r="C120" s="53" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D120" s="53" t="s">
         <v>91</v>
@@ -4013,11 +4019,11 @@
       <c r="E120" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="F120" s="17" t="s">
-        <v>118</v>
+      <c r="F120" s="53" t="s">
+        <v>116</v>
       </c>
       <c r="G120" s="54" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H120" s="53"/>
     </row>
@@ -4029,7 +4035,7 @@
         <v>2050</v>
       </c>
       <c r="C121" s="53" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D121" s="53" t="s">
         <v>91</v>
@@ -4053,7 +4059,7 @@
         <v>2050</v>
       </c>
       <c r="C122" s="53" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D122" s="53" t="s">
         <v>91</v>
@@ -4061,11 +4067,11 @@
       <c r="E122" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="F122" s="53" t="s">
-        <v>116</v>
+      <c r="F122" s="17" t="s">
+        <v>118</v>
       </c>
       <c r="G122" s="54" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H122" s="53"/>
     </row>
@@ -4077,7 +4083,7 @@
         <v>2050</v>
       </c>
       <c r="C123" s="53" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D123" s="53" t="s">
         <v>91</v>
@@ -4101,7 +4107,7 @@
         <v>2050</v>
       </c>
       <c r="C124" s="53" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D124" s="53" t="s">
         <v>91</v>
@@ -4110,10 +4116,10 @@
         <v>38</v>
       </c>
       <c r="F124" s="53" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G124" s="54" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H124" s="53"/>
     </row>
@@ -4125,7 +4131,7 @@
         <v>2050</v>
       </c>
       <c r="C125" s="53" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="D125" s="53" t="s">
         <v>91</v>
@@ -4133,13 +4139,13 @@
       <c r="E125" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="F125" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="G125" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="H125" s="17"/>
+      <c r="F125" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="G125" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="H125" s="53"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="53" t="s">
@@ -4149,7 +4155,7 @@
         <v>2050</v>
       </c>
       <c r="C126" s="53" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D126" s="53" t="s">
         <v>91</v>
@@ -4157,13 +4163,13 @@
       <c r="E126" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="F126" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="G126" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="H126" s="17"/>
+      <c r="F126" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="G126" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="H126" s="53"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="53" t="s">
@@ -4173,7 +4179,7 @@
         <v>2050</v>
       </c>
       <c r="C127" s="53" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="D127" s="53" t="s">
         <v>91</v>
@@ -4182,10 +4188,10 @@
         <v>38</v>
       </c>
       <c r="F127" s="17" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="G127" s="16" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="H127" s="17"/>
     </row>
@@ -4197,7 +4203,7 @@
         <v>2050</v>
       </c>
       <c r="C128" s="53" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="D128" s="53" t="s">
         <v>91</v>
@@ -4206,10 +4212,10 @@
         <v>38</v>
       </c>
       <c r="F128" s="17" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G128" s="16" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H128" s="17"/>
     </row>
@@ -4221,7 +4227,7 @@
         <v>2050</v>
       </c>
       <c r="C129" s="53" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D129" s="53" t="s">
         <v>91</v>
@@ -4235,9 +4241,7 @@
       <c r="G129" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H129" s="17" t="s">
-        <v>43</v>
-      </c>
+      <c r="H129" s="17"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="53" t="s">
@@ -4247,7 +4251,7 @@
         <v>2050</v>
       </c>
       <c r="C130" s="53" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D130" s="53" t="s">
         <v>91</v>
@@ -4271,7 +4275,7 @@
         <v>2050</v>
       </c>
       <c r="C131" s="53" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D131" s="53" t="s">
         <v>91</v>
@@ -4285,7 +4289,9 @@
       <c r="G131" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H131" s="17"/>
+      <c r="H131" s="17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="53" t="s">
@@ -4295,7 +4301,7 @@
         <v>2050</v>
       </c>
       <c r="C132" s="53" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="D132" s="53" t="s">
         <v>91</v>
@@ -4319,7 +4325,7 @@
         <v>2050</v>
       </c>
       <c r="C133" s="53" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="D133" s="53" t="s">
         <v>91</v>
@@ -4343,7 +4349,7 @@
         <v>2050</v>
       </c>
       <c r="C134" s="53" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D134" s="53" t="s">
         <v>91</v>
@@ -4357,57 +4363,57 @@
       <c r="G134" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H134" s="17" t="s">
+      <c r="H134" s="17"/>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A135" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B135" s="54">
+        <v>2050</v>
+      </c>
+      <c r="C135" s="53" t="s">
+        <v>165</v>
+      </c>
+      <c r="D135" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E135" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F135" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="G135" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H135" s="17"/>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A136" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B136" s="54">
+        <v>2050</v>
+      </c>
+      <c r="C136" s="53" t="s">
+        <v>173</v>
+      </c>
+      <c r="D136" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E136" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F136" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="G136" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H136" s="17" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A135" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="B135" s="60">
-        <v>2035</v>
-      </c>
-      <c r="C135" s="59" t="s">
-        <v>186</v>
-      </c>
-      <c r="D135" s="59" t="s">
-        <v>181</v>
-      </c>
-      <c r="E135" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="F135" s="59" t="s">
-        <v>184</v>
-      </c>
-      <c r="G135" s="60" t="s">
-        <v>185</v>
-      </c>
-      <c r="H135" s="59"/>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A136" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="B136" s="60">
-        <v>2050</v>
-      </c>
-      <c r="C136" s="59" t="s">
-        <v>180</v>
-      </c>
-      <c r="D136" s="59" t="s">
-        <v>181</v>
-      </c>
-      <c r="E136" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="F136" s="59" t="s">
-        <v>184</v>
-      </c>
-      <c r="G136" s="60" t="s">
-        <v>185</v>
-      </c>
-      <c r="H136" s="59"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="59" t="s">
@@ -4417,7 +4423,7 @@
         <v>2035</v>
       </c>
       <c r="C137" s="59" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D137" s="59" t="s">
         <v>181</v>
@@ -4426,10 +4432,10 @@
         <v>182</v>
       </c>
       <c r="F137" s="59" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G137" s="60" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="H137" s="59"/>
     </row>
@@ -4441,7 +4447,7 @@
         <v>2050</v>
       </c>
       <c r="C138" s="59" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="D138" s="59" t="s">
         <v>181</v>
@@ -4450,10 +4456,10 @@
         <v>182</v>
       </c>
       <c r="F138" s="59" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G138" s="60" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="H138" s="59"/>
     </row>
@@ -4465,7 +4471,7 @@
         <v>2035</v>
       </c>
       <c r="C139" s="59" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="D139" s="59" t="s">
         <v>181</v>
@@ -4474,14 +4480,12 @@
         <v>182</v>
       </c>
       <c r="F139" s="59" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="G139" s="60" t="s">
-        <v>197</v>
-      </c>
-      <c r="H139" s="59" t="s">
-        <v>43</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="H139" s="59"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="59" t="s">
@@ -4491,7 +4495,7 @@
         <v>2050</v>
       </c>
       <c r="C140" s="59" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="D140" s="59" t="s">
         <v>181</v>
@@ -4500,14 +4504,12 @@
         <v>182</v>
       </c>
       <c r="F140" s="59" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="G140" s="60" t="s">
-        <v>197</v>
-      </c>
-      <c r="H140" s="59" t="s">
-        <v>43</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="H140" s="59"/>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" s="59" t="s">
@@ -4517,21 +4519,23 @@
         <v>2035</v>
       </c>
       <c r="C141" s="59" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="D141" s="59" t="s">
         <v>181</v>
       </c>
       <c r="E141" s="59" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="F141" s="59" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="G141" s="60" t="s">
-        <v>195</v>
-      </c>
-      <c r="H141" s="59"/>
+        <v>197</v>
+      </c>
+      <c r="H141" s="59" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="59" t="s">
@@ -4541,21 +4545,23 @@
         <v>2050</v>
       </c>
       <c r="C142" s="59" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D142" s="59" t="s">
         <v>181</v>
       </c>
       <c r="E142" s="59" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="F142" s="59" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="G142" s="60" t="s">
-        <v>195</v>
-      </c>
-      <c r="H142" s="59"/>
+        <v>197</v>
+      </c>
+      <c r="H142" s="59" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" s="59" t="s">
@@ -4565,7 +4571,7 @@
         <v>2035</v>
       </c>
       <c r="C143" s="59" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D143" s="59" t="s">
         <v>181</v>
@@ -4579,9 +4585,7 @@
       <c r="G143" s="60" t="s">
         <v>195</v>
       </c>
-      <c r="H143" s="59" t="s">
-        <v>43</v>
-      </c>
+      <c r="H143" s="59"/>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" s="59" t="s">
@@ -4591,7 +4595,7 @@
         <v>2050</v>
       </c>
       <c r="C144" s="59" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D144" s="59" t="s">
         <v>181</v>
@@ -4605,33 +4609,83 @@
       <c r="G144" s="60" t="s">
         <v>195</v>
       </c>
-      <c r="H144" s="59" t="s">
+      <c r="H144" s="59"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A145" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B145" s="60">
+        <v>2035</v>
+      </c>
+      <c r="C145" s="59" t="s">
+        <v>201</v>
+      </c>
+      <c r="D145" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="E145" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="F145" s="59" t="s">
+        <v>194</v>
+      </c>
+      <c r="G145" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="H145" s="59" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A145" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="B145" s="65">
-        <v>2035</v>
-      </c>
-      <c r="C145" s="64" t="s">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A146" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B146" s="60">
+        <v>2050</v>
+      </c>
+      <c r="C146" s="59" t="s">
+        <v>202</v>
+      </c>
+      <c r="D146" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="E146" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="F146" s="59" t="s">
+        <v>194</v>
+      </c>
+      <c r="G146" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="H146" s="59" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A147" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="B147" s="65">
+        <v>2035</v>
+      </c>
+      <c r="C147" s="64" t="s">
         <v>203</v>
       </c>
-      <c r="D145" s="64" t="s">
+      <c r="D147" s="64" t="s">
         <v>181</v>
       </c>
-      <c r="E145" s="64" t="s">
+      <c r="E147" s="64" t="s">
         <v>193</v>
       </c>
-      <c r="F145" s="64" t="s">
+      <c r="F147" s="64" t="s">
         <v>194</v>
       </c>
-      <c r="G145" s="65" t="s">
+      <c r="G147" s="65" t="s">
         <v>195</v>
       </c>
-      <c r="H145" s="64"/>
+      <c r="H147" s="64"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Added 2050 FBP PlusCrossing_22 run
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ywang\Documents\GitHub\travel-model-one\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F67A27-F381-4074-AE6D-D62ADE54EDC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8944C472-F895-4E27-AF1F-A3540CBE41ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1460" yWindow="690" windowWidth="19780" windowHeight="12910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="208">
   <si>
     <t>EEJ</t>
   </si>
@@ -646,6 +646,9 @@
   </si>
   <si>
     <t>2040_TM152_FBP_Plus_22</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_PlusCrossing_22</t>
   </si>
 </sst>
 </file>
@@ -1247,11 +1250,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H147"/>
+  <dimension ref="A1:H148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A86" sqref="A86"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -4416,38 +4419,40 @@
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A137" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="B137" s="60">
-        <v>2035</v>
-      </c>
-      <c r="C137" s="59" t="s">
-        <v>186</v>
-      </c>
-      <c r="D137" s="59" t="s">
-        <v>181</v>
-      </c>
-      <c r="E137" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="F137" s="59" t="s">
-        <v>184</v>
-      </c>
-      <c r="G137" s="60" t="s">
-        <v>185</v>
-      </c>
-      <c r="H137" s="59"/>
+      <c r="A137" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B137" s="54">
+        <v>2050</v>
+      </c>
+      <c r="C137" s="53" t="s">
+        <v>207</v>
+      </c>
+      <c r="D137" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E137" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F137" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="G137" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H137" s="17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="59" t="s">
         <v>26</v>
       </c>
       <c r="B138" s="60">
-        <v>2050</v>
+        <v>2035</v>
       </c>
       <c r="C138" s="59" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="D138" s="59" t="s">
         <v>181</v>
@@ -4468,10 +4473,10 @@
         <v>26</v>
       </c>
       <c r="B139" s="60">
-        <v>2035</v>
+        <v>2050</v>
       </c>
       <c r="C139" s="59" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D139" s="59" t="s">
         <v>181</v>
@@ -4480,10 +4485,10 @@
         <v>182</v>
       </c>
       <c r="F139" s="59" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G139" s="60" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="H139" s="59"/>
     </row>
@@ -4492,10 +4497,10 @@
         <v>26</v>
       </c>
       <c r="B140" s="60">
-        <v>2050</v>
+        <v>2035</v>
       </c>
       <c r="C140" s="59" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D140" s="59" t="s">
         <v>181</v>
@@ -4516,10 +4521,10 @@
         <v>26</v>
       </c>
       <c r="B141" s="60">
-        <v>2035</v>
+        <v>2050</v>
       </c>
       <c r="C141" s="59" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D141" s="59" t="s">
         <v>181</v>
@@ -4528,24 +4533,22 @@
         <v>182</v>
       </c>
       <c r="F141" s="59" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="G141" s="60" t="s">
-        <v>197</v>
-      </c>
-      <c r="H141" s="59" t="s">
-        <v>43</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="H141" s="59"/>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="59" t="s">
         <v>26</v>
       </c>
       <c r="B142" s="60">
-        <v>2050</v>
+        <v>2035</v>
       </c>
       <c r="C142" s="59" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D142" s="59" t="s">
         <v>181</v>
@@ -4568,34 +4571,36 @@
         <v>26</v>
       </c>
       <c r="B143" s="60">
-        <v>2035</v>
+        <v>2050</v>
       </c>
       <c r="C143" s="59" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="D143" s="59" t="s">
         <v>181</v>
       </c>
       <c r="E143" s="59" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="F143" s="59" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="G143" s="60" t="s">
-        <v>195</v>
-      </c>
-      <c r="H143" s="59"/>
+        <v>197</v>
+      </c>
+      <c r="H143" s="59" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" s="59" t="s">
         <v>26</v>
       </c>
       <c r="B144" s="60">
-        <v>2050</v>
+        <v>2035</v>
       </c>
       <c r="C144" s="59" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D144" s="59" t="s">
         <v>181</v>
@@ -4616,10 +4621,10 @@
         <v>26</v>
       </c>
       <c r="B145" s="60">
-        <v>2035</v>
+        <v>2050</v>
       </c>
       <c r="C145" s="59" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D145" s="59" t="s">
         <v>181</v>
@@ -4633,19 +4638,17 @@
       <c r="G145" s="60" t="s">
         <v>195</v>
       </c>
-      <c r="H145" s="59" t="s">
-        <v>43</v>
-      </c>
+      <c r="H145" s="59"/>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" s="59" t="s">
         <v>26</v>
       </c>
       <c r="B146" s="60">
-        <v>2050</v>
+        <v>2035</v>
       </c>
       <c r="C146" s="59" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D146" s="59" t="s">
         <v>181</v>
@@ -4664,28 +4667,54 @@
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A147" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="B147" s="65">
-        <v>2035</v>
-      </c>
-      <c r="C147" s="64" t="s">
+      <c r="A147" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B147" s="60">
+        <v>2050</v>
+      </c>
+      <c r="C147" s="59" t="s">
+        <v>202</v>
+      </c>
+      <c r="D147" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="E147" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="F147" s="59" t="s">
+        <v>194</v>
+      </c>
+      <c r="G147" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="H147" s="59" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A148" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="B148" s="65">
+        <v>2035</v>
+      </c>
+      <c r="C148" s="64" t="s">
         <v>203</v>
       </c>
-      <c r="D147" s="64" t="s">
+      <c r="D148" s="64" t="s">
         <v>181</v>
       </c>
-      <c r="E147" s="64" t="s">
+      <c r="E148" s="64" t="s">
         <v>193</v>
       </c>
-      <c r="F147" s="64" t="s">
+      <c r="F148" s="64" t="s">
         <v>194</v>
       </c>
-      <c r="G147" s="65" t="s">
+      <c r="G148" s="65" t="s">
         <v>195</v>
       </c>
-      <c r="H147" s="64"/>
+      <c r="H148" s="64"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Add a couple DEIR tags and  include them in current summaries
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8560F7F-F6EF-424C-AD90-E53087FE145C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F5DA3D-68CB-4F2D-8DA8-ADF1AE8CF6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9585" yWindow="4230" windowWidth="23295" windowHeight="15615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1329,8 +1329,8 @@
   <dimension ref="A1:H163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1747,7 +1747,7 @@
       <c r="F20" s="24"/>
       <c r="G20" s="23"/>
       <c r="H20" s="24" t="s">
-        <v>43</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1959,7 +1959,7 @@
         <v>137</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>43</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
One more update so 2015 lines get parsed correctly by batch
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F5DA3D-68CB-4F2D-8DA8-ADF1AE8CF6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843E13FD-2B2A-40ED-AF73-B41D1280C65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9585" yWindow="4230" windowWidth="23295" windowHeight="15615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="227">
   <si>
     <t>EEJ</t>
   </si>
@@ -703,6 +703,12 @@
   </si>
   <si>
     <t>2015_TM152_IPA_17</t>
+  </si>
+  <si>
+    <t>"census_petrale"</t>
+  </si>
+  <si>
+    <t>na</t>
   </si>
 </sst>
 </file>
@@ -1329,8 +1335,8 @@
   <dimension ref="A1:H163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1786,8 +1792,12 @@
       <c r="E22" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="73"/>
-      <c r="G22" s="72"/>
+      <c r="F22" s="73" t="s">
+        <v>225</v>
+      </c>
+      <c r="G22" s="72" t="s">
+        <v>226</v>
+      </c>
       <c r="H22" s="73" t="s">
         <v>222</v>
       </c>
@@ -1808,8 +1818,12 @@
       <c r="E23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="1"/>
+      <c r="F23" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>226</v>
+      </c>
       <c r="H23" s="2" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
use the latest EIR Alt2 runs for comparison
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ywang\Documents\GitHub\travel-model-one\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843E13FD-2B2A-40ED-AF73-B41D1280C65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8C4743-18A1-49D8-9B2B-DA714F4616E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9585" yWindow="4230" windowWidth="23295" windowHeight="15615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="20200" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -675,18 +675,12 @@
     <t>2035_TM152_EIR_Alt1_04</t>
   </si>
   <si>
-    <t>2035_TM152_EIR_Alt2_03</t>
-  </si>
-  <si>
     <t>2050_TM152_FBP_NoProject_24</t>
   </si>
   <si>
     <t>2050_TM152_EIR_Alt1_04</t>
   </si>
   <si>
-    <t>2050_TM152_EIR_Alt2_03</t>
-  </si>
-  <si>
     <t>2050_TM152_FBP_NoProject_23</t>
   </si>
   <si>
@@ -709,6 +703,12 @@
   </si>
   <si>
     <t>na</t>
+  </si>
+  <si>
+    <t>2035_TM152_EIR_Alt2_04</t>
+  </si>
+  <si>
+    <t>2050_TM152_EIR_Alt2_04</t>
   </si>
 </sst>
 </file>
@@ -1336,19 +1336,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomLeft" activeCell="C164" sqref="C164"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.296875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="70.85546875" customWidth="1"/>
+    <col min="6" max="6" width="70.8984375" customWidth="1"/>
     <col min="7" max="7" width="15" style="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="52" t="s">
         <v>40</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
@@ -1394,7 +1394,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>25</v>
       </c>
@@ -1414,7 +1414,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>25</v>
       </c>
@@ -1434,7 +1434,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>25</v>
       </c>
@@ -1454,7 +1454,7 @@
       <c r="G5" s="11"/>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>25</v>
       </c>
@@ -1474,7 +1474,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>25</v>
       </c>
@@ -1494,7 +1494,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>25</v>
       </c>
@@ -1514,7 +1514,7 @@
       <c r="G8" s="11"/>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>25</v>
       </c>
@@ -1534,7 +1534,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>25</v>
       </c>
@@ -1554,7 +1554,7 @@
       <c r="G10" s="17"/>
       <c r="H10" s="18"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>25</v>
       </c>
@@ -1574,7 +1574,7 @@
       <c r="G11" s="17"/>
       <c r="H11" s="18"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>25</v>
       </c>
@@ -1594,7 +1594,7 @@
       <c r="G12" s="17"/>
       <c r="H12" s="18"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>25</v>
       </c>
@@ -1614,7 +1614,7 @@
       <c r="G13" s="17"/>
       <c r="H13" s="18"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>25</v>
       </c>
@@ -1634,7 +1634,7 @@
       <c r="G14" s="17"/>
       <c r="H14" s="18"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>25</v>
       </c>
@@ -1654,7 +1654,7 @@
       <c r="G15" s="14"/>
       <c r="H15" s="15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>25</v>
       </c>
@@ -1674,7 +1674,7 @@
       <c r="G16" s="14"/>
       <c r="H16" s="15"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
@@ -1694,7 +1694,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="15"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>25</v>
       </c>
@@ -1714,7 +1714,7 @@
       <c r="G18" s="14"/>
       <c r="H18" s="15"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
         <v>25</v>
       </c>
@@ -1734,7 +1734,7 @@
       <c r="G19" s="20"/>
       <c r="H19" s="21"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
         <v>26</v>
       </c>
@@ -1753,10 +1753,10 @@
       <c r="F20" s="24"/>
       <c r="G20" s="23"/>
       <c r="H20" s="24" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
         <v>26</v>
       </c>
@@ -1776,7 +1776,7 @@
       <c r="G21" s="23"/>
       <c r="H21" s="24"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="65" t="s">
         <v>26</v>
       </c>
@@ -1793,16 +1793,16 @@
         <v>28</v>
       </c>
       <c r="F22" s="73" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G22" s="72" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H22" s="73" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>26</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>2015</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>28</v>
@@ -1819,16 +1819,16 @@
         <v>28</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="61" t="s">
         <v>26</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="67" t="s">
         <v>26</v>
       </c>
@@ -1878,7 +1878,7 @@
       </c>
       <c r="H25" s="75"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
         <v>26</v>
       </c>
@@ -1902,7 +1902,7 @@
       </c>
       <c r="H26" s="21"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="57" t="s">
         <v>26</v>
       </c>
@@ -1926,7 +1926,7 @@
       </c>
       <c r="H27" s="59"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
         <v>26</v>
       </c>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="H28" s="18"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
         <v>26</v>
       </c>
@@ -1973,10 +1973,10 @@
         <v>137</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="31" t="s">
         <v>26</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="57" t="s">
         <v>26</v>
       </c>
@@ -2026,7 +2026,7 @@
       </c>
       <c r="H31" s="59"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
         <v>26</v>
       </c>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="H32" s="18"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="16" t="s">
         <v>26</v>
       </c>
@@ -2073,10 +2073,10 @@
         <v>137</v>
       </c>
       <c r="H33" s="18" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="16" t="s">
         <v>26</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="34" t="s">
         <v>26</v>
       </c>
@@ -2122,7 +2122,7 @@
       <c r="G35" s="17"/>
       <c r="H35" s="17"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="16" t="s">
         <v>26</v>
       </c>
@@ -2142,7 +2142,7 @@
       <c r="G36" s="17"/>
       <c r="H36" s="18"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="16" t="s">
         <v>26</v>
       </c>
@@ -2162,7 +2162,7 @@
       <c r="G37" s="17"/>
       <c r="H37" s="18"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="16" t="s">
         <v>26</v>
       </c>
@@ -2181,10 +2181,10 @@
       <c r="F38" s="18"/>
       <c r="G38" s="17"/>
       <c r="H38" s="18" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="34" t="s">
         <v>26</v>
       </c>
@@ -2204,7 +2204,7 @@
       <c r="G39" s="35"/>
       <c r="H39" s="36"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
         <v>26</v>
       </c>
@@ -2224,7 +2224,7 @@
       <c r="G40" s="17"/>
       <c r="H40" s="18"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="16" t="s">
         <v>26</v>
       </c>
@@ -2244,7 +2244,7 @@
       <c r="G41" s="17"/>
       <c r="H41" s="18"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="16" t="s">
         <v>26</v>
       </c>
@@ -2264,7 +2264,7 @@
       <c r="G42" s="17"/>
       <c r="H42" s="18"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="16" t="s">
         <v>26</v>
       </c>
@@ -2288,7 +2288,7 @@
       </c>
       <c r="H43" s="18"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="16" t="s">
         <v>26</v>
       </c>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="H44" s="18"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="31" t="s">
         <v>26</v>
       </c>
@@ -2336,7 +2336,7 @@
       </c>
       <c r="H45" s="33"/>
     </row>
-    <row r="46" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="46" t="s">
         <v>26</v>
       </c>
@@ -2360,7 +2360,7 @@
       </c>
       <c r="H46" s="48"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>26</v>
       </c>
@@ -2384,7 +2384,7 @@
       </c>
       <c r="H47" s="15"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
         <v>26</v>
       </c>
@@ -2408,7 +2408,7 @@
       </c>
       <c r="H48" s="15"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
         <v>26</v>
       </c>
@@ -2432,7 +2432,7 @@
       </c>
       <c r="H49" s="15"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
         <v>26</v>
       </c>
@@ -2456,7 +2456,7 @@
       </c>
       <c r="H50" s="15"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
         <v>26</v>
       </c>
@@ -2480,7 +2480,7 @@
       </c>
       <c r="H51" s="15"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
         <v>26</v>
       </c>
@@ -2504,7 +2504,7 @@
       </c>
       <c r="H52" s="15"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="13" t="s">
         <v>26</v>
       </c>
@@ -2528,7 +2528,7 @@
       </c>
       <c r="H53" s="15"/>
     </row>
-    <row r="54" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="13" t="s">
         <v>26</v>
       </c>
@@ -2551,10 +2551,10 @@
         <v>169</v>
       </c>
       <c r="H54" s="15" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="13" t="s">
         <v>26</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>2035</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D55" s="15" t="s">
         <v>91</v>
@@ -2578,7 +2578,7 @@
       </c>
       <c r="H55" s="15"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="19" t="s">
         <v>26</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="34" t="s">
         <v>26</v>
       </c>
@@ -2624,7 +2624,7 @@
       <c r="G57" s="35"/>
       <c r="H57" s="36"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="31" t="s">
         <v>26</v>
       </c>
@@ -2644,7 +2644,7 @@
       <c r="G58" s="32"/>
       <c r="H58" s="33"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="16" t="s">
         <v>26</v>
       </c>
@@ -2664,7 +2664,7 @@
       <c r="G59" s="17"/>
       <c r="H59" s="18"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="16" t="s">
         <v>26</v>
       </c>
@@ -2684,7 +2684,7 @@
       <c r="G60" s="17"/>
       <c r="H60" s="18"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="16" t="s">
         <v>26</v>
       </c>
@@ -2708,7 +2708,7 @@
       </c>
       <c r="H61" s="18"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="16" t="s">
         <v>26</v>
       </c>
@@ -2732,7 +2732,7 @@
       </c>
       <c r="H62" s="18"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="16" t="s">
         <v>26</v>
       </c>
@@ -2756,7 +2756,7 @@
       </c>
       <c r="H63" s="18"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="16" t="s">
         <v>26</v>
       </c>
@@ -2780,7 +2780,7 @@
       </c>
       <c r="H64" s="18"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="16" t="s">
         <v>26</v>
       </c>
@@ -2804,7 +2804,7 @@
       </c>
       <c r="H65" s="18"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="16" t="s">
         <v>26</v>
       </c>
@@ -2827,10 +2827,10 @@
         <v>82</v>
       </c>
       <c r="H66" s="18" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="45" t="s">
         <v>26</v>
       </c>
@@ -2854,7 +2854,7 @@
       </c>
       <c r="H67" s="26"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="45" t="s">
         <v>26</v>
       </c>
@@ -2878,7 +2878,7 @@
       </c>
       <c r="H68" s="26"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="16" t="s">
         <v>26</v>
       </c>
@@ -2902,7 +2902,7 @@
       </c>
       <c r="H69" s="18"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="16" t="s">
         <v>26</v>
       </c>
@@ -2926,7 +2926,7 @@
       </c>
       <c r="H70" s="18"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
         <v>26</v>
       </c>
@@ -2950,7 +2950,7 @@
       </c>
       <c r="H71" s="18"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="16" t="s">
         <v>26</v>
       </c>
@@ -2974,7 +2974,7 @@
       </c>
       <c r="H72" s="18"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="46" t="s">
         <v>26</v>
       </c>
@@ -2998,7 +2998,7 @@
       </c>
       <c r="H73" s="48"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="13" t="s">
         <v>26</v>
       </c>
@@ -3022,7 +3022,7 @@
       </c>
       <c r="H74" s="15"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="13" t="s">
         <v>26</v>
       </c>
@@ -3046,7 +3046,7 @@
       </c>
       <c r="H75" s="15"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="13" t="s">
         <v>26</v>
       </c>
@@ -3070,7 +3070,7 @@
       </c>
       <c r="H76" s="15"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="13" t="s">
         <v>26</v>
       </c>
@@ -3094,7 +3094,7 @@
       </c>
       <c r="H77" s="15"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="13" t="s">
         <v>26</v>
       </c>
@@ -3118,7 +3118,7 @@
       </c>
       <c r="H78" s="15"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
         <v>26</v>
       </c>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="H79" s="15"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
         <v>26</v>
       </c>
@@ -3166,7 +3166,7 @@
       </c>
       <c r="H80" s="15"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
         <v>26</v>
       </c>
@@ -3190,7 +3190,7 @@
       </c>
       <c r="H81" s="15"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="13" t="s">
         <v>26</v>
       </c>
@@ -3214,7 +3214,7 @@
       </c>
       <c r="H82" s="15"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="13" t="s">
         <v>26</v>
       </c>
@@ -3238,7 +3238,7 @@
       </c>
       <c r="H83" s="15"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="13" t="s">
         <v>26</v>
       </c>
@@ -3262,7 +3262,7 @@
       </c>
       <c r="H84" s="15"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="13" t="s">
         <v>26</v>
       </c>
@@ -3286,7 +3286,7 @@
       </c>
       <c r="H85" s="15"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
         <v>26</v>
       </c>
@@ -3310,7 +3310,7 @@
       </c>
       <c r="H86" s="15"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="13" t="s">
         <v>26</v>
       </c>
@@ -3333,10 +3333,10 @@
         <v>137</v>
       </c>
       <c r="H87" s="15" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="13" t="s">
         <v>26</v>
       </c>
@@ -3360,7 +3360,7 @@
       </c>
       <c r="H88" s="15"/>
     </row>
-    <row r="89" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
         <v>26</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>2035</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D89" s="15" t="s">
         <v>91</v>
@@ -3384,7 +3384,7 @@
       </c>
       <c r="H89" s="15"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="19" t="s">
         <v>26</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="57" t="s">
         <v>26</v>
       </c>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="H91" s="15"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="13" t="s">
         <v>26</v>
       </c>
@@ -3457,10 +3457,10 @@
         <v>137</v>
       </c>
       <c r="H92" s="48" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="13" t="s">
         <v>26</v>
       </c>
@@ -3484,7 +3484,7 @@
       </c>
       <c r="H93" s="15"/>
     </row>
-    <row r="94" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="13" t="s">
         <v>26</v>
       </c>
@@ -3508,7 +3508,7 @@
       </c>
       <c r="H94" s="15"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="13" t="s">
         <v>26</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="37" t="s">
         <v>26</v>
       </c>
@@ -3554,7 +3554,7 @@
       <c r="G96" s="40"/>
       <c r="H96" s="41"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="27" t="s">
         <v>26</v>
       </c>
@@ -3574,7 +3574,7 @@
       <c r="G97" s="40"/>
       <c r="H97" s="41"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="27" t="s">
         <v>26</v>
       </c>
@@ -3598,7 +3598,7 @@
       </c>
       <c r="H98" s="41"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="27" t="s">
         <v>26</v>
       </c>
@@ -3622,7 +3622,7 @@
       </c>
       <c r="H99" s="41"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="27" t="s">
         <v>26</v>
       </c>
@@ -3646,7 +3646,7 @@
       </c>
       <c r="H100" s="41"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="27" t="s">
         <v>26</v>
       </c>
@@ -3670,7 +3670,7 @@
       </c>
       <c r="H101" s="41"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="42" t="s">
         <v>26</v>
       </c>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="H102" s="44"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="13" t="s">
         <v>26</v>
       </c>
@@ -3718,7 +3718,7 @@
       </c>
       <c r="H103" s="15"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="13" t="s">
         <v>26</v>
       </c>
@@ -3742,7 +3742,7 @@
       </c>
       <c r="H104" s="15"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="13" t="s">
         <v>26</v>
       </c>
@@ -3766,7 +3766,7 @@
       </c>
       <c r="H105" s="15"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="13" t="s">
         <v>26</v>
       </c>
@@ -3790,7 +3790,7 @@
       </c>
       <c r="H106" s="15"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="13" t="s">
         <v>26</v>
       </c>
@@ -3814,7 +3814,7 @@
       </c>
       <c r="H107" s="15"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="13" t="s">
         <v>26</v>
       </c>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="H108" s="15"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="13" t="s">
         <v>26</v>
       </c>
@@ -3862,7 +3862,7 @@
       </c>
       <c r="H109" s="15"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="13" t="s">
         <v>26</v>
       </c>
@@ -3886,7 +3886,7 @@
       </c>
       <c r="H110" s="15"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="13" t="s">
         <v>26</v>
       </c>
@@ -3910,7 +3910,7 @@
       </c>
       <c r="H111" s="15"/>
     </row>
-    <row r="112" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="13" t="s">
         <v>26</v>
       </c>
@@ -3933,10 +3933,10 @@
         <v>169</v>
       </c>
       <c r="H112" s="15" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="13" t="s">
         <v>26</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>2050</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D113" s="15" t="s">
         <v>91</v>
@@ -3960,7 +3960,7 @@
       </c>
       <c r="H113" s="15"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="19" t="s">
         <v>26</v>
       </c>
@@ -3968,7 +3968,7 @@
         <v>2050</v>
       </c>
       <c r="C114" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D114" s="21" t="s">
         <v>91</v>
@@ -3986,7 +3986,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="27" t="s">
         <v>26</v>
       </c>
@@ -4006,7 +4006,7 @@
       <c r="G115" s="40"/>
       <c r="H115" s="41"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="42" t="s">
         <v>26</v>
       </c>
@@ -4026,7 +4026,7 @@
       <c r="G116" s="43"/>
       <c r="H116" s="44"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="27" t="s">
         <v>26</v>
       </c>
@@ -4046,7 +4046,7 @@
       <c r="G117" s="28"/>
       <c r="H117" s="29"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="27" t="s">
         <v>26</v>
       </c>
@@ -4066,7 +4066,7 @@
       <c r="G118" s="28"/>
       <c r="H118" s="29"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="27" t="s">
         <v>26</v>
       </c>
@@ -4090,7 +4090,7 @@
       </c>
       <c r="H119" s="29"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="27" t="s">
         <v>26</v>
       </c>
@@ -4114,7 +4114,7 @@
       </c>
       <c r="H120" s="29"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="27" t="s">
         <v>26</v>
       </c>
@@ -4138,7 +4138,7 @@
       </c>
       <c r="H121" s="29"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="27" t="s">
         <v>26</v>
       </c>
@@ -4162,7 +4162,7 @@
       </c>
       <c r="H122" s="29"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="27" t="s">
         <v>26</v>
       </c>
@@ -4186,7 +4186,7 @@
       </c>
       <c r="H123" s="29"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="27" t="s">
         <v>26</v>
       </c>
@@ -4210,7 +4210,7 @@
       </c>
       <c r="H124" s="29"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="27" t="s">
         <v>26</v>
       </c>
@@ -4233,10 +4233,10 @@
         <v>82</v>
       </c>
       <c r="H125" s="29" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="46" t="s">
         <v>26</v>
       </c>
@@ -4260,7 +4260,7 @@
       </c>
       <c r="H126" s="48"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="49" t="s">
         <v>26</v>
       </c>
@@ -4284,7 +4284,7 @@
       </c>
       <c r="H127" s="49"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="49" t="s">
         <v>26</v>
       </c>
@@ -4308,7 +4308,7 @@
       </c>
       <c r="H128" s="49"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="49" t="s">
         <v>26</v>
       </c>
@@ -4332,7 +4332,7 @@
       </c>
       <c r="H129" s="49"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="49" t="s">
         <v>26</v>
       </c>
@@ -4356,7 +4356,7 @@
       </c>
       <c r="H130" s="49"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="49" t="s">
         <v>26</v>
       </c>
@@ -4380,7 +4380,7 @@
       </c>
       <c r="H131" s="49"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="49" t="s">
         <v>26</v>
       </c>
@@ -4404,7 +4404,7 @@
       </c>
       <c r="H132" s="49"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="49" t="s">
         <v>26</v>
       </c>
@@ -4428,7 +4428,7 @@
       </c>
       <c r="H133" s="49"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="49" t="s">
         <v>26</v>
       </c>
@@ -4452,7 +4452,7 @@
       </c>
       <c r="H134" s="49"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="49" t="s">
         <v>26</v>
       </c>
@@ -4476,7 +4476,7 @@
       </c>
       <c r="H135" s="49"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" s="49" t="s">
         <v>26</v>
       </c>
@@ -4500,7 +4500,7 @@
       </c>
       <c r="H136" s="49"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="49" t="s">
         <v>26</v>
       </c>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="H137" s="15"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="49" t="s">
         <v>26</v>
       </c>
@@ -4548,7 +4548,7 @@
       </c>
       <c r="H138" s="15"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="49" t="s">
         <v>26</v>
       </c>
@@ -4572,7 +4572,7 @@
       </c>
       <c r="H139" s="15"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="49" t="s">
         <v>26</v>
       </c>
@@ -4596,7 +4596,7 @@
       </c>
       <c r="H140" s="15"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" s="49" t="s">
         <v>26</v>
       </c>
@@ -4620,7 +4620,7 @@
       </c>
       <c r="H141" s="15"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="49" t="s">
         <v>26</v>
       </c>
@@ -4644,7 +4644,7 @@
       </c>
       <c r="H142" s="15"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" s="49" t="s">
         <v>26</v>
       </c>
@@ -4668,7 +4668,7 @@
       </c>
       <c r="H143" s="15"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" s="49" t="s">
         <v>26</v>
       </c>
@@ -4692,7 +4692,7 @@
       </c>
       <c r="H144" s="15"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" s="49" t="s">
         <v>26</v>
       </c>
@@ -4716,7 +4716,7 @@
       </c>
       <c r="H145" s="15"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" s="13" t="s">
         <v>26</v>
       </c>
@@ -4739,10 +4739,10 @@
         <v>137</v>
       </c>
       <c r="H146" s="15" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" s="13" t="s">
         <v>26</v>
       </c>
@@ -4766,7 +4766,7 @@
       </c>
       <c r="H147" s="15"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" s="19" t="s">
         <v>26</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" s="9" t="s">
         <v>26</v>
       </c>
@@ -4816,7 +4816,7 @@
       </c>
       <c r="H149" s="9"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" s="9" t="s">
         <v>26</v>
       </c>
@@ -4840,7 +4840,7 @@
       </c>
       <c r="H150" s="9"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" s="9" t="s">
         <v>26</v>
       </c>
@@ -4863,10 +4863,10 @@
         <v>197</v>
       </c>
       <c r="H151" s="9" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" s="61" t="s">
         <v>26</v>
       </c>
@@ -4892,7 +4892,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" s="65" t="s">
         <v>26</v>
       </c>
@@ -4916,7 +4916,7 @@
       </c>
       <c r="H153" s="65"/>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" s="9" t="s">
         <v>26</v>
       </c>
@@ -4940,7 +4940,7 @@
       </c>
       <c r="H154" s="9"/>
     </row>
-    <row r="155" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="9" t="s">
         <v>26</v>
       </c>
@@ -4963,10 +4963,10 @@
         <v>197</v>
       </c>
       <c r="H155" s="9" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="61" t="s">
         <v>26</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>2050</v>
       </c>
       <c r="C156" s="61" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D156" s="61" t="s">
         <v>181</v>
@@ -4992,7 +4992,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="67" t="s">
         <v>26</v>
       </c>
@@ -5016,7 +5016,7 @@
       </c>
       <c r="H157" s="67"/>
     </row>
-    <row r="158" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="6" t="s">
         <v>26</v>
       </c>
@@ -5039,10 +5039,10 @@
         <v>195</v>
       </c>
       <c r="H158" s="6" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="70" t="s">
         <v>26</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>2035</v>
       </c>
       <c r="C159" s="70" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="D159" s="70" t="s">
         <v>181</v>
@@ -5068,7 +5068,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="160" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:8" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="55" t="s">
         <v>26</v>
       </c>
@@ -5092,7 +5092,7 @@
       </c>
       <c r="H160" s="55"/>
     </row>
-    <row r="161" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="55" t="s">
         <v>26</v>
       </c>
@@ -5115,10 +5115,10 @@
         <v>195</v>
       </c>
       <c r="H161" s="55" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="55" t="s">
         <v>26</v>
       </c>
@@ -5142,7 +5142,7 @@
       </c>
       <c r="H162" s="55"/>
     </row>
-    <row r="163" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="55" t="s">
         <v>26</v>
       </c>
@@ -5150,7 +5150,7 @@
         <v>2050</v>
       </c>
       <c r="C163" s="55" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="D163" s="55" t="s">
         <v>181</v>
@@ -5169,7 +5169,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H163" xr:uid="{56DFE6B8-B4E7-4E48-A7C9-F6B78001C38B}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add updated 2035 IPA run
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ywang\Documents\GitHub\travel-model-one\utilities\RTP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8C4743-18A1-49D8-9B2B-DA714F4616E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6084E7-7734-424E-B262-C3743E51B374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="20200" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="24765" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$H$163</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$H$164</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="229">
   <si>
     <t>EEJ</t>
   </si>
@@ -709,6 +709,12 @@
   </si>
   <si>
     <t>2050_TM152_EIR_Alt2_04</t>
+  </si>
+  <si>
+    <t>2035_TM152_IPA_04</t>
+  </si>
+  <si>
+    <t>2035_IP_FBPtotals</t>
   </si>
 </sst>
 </file>
@@ -1332,23 +1338,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H163"/>
+  <dimension ref="A1:H164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C164" sqref="C164"/>
+      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="36.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.296875" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="70.8984375" customWidth="1"/>
+    <col min="6" max="6" width="70.85546875" customWidth="1"/>
     <col min="7" max="7" width="15" style="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="52" t="s">
         <v>40</v>
       </c>
@@ -1374,7 +1380,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
@@ -1394,7 +1400,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>25</v>
       </c>
@@ -1414,7 +1420,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>25</v>
       </c>
@@ -1434,7 +1440,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>25</v>
       </c>
@@ -1454,7 +1460,7 @@
       <c r="G5" s="11"/>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>25</v>
       </c>
@@ -1474,7 +1480,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>25</v>
       </c>
@@ -1494,7 +1500,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>25</v>
       </c>
@@ -1514,7 +1520,7 @@
       <c r="G8" s="11"/>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>25</v>
       </c>
@@ -1534,7 +1540,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>25</v>
       </c>
@@ -1554,7 +1560,7 @@
       <c r="G10" s="17"/>
       <c r="H10" s="18"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>25</v>
       </c>
@@ -1574,7 +1580,7 @@
       <c r="G11" s="17"/>
       <c r="H11" s="18"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>25</v>
       </c>
@@ -1594,7 +1600,7 @@
       <c r="G12" s="17"/>
       <c r="H12" s="18"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>25</v>
       </c>
@@ -1614,7 +1620,7 @@
       <c r="G13" s="17"/>
       <c r="H13" s="18"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>25</v>
       </c>
@@ -1634,7 +1640,7 @@
       <c r="G14" s="17"/>
       <c r="H14" s="18"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>25</v>
       </c>
@@ -1654,7 +1660,7 @@
       <c r="G15" s="14"/>
       <c r="H15" s="15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>25</v>
       </c>
@@ -1674,7 +1680,7 @@
       <c r="G16" s="14"/>
       <c r="H16" s="15"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
@@ -1694,7 +1700,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="15"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>25</v>
       </c>
@@ -1714,7 +1720,7 @@
       <c r="G18" s="14"/>
       <c r="H18" s="15"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>25</v>
       </c>
@@ -1734,7 +1740,7 @@
       <c r="G19" s="20"/>
       <c r="H19" s="21"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
         <v>26</v>
       </c>
@@ -1756,7 +1762,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
         <v>26</v>
       </c>
@@ -1776,7 +1782,7 @@
       <c r="G21" s="23"/>
       <c r="H21" s="24"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="65" t="s">
         <v>26</v>
       </c>
@@ -1802,7 +1808,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>26</v>
       </c>
@@ -1828,7 +1834,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="61" t="s">
         <v>26</v>
       </c>
@@ -1854,7 +1860,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="67" t="s">
         <v>26</v>
       </c>
@@ -1878,7 +1884,7 @@
       </c>
       <c r="H25" s="75"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
         <v>26</v>
       </c>
@@ -1902,7 +1908,7 @@
       </c>
       <c r="H26" s="21"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="57" t="s">
         <v>26</v>
       </c>
@@ -1926,7 +1932,7 @@
       </c>
       <c r="H27" s="59"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
         <v>26</v>
       </c>
@@ -1950,7 +1956,7 @@
       </c>
       <c r="H28" s="18"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
         <v>26</v>
       </c>
@@ -1976,7 +1982,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="31" t="s">
         <v>26</v>
       </c>
@@ -2002,7 +2008,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="57" t="s">
         <v>26</v>
       </c>
@@ -2026,7 +2032,7 @@
       </c>
       <c r="H31" s="59"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
         <v>26</v>
       </c>
@@ -2050,7 +2056,7 @@
       </c>
       <c r="H32" s="18"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
         <v>26</v>
       </c>
@@ -2076,7 +2082,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
         <v>26</v>
       </c>
@@ -2102,7 +2108,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="34" t="s">
         <v>26</v>
       </c>
@@ -2122,7 +2128,7 @@
       <c r="G35" s="17"/>
       <c r="H35" s="17"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
         <v>26</v>
       </c>
@@ -2142,7 +2148,7 @@
       <c r="G36" s="17"/>
       <c r="H36" s="18"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
         <v>26</v>
       </c>
@@ -2162,7 +2168,7 @@
       <c r="G37" s="17"/>
       <c r="H37" s="18"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="16" t="s">
         <v>26</v>
       </c>
@@ -2178,61 +2184,71 @@
       <c r="E38" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F38" s="18"/>
-      <c r="G38" s="17"/>
+      <c r="F38" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>224</v>
+      </c>
       <c r="H38" s="18" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="35">
-        <v>2035</v>
-      </c>
-      <c r="C39" s="34" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="17">
+        <v>2035</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="35">
+        <v>2035</v>
+      </c>
+      <c r="C40" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="36" t="s">
+      <c r="D40" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="E39" s="36" t="s">
+      <c r="E40" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="F39" s="36"/>
-      <c r="G39" s="35"/>
-      <c r="H39" s="36"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="17">
-        <v>2035</v>
-      </c>
-      <c r="C40" s="16" t="s">
+      <c r="F40" s="36"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="36"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="17">
+        <v>2035</v>
+      </c>
+      <c r="C41" s="16" t="s">
         <v>44</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" s="18"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="18"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B41" s="17">
-        <v>2035</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>45</v>
       </c>
       <c r="D41" s="18" t="s">
         <v>34</v>
@@ -2244,7 +2260,7 @@
       <c r="G41" s="17"/>
       <c r="H41" s="18"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="s">
         <v>26</v>
       </c>
@@ -2252,7 +2268,7 @@
         <v>2035</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>34</v>
@@ -2264,7 +2280,7 @@
       <c r="G42" s="17"/>
       <c r="H42" s="18"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="s">
         <v>26</v>
       </c>
@@ -2272,7 +2288,7 @@
         <v>2035</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="D43" s="18" t="s">
         <v>34</v>
@@ -2280,15 +2296,11 @@
       <c r="E43" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F43" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="G43" s="17" t="s">
-        <v>74</v>
-      </c>
+      <c r="F43" s="18"/>
+      <c r="G43" s="17"/>
       <c r="H43" s="18"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="16" t="s">
         <v>26</v>
       </c>
@@ -2296,7 +2308,7 @@
         <v>2035</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D44" s="18" t="s">
         <v>34</v>
@@ -2305,94 +2317,94 @@
         <v>7</v>
       </c>
       <c r="F44" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="H44" s="18"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="17">
+        <v>2035</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="G44" s="17" t="s">
+      <c r="G45" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="H44" s="18"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" s="32">
-        <v>2035</v>
-      </c>
-      <c r="C45" s="31" t="s">
+      <c r="H45" s="18"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="32">
+        <v>2035</v>
+      </c>
+      <c r="C46" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="D45" s="33" t="s">
+      <c r="D46" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="E45" s="33" t="s">
+      <c r="E46" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="F45" s="33" t="s">
+      <c r="F46" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="G45" s="32" t="s">
+      <c r="G46" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="H45" s="33"/>
-    </row>
-    <row r="46" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B46" s="47">
-        <v>2035</v>
-      </c>
-      <c r="C46" s="48" t="s">
+      <c r="H46" s="33"/>
+    </row>
+    <row r="47" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="47">
+        <v>2035</v>
+      </c>
+      <c r="C47" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="D46" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="E46" s="48" t="s">
+      <c r="D47" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F46" s="48" t="s">
+      <c r="F47" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="G46" s="47" t="s">
+      <c r="G47" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="H46" s="48"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47" s="14">
-        <v>2035</v>
-      </c>
-      <c r="C47" s="15" t="s">
+      <c r="H47" s="48"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="14">
+        <v>2035</v>
+      </c>
+      <c r="C48" s="15" t="s">
         <v>111</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F47" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="G47" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="H47" s="15"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B48" s="14">
-        <v>2035</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>123</v>
       </c>
       <c r="D48" s="15" t="s">
         <v>91</v>
@@ -2401,14 +2413,14 @@
         <v>7</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G48" s="14" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H48" s="15"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
         <v>26</v>
       </c>
@@ -2416,7 +2428,7 @@
         <v>2035</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="D49" s="15" t="s">
         <v>91</v>
@@ -2425,14 +2437,14 @@
         <v>7</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="G49" s="14" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="H49" s="15"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
         <v>26</v>
       </c>
@@ -2440,7 +2452,7 @@
         <v>2035</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D50" s="15" t="s">
         <v>91</v>
@@ -2456,7 +2468,7 @@
       </c>
       <c r="H50" s="15"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="13" t="s">
         <v>26</v>
       </c>
@@ -2464,7 +2476,7 @@
         <v>2035</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D51" s="15" t="s">
         <v>91</v>
@@ -2480,7 +2492,7 @@
       </c>
       <c r="H51" s="15"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="13" t="s">
         <v>26</v>
       </c>
@@ -2488,7 +2500,7 @@
         <v>2035</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D52" s="15" t="s">
         <v>91</v>
@@ -2497,14 +2509,14 @@
         <v>7</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="G52" s="14" t="s">
         <v>137</v>
       </c>
       <c r="H52" s="15"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="13" t="s">
         <v>26</v>
       </c>
@@ -2512,7 +2524,7 @@
         <v>2035</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D53" s="15" t="s">
         <v>91</v>
@@ -2521,14 +2533,14 @@
         <v>7</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G53" s="14" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="H53" s="15"/>
     </row>
-    <row r="54" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
         <v>26</v>
       </c>
@@ -2536,7 +2548,7 @@
         <v>2035</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="D54" s="15" t="s">
         <v>91</v>
@@ -2545,16 +2557,14 @@
         <v>7</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="G54" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="H54" s="15" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+      <c r="H54" s="15"/>
+    </row>
+    <row r="55" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
         <v>26</v>
       </c>
@@ -2562,7 +2572,7 @@
         <v>2035</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>221</v>
+        <v>170</v>
       </c>
       <c r="D55" s="15" t="s">
         <v>91</v>
@@ -2576,103 +2586,109 @@
       <c r="G55" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="H55" s="15"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A56" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B56" s="20">
-        <v>2035</v>
-      </c>
-      <c r="C56" s="21" t="s">
+      <c r="H55" s="15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="14">
+        <v>2035</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="G56" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H56" s="15"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" s="20">
+        <v>2035</v>
+      </c>
+      <c r="C57" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="D56" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E56" s="21" t="s">
+      <c r="D57" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E57" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F56" s="21" t="s">
+      <c r="F57" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="G56" s="20" t="s">
+      <c r="G57" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="H56" s="21" t="s">
+      <c r="H57" s="21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B57" s="35">
-        <v>2035</v>
-      </c>
-      <c r="C57" s="36" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" s="35">
+        <v>2035</v>
+      </c>
+      <c r="C58" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="D57" s="36" t="s">
+      <c r="D58" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="E57" s="36" t="s">
+      <c r="E58" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="F57" s="36"/>
-      <c r="G57" s="35"/>
-      <c r="H57" s="36"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B58" s="32">
-        <v>2035</v>
-      </c>
-      <c r="C58" s="33" t="s">
+      <c r="F58" s="36"/>
+      <c r="G58" s="35"/>
+      <c r="H58" s="36"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="32">
+        <v>2035</v>
+      </c>
+      <c r="C59" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="D58" s="33" t="s">
+      <c r="D59" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="E58" s="33" t="s">
+      <c r="E59" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="F58" s="33"/>
-      <c r="G58" s="32"/>
-      <c r="H58" s="33"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B59" s="17">
-        <v>2035</v>
-      </c>
-      <c r="C59" s="18" t="s">
+      <c r="F59" s="33"/>
+      <c r="G59" s="32"/>
+      <c r="H59" s="33"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B60" s="17">
+        <v>2035</v>
+      </c>
+      <c r="C60" s="18" t="s">
         <v>47</v>
-      </c>
-      <c r="D59" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E59" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F59" s="18"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="18"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A60" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B60" s="17">
-        <v>2035</v>
-      </c>
-      <c r="C60" s="18" t="s">
-        <v>37</v>
       </c>
       <c r="D60" s="18" t="s">
         <v>34</v>
@@ -2684,7 +2700,7 @@
       <c r="G60" s="17"/>
       <c r="H60" s="18"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="16" t="s">
         <v>26</v>
       </c>
@@ -2692,7 +2708,7 @@
         <v>2035</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D61" s="18" t="s">
         <v>34</v>
@@ -2700,15 +2716,11 @@
       <c r="E61" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="F61" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="G61" s="17" t="s">
-        <v>64</v>
-      </c>
+      <c r="F61" s="18"/>
+      <c r="G61" s="17"/>
       <c r="H61" s="18"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="16" t="s">
         <v>26</v>
       </c>
@@ -2716,7 +2728,7 @@
         <v>2035</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D62" s="18" t="s">
         <v>34</v>
@@ -2725,14 +2737,14 @@
         <v>38</v>
       </c>
       <c r="F62" s="18" t="s">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="G62" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H62" s="18"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="16" t="s">
         <v>26</v>
       </c>
@@ -2740,7 +2752,7 @@
         <v>2035</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D63" s="18" t="s">
         <v>34</v>
@@ -2749,14 +2761,14 @@
         <v>38</v>
       </c>
       <c r="F63" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G63" s="17" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H63" s="18"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="16" t="s">
         <v>26</v>
       </c>
@@ -2764,7 +2776,7 @@
         <v>2035</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D64" s="18" t="s">
         <v>34</v>
@@ -2773,14 +2785,14 @@
         <v>38</v>
       </c>
       <c r="F64" s="18" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G64" s="17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H64" s="18"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="16" t="s">
         <v>26</v>
       </c>
@@ -2788,7 +2800,7 @@
         <v>2035</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D65" s="18" t="s">
         <v>34</v>
@@ -2797,14 +2809,14 @@
         <v>38</v>
       </c>
       <c r="F65" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G65" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H65" s="18"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="16" t="s">
         <v>26</v>
       </c>
@@ -2812,7 +2824,7 @@
         <v>2035</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="D66" s="18" t="s">
         <v>34</v>
@@ -2821,40 +2833,40 @@
         <v>38</v>
       </c>
       <c r="F66" s="18" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G66" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="H66" s="18" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A67" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="B67" s="25">
-        <v>2035</v>
-      </c>
-      <c r="C67" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="D67" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="H66" s="18"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" s="17">
+        <v>2035</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D67" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E67" s="26" t="s">
+      <c r="E67" s="18" t="s">
         <v>38</v>
       </c>
       <c r="F67" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="G67" s="25" t="s">
+      <c r="G67" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="H67" s="26"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H67" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="45" t="s">
         <v>26</v>
       </c>
@@ -2862,7 +2874,7 @@
         <v>2035</v>
       </c>
       <c r="C68" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D68" s="26" t="s">
         <v>34</v>
@@ -2878,31 +2890,31 @@
       </c>
       <c r="H68" s="26"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A69" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B69" s="17">
-        <v>2035</v>
-      </c>
-      <c r="C69" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="D69" s="18" t="s">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B69" s="25">
+        <v>2035</v>
+      </c>
+      <c r="C69" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="D69" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="E69" s="18" t="s">
+      <c r="E69" s="26" t="s">
         <v>38</v>
       </c>
       <c r="F69" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="G69" s="17" t="s">
+      <c r="G69" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="H69" s="18"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H69" s="26"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="16" t="s">
         <v>26</v>
       </c>
@@ -2910,7 +2922,7 @@
         <v>2035</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D70" s="18" t="s">
         <v>34</v>
@@ -2926,7 +2938,7 @@
       </c>
       <c r="H70" s="18"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="16" t="s">
         <v>26</v>
       </c>
@@ -2934,7 +2946,7 @@
         <v>2035</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D71" s="18" t="s">
         <v>34</v>
@@ -2950,7 +2962,7 @@
       </c>
       <c r="H71" s="18"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="16" t="s">
         <v>26</v>
       </c>
@@ -2958,7 +2970,7 @@
         <v>2035</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D72" s="18" t="s">
         <v>34</v>
@@ -2974,63 +2986,63 @@
       </c>
       <c r="H72" s="18"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A73" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B73" s="47">
-        <v>2035</v>
-      </c>
-      <c r="C73" s="48" t="s">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B73" s="17">
+        <v>2035</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D73" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E73" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F73" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="G73" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="H73" s="18"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74" s="47">
+        <v>2035</v>
+      </c>
+      <c r="C74" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="D73" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="E73" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="F73" s="48" t="s">
+      <c r="D74" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E74" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="F74" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="G73" s="47" t="s">
+      <c r="G74" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="H73" s="48"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A74" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B74" s="14">
-        <v>2035</v>
-      </c>
-      <c r="C74" s="15" t="s">
+      <c r="H74" s="48"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B75" s="14">
+        <v>2035</v>
+      </c>
+      <c r="C75" s="15" t="s">
         <v>98</v>
-      </c>
-      <c r="D74" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E74" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F74" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="G74" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="H74" s="15"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A75" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B75" s="14">
-        <v>2035</v>
-      </c>
-      <c r="C75" s="15" t="s">
-        <v>110</v>
       </c>
       <c r="D75" s="15" t="s">
         <v>91</v>
@@ -3046,7 +3058,7 @@
       </c>
       <c r="H75" s="15"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="13" t="s">
         <v>26</v>
       </c>
@@ -3054,7 +3066,7 @@
         <v>2035</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D76" s="15" t="s">
         <v>91</v>
@@ -3070,7 +3082,7 @@
       </c>
       <c r="H76" s="15"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="13" t="s">
         <v>26</v>
       </c>
@@ -3078,7 +3090,7 @@
         <v>2035</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D77" s="15" t="s">
         <v>91</v>
@@ -3094,7 +3106,7 @@
       </c>
       <c r="H77" s="15"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="13" t="s">
         <v>26</v>
       </c>
@@ -3102,79 +3114,79 @@
         <v>2035</v>
       </c>
       <c r="C78" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E78" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F78" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="G78" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="H78" s="15"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B79" s="14">
+        <v>2035</v>
+      </c>
+      <c r="C79" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D78" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E78" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F78" s="15" t="s">
+      <c r="D79" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E79" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F79" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="G78" s="14" t="s">
+      <c r="G79" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="H78" s="15"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A79" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B79" s="14">
-        <v>2035</v>
-      </c>
-      <c r="C79" s="15" t="s">
+      <c r="H79" s="15"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B80" s="14">
+        <v>2035</v>
+      </c>
+      <c r="C80" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="D79" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E79" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F79" s="15" t="s">
+      <c r="D80" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E80" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F80" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="G79" s="14" t="s">
+      <c r="G80" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="H79" s="15"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A80" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B80" s="14">
-        <v>2035</v>
-      </c>
-      <c r="C80" s="15" t="s">
+      <c r="H80" s="15"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B81" s="14">
+        <v>2035</v>
+      </c>
+      <c r="C81" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="D80" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E80" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F80" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="G80" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="H80" s="15"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A81" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B81" s="14">
-        <v>2035</v>
-      </c>
-      <c r="C81" s="15" t="s">
-        <v>133</v>
       </c>
       <c r="D81" s="15" t="s">
         <v>91</v>
@@ -3190,7 +3202,7 @@
       </c>
       <c r="H81" s="15"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="s">
         <v>26</v>
       </c>
@@ -3198,31 +3210,31 @@
         <v>2035</v>
       </c>
       <c r="C82" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="D82" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E82" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F82" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="G82" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="H82" s="15"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B83" s="14">
+        <v>2035</v>
+      </c>
+      <c r="C83" s="15" t="s">
         <v>139</v>
-      </c>
-      <c r="D82" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E82" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F82" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="G82" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="H82" s="15"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A83" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B83" s="14">
-        <v>2035</v>
-      </c>
-      <c r="C83" s="15" t="s">
-        <v>142</v>
       </c>
       <c r="D83" s="15" t="s">
         <v>91</v>
@@ -3238,7 +3250,7 @@
       </c>
       <c r="H83" s="15"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="s">
         <v>26</v>
       </c>
@@ -3246,7 +3258,7 @@
         <v>2035</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D84" s="15" t="s">
         <v>91</v>
@@ -3262,7 +3274,7 @@
       </c>
       <c r="H84" s="15"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
         <v>26</v>
       </c>
@@ -3270,7 +3282,7 @@
         <v>2035</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D85" s="15" t="s">
         <v>91</v>
@@ -3286,7 +3298,7 @@
       </c>
       <c r="H85" s="15"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
         <v>26</v>
       </c>
@@ -3294,7 +3306,7 @@
         <v>2035</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D86" s="15" t="s">
         <v>91</v>
@@ -3310,7 +3322,7 @@
       </c>
       <c r="H86" s="15"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="13" t="s">
         <v>26</v>
       </c>
@@ -3318,7 +3330,7 @@
         <v>2035</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D87" s="15" t="s">
         <v>91</v>
@@ -3332,11 +3344,9 @@
       <c r="G87" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="H87" s="15" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H87" s="15"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="13" t="s">
         <v>26</v>
       </c>
@@ -3344,7 +3354,7 @@
         <v>2035</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="D88" s="15" t="s">
         <v>91</v>
@@ -3358,9 +3368,11 @@
       <c r="G88" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="H88" s="15"/>
-    </row>
-    <row r="89" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H88" s="15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="s">
         <v>26</v>
       </c>
@@ -3368,7 +3380,7 @@
         <v>2035</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="D89" s="15" t="s">
         <v>91</v>
@@ -3384,83 +3396,81 @@
       </c>
       <c r="H89" s="15"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A90" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B90" s="20">
-        <v>2035</v>
-      </c>
-      <c r="C90" s="21" t="s">
+    <row r="90" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B90" s="14">
+        <v>2035</v>
+      </c>
+      <c r="C90" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E90" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F90" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G90" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H90" s="15"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B91" s="20">
+        <v>2035</v>
+      </c>
+      <c r="C91" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="D90" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E90" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="F90" s="21" t="s">
+      <c r="D91" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E91" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F91" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="G90" s="20" t="s">
+      <c r="G91" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="H90" s="21" t="s">
+      <c r="H91" s="21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A91" s="57" t="s">
-        <v>26</v>
-      </c>
-      <c r="B91" s="58">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="B92" s="58">
         <v>2040</v>
       </c>
-      <c r="C91" s="59" t="s">
+      <c r="C92" s="59" t="s">
         <v>183</v>
       </c>
-      <c r="D91" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="E91" s="48" t="s">
+      <c r="D92" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="E92" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F91" s="15" t="s">
+      <c r="F92" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="G91" s="14" t="s">
+      <c r="G92" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="H91" s="15"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A92" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B92" s="14">
-        <v>2040</v>
-      </c>
-      <c r="C92" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="D92" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E92" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="F92" s="48" t="s">
-        <v>147</v>
-      </c>
-      <c r="G92" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="H92" s="48" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H92" s="15"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="13" t="s">
         <v>26</v>
       </c>
@@ -3468,23 +3478,25 @@
         <v>2040</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>205</v>
+        <v>177</v>
       </c>
       <c r="D93" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E93" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F93" s="15" t="s">
+      <c r="E93" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="F93" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="G93" s="14" t="s">
+      <c r="G93" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="H93" s="15"/>
-    </row>
-    <row r="94" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H93" s="48" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="13" t="s">
         <v>26</v>
       </c>
@@ -3492,7 +3504,7 @@
         <v>2040</v>
       </c>
       <c r="C94" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D94" s="15" t="s">
         <v>91</v>
@@ -3508,7 +3520,7 @@
       </c>
       <c r="H94" s="15"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="13" t="s">
         <v>26</v>
       </c>
@@ -3516,55 +3528,59 @@
         <v>2040</v>
       </c>
       <c r="C95" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="D95" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E95" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F95" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G95" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H95" s="15"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B96" s="14">
+        <v>2040</v>
+      </c>
+      <c r="C96" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="D95" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E95" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="F95" s="21" t="s">
+      <c r="D96" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E96" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F96" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="G95" s="20" t="s">
+      <c r="G96" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="H95" s="21" t="s">
+      <c r="H96" s="21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A96" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="B96" s="38">
-        <v>2050</v>
-      </c>
-      <c r="C96" s="39" t="s">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B97" s="38">
+        <v>2050</v>
+      </c>
+      <c r="C97" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="D96" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="E96" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="F96" s="41"/>
-      <c r="G96" s="40"/>
-      <c r="H96" s="41"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A97" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B97" s="40">
-        <v>2050</v>
-      </c>
-      <c r="C97" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="D97" s="41" t="s">
+      <c r="D97" s="39" t="s">
         <v>34</v>
       </c>
       <c r="E97" s="41" t="s">
@@ -3574,7 +3590,7 @@
       <c r="G97" s="40"/>
       <c r="H97" s="41"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="27" t="s">
         <v>26</v>
       </c>
@@ -3582,7 +3598,7 @@
         <v>2050</v>
       </c>
       <c r="C98" s="41" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D98" s="41" t="s">
         <v>34</v>
@@ -3590,15 +3606,11 @@
       <c r="E98" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F98" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="G98" s="40" t="s">
-        <v>65</v>
-      </c>
+      <c r="F98" s="41"/>
+      <c r="G98" s="40"/>
       <c r="H98" s="41"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="27" t="s">
         <v>26</v>
       </c>
@@ -3606,7 +3618,7 @@
         <v>2050</v>
       </c>
       <c r="C99" s="41" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D99" s="41" t="s">
         <v>34</v>
@@ -3622,7 +3634,7 @@
       </c>
       <c r="H99" s="41"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="27" t="s">
         <v>26</v>
       </c>
@@ -3630,7 +3642,7 @@
         <v>2050</v>
       </c>
       <c r="C100" s="41" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D100" s="41" t="s">
         <v>34</v>
@@ -3639,14 +3651,14 @@
         <v>7</v>
       </c>
       <c r="F100" s="41" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G100" s="40" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H100" s="41"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="27" t="s">
         <v>26</v>
       </c>
@@ -3654,7 +3666,7 @@
         <v>2050</v>
       </c>
       <c r="C101" s="41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D101" s="41" t="s">
         <v>34</v>
@@ -3663,86 +3675,86 @@
         <v>7</v>
       </c>
       <c r="F101" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="G101" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="H101" s="41"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B102" s="40">
+        <v>2050</v>
+      </c>
+      <c r="C102" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D102" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="E102" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="F102" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="G101" s="40" t="s">
+      <c r="G102" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="H101" s="41"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A102" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="B102" s="43">
-        <v>2050</v>
-      </c>
-      <c r="C102" s="44" t="s">
+      <c r="H102" s="41"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B103" s="43">
+        <v>2050</v>
+      </c>
+      <c r="C103" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="D102" s="44" t="s">
+      <c r="D103" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="E102" s="44" t="s">
+      <c r="E103" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="F102" s="44" t="s">
+      <c r="F103" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="G102" s="43" t="s">
+      <c r="G103" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="H102" s="44"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A103" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B103" s="14">
-        <v>2050</v>
-      </c>
-      <c r="C103" s="15" t="s">
+      <c r="H103" s="44"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B104" s="14">
+        <v>2050</v>
+      </c>
+      <c r="C104" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="D103" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="E103" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F103" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="G103" s="50" t="s">
-        <v>75</v>
-      </c>
-      <c r="H103" s="15"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A104" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B104" s="14">
-        <v>2050</v>
-      </c>
-      <c r="C104" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="D104" s="15" t="s">
+      <c r="D104" s="48" t="s">
         <v>91</v>
       </c>
       <c r="E104" s="15" t="s">
         <v>7</v>
       </c>
       <c r="F104" s="15" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G104" s="50" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H104" s="15"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="13" t="s">
         <v>26</v>
       </c>
@@ -3750,7 +3762,7 @@
         <v>2050</v>
       </c>
       <c r="C105" s="15" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="D105" s="15" t="s">
         <v>91</v>
@@ -3759,14 +3771,14 @@
         <v>7</v>
       </c>
       <c r="F105" s="15" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G105" s="50" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H105" s="15"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="13" t="s">
         <v>26</v>
       </c>
@@ -3774,7 +3786,7 @@
         <v>2050</v>
       </c>
       <c r="C106" s="15" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="D106" s="15" t="s">
         <v>91</v>
@@ -3783,14 +3795,14 @@
         <v>7</v>
       </c>
       <c r="F106" s="15" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="G106" s="50" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="H106" s="15"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="13" t="s">
         <v>26</v>
       </c>
@@ -3798,7 +3810,7 @@
         <v>2050</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D107" s="15" t="s">
         <v>91</v>
@@ -3809,12 +3821,12 @@
       <c r="F107" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="G107" s="14" t="s">
+      <c r="G107" s="50" t="s">
         <v>137</v>
       </c>
       <c r="H107" s="15"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="13" t="s">
         <v>26</v>
       </c>
@@ -3822,7 +3834,7 @@
         <v>2050</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D108" s="15" t="s">
         <v>91</v>
@@ -3838,7 +3850,7 @@
       </c>
       <c r="H108" s="15"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="13" t="s">
         <v>26</v>
       </c>
@@ -3846,7 +3858,7 @@
         <v>2050</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D109" s="15" t="s">
         <v>91</v>
@@ -3855,14 +3867,14 @@
         <v>7</v>
       </c>
       <c r="F109" s="15" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="G109" s="14" t="s">
         <v>137</v>
       </c>
       <c r="H109" s="15"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="13" t="s">
         <v>26</v>
       </c>
@@ -3870,7 +3882,7 @@
         <v>2050</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D110" s="15" t="s">
         <v>91</v>
@@ -3879,14 +3891,14 @@
         <v>7</v>
       </c>
       <c r="F110" s="15" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G110" s="14" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="H110" s="15"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="13" t="s">
         <v>26</v>
       </c>
@@ -3894,7 +3906,7 @@
         <v>2050</v>
       </c>
       <c r="C111" s="15" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D111" s="15" t="s">
         <v>91</v>
@@ -3903,14 +3915,14 @@
         <v>7</v>
       </c>
       <c r="F111" s="15" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="G111" s="14" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="H111" s="15"/>
     </row>
-    <row r="112" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="13" t="s">
         <v>26</v>
       </c>
@@ -3918,7 +3930,7 @@
         <v>2050</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D112" s="15" t="s">
         <v>91</v>
@@ -3932,11 +3944,9 @@
       <c r="G112" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="H112" s="15" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H112" s="15"/>
+    </row>
+    <row r="113" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="13" t="s">
         <v>26</v>
       </c>
@@ -3944,7 +3954,7 @@
         <v>2050</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>217</v>
+        <v>174</v>
       </c>
       <c r="D113" s="15" t="s">
         <v>91</v>
@@ -3958,103 +3968,109 @@
       <c r="G113" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="H113" s="15"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A114" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B114" s="20">
-        <v>2050</v>
-      </c>
-      <c r="C114" s="21" t="s">
+      <c r="H113" s="15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B114" s="14">
+        <v>2050</v>
+      </c>
+      <c r="C114" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D114" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E114" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F114" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="G114" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H114" s="15"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B115" s="20">
+        <v>2050</v>
+      </c>
+      <c r="C115" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="D114" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E114" s="21" t="s">
+      <c r="D115" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E115" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F114" s="21" t="s">
+      <c r="F115" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="G114" s="20" t="s">
+      <c r="G115" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="H114" s="21" t="s">
+      <c r="H115" s="21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A115" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B115" s="40">
-        <v>2050</v>
-      </c>
-      <c r="C115" s="41" t="s">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B116" s="40">
+        <v>2050</v>
+      </c>
+      <c r="C116" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="D115" s="41" t="s">
+      <c r="D116" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="E115" s="41" t="s">
+      <c r="E116" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="F115" s="41"/>
-      <c r="G115" s="40"/>
-      <c r="H115" s="41"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A116" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="B116" s="43">
-        <v>2050</v>
-      </c>
-      <c r="C116" s="44" t="s">
+      <c r="F116" s="41"/>
+      <c r="G116" s="40"/>
+      <c r="H116" s="41"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B117" s="43">
+        <v>2050</v>
+      </c>
+      <c r="C117" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="D116" s="44" t="s">
+      <c r="D117" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="E116" s="44" t="s">
+      <c r="E117" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="F116" s="44"/>
-      <c r="G116" s="43"/>
-      <c r="H116" s="44"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A117" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B117" s="28">
-        <v>2050</v>
-      </c>
-      <c r="C117" s="29" t="s">
+      <c r="F117" s="44"/>
+      <c r="G117" s="43"/>
+      <c r="H117" s="44"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B118" s="28">
+        <v>2050</v>
+      </c>
+      <c r="C118" s="29" t="s">
         <v>51</v>
-      </c>
-      <c r="D117" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="E117" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F117" s="29"/>
-      <c r="G117" s="28"/>
-      <c r="H117" s="29"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A118" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B118" s="28">
-        <v>2050</v>
-      </c>
-      <c r="C118" s="29" t="s">
-        <v>39</v>
       </c>
       <c r="D118" s="29" t="s">
         <v>34</v>
@@ -4066,7 +4082,7 @@
       <c r="G118" s="28"/>
       <c r="H118" s="29"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="27" t="s">
         <v>26</v>
       </c>
@@ -4074,7 +4090,7 @@
         <v>2050</v>
       </c>
       <c r="C119" s="29" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D119" s="29" t="s">
         <v>34</v>
@@ -4082,15 +4098,11 @@
       <c r="E119" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="F119" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="G119" s="28" t="s">
-        <v>63</v>
-      </c>
+      <c r="F119" s="29"/>
+      <c r="G119" s="28"/>
       <c r="H119" s="29"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="27" t="s">
         <v>26</v>
       </c>
@@ -4098,7 +4110,7 @@
         <v>2050</v>
       </c>
       <c r="C120" s="29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D120" s="29" t="s">
         <v>34</v>
@@ -4114,7 +4126,7 @@
       </c>
       <c r="H120" s="29"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="27" t="s">
         <v>26</v>
       </c>
@@ -4122,7 +4134,7 @@
         <v>2050</v>
       </c>
       <c r="C121" s="29" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D121" s="29" t="s">
         <v>34</v>
@@ -4131,14 +4143,14 @@
         <v>38</v>
       </c>
       <c r="F121" s="29" t="s">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="G121" s="28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H121" s="29"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="27" t="s">
         <v>26</v>
       </c>
@@ -4146,7 +4158,7 @@
         <v>2050</v>
       </c>
       <c r="C122" s="29" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D122" s="29" t="s">
         <v>34</v>
@@ -4155,14 +4167,14 @@
         <v>38</v>
       </c>
       <c r="F122" s="29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G122" s="28" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H122" s="29"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="27" t="s">
         <v>26</v>
       </c>
@@ -4170,7 +4182,7 @@
         <v>2050</v>
       </c>
       <c r="C123" s="29" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D123" s="29" t="s">
         <v>34</v>
@@ -4179,14 +4191,14 @@
         <v>38</v>
       </c>
       <c r="F123" s="29" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G123" s="28" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H123" s="29"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="27" t="s">
         <v>26</v>
       </c>
@@ -4194,7 +4206,7 @@
         <v>2050</v>
       </c>
       <c r="C124" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D124" s="29" t="s">
         <v>34</v>
@@ -4203,14 +4215,14 @@
         <v>38</v>
       </c>
       <c r="F124" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G124" s="28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H124" s="29"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="27" t="s">
         <v>26</v>
       </c>
@@ -4218,7 +4230,7 @@
         <v>2050</v>
       </c>
       <c r="C125" s="29" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D125" s="29" t="s">
         <v>34</v>
@@ -4227,72 +4239,72 @@
         <v>38</v>
       </c>
       <c r="F125" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="G125" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="H125" s="29"/>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A126" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B126" s="28">
+        <v>2050</v>
+      </c>
+      <c r="C126" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D126" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E126" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="F126" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="G125" s="28" t="s">
+      <c r="G126" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="H125" s="29" t="s">
+      <c r="H126" s="29" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A126" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B126" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C126" s="48" t="s">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A127" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B127" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C127" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="D126" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="E126" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="F126" s="48" t="s">
+      <c r="D127" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E127" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="F127" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="G126" s="47" t="s">
+      <c r="G127" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="H126" s="48"/>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A127" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B127" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C127" s="49" t="s">
+      <c r="H127" s="48"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A128" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B128" s="50">
+        <v>2050</v>
+      </c>
+      <c r="C128" s="49" t="s">
         <v>101</v>
-      </c>
-      <c r="D127" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E127" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F127" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="G127" s="50" t="s">
-        <v>82</v>
-      </c>
-      <c r="H127" s="49"/>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A128" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B128" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C128" s="49" t="s">
-        <v>102</v>
       </c>
       <c r="D128" s="49" t="s">
         <v>91</v>
@@ -4308,7 +4320,7 @@
       </c>
       <c r="H128" s="49"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="49" t="s">
         <v>26</v>
       </c>
@@ -4316,7 +4328,7 @@
         <v>2050</v>
       </c>
       <c r="C129" s="49" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D129" s="49" t="s">
         <v>91</v>
@@ -4332,7 +4344,7 @@
       </c>
       <c r="H129" s="49"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="49" t="s">
         <v>26</v>
       </c>
@@ -4340,7 +4352,7 @@
         <v>2050</v>
       </c>
       <c r="C130" s="49" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D130" s="49" t="s">
         <v>91</v>
@@ -4356,7 +4368,7 @@
       </c>
       <c r="H130" s="49"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="49" t="s">
         <v>26</v>
       </c>
@@ -4364,7 +4376,7 @@
         <v>2050</v>
       </c>
       <c r="C131" s="49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D131" s="49" t="s">
         <v>91</v>
@@ -4380,7 +4392,7 @@
       </c>
       <c r="H131" s="49"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="49" t="s">
         <v>26</v>
       </c>
@@ -4388,55 +4400,55 @@
         <v>2050</v>
       </c>
       <c r="C132" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="D132" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E132" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="F132" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="G132" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="H132" s="49"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A133" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B133" s="50">
+        <v>2050</v>
+      </c>
+      <c r="C133" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="D132" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E132" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F132" s="15" t="s">
+      <c r="D133" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E133" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="F133" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="G132" s="50" t="s">
+      <c r="G133" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="H132" s="49"/>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A133" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B133" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C133" s="49" t="s">
+      <c r="H133" s="49"/>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A134" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B134" s="50">
+        <v>2050</v>
+      </c>
+      <c r="C134" s="49" t="s">
         <v>107</v>
-      </c>
-      <c r="D133" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E133" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F133" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="G133" s="50" t="s">
-        <v>82</v>
-      </c>
-      <c r="H133" s="49"/>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A134" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B134" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C134" s="49" t="s">
-        <v>109</v>
       </c>
       <c r="D134" s="49" t="s">
         <v>91</v>
@@ -4452,7 +4464,7 @@
       </c>
       <c r="H134" s="49"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" s="49" t="s">
         <v>26</v>
       </c>
@@ -4460,7 +4472,7 @@
         <v>2050</v>
       </c>
       <c r="C135" s="49" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D135" s="49" t="s">
         <v>91</v>
@@ -4476,7 +4488,7 @@
       </c>
       <c r="H135" s="49"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" s="49" t="s">
         <v>26</v>
       </c>
@@ -4484,103 +4496,103 @@
         <v>2050</v>
       </c>
       <c r="C136" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="D136" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E136" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="F136" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="G136" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="H136" s="49"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A137" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B137" s="50">
+        <v>2050</v>
+      </c>
+      <c r="C137" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="D136" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E136" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F136" s="49" t="s">
+      <c r="D137" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E137" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="F137" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="G136" s="50" t="s">
+      <c r="G137" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="H136" s="49"/>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A137" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B137" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C137" s="49" t="s">
+      <c r="H137" s="49"/>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A138" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B138" s="50">
+        <v>2050</v>
+      </c>
+      <c r="C138" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="D137" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E137" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F137" s="15" t="s">
+      <c r="D138" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E138" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="F138" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="G137" s="14" t="s">
+      <c r="G138" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="H137" s="15"/>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A138" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B138" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C138" s="49" t="s">
+      <c r="H138" s="15"/>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A139" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B139" s="50">
+        <v>2050</v>
+      </c>
+      <c r="C139" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="D138" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E138" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F138" s="15" t="s">
+      <c r="D139" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E139" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="F139" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="G138" s="14" t="s">
+      <c r="G139" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="H138" s="15"/>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A139" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B139" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C139" s="49" t="s">
+      <c r="H139" s="15"/>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A140" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B140" s="50">
+        <v>2050</v>
+      </c>
+      <c r="C140" s="49" t="s">
         <v>140</v>
-      </c>
-      <c r="D139" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E139" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F139" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="G139" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="H139" s="15"/>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A140" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B140" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C140" s="49" t="s">
-        <v>144</v>
       </c>
       <c r="D140" s="49" t="s">
         <v>91</v>
@@ -4596,7 +4608,7 @@
       </c>
       <c r="H140" s="15"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" s="49" t="s">
         <v>26</v>
       </c>
@@ -4604,7 +4616,7 @@
         <v>2050</v>
       </c>
       <c r="C141" s="49" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D141" s="49" t="s">
         <v>91</v>
@@ -4620,7 +4632,7 @@
       </c>
       <c r="H141" s="15"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" s="49" t="s">
         <v>26</v>
       </c>
@@ -4628,7 +4640,7 @@
         <v>2050</v>
       </c>
       <c r="C142" s="49" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D142" s="49" t="s">
         <v>91</v>
@@ -4644,7 +4656,7 @@
       </c>
       <c r="H142" s="15"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" s="49" t="s">
         <v>26</v>
       </c>
@@ -4652,7 +4664,7 @@
         <v>2050</v>
       </c>
       <c r="C143" s="49" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D143" s="49" t="s">
         <v>91</v>
@@ -4668,7 +4680,7 @@
       </c>
       <c r="H143" s="15"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" s="49" t="s">
         <v>26</v>
       </c>
@@ -4676,7 +4688,7 @@
         <v>2050</v>
       </c>
       <c r="C144" s="49" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D144" s="49" t="s">
         <v>91</v>
@@ -4692,7 +4704,7 @@
       </c>
       <c r="H144" s="15"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="49" t="s">
         <v>26</v>
       </c>
@@ -4700,7 +4712,7 @@
         <v>2050</v>
       </c>
       <c r="C145" s="49" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D145" s="49" t="s">
         <v>91</v>
@@ -4716,20 +4728,20 @@
       </c>
       <c r="H145" s="15"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A146" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B146" s="63">
-        <v>2050</v>
-      </c>
-      <c r="C146" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="D146" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="E146" s="13" t="s">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A146" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B146" s="50">
+        <v>2050</v>
+      </c>
+      <c r="C146" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="D146" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E146" s="49" t="s">
         <v>38</v>
       </c>
       <c r="F146" s="15" t="s">
@@ -4738,11 +4750,9 @@
       <c r="G146" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="H146" s="15" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H146" s="15"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="13" t="s">
         <v>26</v>
       </c>
@@ -4750,7 +4760,7 @@
         <v>2050</v>
       </c>
       <c r="C147" s="13" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
       <c r="D147" s="13" t="s">
         <v>91</v>
@@ -4764,67 +4774,69 @@
       <c r="G147" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="H147" s="15"/>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A148" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B148" s="64">
-        <v>2050</v>
-      </c>
-      <c r="C148" s="19" t="s">
+      <c r="H147" s="15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A148" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B148" s="63">
+        <v>2050</v>
+      </c>
+      <c r="C148" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="D148" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E148" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F148" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G148" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H148" s="15"/>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A149" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B149" s="64">
+        <v>2050</v>
+      </c>
+      <c r="C149" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="D148" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E148" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F148" s="21" t="s">
+      <c r="D149" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E149" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F149" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="G148" s="20" t="s">
+      <c r="G149" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="H148" s="21" t="s">
+      <c r="H149" s="21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A149" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B149" s="60">
-        <v>2035</v>
-      </c>
-      <c r="C149" s="9" t="s">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A150" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B150" s="60">
+        <v>2035</v>
+      </c>
+      <c r="C150" s="9" t="s">
         <v>186</v>
-      </c>
-      <c r="D149" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="E149" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="F149" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="G149" s="60" t="s">
-        <v>185</v>
-      </c>
-      <c r="H149" s="9"/>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A150" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B150" s="60">
-        <v>2035</v>
-      </c>
-      <c r="C150" s="9" t="s">
-        <v>188</v>
       </c>
       <c r="D150" s="9" t="s">
         <v>181</v>
@@ -4833,14 +4845,14 @@
         <v>182</v>
       </c>
       <c r="F150" s="9" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G150" s="60" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="H150" s="9"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="9" t="s">
         <v>26</v>
       </c>
@@ -4848,7 +4860,7 @@
         <v>2035</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="D151" s="9" t="s">
         <v>181</v>
@@ -4857,98 +4869,98 @@
         <v>182</v>
       </c>
       <c r="F151" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="G151" s="60" t="s">
+        <v>190</v>
+      </c>
+      <c r="H151" s="9"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A152" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B152" s="60">
+        <v>2035</v>
+      </c>
+      <c r="C152" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D152" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E152" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F152" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="G151" s="60" t="s">
+      <c r="G152" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="H151" s="9" t="s">
+      <c r="H152" s="9" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A152" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="B152" s="62">
-        <v>2035</v>
-      </c>
-      <c r="C152" s="61" t="s">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A153" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B153" s="62">
+        <v>2035</v>
+      </c>
+      <c r="C153" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="D152" s="61" t="s">
+      <c r="D153" s="61" t="s">
         <v>181</v>
       </c>
-      <c r="E152" s="61" t="s">
+      <c r="E153" s="61" t="s">
         <v>182</v>
       </c>
-      <c r="F152" s="61" t="s">
+      <c r="F153" s="61" t="s">
         <v>200</v>
       </c>
-      <c r="G152" s="62" t="s">
+      <c r="G153" s="62" t="s">
         <v>197</v>
       </c>
-      <c r="H152" s="61" t="s">
+      <c r="H153" s="61" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A153" s="65" t="s">
-        <v>26</v>
-      </c>
-      <c r="B153" s="66">
-        <v>2050</v>
-      </c>
-      <c r="C153" s="65" t="s">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A154" s="65" t="s">
+        <v>26</v>
+      </c>
+      <c r="B154" s="66">
+        <v>2050</v>
+      </c>
+      <c r="C154" s="65" t="s">
         <v>180</v>
       </c>
-      <c r="D153" s="65" t="s">
+      <c r="D154" s="65" t="s">
         <v>181</v>
       </c>
-      <c r="E153" s="65" t="s">
+      <c r="E154" s="65" t="s">
         <v>182</v>
       </c>
-      <c r="F153" s="65" t="s">
+      <c r="F154" s="65" t="s">
         <v>184</v>
       </c>
-      <c r="G153" s="66" t="s">
+      <c r="G154" s="66" t="s">
         <v>185</v>
       </c>
-      <c r="H153" s="65"/>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A154" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B154" s="60">
-        <v>2050</v>
-      </c>
-      <c r="C154" s="9" t="s">
+      <c r="H154" s="65"/>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A155" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B155" s="60">
+        <v>2050</v>
+      </c>
+      <c r="C155" s="9" t="s">
         <v>191</v>
-      </c>
-      <c r="D154" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="E154" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="F154" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="G154" s="60" t="s">
-        <v>190</v>
-      </c>
-      <c r="H154" s="9"/>
-    </row>
-    <row r="155" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B155" s="60">
-        <v>2050</v>
-      </c>
-      <c r="C155" s="9" t="s">
-        <v>199</v>
       </c>
       <c r="D155" s="9" t="s">
         <v>181</v>
@@ -4957,150 +4969,150 @@
         <v>182</v>
       </c>
       <c r="F155" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="G155" s="60" t="s">
+        <v>190</v>
+      </c>
+      <c r="H155" s="9"/>
+    </row>
+    <row r="156" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B156" s="60">
+        <v>2050</v>
+      </c>
+      <c r="C156" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="D156" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E156" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F156" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="G155" s="60" t="s">
+      <c r="G156" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="H155" s="9" t="s">
+      <c r="H156" s="9" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="156" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="B156" s="62">
-        <v>2050</v>
-      </c>
-      <c r="C156" s="61" t="s">
+    <row r="157" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B157" s="62">
+        <v>2050</v>
+      </c>
+      <c r="C157" s="61" t="s">
         <v>216</v>
       </c>
-      <c r="D156" s="61" t="s">
+      <c r="D157" s="61" t="s">
         <v>181</v>
       </c>
-      <c r="E156" s="61" t="s">
+      <c r="E157" s="61" t="s">
         <v>182</v>
       </c>
-      <c r="F156" s="61" t="s">
+      <c r="F157" s="61" t="s">
         <v>200</v>
       </c>
-      <c r="G156" s="62" t="s">
+      <c r="G157" s="62" t="s">
         <v>197</v>
       </c>
-      <c r="H156" s="61" t="s">
+      <c r="H157" s="61" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="B157" s="68">
-        <v>2035</v>
-      </c>
-      <c r="C157" s="67" t="s">
+    <row r="158" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="B158" s="68">
+        <v>2035</v>
+      </c>
+      <c r="C158" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="D157" s="67" t="s">
+      <c r="D158" s="67" t="s">
         <v>181</v>
       </c>
-      <c r="E157" s="67" t="s">
+      <c r="E158" s="67" t="s">
         <v>193</v>
       </c>
-      <c r="F157" s="67" t="s">
+      <c r="F158" s="67" t="s">
         <v>194</v>
       </c>
-      <c r="G157" s="68" t="s">
+      <c r="G158" s="68" t="s">
         <v>195</v>
       </c>
-      <c r="H157" s="67"/>
-    </row>
-    <row r="158" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B158" s="69">
-        <v>2035</v>
-      </c>
-      <c r="C158" s="6" t="s">
+      <c r="H158" s="67"/>
+    </row>
+    <row r="159" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B159" s="69">
+        <v>2035</v>
+      </c>
+      <c r="C159" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="D158" s="6" t="s">
+      <c r="D159" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="E158" s="6" t="s">
+      <c r="E159" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="F158" s="6" t="s">
+      <c r="F159" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="G158" s="69" t="s">
+      <c r="G159" s="69" t="s">
         <v>195</v>
       </c>
-      <c r="H158" s="6" t="s">
+      <c r="H159" s="6" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="159" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="B159" s="71">
-        <v>2035</v>
-      </c>
-      <c r="C159" s="70" t="s">
+    <row r="160" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="B160" s="71">
+        <v>2035</v>
+      </c>
+      <c r="C160" s="70" t="s">
         <v>225</v>
       </c>
-      <c r="D159" s="70" t="s">
+      <c r="D160" s="70" t="s">
         <v>181</v>
       </c>
-      <c r="E159" s="70" t="s">
+      <c r="E160" s="70" t="s">
         <v>193</v>
       </c>
-      <c r="F159" s="70" t="s">
+      <c r="F160" s="70" t="s">
         <v>194</v>
       </c>
-      <c r="G159" s="71" t="s">
+      <c r="G160" s="71" t="s">
         <v>195</v>
       </c>
-      <c r="H159" s="70" t="s">
+      <c r="H160" s="70" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="160" spans="1:8" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B160" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C160" s="55" t="s">
+    <row r="161" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B161" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C161" s="55" t="s">
         <v>196</v>
-      </c>
-      <c r="D160" s="55" t="s">
-        <v>181</v>
-      </c>
-      <c r="E160" s="55" t="s">
-        <v>193</v>
-      </c>
-      <c r="F160" s="55" t="s">
-        <v>194</v>
-      </c>
-      <c r="G160" s="56" t="s">
-        <v>195</v>
-      </c>
-      <c r="H160" s="55"/>
-    </row>
-    <row r="161" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B161" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C161" s="55" t="s">
-        <v>202</v>
       </c>
       <c r="D161" s="55" t="s">
         <v>181</v>
@@ -5114,19 +5126,17 @@
       <c r="G161" s="56" t="s">
         <v>195</v>
       </c>
-      <c r="H161" s="55" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H161" s="55"/>
+    </row>
+    <row r="162" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="55" t="s">
         <v>26</v>
       </c>
       <c r="B162" s="56">
-        <v>2035</v>
+        <v>2050</v>
       </c>
       <c r="C162" s="55" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D162" s="55" t="s">
         <v>181</v>
@@ -5140,17 +5150,19 @@
       <c r="G162" s="56" t="s">
         <v>195</v>
       </c>
-      <c r="H162" s="55"/>
-    </row>
-    <row r="163" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H162" s="55" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="55" t="s">
         <v>26</v>
       </c>
       <c r="B163" s="56">
-        <v>2050</v>
+        <v>2035</v>
       </c>
       <c r="C163" s="55" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
       <c r="D163" s="55" t="s">
         <v>181</v>
@@ -5164,7 +5176,31 @@
       <c r="G163" s="56" t="s">
         <v>195</v>
       </c>
-      <c r="H163" s="55" t="s">
+      <c r="H163" s="55"/>
+    </row>
+    <row r="164" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B164" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C164" s="55" t="s">
+        <v>226</v>
+      </c>
+      <c r="D164" s="55" t="s">
+        <v>181</v>
+      </c>
+      <c r="E164" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="F164" s="55" t="s">
+        <v>194</v>
+      </c>
+      <c r="G164" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="H164" s="55" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add seven new runs as current
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6084E7-7734-424E-B262-C3743E51B374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5C50C7-C915-4B6F-8F39-C5A3FE7F8DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="24765" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19575" yWindow="1770" windowWidth="17400" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$H$164</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$H$170</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="236">
   <si>
     <t>EEJ</t>
   </si>
@@ -715,6 +715,27 @@
   </si>
   <si>
     <t>2035_IP_FBPtotals</t>
+  </si>
+  <si>
+    <t>2030_TM152_FBP_Plus_23</t>
+  </si>
+  <si>
+    <t>2035_TM152_FBP_Plus_24</t>
+  </si>
+  <si>
+    <t>2040_TM152_FBP_Plus_24</t>
+  </si>
+  <si>
+    <t>2050_TM152_FBP_PlusCrossing_24</t>
+  </si>
+  <si>
+    <t>2035_TM152_EIR_Alt1_05</t>
+  </si>
+  <si>
+    <t>2050_TM152_EIR_Alt1_05</t>
+  </si>
+  <si>
+    <t>2050_TM152_EIR_Alt2_05</t>
   </si>
 </sst>
 </file>
@@ -1338,11 +1359,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H164"/>
+  <dimension ref="A1:H171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A170" sqref="A170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2098,55 +2119,61 @@
       <c r="E34" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="F34" s="33" t="s">
+      <c r="F34" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="G34" s="32" t="s">
+      <c r="G34" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="H34" s="33" t="s">
+      <c r="H34" s="18" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="35">
-        <v>2035</v>
-      </c>
-      <c r="C35" s="36" t="s">
+      <c r="A35" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="32">
+        <v>2030</v>
+      </c>
+      <c r="C35" s="33" t="s">
+        <v>229</v>
+      </c>
+      <c r="D35" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="G35" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="H35" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="35">
+        <v>2035</v>
+      </c>
+      <c r="C36" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="36" t="s">
+      <c r="D36" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="E35" s="36" t="s">
+      <c r="E36" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="36"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="17">
-        <v>2035</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E36" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F36" s="18"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="17"/>
-      <c r="H36" s="18"/>
+      <c r="H36" s="17"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
@@ -2156,7 +2183,7 @@
         <v>2035</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>152</v>
+        <v>93</v>
       </c>
       <c r="D37" s="18" t="s">
         <v>28</v>
@@ -2176,7 +2203,7 @@
         <v>2035</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>28</v>
@@ -2184,15 +2211,9 @@
       <c r="E38" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F38" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="G38" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="H38" s="18" t="s">
-        <v>220</v>
-      </c>
+      <c r="F38" s="18"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="18"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="s">
@@ -2202,7 +2223,7 @@
         <v>2035</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>227</v>
+        <v>158</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>28</v>
@@ -2217,48 +2238,54 @@
         <v>224</v>
       </c>
       <c r="H39" s="18" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="17">
+        <v>2035</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="H40" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="35">
-        <v>2035</v>
-      </c>
-      <c r="C40" s="34" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="35">
+        <v>2035</v>
+      </c>
+      <c r="C41" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="D40" s="36" t="s">
+      <c r="D41" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="E40" s="36" t="s">
+      <c r="E41" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="F40" s="36"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="36"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B41" s="17">
-        <v>2035</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E41" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" s="18"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="18"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="36"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="s">
@@ -2268,7 +2295,7 @@
         <v>2035</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>34</v>
@@ -2288,7 +2315,7 @@
         <v>2035</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D43" s="18" t="s">
         <v>34</v>
@@ -2308,7 +2335,7 @@
         <v>2035</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="D44" s="18" t="s">
         <v>34</v>
@@ -2316,12 +2343,8 @@
       <c r="E44" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F44" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="G44" s="17" t="s">
-        <v>74</v>
-      </c>
+      <c r="F44" s="18"/>
+      <c r="G44" s="17"/>
       <c r="H44" s="18"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -2332,7 +2355,7 @@
         <v>2035</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D45" s="18" t="s">
         <v>34</v>
@@ -2341,84 +2364,84 @@
         <v>7</v>
       </c>
       <c r="F45" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="G45" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="H45" s="18"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="17">
+        <v>2035</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="G45" s="17" t="s">
+      <c r="G46" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="H45" s="18"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B46" s="32">
-        <v>2035</v>
-      </c>
-      <c r="C46" s="31" t="s">
+      <c r="H46" s="18"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="32">
+        <v>2035</v>
+      </c>
+      <c r="C47" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="D46" s="33" t="s">
+      <c r="D47" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="E46" s="33" t="s">
+      <c r="E47" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="F46" s="33" t="s">
+      <c r="F47" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="G46" s="32" t="s">
+      <c r="G47" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="H46" s="33"/>
-    </row>
-    <row r="47" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47" s="47">
-        <v>2035</v>
-      </c>
-      <c r="C47" s="48" t="s">
+      <c r="H47" s="33"/>
+    </row>
+    <row r="48" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="47">
+        <v>2035</v>
+      </c>
+      <c r="C48" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="D47" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="E47" s="48" t="s">
+      <c r="D48" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F47" s="48" t="s">
+      <c r="F48" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="G47" s="47" t="s">
+      <c r="G48" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="H47" s="48"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B48" s="14">
-        <v>2035</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="D48" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="G48" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="H48" s="15"/>
+      <c r="H48" s="48"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
@@ -2428,7 +2451,7 @@
         <v>2035</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D49" s="15" t="s">
         <v>91</v>
@@ -2437,10 +2460,10 @@
         <v>7</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G49" s="14" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H49" s="15"/>
     </row>
@@ -2452,7 +2475,7 @@
         <v>2035</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="D50" s="15" t="s">
         <v>91</v>
@@ -2461,10 +2484,10 @@
         <v>7</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="G50" s="14" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="H50" s="15"/>
     </row>
@@ -2476,7 +2499,7 @@
         <v>2035</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D51" s="15" t="s">
         <v>91</v>
@@ -2500,7 +2523,7 @@
         <v>2035</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D52" s="15" t="s">
         <v>91</v>
@@ -2524,7 +2547,7 @@
         <v>2035</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D53" s="15" t="s">
         <v>91</v>
@@ -2533,7 +2556,7 @@
         <v>7</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="G53" s="14" t="s">
         <v>137</v>
@@ -2548,7 +2571,7 @@
         <v>2035</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D54" s="15" t="s">
         <v>91</v>
@@ -2557,14 +2580,14 @@
         <v>7</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G54" s="14" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="H54" s="15"/>
     </row>
-    <row r="55" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
         <v>26</v>
       </c>
@@ -2572,7 +2595,7 @@
         <v>2035</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="D55" s="15" t="s">
         <v>91</v>
@@ -2581,14 +2604,12 @@
         <v>7</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="G55" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="H55" s="15" t="s">
-        <v>220</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="H55" s="15"/>
     </row>
     <row r="56" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
@@ -2598,7 +2619,7 @@
         <v>2035</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>221</v>
+        <v>170</v>
       </c>
       <c r="D56" s="15" t="s">
         <v>91</v>
@@ -2612,93 +2633,99 @@
       <c r="G56" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="H56" s="15"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B57" s="20">
-        <v>2035</v>
-      </c>
-      <c r="C57" s="21" t="s">
+      <c r="H56" s="15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" s="14">
+        <v>2035</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E57" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="G57" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H57" s="15"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" s="20">
+        <v>2035</v>
+      </c>
+      <c r="C58" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="D57" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E57" s="21" t="s">
+      <c r="D58" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E58" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F57" s="21" t="s">
+      <c r="F58" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="G57" s="20" t="s">
+      <c r="G58" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="H57" s="21" t="s">
+      <c r="H58" s="21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B58" s="35">
-        <v>2035</v>
-      </c>
-      <c r="C58" s="36" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="35">
+        <v>2035</v>
+      </c>
+      <c r="C59" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="D58" s="36" t="s">
+      <c r="D59" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="E58" s="36" t="s">
+      <c r="E59" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="F58" s="36"/>
-      <c r="G58" s="35"/>
-      <c r="H58" s="36"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B59" s="32">
-        <v>2035</v>
-      </c>
-      <c r="C59" s="33" t="s">
+      <c r="F59" s="36"/>
+      <c r="G59" s="35"/>
+      <c r="H59" s="36"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B60" s="32">
+        <v>2035</v>
+      </c>
+      <c r="C60" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="D59" s="33" t="s">
+      <c r="D60" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="E59" s="33" t="s">
+      <c r="E60" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="F59" s="33"/>
-      <c r="G59" s="32"/>
-      <c r="H59" s="33"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B60" s="17">
-        <v>2035</v>
-      </c>
-      <c r="C60" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E60" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F60" s="18"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="18"/>
+      <c r="F60" s="33"/>
+      <c r="G60" s="32"/>
+      <c r="H60" s="33"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="16" t="s">
@@ -2708,7 +2735,7 @@
         <v>2035</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D61" s="18" t="s">
         <v>34</v>
@@ -2728,7 +2755,7 @@
         <v>2035</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D62" s="18" t="s">
         <v>34</v>
@@ -2736,12 +2763,8 @@
       <c r="E62" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="F62" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="G62" s="17" t="s">
-        <v>64</v>
-      </c>
+      <c r="F62" s="18"/>
+      <c r="G62" s="17"/>
       <c r="H62" s="18"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -2752,7 +2775,7 @@
         <v>2035</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D63" s="18" t="s">
         <v>34</v>
@@ -2761,10 +2784,10 @@
         <v>38</v>
       </c>
       <c r="F63" s="18" t="s">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="G63" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H63" s="18"/>
     </row>
@@ -2776,7 +2799,7 @@
         <v>2035</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D64" s="18" t="s">
         <v>34</v>
@@ -2785,10 +2808,10 @@
         <v>38</v>
       </c>
       <c r="F64" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G64" s="17" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H64" s="18"/>
     </row>
@@ -2800,7 +2823,7 @@
         <v>2035</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D65" s="18" t="s">
         <v>34</v>
@@ -2809,10 +2832,10 @@
         <v>38</v>
       </c>
       <c r="F65" s="18" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G65" s="17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H65" s="18"/>
     </row>
@@ -2824,7 +2847,7 @@
         <v>2035</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D66" s="18" t="s">
         <v>34</v>
@@ -2833,10 +2856,10 @@
         <v>38</v>
       </c>
       <c r="F66" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G66" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H66" s="18"/>
     </row>
@@ -2848,7 +2871,7 @@
         <v>2035</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="D67" s="18" t="s">
         <v>34</v>
@@ -2857,38 +2880,38 @@
         <v>38</v>
       </c>
       <c r="F67" s="18" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G67" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="H67" s="18" t="s">
-        <v>218</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="H67" s="18"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="B68" s="25">
-        <v>2035</v>
-      </c>
-      <c r="C68" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="D68" s="26" t="s">
+      <c r="A68" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" s="17">
+        <v>2035</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D68" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E68" s="26" t="s">
+      <c r="E68" s="18" t="s">
         <v>38</v>
       </c>
       <c r="F68" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="G68" s="25" t="s">
+      <c r="G68" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="H68" s="26"/>
+      <c r="H68" s="18" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="45" t="s">
@@ -2898,7 +2921,7 @@
         <v>2035</v>
       </c>
       <c r="C69" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D69" s="26" t="s">
         <v>34</v>
@@ -2915,28 +2938,28 @@
       <c r="H69" s="26"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B70" s="17">
-        <v>2035</v>
-      </c>
-      <c r="C70" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="D70" s="18" t="s">
+      <c r="A70" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B70" s="25">
+        <v>2035</v>
+      </c>
+      <c r="C70" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="D70" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="E70" s="18" t="s">
+      <c r="E70" s="26" t="s">
         <v>38</v>
       </c>
       <c r="F70" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="G70" s="17" t="s">
+      <c r="G70" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="H70" s="18"/>
+      <c r="H70" s="26"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="16" t="s">
@@ -2946,7 +2969,7 @@
         <v>2035</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D71" s="18" t="s">
         <v>34</v>
@@ -2970,7 +2993,7 @@
         <v>2035</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D72" s="18" t="s">
         <v>34</v>
@@ -2994,7 +3017,7 @@
         <v>2035</v>
       </c>
       <c r="C73" s="18" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D73" s="18" t="s">
         <v>34</v>
@@ -3011,52 +3034,52 @@
       <c r="H73" s="18"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B74" s="47">
-        <v>2035</v>
-      </c>
-      <c r="C74" s="48" t="s">
+      <c r="A74" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74" s="17">
+        <v>2035</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D74" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E74" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F74" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="G74" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="H74" s="18"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B75" s="47">
+        <v>2035</v>
+      </c>
+      <c r="C75" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="D74" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="E74" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="F74" s="48" t="s">
+      <c r="D75" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E75" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="F75" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="G74" s="47" t="s">
+      <c r="G75" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="H74" s="48"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B75" s="14">
-        <v>2035</v>
-      </c>
-      <c r="C75" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="D75" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E75" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F75" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="G75" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="H75" s="15"/>
+      <c r="H75" s="48"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="13" t="s">
@@ -3066,7 +3089,7 @@
         <v>2035</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D76" s="15" t="s">
         <v>91</v>
@@ -3090,7 +3113,7 @@
         <v>2035</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D77" s="15" t="s">
         <v>91</v>
@@ -3114,7 +3137,7 @@
         <v>2035</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D78" s="15" t="s">
         <v>91</v>
@@ -3138,7 +3161,7 @@
         <v>2035</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D79" s="15" t="s">
         <v>91</v>
@@ -3147,10 +3170,10 @@
         <v>38</v>
       </c>
       <c r="F79" s="15" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G79" s="14" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H79" s="15"/>
     </row>
@@ -3162,7 +3185,7 @@
         <v>2035</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D80" s="15" t="s">
         <v>91</v>
@@ -3171,10 +3194,10 @@
         <v>38</v>
       </c>
       <c r="F80" s="15" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="G80" s="14" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H80" s="15"/>
     </row>
@@ -3186,7 +3209,7 @@
         <v>2035</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D81" s="15" t="s">
         <v>91</v>
@@ -3195,10 +3218,10 @@
         <v>38</v>
       </c>
       <c r="F81" s="15" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G81" s="14" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H81" s="15"/>
     </row>
@@ -3210,7 +3233,7 @@
         <v>2035</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D82" s="15" t="s">
         <v>91</v>
@@ -3234,7 +3257,7 @@
         <v>2035</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D83" s="15" t="s">
         <v>91</v>
@@ -3243,10 +3266,10 @@
         <v>38</v>
       </c>
       <c r="F83" s="15" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G83" s="14" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H83" s="15"/>
     </row>
@@ -3258,7 +3281,7 @@
         <v>2035</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D84" s="15" t="s">
         <v>91</v>
@@ -3282,7 +3305,7 @@
         <v>2035</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D85" s="15" t="s">
         <v>91</v>
@@ -3306,7 +3329,7 @@
         <v>2035</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D86" s="15" t="s">
         <v>91</v>
@@ -3330,7 +3353,7 @@
         <v>2035</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D87" s="15" t="s">
         <v>91</v>
@@ -3354,7 +3377,7 @@
         <v>2035</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D88" s="15" t="s">
         <v>91</v>
@@ -3368,11 +3391,9 @@
       <c r="G88" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="H88" s="15" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H88" s="15"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="s">
         <v>26</v>
       </c>
@@ -3380,7 +3401,7 @@
         <v>2035</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="D89" s="15" t="s">
         <v>91</v>
@@ -3394,7 +3415,9 @@
       <c r="G89" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="H89" s="15"/>
+      <c r="H89" s="15" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="90" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="13" t="s">
@@ -3404,7 +3427,7 @@
         <v>2035</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="D90" s="15" t="s">
         <v>91</v>
@@ -3420,107 +3443,107 @@
       </c>
       <c r="H90" s="15"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B91" s="20">
-        <v>2035</v>
-      </c>
-      <c r="C91" s="21" t="s">
+    <row r="91" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B91" s="14">
+        <v>2035</v>
+      </c>
+      <c r="C91" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="D91" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E91" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F91" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G91" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H91" s="15"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B92" s="14">
+        <v>2035</v>
+      </c>
+      <c r="C92" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="D91" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E91" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="F91" s="21" t="s">
+      <c r="D92" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E92" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F92" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="G91" s="20" t="s">
+      <c r="G92" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="H91" s="21" t="s">
+      <c r="H92" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="57" t="s">
-        <v>26</v>
-      </c>
-      <c r="B92" s="58">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B93" s="20">
+        <v>2035</v>
+      </c>
+      <c r="C93" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="D93" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E93" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F93" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="G93" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="H93" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="B94" s="58">
         <v>2040</v>
       </c>
-      <c r="C92" s="59" t="s">
+      <c r="C94" s="59" t="s">
         <v>183</v>
       </c>
-      <c r="D92" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="E92" s="48" t="s">
+      <c r="D94" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="E94" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F92" s="15" t="s">
+      <c r="F94" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="G92" s="14" t="s">
+      <c r="G94" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="H92" s="15"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B93" s="14">
-        <v>2040</v>
-      </c>
-      <c r="C93" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="D93" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E93" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="F93" s="48" t="s">
-        <v>147</v>
-      </c>
-      <c r="G93" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="H93" s="48" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B94" s="14">
-        <v>2040</v>
-      </c>
-      <c r="C94" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="D94" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E94" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F94" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="G94" s="14" t="s">
-        <v>137</v>
-      </c>
       <c r="H94" s="15"/>
     </row>
-    <row r="95" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="13" t="s">
         <v>26</v>
       </c>
@@ -3528,21 +3551,23 @@
         <v>2040</v>
       </c>
       <c r="C95" s="15" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
       <c r="D95" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E95" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F95" s="15" t="s">
+      <c r="E95" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="F95" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="G95" s="14" t="s">
+      <c r="G95" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="H95" s="15"/>
+      <c r="H95" s="48" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="13" t="s">
@@ -3552,110 +3577,116 @@
         <v>2040</v>
       </c>
       <c r="C96" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="D96" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E96" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F96" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G96" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H96" s="15"/>
+    </row>
+    <row r="97" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B97" s="14">
+        <v>2040</v>
+      </c>
+      <c r="C97" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="D97" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E97" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F97" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G97" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H97" s="15"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B98" s="14">
+        <v>2040</v>
+      </c>
+      <c r="C98" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="D96" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E96" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="F96" s="21" t="s">
+      <c r="D98" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E98" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F98" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="G96" s="20" t="s">
+      <c r="G98" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="H96" s="21" t="s">
+      <c r="H98" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="B97" s="38">
-        <v>2050</v>
-      </c>
-      <c r="C97" s="39" t="s">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B99" s="20">
+        <v>2040</v>
+      </c>
+      <c r="C99" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="D99" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E99" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F99" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="G99" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="H99" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B100" s="38">
+        <v>2050</v>
+      </c>
+      <c r="C100" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="D97" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="E97" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="F97" s="41"/>
-      <c r="G97" s="40"/>
-      <c r="H97" s="41"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B98" s="40">
-        <v>2050</v>
-      </c>
-      <c r="C98" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="D98" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="E98" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="F98" s="41"/>
-      <c r="G98" s="40"/>
-      <c r="H98" s="41"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B99" s="40">
-        <v>2050</v>
-      </c>
-      <c r="C99" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="D99" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="E99" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="F99" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="G99" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="H99" s="41"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B100" s="40">
-        <v>2050</v>
-      </c>
-      <c r="C100" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="D100" s="41" t="s">
+      <c r="D100" s="39" t="s">
         <v>34</v>
       </c>
       <c r="E100" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F100" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="G100" s="40" t="s">
-        <v>65</v>
-      </c>
+      <c r="F100" s="41"/>
+      <c r="G100" s="40"/>
       <c r="H100" s="41"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
@@ -3666,7 +3697,7 @@
         <v>2050</v>
       </c>
       <c r="C101" s="41" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="D101" s="41" t="s">
         <v>34</v>
@@ -3674,12 +3705,8 @@
       <c r="E101" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F101" s="41" t="s">
-        <v>117</v>
-      </c>
-      <c r="G101" s="40" t="s">
-        <v>74</v>
-      </c>
+      <c r="F101" s="41"/>
+      <c r="G101" s="40"/>
       <c r="H101" s="41"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
@@ -3690,7 +3717,7 @@
         <v>2050</v>
       </c>
       <c r="C102" s="41" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="D102" s="41" t="s">
         <v>34</v>
@@ -3699,108 +3726,108 @@
         <v>7</v>
       </c>
       <c r="F102" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="G102" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="H102" s="41"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B103" s="40">
+        <v>2050</v>
+      </c>
+      <c r="C103" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D103" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="E103" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="F103" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="G103" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="H103" s="41"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B104" s="40">
+        <v>2050</v>
+      </c>
+      <c r="C104" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="D104" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="E104" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="F104" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="G104" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="H104" s="41"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B105" s="40">
+        <v>2050</v>
+      </c>
+      <c r="C105" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D105" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="E105" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="F105" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="G102" s="40" t="s">
+      <c r="G105" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="H102" s="41"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="B103" s="43">
-        <v>2050</v>
-      </c>
-      <c r="C103" s="44" t="s">
+      <c r="H105" s="41"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B106" s="43">
+        <v>2050</v>
+      </c>
+      <c r="C106" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="D103" s="44" t="s">
+      <c r="D106" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="E103" s="44" t="s">
+      <c r="E106" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="F103" s="44" t="s">
+      <c r="F106" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="G103" s="43" t="s">
+      <c r="G106" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="H103" s="44"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B104" s="14">
-        <v>2050</v>
-      </c>
-      <c r="C104" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="D104" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="E104" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F104" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="G104" s="50" t="s">
-        <v>75</v>
-      </c>
-      <c r="H104" s="15"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B105" s="14">
-        <v>2050</v>
-      </c>
-      <c r="C105" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="D105" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E105" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F105" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="G105" s="50" t="s">
-        <v>82</v>
-      </c>
-      <c r="H105" s="15"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B106" s="14">
-        <v>2050</v>
-      </c>
-      <c r="C106" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="D106" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E106" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F106" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="G106" s="50" t="s">
-        <v>122</v>
-      </c>
-      <c r="H106" s="15"/>
+      <c r="H106" s="44"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="13" t="s">
@@ -3810,19 +3837,19 @@
         <v>2050</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="D107" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D107" s="48" t="s">
         <v>91</v>
       </c>
       <c r="E107" s="15" t="s">
         <v>7</v>
       </c>
       <c r="F107" s="15" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="G107" s="50" t="s">
-        <v>137</v>
+        <v>75</v>
       </c>
       <c r="H107" s="15"/>
     </row>
@@ -3834,7 +3861,7 @@
         <v>2050</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>143</v>
+        <v>100</v>
       </c>
       <c r="D108" s="15" t="s">
         <v>91</v>
@@ -3843,10 +3870,10 @@
         <v>7</v>
       </c>
       <c r="F108" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="G108" s="14" t="s">
-        <v>137</v>
+        <v>116</v>
+      </c>
+      <c r="G108" s="50" t="s">
+        <v>82</v>
       </c>
       <c r="H108" s="15"/>
     </row>
@@ -3858,7 +3885,7 @@
         <v>2050</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="D109" s="15" t="s">
         <v>91</v>
@@ -3867,10 +3894,10 @@
         <v>7</v>
       </c>
       <c r="F109" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="G109" s="14" t="s">
-        <v>137</v>
+        <v>121</v>
+      </c>
+      <c r="G109" s="50" t="s">
+        <v>122</v>
       </c>
       <c r="H109" s="15"/>
     </row>
@@ -3882,7 +3909,7 @@
         <v>2050</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="D110" s="15" t="s">
         <v>91</v>
@@ -3891,9 +3918,9 @@
         <v>7</v>
       </c>
       <c r="F110" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="G110" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G110" s="50" t="s">
         <v>137</v>
       </c>
       <c r="H110" s="15"/>
@@ -3906,7 +3933,7 @@
         <v>2050</v>
       </c>
       <c r="C111" s="15" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="D111" s="15" t="s">
         <v>91</v>
@@ -3915,10 +3942,10 @@
         <v>7</v>
       </c>
       <c r="F111" s="15" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="G111" s="14" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="H111" s="15"/>
     </row>
@@ -3930,7 +3957,7 @@
         <v>2050</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="D112" s="15" t="s">
         <v>91</v>
@@ -3939,14 +3966,14 @@
         <v>7</v>
       </c>
       <c r="F112" s="15" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="G112" s="14" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
       <c r="H112" s="15"/>
     </row>
-    <row r="113" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="13" t="s">
         <v>26</v>
       </c>
@@ -3954,7 +3981,7 @@
         <v>2050</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="D113" s="15" t="s">
         <v>91</v>
@@ -3963,16 +3990,14 @@
         <v>7</v>
       </c>
       <c r="F113" s="15" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="G113" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="H113" s="15" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+      <c r="H113" s="15"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="13" t="s">
         <v>26</v>
       </c>
@@ -3980,7 +4005,7 @@
         <v>2050</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>217</v>
+        <v>159</v>
       </c>
       <c r="D114" s="15" t="s">
         <v>91</v>
@@ -3989,142 +4014,152 @@
         <v>7</v>
       </c>
       <c r="F114" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G114" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="H114" s="15"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B115" s="14">
+        <v>2050</v>
+      </c>
+      <c r="C115" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="D115" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E115" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F115" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="G114" s="14" t="s">
+      <c r="G115" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="H114" s="15"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A115" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B115" s="20">
-        <v>2050</v>
-      </c>
-      <c r="C115" s="21" t="s">
+      <c r="H115" s="15"/>
+    </row>
+    <row r="116" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B116" s="14">
+        <v>2050</v>
+      </c>
+      <c r="C116" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="D116" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E116" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F116" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="G116" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H116" s="15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B117" s="14">
+        <v>2050</v>
+      </c>
+      <c r="C117" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D117" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E117" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F117" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="G117" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H117" s="15"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B118" s="20">
+        <v>2050</v>
+      </c>
+      <c r="C118" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="D115" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E115" s="21" t="s">
+      <c r="D118" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E118" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F115" s="21" t="s">
+      <c r="F118" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="G115" s="20" t="s">
+      <c r="G118" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="H115" s="21" t="s">
+      <c r="H118" s="21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A116" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B116" s="40">
-        <v>2050</v>
-      </c>
-      <c r="C116" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="D116" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="E116" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="F116" s="41"/>
-      <c r="G116" s="40"/>
-      <c r="H116" s="41"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A117" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="B117" s="43">
-        <v>2050</v>
-      </c>
-      <c r="C117" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="D117" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="E117" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="F117" s="44"/>
-      <c r="G117" s="43"/>
-      <c r="H117" s="44"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A118" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B118" s="28">
-        <v>2050</v>
-      </c>
-      <c r="C118" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="D118" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="E118" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F118" s="29"/>
-      <c r="G118" s="28"/>
-      <c r="H118" s="29"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B119" s="28">
-        <v>2050</v>
-      </c>
-      <c r="C119" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D119" s="29" t="s">
+      <c r="B119" s="40">
+        <v>2050</v>
+      </c>
+      <c r="C119" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="D119" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="E119" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F119" s="29"/>
-      <c r="G119" s="28"/>
-      <c r="H119" s="29"/>
+      <c r="E119" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="F119" s="41"/>
+      <c r="G119" s="40"/>
+      <c r="H119" s="41"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A120" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B120" s="28">
-        <v>2050</v>
-      </c>
-      <c r="C120" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="D120" s="29" t="s">
+      <c r="A120" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B120" s="43">
+        <v>2050</v>
+      </c>
+      <c r="C120" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="D120" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="E120" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F120" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="G120" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="H120" s="29"/>
+      <c r="E120" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="F120" s="44"/>
+      <c r="G120" s="43"/>
+      <c r="H120" s="44"/>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="27" t="s">
@@ -4134,7 +4169,7 @@
         <v>2050</v>
       </c>
       <c r="C121" s="29" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D121" s="29" t="s">
         <v>34</v>
@@ -4142,12 +4177,8 @@
       <c r="E121" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="F121" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="G121" s="28" t="s">
-        <v>63</v>
-      </c>
+      <c r="F121" s="29"/>
+      <c r="G121" s="28"/>
       <c r="H121" s="29"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
@@ -4158,7 +4189,7 @@
         <v>2050</v>
       </c>
       <c r="C122" s="29" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="D122" s="29" t="s">
         <v>34</v>
@@ -4166,12 +4197,8 @@
       <c r="E122" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="F122" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="G122" s="28" t="s">
-        <v>65</v>
-      </c>
+      <c r="F122" s="29"/>
+      <c r="G122" s="28"/>
       <c r="H122" s="29"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
@@ -4182,7 +4209,7 @@
         <v>2050</v>
       </c>
       <c r="C123" s="29" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D123" s="29" t="s">
         <v>34</v>
@@ -4191,10 +4218,10 @@
         <v>38</v>
       </c>
       <c r="F123" s="29" t="s">
-        <v>120</v>
+        <v>66</v>
       </c>
       <c r="G123" s="28" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H123" s="29"/>
     </row>
@@ -4206,7 +4233,7 @@
         <v>2050</v>
       </c>
       <c r="C124" s="29" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="D124" s="29" t="s">
         <v>34</v>
@@ -4215,10 +4242,10 @@
         <v>38</v>
       </c>
       <c r="F124" s="29" t="s">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="G124" s="28" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="H124" s="29"/>
     </row>
@@ -4230,7 +4257,7 @@
         <v>2050</v>
       </c>
       <c r="C125" s="29" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="D125" s="29" t="s">
         <v>34</v>
@@ -4239,10 +4266,10 @@
         <v>38</v>
       </c>
       <c r="F125" s="29" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G125" s="28" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="H125" s="29"/>
     </row>
@@ -4254,7 +4281,7 @@
         <v>2050</v>
       </c>
       <c r="C126" s="29" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="D126" s="29" t="s">
         <v>34</v>
@@ -4263,110 +4290,110 @@
         <v>38</v>
       </c>
       <c r="F126" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="G126" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H126" s="29"/>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A127" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B127" s="28">
+        <v>2050</v>
+      </c>
+      <c r="C127" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D127" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E127" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="F127" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="G127" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="H127" s="29"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A128" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B128" s="28">
+        <v>2050</v>
+      </c>
+      <c r="C128" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D128" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E128" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="F128" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="G128" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="H128" s="29"/>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A129" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B129" s="28">
+        <v>2050</v>
+      </c>
+      <c r="C129" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D129" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E129" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="F129" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="G126" s="28" t="s">
+      <c r="G129" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="H126" s="29" t="s">
+      <c r="H129" s="29" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A127" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B127" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C127" s="48" t="s">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A130" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B130" s="47">
+        <v>2050</v>
+      </c>
+      <c r="C130" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="D127" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="E127" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="F127" s="48" t="s">
+      <c r="D130" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E130" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="F130" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="G127" s="47" t="s">
+      <c r="G130" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="H127" s="48"/>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A128" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B128" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C128" s="49" t="s">
-        <v>101</v>
-      </c>
-      <c r="D128" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E128" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F128" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="G128" s="50" t="s">
-        <v>82</v>
-      </c>
-      <c r="H128" s="49"/>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A129" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B129" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C129" s="49" t="s">
-        <v>102</v>
-      </c>
-      <c r="D129" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E129" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F129" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="G129" s="50" t="s">
-        <v>82</v>
-      </c>
-      <c r="H129" s="49"/>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A130" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B130" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C130" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="D130" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E130" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F130" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="G130" s="50" t="s">
-        <v>82</v>
-      </c>
-      <c r="H130" s="49"/>
+      <c r="H130" s="48"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="49" t="s">
@@ -4376,7 +4403,7 @@
         <v>2050</v>
       </c>
       <c r="C131" s="49" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D131" s="49" t="s">
         <v>91</v>
@@ -4400,7 +4427,7 @@
         <v>2050</v>
       </c>
       <c r="C132" s="49" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D132" s="49" t="s">
         <v>91</v>
@@ -4424,7 +4451,7 @@
         <v>2050</v>
       </c>
       <c r="C133" s="49" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D133" s="49" t="s">
         <v>91</v>
@@ -4432,11 +4459,11 @@
       <c r="E133" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="F133" s="15" t="s">
-        <v>118</v>
+      <c r="F133" s="49" t="s">
+        <v>116</v>
       </c>
       <c r="G133" s="50" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H133" s="49"/>
     </row>
@@ -4448,7 +4475,7 @@
         <v>2050</v>
       </c>
       <c r="C134" s="49" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D134" s="49" t="s">
         <v>91</v>
@@ -4472,7 +4499,7 @@
         <v>2050</v>
       </c>
       <c r="C135" s="49" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D135" s="49" t="s">
         <v>91</v>
@@ -4496,7 +4523,7 @@
         <v>2050</v>
       </c>
       <c r="C136" s="49" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D136" s="49" t="s">
         <v>91</v>
@@ -4504,11 +4531,11 @@
       <c r="E136" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="F136" s="49" t="s">
-        <v>116</v>
+      <c r="F136" s="15" t="s">
+        <v>118</v>
       </c>
       <c r="G136" s="50" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H136" s="49"/>
     </row>
@@ -4520,7 +4547,7 @@
         <v>2050</v>
       </c>
       <c r="C137" s="49" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="D137" s="49" t="s">
         <v>91</v>
@@ -4529,10 +4556,10 @@
         <v>38</v>
       </c>
       <c r="F137" s="49" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G137" s="50" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="H137" s="49"/>
     </row>
@@ -4544,7 +4571,7 @@
         <v>2050</v>
       </c>
       <c r="C138" s="49" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="D138" s="49" t="s">
         <v>91</v>
@@ -4552,13 +4579,13 @@
       <c r="E138" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="F138" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="G138" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="H138" s="15"/>
+      <c r="F138" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="G138" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="H138" s="49"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="49" t="s">
@@ -4568,7 +4595,7 @@
         <v>2050</v>
       </c>
       <c r="C139" s="49" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="D139" s="49" t="s">
         <v>91</v>
@@ -4576,13 +4603,13 @@
       <c r="E139" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="F139" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="G139" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="H139" s="15"/>
+      <c r="F139" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="G139" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="H139" s="49"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" s="49" t="s">
@@ -4592,7 +4619,7 @@
         <v>2050</v>
       </c>
       <c r="C140" s="49" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="D140" s="49" t="s">
         <v>91</v>
@@ -4600,13 +4627,13 @@
       <c r="E140" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="F140" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="G140" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="H140" s="15"/>
+      <c r="F140" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="G140" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="H140" s="49"/>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" s="49" t="s">
@@ -4616,7 +4643,7 @@
         <v>2050</v>
       </c>
       <c r="C141" s="49" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="D141" s="49" t="s">
         <v>91</v>
@@ -4625,10 +4652,10 @@
         <v>38</v>
       </c>
       <c r="F141" s="15" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="G141" s="14" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="H141" s="15"/>
     </row>
@@ -4640,7 +4667,7 @@
         <v>2050</v>
       </c>
       <c r="C142" s="49" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="D142" s="49" t="s">
         <v>91</v>
@@ -4649,10 +4676,10 @@
         <v>38</v>
       </c>
       <c r="F142" s="15" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G142" s="14" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H142" s="15"/>
     </row>
@@ -4664,7 +4691,7 @@
         <v>2050</v>
       </c>
       <c r="C143" s="49" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D143" s="49" t="s">
         <v>91</v>
@@ -4688,7 +4715,7 @@
         <v>2050</v>
       </c>
       <c r="C144" s="49" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D144" s="49" t="s">
         <v>91</v>
@@ -4712,7 +4739,7 @@
         <v>2050</v>
       </c>
       <c r="C145" s="49" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="D145" s="49" t="s">
         <v>91</v>
@@ -4736,7 +4763,7 @@
         <v>2050</v>
       </c>
       <c r="C146" s="49" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="D146" s="49" t="s">
         <v>91</v>
@@ -4753,19 +4780,19 @@
       <c r="H146" s="15"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A147" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B147" s="63">
-        <v>2050</v>
-      </c>
-      <c r="C147" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="D147" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="E147" s="13" t="s">
+      <c r="A147" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B147" s="50">
+        <v>2050</v>
+      </c>
+      <c r="C147" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="D147" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E147" s="49" t="s">
         <v>38</v>
       </c>
       <c r="F147" s="15" t="s">
@@ -4774,24 +4801,22 @@
       <c r="G147" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="H147" s="15" t="s">
-        <v>220</v>
-      </c>
+      <c r="H147" s="15"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A148" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B148" s="63">
-        <v>2050</v>
-      </c>
-      <c r="C148" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="D148" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="E148" s="13" t="s">
+      <c r="A148" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B148" s="50">
+        <v>2050</v>
+      </c>
+      <c r="C148" s="49" t="s">
+        <v>164</v>
+      </c>
+      <c r="D148" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E148" s="49" t="s">
         <v>38</v>
       </c>
       <c r="F148" s="15" t="s">
@@ -4803,164 +4828,164 @@
       <c r="H148" s="15"/>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A149" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B149" s="64">
-        <v>2050</v>
-      </c>
-      <c r="C149" s="19" t="s">
+      <c r="A149" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B149" s="50">
+        <v>2050</v>
+      </c>
+      <c r="C149" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="D149" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E149" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="F149" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G149" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H149" s="15"/>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A150" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B150" s="63">
+        <v>2050</v>
+      </c>
+      <c r="C150" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="D150" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E150" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F150" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G150" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H150" s="15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A151" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B151" s="63">
+        <v>2050</v>
+      </c>
+      <c r="C151" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="D151" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E151" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F151" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G151" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H151" s="15"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A152" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B152" s="63">
+        <v>2050</v>
+      </c>
+      <c r="C152" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="D149" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E149" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F149" s="21" t="s">
+      <c r="D152" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E152" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F152" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="G149" s="20" t="s">
+      <c r="G152" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="H149" s="21" t="s">
+      <c r="H152" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A150" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B150" s="60">
-        <v>2035</v>
-      </c>
-      <c r="C150" s="9" t="s">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A153" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B153" s="64">
+        <v>2050</v>
+      </c>
+      <c r="C153" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="D153" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E153" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F153" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="G153" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="H153" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A154" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B154" s="60">
+        <v>2035</v>
+      </c>
+      <c r="C154" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="D150" s="9" t="s">
+      <c r="D154" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="E150" s="9" t="s">
+      <c r="E154" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="F150" s="9" t="s">
+      <c r="F154" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="G150" s="60" t="s">
+      <c r="G154" s="60" t="s">
         <v>185</v>
       </c>
-      <c r="H150" s="9"/>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A151" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B151" s="60">
-        <v>2035</v>
-      </c>
-      <c r="C151" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="D151" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="E151" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="F151" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="G151" s="60" t="s">
-        <v>190</v>
-      </c>
-      <c r="H151" s="9"/>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A152" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B152" s="60">
-        <v>2035</v>
-      </c>
-      <c r="C152" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="D152" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="E152" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="F152" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="G152" s="60" t="s">
-        <v>197</v>
-      </c>
-      <c r="H152" s="9" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A153" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="B153" s="62">
-        <v>2035</v>
-      </c>
-      <c r="C153" s="61" t="s">
-        <v>214</v>
-      </c>
-      <c r="D153" s="61" t="s">
-        <v>181</v>
-      </c>
-      <c r="E153" s="61" t="s">
-        <v>182</v>
-      </c>
-      <c r="F153" s="61" t="s">
-        <v>200</v>
-      </c>
-      <c r="G153" s="62" t="s">
-        <v>197</v>
-      </c>
-      <c r="H153" s="61" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A154" s="65" t="s">
-        <v>26</v>
-      </c>
-      <c r="B154" s="66">
-        <v>2050</v>
-      </c>
-      <c r="C154" s="65" t="s">
-        <v>180</v>
-      </c>
-      <c r="D154" s="65" t="s">
-        <v>181</v>
-      </c>
-      <c r="E154" s="65" t="s">
-        <v>182</v>
-      </c>
-      <c r="F154" s="65" t="s">
-        <v>184</v>
-      </c>
-      <c r="G154" s="66" t="s">
-        <v>185</v>
-      </c>
-      <c r="H154" s="65"/>
+      <c r="H154" s="9"/>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B155" s="60">
-        <v>2050</v>
+        <v>2035</v>
       </c>
       <c r="C155" s="9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D155" s="9" t="s">
         <v>181</v>
@@ -4976,15 +5001,15 @@
       </c>
       <c r="H155" s="9"/>
     </row>
-    <row r="156" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B156" s="60">
-        <v>2050</v>
+        <v>2035</v>
       </c>
       <c r="C156" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D156" s="9" t="s">
         <v>181</v>
@@ -5002,205 +5027,383 @@
         <v>220</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="B157" s="62">
-        <v>2050</v>
-      </c>
-      <c r="C157" s="61" t="s">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A157" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B157" s="60">
+        <v>2035</v>
+      </c>
+      <c r="C157" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="D157" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E157" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F157" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="G157" s="60" t="s">
+        <v>197</v>
+      </c>
+      <c r="H157" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A158" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B158" s="62">
+        <v>2035</v>
+      </c>
+      <c r="C158" s="61" t="s">
+        <v>233</v>
+      </c>
+      <c r="D158" s="61" t="s">
+        <v>181</v>
+      </c>
+      <c r="E158" s="61" t="s">
+        <v>182</v>
+      </c>
+      <c r="F158" s="61" t="s">
+        <v>200</v>
+      </c>
+      <c r="G158" s="62" t="s">
+        <v>197</v>
+      </c>
+      <c r="H158" s="61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A159" s="65" t="s">
+        <v>26</v>
+      </c>
+      <c r="B159" s="66">
+        <v>2050</v>
+      </c>
+      <c r="C159" s="65" t="s">
+        <v>180</v>
+      </c>
+      <c r="D159" s="65" t="s">
+        <v>181</v>
+      </c>
+      <c r="E159" s="65" t="s">
+        <v>182</v>
+      </c>
+      <c r="F159" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="G159" s="66" t="s">
+        <v>185</v>
+      </c>
+      <c r="H159" s="65"/>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A160" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B160" s="60">
+        <v>2050</v>
+      </c>
+      <c r="C160" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D160" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E160" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F160" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="G160" s="60" t="s">
+        <v>190</v>
+      </c>
+      <c r="H160" s="9"/>
+    </row>
+    <row r="161" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B161" s="60">
+        <v>2050</v>
+      </c>
+      <c r="C161" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="D161" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E161" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F161" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="G161" s="60" t="s">
+        <v>197</v>
+      </c>
+      <c r="H161" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B162" s="60">
+        <v>2050</v>
+      </c>
+      <c r="C162" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="D157" s="61" t="s">
+      <c r="D162" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="E157" s="61" t="s">
+      <c r="E162" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="F157" s="61" t="s">
+      <c r="F162" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="G157" s="62" t="s">
+      <c r="G162" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="H157" s="61" t="s">
+      <c r="H162" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="158" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A158" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="B158" s="68">
-        <v>2035</v>
-      </c>
-      <c r="C158" s="67" t="s">
+    <row r="163" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B163" s="62">
+        <v>2050</v>
+      </c>
+      <c r="C163" s="61" t="s">
+        <v>234</v>
+      </c>
+      <c r="D163" s="61" t="s">
+        <v>181</v>
+      </c>
+      <c r="E163" s="61" t="s">
+        <v>182</v>
+      </c>
+      <c r="F163" s="61" t="s">
+        <v>200</v>
+      </c>
+      <c r="G163" s="62" t="s">
+        <v>197</v>
+      </c>
+      <c r="H163" s="61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="B164" s="68">
+        <v>2035</v>
+      </c>
+      <c r="C164" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="D158" s="67" t="s">
+      <c r="D164" s="67" t="s">
         <v>181</v>
       </c>
-      <c r="E158" s="67" t="s">
+      <c r="E164" s="67" t="s">
         <v>193</v>
       </c>
-      <c r="F158" s="67" t="s">
+      <c r="F164" s="67" t="s">
         <v>194</v>
       </c>
-      <c r="G158" s="68" t="s">
+      <c r="G164" s="68" t="s">
         <v>195</v>
       </c>
-      <c r="H158" s="67"/>
-    </row>
-    <row r="159" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B159" s="69">
-        <v>2035</v>
-      </c>
-      <c r="C159" s="6" t="s">
+      <c r="H164" s="67"/>
+    </row>
+    <row r="165" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B165" s="69">
+        <v>2035</v>
+      </c>
+      <c r="C165" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="D159" s="6" t="s">
+      <c r="D165" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="E159" s="6" t="s">
+      <c r="E165" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="F159" s="6" t="s">
+      <c r="F165" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="G159" s="69" t="s">
+      <c r="G165" s="69" t="s">
         <v>195</v>
       </c>
-      <c r="H159" s="6" t="s">
+      <c r="H165" s="6" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="160" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A160" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="B160" s="71">
-        <v>2035</v>
-      </c>
-      <c r="C160" s="70" t="s">
+    <row r="166" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B166" s="56">
+        <v>2035</v>
+      </c>
+      <c r="C166" s="55" t="s">
+        <v>203</v>
+      </c>
+      <c r="D166" s="55" t="s">
+        <v>181</v>
+      </c>
+      <c r="E166" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="F166" s="55" t="s">
+        <v>194</v>
+      </c>
+      <c r="G166" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="H166" s="55"/>
+    </row>
+    <row r="167" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="B167" s="71">
+        <v>2035</v>
+      </c>
+      <c r="C167" s="70" t="s">
         <v>225</v>
       </c>
-      <c r="D160" s="70" t="s">
+      <c r="D167" s="70" t="s">
         <v>181</v>
       </c>
-      <c r="E160" s="70" t="s">
+      <c r="E167" s="70" t="s">
         <v>193</v>
       </c>
-      <c r="F160" s="70" t="s">
+      <c r="F167" s="70" t="s">
         <v>194</v>
       </c>
-      <c r="G160" s="71" t="s">
+      <c r="G167" s="71" t="s">
         <v>195</v>
       </c>
-      <c r="H160" s="70" t="s">
+      <c r="H167" s="70" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="161" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B161" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C161" s="55" t="s">
+    <row r="168" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B168" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C168" s="55" t="s">
         <v>196</v>
       </c>
-      <c r="D161" s="55" t="s">
+      <c r="D168" s="55" t="s">
         <v>181</v>
       </c>
-      <c r="E161" s="55" t="s">
+      <c r="E168" s="55" t="s">
         <v>193</v>
       </c>
-      <c r="F161" s="55" t="s">
+      <c r="F168" s="55" t="s">
         <v>194</v>
       </c>
-      <c r="G161" s="56" t="s">
+      <c r="G168" s="56" t="s">
         <v>195</v>
       </c>
-      <c r="H161" s="55"/>
-    </row>
-    <row r="162" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B162" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C162" s="55" t="s">
+      <c r="H168" s="55"/>
+    </row>
+    <row r="169" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B169" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C169" s="55" t="s">
         <v>202</v>
       </c>
-      <c r="D162" s="55" t="s">
+      <c r="D169" s="55" t="s">
         <v>181</v>
       </c>
-      <c r="E162" s="55" t="s">
+      <c r="E169" s="55" t="s">
         <v>193</v>
       </c>
-      <c r="F162" s="55" t="s">
+      <c r="F169" s="55" t="s">
         <v>194</v>
       </c>
-      <c r="G162" s="56" t="s">
+      <c r="G169" s="56" t="s">
         <v>195</v>
       </c>
-      <c r="H162" s="55" t="s">
+      <c r="H169" s="55" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="163" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B163" s="56">
-        <v>2035</v>
-      </c>
-      <c r="C163" s="55" t="s">
-        <v>203</v>
-      </c>
-      <c r="D163" s="55" t="s">
+    <row r="170" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B170" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C170" s="55" t="s">
+        <v>226</v>
+      </c>
+      <c r="D170" s="55" t="s">
         <v>181</v>
       </c>
-      <c r="E163" s="55" t="s">
+      <c r="E170" s="55" t="s">
         <v>193</v>
       </c>
-      <c r="F163" s="55" t="s">
+      <c r="F170" s="55" t="s">
         <v>194</v>
       </c>
-      <c r="G163" s="56" t="s">
+      <c r="G170" s="56" t="s">
         <v>195</v>
       </c>
-      <c r="H163" s="55"/>
-    </row>
-    <row r="164" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A164" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B164" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C164" s="55" t="s">
-        <v>226</v>
-      </c>
-      <c r="D164" s="55" t="s">
+      <c r="H170" s="55" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A171" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B171" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C171" s="55" t="s">
+        <v>235</v>
+      </c>
+      <c r="D171" s="55" t="s">
         <v>181</v>
       </c>
-      <c r="E164" s="55" t="s">
+      <c r="E171" s="55" t="s">
         <v>193</v>
       </c>
-      <c r="F164" s="55" t="s">
+      <c r="F171" s="55" t="s">
         <v>194</v>
       </c>
-      <c r="G164" s="56" t="s">
+      <c r="G171" s="56" t="s">
         <v>195</v>
       </c>
-      <c r="H164" s="55" t="s">
+      <c r="H171" s="55" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Demoting 6 runs that are no longer current
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5C50C7-C915-4B6F-8F39-C5A3FE7F8DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF66123F-5DB6-420A-BCC3-C58B231BF180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19575" yWindow="1770" windowWidth="17400" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14580" yWindow="1935" windowWidth="22155" windowHeight="17670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="236">
   <si>
     <t>EEJ</t>
   </si>
@@ -1363,7 +1363,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A170" sqref="A170"/>
+      <selection pane="bottomLeft" activeCell="H170" sqref="H170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2125,9 +2125,7 @@
       <c r="G34" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="H34" s="18" t="s">
-        <v>43</v>
-      </c>
+      <c r="H34" s="18"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="31" t="s">
@@ -3489,9 +3487,7 @@
       <c r="G92" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="H92" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="H92" s="15"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="19" t="s">
@@ -3639,9 +3635,7 @@
       <c r="G98" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="H98" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="H98" s="15"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="19" t="s">
@@ -4923,9 +4917,7 @@
       <c r="G152" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="H152" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="H152" s="15"/>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" s="19" t="s">
@@ -5049,9 +5041,7 @@
       <c r="G157" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="H157" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="H157" s="9"/>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" s="61" t="s">
@@ -5175,9 +5165,7 @@
       <c r="G162" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="H162" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="H162" s="9"/>
     </row>
     <row r="163" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="61" t="s">

</xml_diff>

<commit_message>
Demoting one more run from current
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF66123F-5DB6-420A-BCC3-C58B231BF180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5500DB6-D0D2-4D57-8788-38989E911FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14580" yWindow="1935" windowWidth="22155" windowHeight="17670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="236">
   <si>
     <t>EEJ</t>
   </si>
@@ -1363,7 +1363,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H170" sqref="H170"/>
+      <selection pane="bottomLeft" activeCell="F173" sqref="F173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5365,9 +5365,7 @@
       <c r="G170" s="56" t="s">
         <v>195</v>
       </c>
-      <c r="H170" s="55" t="s">
-        <v>43</v>
-      </c>
+      <c r="H170" s="55"/>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" s="55" t="s">

</xml_diff>

<commit_message>
Added Alt1 run updates
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0D41E6-7520-4DEE-AC37-B1343F79EFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96D6C41-06FF-4358-A864-95CB8F90AEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="375" windowWidth="29115" windowHeight="16530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="2790" windowWidth="30270" windowHeight="16845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$H$173</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$H$175</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="241">
   <si>
     <t>EEJ</t>
   </si>
@@ -745,6 +745,12 @@
   </si>
   <si>
     <t>2030_TM152_FBP_NoProject_22</t>
+  </si>
+  <si>
+    <t>2035_TM152_EIR_Alt1_06</t>
+  </si>
+  <si>
+    <t>2050_TM152_EIR_Alt1_06</t>
   </si>
 </sst>
 </file>
@@ -1352,11 +1358,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H174"/>
+  <dimension ref="A1:H176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5121,88 +5127,90 @@
       <c r="H160" s="9"/>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A161" s="58" t="s">
-        <v>26</v>
-      </c>
-      <c r="B161" s="59">
-        <v>2035</v>
-      </c>
-      <c r="C161" s="58" t="s">
+      <c r="A161" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B161" s="57">
+        <v>2035</v>
+      </c>
+      <c r="C161" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="D161" s="58" t="s">
+      <c r="D161" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="E161" s="58" t="s">
+      <c r="E161" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="F161" s="58" t="s">
+      <c r="F161" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="G161" s="59" t="s">
+      <c r="G161" s="57" t="s">
         <v>197</v>
       </c>
-      <c r="H161" s="58" t="s">
+      <c r="H161" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A162" s="62" t="s">
-        <v>26</v>
-      </c>
-      <c r="B162" s="63">
-        <v>2050</v>
-      </c>
-      <c r="C162" s="62" t="s">
+      <c r="A162" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="B162" s="59">
+        <v>2035</v>
+      </c>
+      <c r="C162" s="58" t="s">
+        <v>239</v>
+      </c>
+      <c r="D162" s="58" t="s">
+        <v>181</v>
+      </c>
+      <c r="E162" s="58" t="s">
+        <v>182</v>
+      </c>
+      <c r="F162" s="58" t="s">
+        <v>200</v>
+      </c>
+      <c r="G162" s="59" t="s">
+        <v>197</v>
+      </c>
+      <c r="H162" s="58" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A163" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="B163" s="63">
+        <v>2050</v>
+      </c>
+      <c r="C163" s="62" t="s">
         <v>180</v>
       </c>
-      <c r="D162" s="62" t="s">
+      <c r="D163" s="62" t="s">
         <v>181</v>
       </c>
-      <c r="E162" s="62" t="s">
+      <c r="E163" s="62" t="s">
         <v>182</v>
       </c>
-      <c r="F162" s="62" t="s">
+      <c r="F163" s="62" t="s">
         <v>184</v>
       </c>
-      <c r="G162" s="63" t="s">
+      <c r="G163" s="63" t="s">
         <v>185</v>
       </c>
-      <c r="H162" s="62"/>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A163" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B163" s="57">
-        <v>2050</v>
-      </c>
-      <c r="C163" s="9" t="s">
+      <c r="H163" s="62"/>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A164" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B164" s="57">
+        <v>2050</v>
+      </c>
+      <c r="C164" s="9" t="s">
         <v>191</v>
-      </c>
-      <c r="D163" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="E163" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="F163" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="G163" s="57" t="s">
-        <v>190</v>
-      </c>
-      <c r="H163" s="9"/>
-    </row>
-    <row r="164" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A164" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B164" s="57">
-        <v>2050</v>
-      </c>
-      <c r="C164" s="9" t="s">
-        <v>199</v>
       </c>
       <c r="D164" s="9" t="s">
         <v>181</v>
@@ -5211,14 +5219,12 @@
         <v>182</v>
       </c>
       <c r="F164" s="9" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="G164" s="57" t="s">
-        <v>197</v>
-      </c>
-      <c r="H164" s="9" t="s">
-        <v>220</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="H164" s="9"/>
     </row>
     <row r="165" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="9" t="s">
@@ -5228,7 +5234,7 @@
         <v>2050</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="D165" s="9" t="s">
         <v>181</v>
@@ -5242,143 +5248,145 @@
       <c r="G165" s="57" t="s">
         <v>197</v>
       </c>
-      <c r="H165" s="9"/>
+      <c r="H165" s="9" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="166" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A166" s="58" t="s">
-        <v>26</v>
-      </c>
-      <c r="B166" s="59">
-        <v>2050</v>
-      </c>
-      <c r="C166" s="58" t="s">
+      <c r="A166" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B166" s="57">
+        <v>2050</v>
+      </c>
+      <c r="C166" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D166" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E166" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F166" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="G166" s="57" t="s">
+        <v>197</v>
+      </c>
+      <c r="H166" s="9"/>
+    </row>
+    <row r="167" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B167" s="57">
+        <v>2050</v>
+      </c>
+      <c r="C167" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="D166" s="58" t="s">
+      <c r="D167" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="E166" s="58" t="s">
+      <c r="E167" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="F166" s="58" t="s">
+      <c r="F167" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="G166" s="59" t="s">
+      <c r="G167" s="57" t="s">
         <v>197</v>
       </c>
-      <c r="H166" s="58" t="s">
+      <c r="H167" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="167" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="B167" s="65">
-        <v>2035</v>
-      </c>
-      <c r="C167" s="64" t="s">
+    <row r="168" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="B168" s="59">
+        <v>2050</v>
+      </c>
+      <c r="C168" s="58" t="s">
+        <v>240</v>
+      </c>
+      <c r="D168" s="58" t="s">
+        <v>181</v>
+      </c>
+      <c r="E168" s="58" t="s">
+        <v>182</v>
+      </c>
+      <c r="F168" s="58" t="s">
+        <v>200</v>
+      </c>
+      <c r="G168" s="59" t="s">
+        <v>197</v>
+      </c>
+      <c r="H168" s="58" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="B169" s="65">
+        <v>2035</v>
+      </c>
+      <c r="C169" s="64" t="s">
         <v>192</v>
       </c>
-      <c r="D167" s="64" t="s">
+      <c r="D169" s="64" t="s">
         <v>181</v>
       </c>
-      <c r="E167" s="64" t="s">
+      <c r="E169" s="64" t="s">
         <v>193</v>
       </c>
-      <c r="F167" s="64" t="s">
+      <c r="F169" s="64" t="s">
         <v>194</v>
       </c>
-      <c r="G167" s="65" t="s">
+      <c r="G169" s="65" t="s">
         <v>195</v>
       </c>
-      <c r="H167" s="64"/>
-    </row>
-    <row r="168" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B168" s="66">
-        <v>2035</v>
-      </c>
-      <c r="C168" s="6" t="s">
+      <c r="H169" s="64"/>
+    </row>
+    <row r="170" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B170" s="66">
+        <v>2035</v>
+      </c>
+      <c r="C170" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="D168" s="6" t="s">
+      <c r="D170" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="E168" s="6" t="s">
+      <c r="E170" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="F168" s="6" t="s">
+      <c r="F170" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="G168" s="66" t="s">
+      <c r="G170" s="66" t="s">
         <v>195</v>
       </c>
-      <c r="H168" s="6" t="s">
+      <c r="H170" s="6" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="169" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A169" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B169" s="56">
-        <v>2035</v>
-      </c>
-      <c r="C169" s="55" t="s">
+    <row r="171" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B171" s="56">
+        <v>2035</v>
+      </c>
+      <c r="C171" s="55" t="s">
         <v>203</v>
-      </c>
-      <c r="D169" s="55" t="s">
-        <v>181</v>
-      </c>
-      <c r="E169" s="55" t="s">
-        <v>193</v>
-      </c>
-      <c r="F169" s="55" t="s">
-        <v>194</v>
-      </c>
-      <c r="G169" s="56" t="s">
-        <v>195</v>
-      </c>
-      <c r="H169" s="55"/>
-    </row>
-    <row r="170" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="B170" s="68">
-        <v>2035</v>
-      </c>
-      <c r="C170" s="67" t="s">
-        <v>225</v>
-      </c>
-      <c r="D170" s="67" t="s">
-        <v>181</v>
-      </c>
-      <c r="E170" s="67" t="s">
-        <v>193</v>
-      </c>
-      <c r="F170" s="67" t="s">
-        <v>194</v>
-      </c>
-      <c r="G170" s="68" t="s">
-        <v>195</v>
-      </c>
-      <c r="H170" s="67" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B171" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C171" s="55" t="s">
-        <v>196</v>
       </c>
       <c r="D171" s="55" t="s">
         <v>181</v>
@@ -5394,33 +5402,33 @@
       </c>
       <c r="H171" s="55"/>
     </row>
-    <row r="172" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B172" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C172" s="55" t="s">
-        <v>202</v>
-      </c>
-      <c r="D172" s="55" t="s">
+    <row r="172" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="B172" s="68">
+        <v>2035</v>
+      </c>
+      <c r="C172" s="67" t="s">
+        <v>225</v>
+      </c>
+      <c r="D172" s="67" t="s">
         <v>181</v>
       </c>
-      <c r="E172" s="55" t="s">
+      <c r="E172" s="67" t="s">
         <v>193</v>
       </c>
-      <c r="F172" s="55" t="s">
+      <c r="F172" s="67" t="s">
         <v>194</v>
       </c>
-      <c r="G172" s="56" t="s">
+      <c r="G172" s="68" t="s">
         <v>195</v>
       </c>
-      <c r="H172" s="55" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H172" s="67" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="55" t="s">
         <v>26</v>
       </c>
@@ -5428,7 +5436,7 @@
         <v>2050</v>
       </c>
       <c r="C173" s="55" t="s">
-        <v>226</v>
+        <v>196</v>
       </c>
       <c r="D173" s="55" t="s">
         <v>181</v>
@@ -5444,7 +5452,7 @@
       </c>
       <c r="H173" s="55"/>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="55" t="s">
         <v>26</v>
       </c>
@@ -5452,7 +5460,7 @@
         <v>2050</v>
       </c>
       <c r="C174" s="55" t="s">
-        <v>235</v>
+        <v>202</v>
       </c>
       <c r="D174" s="55" t="s">
         <v>181</v>
@@ -5467,6 +5475,56 @@
         <v>195</v>
       </c>
       <c r="H174" s="55" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B175" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C175" s="55" t="s">
+        <v>226</v>
+      </c>
+      <c r="D175" s="55" t="s">
+        <v>181</v>
+      </c>
+      <c r="E175" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="F175" s="55" t="s">
+        <v>194</v>
+      </c>
+      <c r="G175" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="H175" s="55"/>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A176" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B176" s="56">
+        <v>2050</v>
+      </c>
+      <c r="C176" s="55" t="s">
+        <v>235</v>
+      </c>
+      <c r="D176" s="55" t="s">
+        <v>181</v>
+      </c>
+      <c r="E176" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="F176" s="55" t="s">
+        <v>194</v>
+      </c>
+      <c r="G176" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="H176" s="55" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Demoting v5 versions of Alt1 runs from current
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96D6C41-06FF-4358-A864-95CB8F90AEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D698E5-532E-43F4-B509-1BAEE29E0D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="2790" windowWidth="30270" windowHeight="16845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="241">
   <si>
     <t>EEJ</t>
   </si>
@@ -1362,7 +1362,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A168" sqref="A168"/>
+      <selection pane="bottomLeft" activeCell="G167" sqref="G167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5148,9 +5148,7 @@
       <c r="G161" s="57" t="s">
         <v>197</v>
       </c>
-      <c r="H161" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="H161" s="9"/>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" s="58" t="s">
@@ -5298,9 +5296,7 @@
       <c r="G167" s="57" t="s">
         <v>197</v>
       </c>
-      <c r="H167" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="H167" s="9"/>
     </row>
     <row r="168" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="58" t="s">

</xml_diff>

<commit_message>
Added column for networks
</commit_message>
<xml_diff>
--- a/utilities/RTP/ModelRuns.xlsx
+++ b/utilities/RTP/ModelRuns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\RTP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\RTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DC71E3-B860-49DE-85F5-05F0B728A61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A6999A-B1CA-452D-860D-928043490CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13695" yWindow="315" windowWidth="24300" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="259">
   <si>
     <t>EEJ</t>
   </si>
@@ -757,6 +757,54 @@
   </si>
   <si>
     <t>2015_TM152_IPA_17_Sens_FaresX1.5</t>
+  </si>
+  <si>
+    <t>network</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_60\net_2015_Baseline</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_62\net_2025_Baseline_TransitCuts_v01</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_62\net_2030_Baseline_TransitCuts_v01</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_64\net_2030_Blueprint_TransitCuts_v01</t>
+  </si>
+  <si>
+    <t>net_2035_IP_02</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_61\net_2035_Baseline</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_64\net_2035_Blueprint</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_62\net_2040_Baseline</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_64\net_2040_Blueprint</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_62\net_2050_Baseline</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_64\net_2050_Blueprint</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_65\net_2035_Alt1</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_65\net_2050_Alt1</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_63\net_2035_Alt2</t>
+  </si>
+  <si>
+    <t>BlueprintNetworks_64\net_2050_Alt2</t>
   </si>
 </sst>
 </file>
@@ -878,53 +926,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -947,43 +991,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -995,9 +1028,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1364,49 +1394,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H178"/>
+  <dimension ref="A1:I178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I178" sqref="I178"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="36.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.296875" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="70.8984375" customWidth="1"/>
-    <col min="7" max="7" width="15" style="30" customWidth="1"/>
+    <col min="6" max="6" width="70.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15" style="28" customWidth="1"/>
+    <col min="9" max="9" width="49.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="54" t="s">
+      <c r="H1" s="47" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="45" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
@@ -1425,8 +1459,9 @@
       <c r="F2" s="5"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>25</v>
       </c>
@@ -1445,8 +1480,9 @@
       <c r="F3" s="8"/>
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>25</v>
       </c>
@@ -1465,8 +1501,9 @@
       <c r="F4" s="2"/>
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>25</v>
       </c>
@@ -1485,8 +1522,9 @@
       <c r="F5" s="12"/>
       <c r="G5" s="11"/>
       <c r="H5" s="12"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>25</v>
       </c>
@@ -1505,8 +1543,9 @@
       <c r="F6" s="12"/>
       <c r="G6" s="11"/>
       <c r="H6" s="12"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>25</v>
       </c>
@@ -1525,8 +1564,9 @@
       <c r="F7" s="12"/>
       <c r="G7" s="11"/>
       <c r="H7" s="12"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>25</v>
       </c>
@@ -1545,8 +1585,9 @@
       <c r="F8" s="12"/>
       <c r="G8" s="11"/>
       <c r="H8" s="12"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>25</v>
       </c>
@@ -1565,8 +1606,9 @@
       <c r="F9" s="12"/>
       <c r="G9" s="11"/>
       <c r="H9" s="12"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>25</v>
       </c>
@@ -1585,8 +1627,9 @@
       <c r="F10" s="18"/>
       <c r="G10" s="17"/>
       <c r="H10" s="18"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="18"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>25</v>
       </c>
@@ -1605,8 +1648,9 @@
       <c r="F11" s="18"/>
       <c r="G11" s="17"/>
       <c r="H11" s="18"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" s="18"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>25</v>
       </c>
@@ -1625,8 +1669,9 @@
       <c r="F12" s="18"/>
       <c r="G12" s="17"/>
       <c r="H12" s="18"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" s="18"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>25</v>
       </c>
@@ -1645,8 +1690,9 @@
       <c r="F13" s="18"/>
       <c r="G13" s="17"/>
       <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" s="18"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>25</v>
       </c>
@@ -1665,8 +1711,9 @@
       <c r="F14" s="18"/>
       <c r="G14" s="17"/>
       <c r="H14" s="18"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" s="18"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>25</v>
       </c>
@@ -1685,8 +1732,9 @@
       <c r="F15" s="15"/>
       <c r="G15" s="14"/>
       <c r="H15" s="15"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" s="15"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>25</v>
       </c>
@@ -1705,8 +1753,9 @@
       <c r="F16" s="15"/>
       <c r="G16" s="14"/>
       <c r="H16" s="15"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
@@ -1725,8 +1774,9 @@
       <c r="F17" s="15"/>
       <c r="G17" s="14"/>
       <c r="H17" s="15"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>25</v>
       </c>
@@ -1745,8 +1795,9 @@
       <c r="F18" s="15"/>
       <c r="G18" s="14"/>
       <c r="H18" s="15"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" s="15"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>25</v>
       </c>
@@ -1765,8 +1816,9 @@
       <c r="F19" s="21"/>
       <c r="G19" s="20"/>
       <c r="H19" s="21"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19" s="21"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
         <v>26</v>
       </c>
@@ -1787,8 +1839,9 @@
       <c r="H20" s="24" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20" s="24"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
         <v>26</v>
       </c>
@@ -1807,34 +1860,36 @@
       <c r="F21" s="24"/>
       <c r="G21" s="23"/>
       <c r="H21" s="24"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="62" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="69">
+      <c r="I21" s="24"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="59">
         <v>2015</v>
       </c>
-      <c r="C22" s="70" t="s">
+      <c r="C22" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="70" t="s">
+      <c r="D22" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="E22" s="70" t="s">
+      <c r="E22" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="70" t="s">
+      <c r="F22" s="60" t="s">
         <v>223</v>
       </c>
-      <c r="G22" s="69" t="s">
+      <c r="G22" s="59" t="s">
         <v>224</v>
       </c>
-      <c r="H22" s="70" t="s">
+      <c r="H22" s="60" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22" s="60"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>26</v>
       </c>
@@ -1859,8 +1914,11 @@
       <c r="H23" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I23" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>26</v>
       </c>
@@ -1885,8 +1943,9 @@
       <c r="H24" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>26</v>
       </c>
@@ -1909,56 +1968,59 @@
         <v>224</v>
       </c>
       <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="58" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="73">
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="63">
         <v>2015</v>
       </c>
-      <c r="C26" s="74" t="s">
+      <c r="C26" s="64" t="s">
         <v>242</v>
       </c>
-      <c r="D26" s="74" t="s">
+      <c r="D26" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="74" t="s">
+      <c r="E26" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="74" t="s">
+      <c r="F26" s="64" t="s">
         <v>223</v>
       </c>
-      <c r="G26" s="73" t="s">
+      <c r="G26" s="63" t="s">
         <v>224</v>
       </c>
-      <c r="H26" s="74"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="71">
+      <c r="H26" s="64"/>
+      <c r="I26" s="64"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="61">
         <v>2020</v>
       </c>
-      <c r="C27" s="72" t="s">
+      <c r="C27" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="D27" s="72" t="s">
+      <c r="D27" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="72" t="s">
+      <c r="E27" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="72" t="s">
+      <c r="F27" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="G27" s="71" t="s">
+      <c r="G27" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="H27" s="72"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H27" s="62"/>
+      <c r="I27" s="62"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
         <v>26</v>
       </c>
@@ -1981,34 +2043,36 @@
         <v>137</v>
       </c>
       <c r="H28" s="21"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="47">
+      <c r="I28" s="21"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="42">
         <v>2025</v>
       </c>
-      <c r="C29" s="48" t="s">
+      <c r="C29" s="43" t="s">
         <v>171</v>
       </c>
-      <c r="D29" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" s="48" t="s">
+      <c r="D29" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F29" s="48" t="s">
+      <c r="F29" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="G29" s="47" t="s">
+      <c r="G29" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="H29" s="48" t="s">
+      <c r="H29" s="43" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I29" s="43"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
         <v>26</v>
       </c>
@@ -2033,8 +2097,11 @@
       <c r="H30" s="21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30" s="21" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
         <v>26</v>
       </c>
@@ -2057,8 +2124,9 @@
         <v>137</v>
       </c>
       <c r="H31" s="18"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I31" s="18"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
         <v>26</v>
       </c>
@@ -2083,60 +2151,63 @@
       <c r="H32" s="18" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="32">
+      <c r="I32" s="18"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="30">
         <v>2025</v>
       </c>
-      <c r="C33" s="33" t="s">
+      <c r="C33" s="31" t="s">
         <v>209</v>
       </c>
-      <c r="D33" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="E33" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F33" s="33" t="s">
+      <c r="D33" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="G33" s="32" t="s">
+      <c r="G33" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="H33" s="33" t="s">
+      <c r="H33" s="31" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="47">
+      <c r="I33" s="31"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="42">
         <v>2030</v>
       </c>
-      <c r="C34" s="48" t="s">
+      <c r="C34" s="43" t="s">
         <v>172</v>
       </c>
-      <c r="D34" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="E34" s="48" t="s">
+      <c r="D34" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="E34" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="48" t="s">
+      <c r="F34" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="G34" s="47" t="s">
+      <c r="G34" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="H34" s="48" t="s">
+      <c r="H34" s="43" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I34" s="43"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
         <v>26</v>
       </c>
@@ -2161,8 +2232,11 @@
       <c r="H35" s="21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I35" s="21" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
         <v>26</v>
       </c>
@@ -2185,8 +2259,9 @@
         <v>137</v>
       </c>
       <c r="H36" s="18"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I36" s="18"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
         <v>26</v>
       </c>
@@ -2211,8 +2286,9 @@
       <c r="H37" s="18" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I37" s="18"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="16" t="s">
         <v>26</v>
       </c>
@@ -2235,54 +2311,59 @@
         <v>137</v>
       </c>
       <c r="H38" s="18"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="32">
+      <c r="I38" s="18"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="30">
         <v>2030</v>
       </c>
-      <c r="C39" s="33" t="s">
+      <c r="C39" s="31" t="s">
         <v>229</v>
       </c>
-      <c r="D39" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="E39" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F39" s="33" t="s">
+      <c r="D39" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E39" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F39" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="G39" s="32" t="s">
+      <c r="G39" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="H39" s="33" t="s">
+      <c r="H39" s="31" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="35">
-        <v>2035</v>
-      </c>
-      <c r="C40" s="36" t="s">
+      <c r="I39" s="31" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="33">
+        <v>2035</v>
+      </c>
+      <c r="C40" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D40" s="36" t="s">
+      <c r="D40" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="E40" s="36" t="s">
+      <c r="E40" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="36"/>
+      <c r="F40" s="34"/>
       <c r="G40" s="17"/>
       <c r="H40" s="17"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I40" s="17"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="s">
         <v>26</v>
       </c>
@@ -2301,8 +2382,9 @@
       <c r="F41" s="18"/>
       <c r="G41" s="17"/>
       <c r="H41" s="18"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I41" s="18"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="s">
         <v>26</v>
       </c>
@@ -2321,8 +2403,9 @@
       <c r="F42" s="18"/>
       <c r="G42" s="17"/>
       <c r="H42" s="18"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I42" s="18"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="s">
         <v>26</v>
       </c>
@@ -2347,8 +2430,9 @@
       <c r="H43" s="18" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I43" s="18"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="16" t="s">
         <v>26</v>
       </c>
@@ -2373,28 +2457,32 @@
       <c r="H44" s="18" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" s="35">
-        <v>2035</v>
-      </c>
-      <c r="C45" s="34" t="s">
+      <c r="I44" s="18" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="33">
+        <v>2035</v>
+      </c>
+      <c r="C45" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="D45" s="36" t="s">
+      <c r="D45" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="E45" s="36" t="s">
+      <c r="E45" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="F45" s="36"/>
-      <c r="G45" s="35"/>
-      <c r="H45" s="36"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F45" s="34"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="34"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="16" t="s">
         <v>26</v>
       </c>
@@ -2413,8 +2501,9 @@
       <c r="F46" s="18"/>
       <c r="G46" s="17"/>
       <c r="H46" s="18"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I46" s="18"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="16" t="s">
         <v>26</v>
       </c>
@@ -2433,8 +2522,9 @@
       <c r="F47" s="18"/>
       <c r="G47" s="17"/>
       <c r="H47" s="18"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I47" s="18"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
         <v>26</v>
       </c>
@@ -2453,8 +2543,9 @@
       <c r="F48" s="18"/>
       <c r="G48" s="17"/>
       <c r="H48" s="18"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I48" s="18"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="16" t="s">
         <v>26</v>
       </c>
@@ -2477,8 +2568,9 @@
         <v>74</v>
       </c>
       <c r="H49" s="18"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I49" s="18"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="16" t="s">
         <v>26</v>
       </c>
@@ -2501,56 +2593,59 @@
         <v>75</v>
       </c>
       <c r="H50" s="18"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B51" s="32">
-        <v>2035</v>
-      </c>
-      <c r="C51" s="31" t="s">
+      <c r="I50" s="18"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C51" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="D51" s="33" t="s">
+      <c r="D51" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E51" s="33" t="s">
+      <c r="E51" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F51" s="33" t="s">
+      <c r="F51" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="G51" s="32" t="s">
+      <c r="G51" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="H51" s="33"/>
-    </row>
-    <row r="52" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B52" s="47">
-        <v>2035</v>
-      </c>
-      <c r="C52" s="48" t="s">
+      <c r="H51" s="31"/>
+      <c r="I51" s="31"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="42">
+        <v>2035</v>
+      </c>
+      <c r="C52" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="D52" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="E52" s="48" t="s">
+      <c r="D52" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="E52" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F52" s="48" t="s">
+      <c r="F52" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="G52" s="47" t="s">
+      <c r="G52" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="H52" s="48"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H52" s="43"/>
+      <c r="I52" s="43"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="13" t="s">
         <v>26</v>
       </c>
@@ -2573,8 +2668,9 @@
         <v>82</v>
       </c>
       <c r="H53" s="15"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I53" s="15"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
         <v>26</v>
       </c>
@@ -2597,8 +2693,9 @@
         <v>122</v>
       </c>
       <c r="H54" s="15"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I54" s="15"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
         <v>26</v>
       </c>
@@ -2621,8 +2718,9 @@
         <v>137</v>
       </c>
       <c r="H55" s="15"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I55" s="15"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
         <v>26</v>
       </c>
@@ -2645,8 +2743,9 @@
         <v>137</v>
       </c>
       <c r="H56" s="15"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I56" s="15"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="13" t="s">
         <v>26</v>
       </c>
@@ -2669,8 +2768,9 @@
         <v>137</v>
       </c>
       <c r="H57" s="15"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I57" s="15"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="13" t="s">
         <v>26</v>
       </c>
@@ -2693,8 +2793,9 @@
         <v>137</v>
       </c>
       <c r="H58" s="15"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I58" s="15"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="13" t="s">
         <v>26</v>
       </c>
@@ -2717,8 +2818,9 @@
         <v>161</v>
       </c>
       <c r="H59" s="15"/>
-    </row>
-    <row r="60" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I59" s="15"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="13" t="s">
         <v>26</v>
       </c>
@@ -2743,8 +2845,9 @@
       <c r="H60" s="15" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I60" s="15"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="13" t="s">
         <v>26</v>
       </c>
@@ -2767,8 +2870,9 @@
         <v>169</v>
       </c>
       <c r="H61" s="15"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I61" s="15"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="19" t="s">
         <v>26</v>
       </c>
@@ -2793,48 +2897,53 @@
       <c r="H62" s="21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B63" s="35">
-        <v>2035</v>
-      </c>
-      <c r="C63" s="36" t="s">
+      <c r="I62" s="21" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" s="33">
+        <v>2035</v>
+      </c>
+      <c r="C63" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="D63" s="36" t="s">
+      <c r="D63" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="E63" s="36" t="s">
+      <c r="E63" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F63" s="36"/>
-      <c r="G63" s="35"/>
-      <c r="H63" s="36"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B64" s="32">
-        <v>2035</v>
-      </c>
-      <c r="C64" s="33" t="s">
+      <c r="F63" s="34"/>
+      <c r="G63" s="33"/>
+      <c r="H63" s="34"/>
+      <c r="I63" s="34"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B64" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C64" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="D64" s="33" t="s">
+      <c r="D64" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E64" s="33" t="s">
+      <c r="E64" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F64" s="33"/>
-      <c r="G64" s="32"/>
-      <c r="H64" s="33"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F64" s="31"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="31"/>
+      <c r="I64" s="31"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="16" t="s">
         <v>26</v>
       </c>
@@ -2853,8 +2962,9 @@
       <c r="F65" s="18"/>
       <c r="G65" s="17"/>
       <c r="H65" s="18"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I65" s="18"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="16" t="s">
         <v>26</v>
       </c>
@@ -2873,8 +2983,9 @@
       <c r="F66" s="18"/>
       <c r="G66" s="17"/>
       <c r="H66" s="18"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I66" s="18"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="16" t="s">
         <v>26</v>
       </c>
@@ -2897,8 +3008,9 @@
         <v>64</v>
       </c>
       <c r="H67" s="18"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I67" s="18"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="16" t="s">
         <v>26</v>
       </c>
@@ -2921,8 +3033,9 @@
         <v>65</v>
       </c>
       <c r="H68" s="18"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I68" s="18"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="16" t="s">
         <v>26</v>
       </c>
@@ -2945,8 +3058,9 @@
         <v>70</v>
       </c>
       <c r="H69" s="18"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I69" s="18"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="16" t="s">
         <v>26</v>
       </c>
@@ -2969,8 +3083,9 @@
         <v>74</v>
       </c>
       <c r="H70" s="18"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I70" s="18"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="16" t="s">
         <v>26</v>
       </c>
@@ -2993,8 +3108,9 @@
         <v>75</v>
       </c>
       <c r="H71" s="18"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I71" s="18"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="16" t="s">
         <v>26</v>
       </c>
@@ -3019,56 +3135,59 @@
       <c r="H72" s="18" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A73" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="B73" s="25">
-        <v>2035</v>
-      </c>
-      <c r="C73" s="26" t="s">
+      <c r="I72" s="18"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B73" s="17">
+        <v>2035</v>
+      </c>
+      <c r="C73" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="D73" s="26" t="s">
+      <c r="D73" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E73" s="26" t="s">
+      <c r="E73" s="18" t="s">
         <v>38</v>
       </c>
       <c r="F73" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="G73" s="25" t="s">
+      <c r="G73" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="H73" s="26"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A74" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="B74" s="25">
-        <v>2035</v>
-      </c>
-      <c r="C74" s="26" t="s">
+      <c r="H73" s="18"/>
+      <c r="I73" s="18"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74" s="17">
+        <v>2035</v>
+      </c>
+      <c r="C74" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="D74" s="26" t="s">
+      <c r="D74" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E74" s="26" t="s">
+      <c r="E74" s="18" t="s">
         <v>38</v>
       </c>
       <c r="F74" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="G74" s="25" t="s">
+      <c r="G74" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="H74" s="26"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H74" s="18"/>
+      <c r="I74" s="18"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="16" t="s">
         <v>26</v>
       </c>
@@ -3091,8 +3210,9 @@
         <v>82</v>
       </c>
       <c r="H75" s="18"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I75" s="18"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="16" t="s">
         <v>26</v>
       </c>
@@ -3115,8 +3235,9 @@
         <v>82</v>
       </c>
       <c r="H76" s="18"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I76" s="18"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="16" t="s">
         <v>26</v>
       </c>
@@ -3139,8 +3260,9 @@
         <v>82</v>
       </c>
       <c r="H77" s="18"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I77" s="18"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="16" t="s">
         <v>26</v>
       </c>
@@ -3163,32 +3285,34 @@
         <v>82</v>
       </c>
       <c r="H78" s="18"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A79" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B79" s="47">
-        <v>2035</v>
-      </c>
-      <c r="C79" s="48" t="s">
+      <c r="I78" s="18"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B79" s="42">
+        <v>2035</v>
+      </c>
+      <c r="C79" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="D79" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="E79" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="F79" s="48" t="s">
+      <c r="D79" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="E79" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="F79" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="G79" s="47" t="s">
+      <c r="G79" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="H79" s="48"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H79" s="43"/>
+      <c r="I79" s="43"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="13" t="s">
         <v>26</v>
       </c>
@@ -3211,8 +3335,9 @@
         <v>82</v>
       </c>
       <c r="H80" s="15"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I80" s="15"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="13" t="s">
         <v>26</v>
       </c>
@@ -3235,8 +3360,9 @@
         <v>82</v>
       </c>
       <c r="H81" s="15"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I81" s="15"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="s">
         <v>26</v>
       </c>
@@ -3259,8 +3385,9 @@
         <v>82</v>
       </c>
       <c r="H82" s="15"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I82" s="15"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="13" t="s">
         <v>26</v>
       </c>
@@ -3283,8 +3410,9 @@
         <v>82</v>
       </c>
       <c r="H83" s="15"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I83" s="15"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="s">
         <v>26</v>
       </c>
@@ -3307,8 +3435,9 @@
         <v>122</v>
       </c>
       <c r="H84" s="15"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I84" s="15"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
         <v>26</v>
       </c>
@@ -3331,8 +3460,9 @@
         <v>128</v>
       </c>
       <c r="H85" s="15"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I85" s="15"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
         <v>26</v>
       </c>
@@ -3355,8 +3485,9 @@
         <v>132</v>
       </c>
       <c r="H86" s="15"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I86" s="15"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="13" t="s">
         <v>26</v>
       </c>
@@ -3379,8 +3510,9 @@
         <v>132</v>
       </c>
       <c r="H87" s="15"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I87" s="15"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="13" t="s">
         <v>26</v>
       </c>
@@ -3403,8 +3535,9 @@
         <v>137</v>
       </c>
       <c r="H88" s="15"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I88" s="15"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="s">
         <v>26</v>
       </c>
@@ -3427,8 +3560,9 @@
         <v>137</v>
       </c>
       <c r="H89" s="15"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I89" s="15"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="13" t="s">
         <v>26</v>
       </c>
@@ -3451,8 +3585,9 @@
         <v>137</v>
       </c>
       <c r="H90" s="15"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I90" s="15"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="13" t="s">
         <v>26</v>
       </c>
@@ -3475,8 +3610,9 @@
         <v>137</v>
       </c>
       <c r="H91" s="15"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I91" s="15"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="13" t="s">
         <v>26</v>
       </c>
@@ -3499,8 +3635,9 @@
         <v>137</v>
       </c>
       <c r="H92" s="15"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I92" s="15"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="13" t="s">
         <v>26</v>
       </c>
@@ -3525,8 +3662,9 @@
       <c r="H93" s="15" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I93" s="15"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="13" t="s">
         <v>26</v>
       </c>
@@ -3549,8 +3687,9 @@
         <v>137</v>
       </c>
       <c r="H94" s="15"/>
-    </row>
-    <row r="95" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I94" s="15"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="13" t="s">
         <v>26</v>
       </c>
@@ -3573,8 +3712,9 @@
         <v>137</v>
       </c>
       <c r="H95" s="15"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I95" s="15"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="13" t="s">
         <v>26</v>
       </c>
@@ -3597,8 +3737,9 @@
         <v>137</v>
       </c>
       <c r="H96" s="15"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I96" s="15"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="19" t="s">
         <v>26</v>
       </c>
@@ -3623,34 +3764,38 @@
       <c r="H97" s="21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A98" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B98" s="47">
+      <c r="I97" s="21" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B98" s="42">
         <v>2040</v>
       </c>
-      <c r="C98" s="48" t="s">
+      <c r="C98" s="43" t="s">
         <v>183</v>
       </c>
-      <c r="D98" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="E98" s="48" t="s">
+      <c r="D98" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="E98" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F98" s="48" t="s">
+      <c r="F98" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="G98" s="47" t="s">
+      <c r="G98" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="H98" s="48" t="s">
+      <c r="H98" s="43" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I98" s="43"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="19" t="s">
         <v>26</v>
       </c>
@@ -3675,8 +3820,11 @@
       <c r="H99" s="21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I99" s="21" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="13" t="s">
         <v>26</v>
       </c>
@@ -3689,20 +3837,21 @@
       <c r="D100" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E100" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="F100" s="48" t="s">
+      <c r="E100" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="F100" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="G100" s="47" t="s">
+      <c r="G100" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="H100" s="48" t="s">
+      <c r="H100" s="43" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I100" s="43"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="13" t="s">
         <v>26</v>
       </c>
@@ -3725,8 +3874,9 @@
         <v>137</v>
       </c>
       <c r="H101" s="15"/>
-    </row>
-    <row r="102" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I101" s="15"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="13" t="s">
         <v>26</v>
       </c>
@@ -3749,8 +3899,9 @@
         <v>137</v>
       </c>
       <c r="H102" s="15"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I102" s="15"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="13" t="s">
         <v>26</v>
       </c>
@@ -3773,8 +3924,9 @@
         <v>137</v>
       </c>
       <c r="H103" s="15"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I103" s="15"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="19" t="s">
         <v>26</v>
       </c>
@@ -3799,168 +3951,178 @@
       <c r="H104" s="21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A105" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="B105" s="38">
-        <v>2050</v>
-      </c>
-      <c r="C105" s="39" t="s">
+      <c r="I104" s="21" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A105" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B105" s="36">
+        <v>2050</v>
+      </c>
+      <c r="C105" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="D105" s="39" t="s">
+      <c r="D105" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="E105" s="41" t="s">
+      <c r="E105" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="F105" s="41"/>
-      <c r="G105" s="40"/>
-      <c r="H105" s="41"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A106" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B106" s="40">
-        <v>2050</v>
-      </c>
-      <c r="C106" s="41" t="s">
+      <c r="F105" s="27"/>
+      <c r="G105" s="26"/>
+      <c r="H105" s="27"/>
+      <c r="I105" s="27"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A106" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B106" s="26">
+        <v>2050</v>
+      </c>
+      <c r="C106" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="D106" s="41" t="s">
+      <c r="D106" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E106" s="41" t="s">
+      <c r="E106" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="F106" s="41"/>
-      <c r="G106" s="40"/>
-      <c r="H106" s="41"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A107" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B107" s="40">
-        <v>2050</v>
-      </c>
-      <c r="C107" s="41" t="s">
+      <c r="F106" s="27"/>
+      <c r="G106" s="26"/>
+      <c r="H106" s="27"/>
+      <c r="I106" s="27"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A107" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B107" s="26">
+        <v>2050</v>
+      </c>
+      <c r="C107" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="D107" s="41" t="s">
+      <c r="D107" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E107" s="41" t="s">
+      <c r="E107" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="F107" s="41" t="s">
+      <c r="F107" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="G107" s="40" t="s">
+      <c r="G107" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="H107" s="41"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A108" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B108" s="40">
-        <v>2050</v>
-      </c>
-      <c r="C108" s="41" t="s">
+      <c r="H107" s="27"/>
+      <c r="I107" s="27"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A108" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B108" s="26">
+        <v>2050</v>
+      </c>
+      <c r="C108" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D108" s="41" t="s">
+      <c r="D108" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E108" s="41" t="s">
+      <c r="E108" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="F108" s="41" t="s">
+      <c r="F108" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="G108" s="40" t="s">
+      <c r="G108" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="H108" s="41"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A109" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B109" s="40">
-        <v>2050</v>
-      </c>
-      <c r="C109" s="41" t="s">
+      <c r="H108" s="27"/>
+      <c r="I108" s="27"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A109" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B109" s="26">
+        <v>2050</v>
+      </c>
+      <c r="C109" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="D109" s="41" t="s">
+      <c r="D109" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E109" s="41" t="s">
+      <c r="E109" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="F109" s="41" t="s">
+      <c r="F109" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="G109" s="40" t="s">
+      <c r="G109" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="H109" s="41"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A110" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B110" s="40">
-        <v>2050</v>
-      </c>
-      <c r="C110" s="41" t="s">
+      <c r="H109" s="27"/>
+      <c r="I109" s="27"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A110" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B110" s="26">
+        <v>2050</v>
+      </c>
+      <c r="C110" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="D110" s="41" t="s">
+      <c r="D110" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E110" s="41" t="s">
+      <c r="E110" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="F110" s="41" t="s">
+      <c r="F110" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="G110" s="40" t="s">
+      <c r="G110" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="H110" s="41"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A111" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="B111" s="43">
-        <v>2050</v>
-      </c>
-      <c r="C111" s="44" t="s">
+      <c r="H110" s="27"/>
+      <c r="I110" s="27"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B111" s="39">
+        <v>2050</v>
+      </c>
+      <c r="C111" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="D111" s="44" t="s">
+      <c r="D111" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="E111" s="44" t="s">
+      <c r="E111" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F111" s="44" t="s">
+      <c r="F111" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="G111" s="43" t="s">
+      <c r="G111" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="H111" s="44"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H111" s="40"/>
+      <c r="I111" s="40"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="13" t="s">
         <v>26</v>
       </c>
@@ -3970,7 +4132,7 @@
       <c r="C112" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="D112" s="48" t="s">
+      <c r="D112" s="43" t="s">
         <v>91</v>
       </c>
       <c r="E112" s="15" t="s">
@@ -3979,12 +4141,13 @@
       <c r="F112" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="G112" s="50" t="s">
+      <c r="G112" s="44" t="s">
         <v>75</v>
       </c>
       <c r="H112" s="15"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I112" s="15"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="13" t="s">
         <v>26</v>
       </c>
@@ -4003,12 +4166,13 @@
       <c r="F113" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="G113" s="50" t="s">
+      <c r="G113" s="44" t="s">
         <v>82</v>
       </c>
       <c r="H113" s="15"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I113" s="15"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="13" t="s">
         <v>26</v>
       </c>
@@ -4027,12 +4191,13 @@
       <c r="F114" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="G114" s="50" t="s">
+      <c r="G114" s="44" t="s">
         <v>122</v>
       </c>
       <c r="H114" s="15"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I114" s="15"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="13" t="s">
         <v>26</v>
       </c>
@@ -4051,12 +4216,13 @@
       <c r="F115" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="G115" s="50" t="s">
+      <c r="G115" s="44" t="s">
         <v>137</v>
       </c>
       <c r="H115" s="15"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I115" s="15"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" s="13" t="s">
         <v>26</v>
       </c>
@@ -4079,8 +4245,9 @@
         <v>137</v>
       </c>
       <c r="H116" s="15"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I116" s="15"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" s="13" t="s">
         <v>26</v>
       </c>
@@ -4103,8 +4270,9 @@
         <v>137</v>
       </c>
       <c r="H117" s="15"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I117" s="15"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" s="13" t="s">
         <v>26</v>
       </c>
@@ -4127,8 +4295,9 @@
         <v>137</v>
       </c>
       <c r="H118" s="15"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I118" s="15"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" s="13" t="s">
         <v>26</v>
       </c>
@@ -4151,8 +4320,9 @@
         <v>161</v>
       </c>
       <c r="H119" s="15"/>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I119" s="15"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="13" t="s">
         <v>26</v>
       </c>
@@ -4175,8 +4345,9 @@
         <v>169</v>
       </c>
       <c r="H120" s="15"/>
-    </row>
-    <row r="121" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I120" s="15"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" s="13" t="s">
         <v>26</v>
       </c>
@@ -4201,8 +4372,9 @@
       <c r="H121" s="15" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I121" s="15"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" s="13" t="s">
         <v>26</v>
       </c>
@@ -4225,8 +4397,9 @@
         <v>169</v>
       </c>
       <c r="H122" s="15"/>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I122" s="15"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="19" t="s">
         <v>26</v>
       </c>
@@ -4251,535 +4424,560 @@
       <c r="H123" s="21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A124" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B124" s="40">
-        <v>2050</v>
-      </c>
-      <c r="C124" s="41" t="s">
+      <c r="I123" s="21" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A124" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B124" s="26">
+        <v>2050</v>
+      </c>
+      <c r="C124" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D124" s="41" t="s">
+      <c r="D124" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E124" s="41" t="s">
+      <c r="E124" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="F124" s="41"/>
-      <c r="G124" s="40"/>
-      <c r="H124" s="41"/>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A125" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="B125" s="43">
-        <v>2050</v>
-      </c>
-      <c r="C125" s="44" t="s">
+      <c r="F124" s="27"/>
+      <c r="G124" s="26"/>
+      <c r="H124" s="27"/>
+      <c r="I124" s="27"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A125" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B125" s="39">
+        <v>2050</v>
+      </c>
+      <c r="C125" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="D125" s="44" t="s">
+      <c r="D125" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="E125" s="44" t="s">
+      <c r="E125" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F125" s="44"/>
-      <c r="G125" s="43"/>
-      <c r="H125" s="44"/>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A126" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B126" s="28">
-        <v>2050</v>
-      </c>
-      <c r="C126" s="29" t="s">
+      <c r="F125" s="40"/>
+      <c r="G125" s="39"/>
+      <c r="H125" s="40"/>
+      <c r="I125" s="40"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A126" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B126" s="26">
+        <v>2050</v>
+      </c>
+      <c r="C126" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D126" s="29" t="s">
+      <c r="D126" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E126" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F126" s="29"/>
-      <c r="G126" s="28"/>
-      <c r="H126" s="29"/>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A127" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B127" s="28">
-        <v>2050</v>
-      </c>
-      <c r="C127" s="29" t="s">
+      <c r="E126" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F126" s="27"/>
+      <c r="G126" s="26"/>
+      <c r="H126" s="27"/>
+      <c r="I126" s="27"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A127" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B127" s="26">
+        <v>2050</v>
+      </c>
+      <c r="C127" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D127" s="29" t="s">
+      <c r="D127" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E127" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F127" s="29"/>
-      <c r="G127" s="28"/>
-      <c r="H127" s="29"/>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A128" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B128" s="28">
-        <v>2050</v>
-      </c>
-      <c r="C128" s="29" t="s">
+      <c r="E127" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F127" s="27"/>
+      <c r="G127" s="26"/>
+      <c r="H127" s="27"/>
+      <c r="I127" s="27"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A128" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B128" s="26">
+        <v>2050</v>
+      </c>
+      <c r="C128" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="D128" s="29" t="s">
+      <c r="D128" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E128" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F128" s="29" t="s">
+      <c r="E128" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F128" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="G128" s="28" t="s">
+      <c r="G128" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="H128" s="29"/>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A129" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B129" s="28">
-        <v>2050</v>
-      </c>
-      <c r="C129" s="29" t="s">
+      <c r="H128" s="27"/>
+      <c r="I128" s="27"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A129" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B129" s="26">
+        <v>2050</v>
+      </c>
+      <c r="C129" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D129" s="29" t="s">
+      <c r="D129" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E129" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F129" s="29" t="s">
+      <c r="E129" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F129" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="G129" s="28" t="s">
+      <c r="G129" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="H129" s="29"/>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A130" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B130" s="28">
-        <v>2050</v>
-      </c>
-      <c r="C130" s="29" t="s">
+      <c r="H129" s="27"/>
+      <c r="I129" s="27"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A130" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B130" s="26">
+        <v>2050</v>
+      </c>
+      <c r="C130" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="D130" s="29" t="s">
+      <c r="D130" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E130" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F130" s="29" t="s">
+      <c r="E130" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F130" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="G130" s="28" t="s">
+      <c r="G130" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="H130" s="29"/>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A131" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B131" s="28">
-        <v>2050</v>
-      </c>
-      <c r="C131" s="29" t="s">
+      <c r="H130" s="27"/>
+      <c r="I130" s="27"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A131" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B131" s="26">
+        <v>2050</v>
+      </c>
+      <c r="C131" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D131" s="29" t="s">
+      <c r="D131" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E131" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F131" s="29" t="s">
+      <c r="E131" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F131" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="G131" s="28" t="s">
+      <c r="G131" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="H131" s="29"/>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A132" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B132" s="28">
-        <v>2050</v>
-      </c>
-      <c r="C132" s="29" t="s">
+      <c r="H131" s="27"/>
+      <c r="I131" s="27"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A132" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B132" s="26">
+        <v>2050</v>
+      </c>
+      <c r="C132" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="D132" s="29" t="s">
+      <c r="D132" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E132" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F132" s="29" t="s">
+      <c r="E132" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F132" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="G132" s="28" t="s">
+      <c r="G132" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="H132" s="29"/>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A133" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B133" s="28">
-        <v>2050</v>
-      </c>
-      <c r="C133" s="29" t="s">
+      <c r="H132" s="27"/>
+      <c r="I132" s="27"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A133" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B133" s="26">
+        <v>2050</v>
+      </c>
+      <c r="C133" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="D133" s="29" t="s">
+      <c r="D133" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E133" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F133" s="29" t="s">
+      <c r="E133" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F133" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="G133" s="28" t="s">
+      <c r="G133" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="H133" s="29"/>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A134" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B134" s="28">
-        <v>2050</v>
-      </c>
-      <c r="C134" s="29" t="s">
+      <c r="H133" s="27"/>
+      <c r="I133" s="27"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A134" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B134" s="26">
+        <v>2050</v>
+      </c>
+      <c r="C134" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="D134" s="29" t="s">
+      <c r="D134" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E134" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F134" s="29" t="s">
+      <c r="E134" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F134" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="G134" s="28" t="s">
+      <c r="G134" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="H134" s="29" t="s">
+      <c r="H134" s="27" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A135" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B135" s="47">
-        <v>2050</v>
-      </c>
-      <c r="C135" s="48" t="s">
+      <c r="I134" s="27"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A135" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B135" s="42">
+        <v>2050</v>
+      </c>
+      <c r="C135" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="D135" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="E135" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="F135" s="48" t="s">
+      <c r="D135" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="E135" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="F135" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="G135" s="47" t="s">
+      <c r="G135" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="H135" s="48"/>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A136" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B136" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C136" s="49" t="s">
+      <c r="H135" s="43"/>
+      <c r="I135" s="43"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A136" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B136" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C136" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D136" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E136" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F136" s="49" t="s">
+      <c r="D136" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E136" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F136" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="G136" s="50" t="s">
+      <c r="G136" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="H136" s="49"/>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A137" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B137" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C137" s="49" t="s">
+      <c r="H136" s="13"/>
+      <c r="I136" s="13"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A137" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B137" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C137" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D137" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E137" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F137" s="49" t="s">
+      <c r="D137" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E137" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F137" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="G137" s="50" t="s">
+      <c r="G137" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="H137" s="49"/>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A138" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B138" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C138" s="49" t="s">
+      <c r="H137" s="13"/>
+      <c r="I137" s="13"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A138" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B138" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C138" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D138" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E138" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F138" s="49" t="s">
+      <c r="D138" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E138" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F138" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="G138" s="50" t="s">
+      <c r="G138" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="H138" s="49"/>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A139" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B139" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C139" s="49" t="s">
+      <c r="H138" s="13"/>
+      <c r="I138" s="13"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A139" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B139" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C139" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D139" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E139" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F139" s="49" t="s">
+      <c r="D139" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E139" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F139" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="G139" s="50" t="s">
+      <c r="G139" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="H139" s="49"/>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A140" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B140" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C140" s="49" t="s">
+      <c r="H139" s="13"/>
+      <c r="I139" s="13"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A140" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B140" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C140" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D140" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E140" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F140" s="49" t="s">
+      <c r="D140" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E140" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F140" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="G140" s="50" t="s">
+      <c r="G140" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="H140" s="49"/>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A141" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B141" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C141" s="49" t="s">
+      <c r="H140" s="13"/>
+      <c r="I140" s="13"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A141" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B141" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C141" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D141" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E141" s="49" t="s">
+      <c r="D141" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E141" s="13" t="s">
         <v>38</v>
       </c>
       <c r="F141" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="G141" s="50" t="s">
+      <c r="G141" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="H141" s="49"/>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A142" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B142" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C142" s="49" t="s">
+      <c r="H141" s="13"/>
+      <c r="I141" s="13"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A142" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B142" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C142" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D142" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E142" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F142" s="49" t="s">
+      <c r="D142" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E142" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F142" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="G142" s="50" t="s">
+      <c r="G142" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="H142" s="49"/>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A143" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B143" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C143" s="49" t="s">
+      <c r="H142" s="13"/>
+      <c r="I142" s="13"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A143" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B143" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C143" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D143" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E143" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F143" s="49" t="s">
+      <c r="D143" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E143" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F143" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="G143" s="50" t="s">
+      <c r="G143" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="H143" s="49"/>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A144" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B144" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C144" s="49" t="s">
+      <c r="H143" s="13"/>
+      <c r="I143" s="13"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A144" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B144" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C144" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D144" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E144" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F144" s="49" t="s">
+      <c r="D144" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E144" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F144" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="G144" s="50" t="s">
+      <c r="G144" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="H144" s="49"/>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A145" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B145" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C145" s="49" t="s">
+      <c r="H144" s="13"/>
+      <c r="I144" s="13"/>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A145" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B145" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C145" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D145" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E145" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F145" s="49" t="s">
+      <c r="D145" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E145" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F145" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="G145" s="50" t="s">
+      <c r="G145" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="H145" s="49"/>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A146" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B146" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C146" s="49" t="s">
+      <c r="H145" s="13"/>
+      <c r="I145" s="13"/>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A146" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B146" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C146" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="D146" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E146" s="49" t="s">
+      <c r="D146" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E146" s="13" t="s">
         <v>38</v>
       </c>
       <c r="F146" s="15" t="s">
@@ -4789,21 +4987,22 @@
         <v>128</v>
       </c>
       <c r="H146" s="15"/>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A147" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B147" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C147" s="49" t="s">
+      <c r="I146" s="15"/>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A147" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B147" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C147" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D147" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E147" s="49" t="s">
+      <c r="D147" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E147" s="13" t="s">
         <v>38</v>
       </c>
       <c r="F147" s="15" t="s">
@@ -4813,21 +5012,22 @@
         <v>132</v>
       </c>
       <c r="H147" s="15"/>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A148" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B148" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C148" s="49" t="s">
+      <c r="I147" s="15"/>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A148" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B148" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C148" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="D148" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E148" s="49" t="s">
+      <c r="D148" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E148" s="13" t="s">
         <v>38</v>
       </c>
       <c r="F148" s="15" t="s">
@@ -4837,21 +5037,22 @@
         <v>137</v>
       </c>
       <c r="H148" s="15"/>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A149" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B149" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C149" s="49" t="s">
+      <c r="I148" s="15"/>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A149" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B149" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C149" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="D149" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E149" s="49" t="s">
+      <c r="D149" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E149" s="13" t="s">
         <v>38</v>
       </c>
       <c r="F149" s="15" t="s">
@@ -4861,21 +5062,22 @@
         <v>137</v>
       </c>
       <c r="H149" s="15"/>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A150" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B150" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C150" s="49" t="s">
+      <c r="I149" s="15"/>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A150" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B150" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C150" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="D150" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E150" s="49" t="s">
+      <c r="D150" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E150" s="13" t="s">
         <v>38</v>
       </c>
       <c r="F150" s="15" t="s">
@@ -4885,21 +5087,22 @@
         <v>137</v>
       </c>
       <c r="H150" s="15"/>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A151" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B151" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C151" s="49" t="s">
+      <c r="I150" s="15"/>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A151" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B151" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C151" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="D151" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E151" s="49" t="s">
+      <c r="D151" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E151" s="13" t="s">
         <v>38</v>
       </c>
       <c r="F151" s="15" t="s">
@@ -4909,21 +5112,22 @@
         <v>137</v>
       </c>
       <c r="H151" s="15"/>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A152" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B152" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C152" s="49" t="s">
+      <c r="I151" s="15"/>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A152" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B152" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C152" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="D152" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E152" s="49" t="s">
+      <c r="D152" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E152" s="13" t="s">
         <v>38</v>
       </c>
       <c r="F152" s="15" t="s">
@@ -4933,21 +5137,22 @@
         <v>137</v>
       </c>
       <c r="H152" s="15"/>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A153" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B153" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C153" s="49" t="s">
+      <c r="I152" s="15"/>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A153" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B153" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C153" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="D153" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E153" s="49" t="s">
+      <c r="D153" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E153" s="13" t="s">
         <v>38</v>
       </c>
       <c r="F153" s="15" t="s">
@@ -4957,21 +5162,22 @@
         <v>137</v>
       </c>
       <c r="H153" s="15"/>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A154" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B154" s="50">
-        <v>2050</v>
-      </c>
-      <c r="C154" s="49" t="s">
+      <c r="I153" s="15"/>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A154" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B154" s="44">
+        <v>2050</v>
+      </c>
+      <c r="C154" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="D154" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E154" s="49" t="s">
+      <c r="D154" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E154" s="13" t="s">
         <v>38</v>
       </c>
       <c r="F154" s="15" t="s">
@@ -4981,12 +5187,13 @@
         <v>137</v>
       </c>
       <c r="H154" s="15"/>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I154" s="15"/>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B155" s="60">
+      <c r="B155" s="44">
         <v>2050</v>
       </c>
       <c r="C155" s="13" t="s">
@@ -5007,12 +5214,13 @@
       <c r="H155" s="15" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I155" s="15"/>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B156" s="60">
+      <c r="B156" s="44">
         <v>2050</v>
       </c>
       <c r="C156" s="13" t="s">
@@ -5031,12 +5239,13 @@
         <v>137</v>
       </c>
       <c r="H156" s="15"/>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I156" s="15"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B157" s="60">
+      <c r="B157" s="44">
         <v>2050</v>
       </c>
       <c r="C157" s="13" t="s">
@@ -5055,12 +5264,13 @@
         <v>137</v>
       </c>
       <c r="H157" s="15"/>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I157" s="15"/>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B158" s="61">
+      <c r="B158" s="52">
         <v>2050</v>
       </c>
       <c r="C158" s="19" t="s">
@@ -5081,12 +5291,15 @@
       <c r="H158" s="21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I158" s="21" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B159" s="57">
+      <c r="B159" s="49">
         <v>2035</v>
       </c>
       <c r="C159" s="9" t="s">
@@ -5101,16 +5314,17 @@
       <c r="F159" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="G159" s="57" t="s">
+      <c r="G159" s="49" t="s">
         <v>185</v>
       </c>
       <c r="H159" s="9"/>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I159" s="9"/>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B160" s="57">
+      <c r="B160" s="49">
         <v>2035</v>
       </c>
       <c r="C160" s="9" t="s">
@@ -5125,16 +5339,17 @@
       <c r="F160" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="G160" s="57" t="s">
+      <c r="G160" s="49" t="s">
         <v>190</v>
       </c>
       <c r="H160" s="9"/>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I160" s="9"/>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B161" s="57">
+      <c r="B161" s="49">
         <v>2035</v>
       </c>
       <c r="C161" s="9" t="s">
@@ -5149,18 +5364,19 @@
       <c r="F161" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="G161" s="57" t="s">
+      <c r="G161" s="49" t="s">
         <v>197</v>
       </c>
       <c r="H161" s="9" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I161" s="9"/>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B162" s="57">
+      <c r="B162" s="49">
         <v>2035</v>
       </c>
       <c r="C162" s="9" t="s">
@@ -5175,16 +5391,17 @@
       <c r="F162" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="G162" s="57" t="s">
+      <c r="G162" s="49" t="s">
         <v>197</v>
       </c>
       <c r="H162" s="9"/>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I162" s="9"/>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B163" s="57">
+      <c r="B163" s="49">
         <v>2035</v>
       </c>
       <c r="C163" s="9" t="s">
@@ -5199,66 +5416,71 @@
       <c r="F163" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="G163" s="57" t="s">
+      <c r="G163" s="49" t="s">
         <v>197</v>
       </c>
       <c r="H163" s="9"/>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A164" s="58" t="s">
-        <v>26</v>
-      </c>
-      <c r="B164" s="59">
-        <v>2035</v>
-      </c>
-      <c r="C164" s="58" t="s">
+      <c r="I163" s="9"/>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A164" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B164" s="51">
+        <v>2035</v>
+      </c>
+      <c r="C164" s="50" t="s">
         <v>239</v>
       </c>
-      <c r="D164" s="58" t="s">
+      <c r="D164" s="50" t="s">
         <v>181</v>
       </c>
-      <c r="E164" s="58" t="s">
+      <c r="E164" s="50" t="s">
         <v>182</v>
       </c>
-      <c r="F164" s="58" t="s">
+      <c r="F164" s="50" t="s">
         <v>200</v>
       </c>
-      <c r="G164" s="59" t="s">
+      <c r="G164" s="51" t="s">
         <v>197</v>
       </c>
-      <c r="H164" s="58" t="s">
+      <c r="H164" s="50" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A165" s="62" t="s">
-        <v>26</v>
-      </c>
-      <c r="B165" s="63">
-        <v>2050</v>
-      </c>
-      <c r="C165" s="62" t="s">
+      <c r="I164" s="50" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A165" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B165" s="54">
+        <v>2050</v>
+      </c>
+      <c r="C165" s="53" t="s">
         <v>180</v>
       </c>
-      <c r="D165" s="62" t="s">
+      <c r="D165" s="53" t="s">
         <v>181</v>
       </c>
-      <c r="E165" s="62" t="s">
+      <c r="E165" s="53" t="s">
         <v>182</v>
       </c>
-      <c r="F165" s="62" t="s">
+      <c r="F165" s="53" t="s">
         <v>184</v>
       </c>
-      <c r="G165" s="63" t="s">
+      <c r="G165" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="H165" s="62"/>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H165" s="53"/>
+      <c r="I165" s="53"/>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B166" s="57">
+      <c r="B166" s="49">
         <v>2050</v>
       </c>
       <c r="C166" s="9" t="s">
@@ -5273,16 +5495,17 @@
       <c r="F166" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="G166" s="57" t="s">
+      <c r="G166" s="49" t="s">
         <v>190</v>
       </c>
       <c r="H166" s="9"/>
-    </row>
-    <row r="167" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I166" s="9"/>
+    </row>
+    <row r="167" spans="1:9" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B167" s="57">
+      <c r="B167" s="49">
         <v>2050</v>
       </c>
       <c r="C167" s="9" t="s">
@@ -5297,18 +5520,19 @@
       <c r="F167" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="G167" s="57" t="s">
+      <c r="G167" s="49" t="s">
         <v>197</v>
       </c>
       <c r="H167" s="9" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="168" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I167" s="9"/>
+    </row>
+    <row r="168" spans="1:9" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B168" s="57">
+      <c r="B168" s="49">
         <v>2050</v>
       </c>
       <c r="C168" s="9" t="s">
@@ -5323,16 +5547,17 @@
       <c r="F168" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="G168" s="57" t="s">
+      <c r="G168" s="49" t="s">
         <v>197</v>
       </c>
       <c r="H168" s="9"/>
-    </row>
-    <row r="169" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I168" s="9"/>
+    </row>
+    <row r="169" spans="1:9" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B169" s="57">
+      <c r="B169" s="49">
         <v>2050</v>
       </c>
       <c r="C169" s="9" t="s">
@@ -5347,66 +5572,71 @@
       <c r="F169" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="G169" s="57" t="s">
+      <c r="G169" s="49" t="s">
         <v>197</v>
       </c>
       <c r="H169" s="9"/>
-    </row>
-    <row r="170" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="58" t="s">
-        <v>26</v>
-      </c>
-      <c r="B170" s="59">
-        <v>2050</v>
-      </c>
-      <c r="C170" s="58" t="s">
+      <c r="I169" s="9"/>
+    </row>
+    <row r="170" spans="1:9" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B170" s="51">
+        <v>2050</v>
+      </c>
+      <c r="C170" s="50" t="s">
         <v>240</v>
       </c>
-      <c r="D170" s="58" t="s">
+      <c r="D170" s="50" t="s">
         <v>181</v>
       </c>
-      <c r="E170" s="58" t="s">
+      <c r="E170" s="50" t="s">
         <v>182</v>
       </c>
-      <c r="F170" s="58" t="s">
+      <c r="F170" s="50" t="s">
         <v>200</v>
       </c>
-      <c r="G170" s="59" t="s">
+      <c r="G170" s="51" t="s">
         <v>197</v>
       </c>
-      <c r="H170" s="58" t="s">
+      <c r="H170" s="50" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="171" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="B171" s="65">
-        <v>2035</v>
-      </c>
-      <c r="C171" s="64" t="s">
+      <c r="I170" s="50" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B171" s="56">
+        <v>2035</v>
+      </c>
+      <c r="C171" s="55" t="s">
         <v>192</v>
       </c>
-      <c r="D171" s="64" t="s">
+      <c r="D171" s="55" t="s">
         <v>181</v>
       </c>
-      <c r="E171" s="64" t="s">
+      <c r="E171" s="55" t="s">
         <v>193</v>
       </c>
-      <c r="F171" s="64" t="s">
+      <c r="F171" s="55" t="s">
         <v>194</v>
       </c>
-      <c r="G171" s="65" t="s">
+      <c r="G171" s="56" t="s">
         <v>195</v>
       </c>
-      <c r="H171" s="64"/>
-    </row>
-    <row r="172" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H171" s="55"/>
+      <c r="I171" s="55"/>
+    </row>
+    <row r="172" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B172" s="66">
+      <c r="B172" s="48">
         <v>2035</v>
       </c>
       <c r="C172" s="6" t="s">
@@ -5421,161 +5651,172 @@
       <c r="F172" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="G172" s="66" t="s">
+      <c r="G172" s="48" t="s">
         <v>195</v>
       </c>
       <c r="H172" s="6" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="173" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B173" s="56">
-        <v>2035</v>
-      </c>
-      <c r="C173" s="55" t="s">
+      <c r="I172" s="6"/>
+    </row>
+    <row r="173" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B173" s="48">
+        <v>2035</v>
+      </c>
+      <c r="C173" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="D173" s="55" t="s">
+      <c r="D173" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="E173" s="55" t="s">
+      <c r="E173" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="F173" s="55" t="s">
+      <c r="F173" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="G173" s="56" t="s">
+      <c r="G173" s="48" t="s">
         <v>195</v>
       </c>
-      <c r="H173" s="55"/>
-    </row>
-    <row r="174" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="B174" s="68">
-        <v>2035</v>
-      </c>
-      <c r="C174" s="67" t="s">
+      <c r="H173" s="6"/>
+      <c r="I173" s="6"/>
+    </row>
+    <row r="174" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A174" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="B174" s="58">
+        <v>2035</v>
+      </c>
+      <c r="C174" s="57" t="s">
         <v>225</v>
       </c>
-      <c r="D174" s="67" t="s">
+      <c r="D174" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="E174" s="67" t="s">
+      <c r="E174" s="57" t="s">
         <v>193</v>
       </c>
-      <c r="F174" s="67" t="s">
+      <c r="F174" s="57" t="s">
         <v>194</v>
       </c>
-      <c r="G174" s="68" t="s">
+      <c r="G174" s="58" t="s">
         <v>195</v>
       </c>
-      <c r="H174" s="67" t="s">
+      <c r="H174" s="57" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="175" spans="1:8" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B175" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C175" s="55" t="s">
+      <c r="I174" s="57" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B175" s="48">
+        <v>2050</v>
+      </c>
+      <c r="C175" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="D175" s="55" t="s">
+      <c r="D175" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="E175" s="55" t="s">
+      <c r="E175" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="F175" s="55" t="s">
+      <c r="F175" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="G175" s="56" t="s">
+      <c r="G175" s="48" t="s">
         <v>195</v>
       </c>
-      <c r="H175" s="55"/>
-    </row>
-    <row r="176" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B176" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C176" s="55" t="s">
+      <c r="H175" s="6"/>
+      <c r="I175" s="6"/>
+    </row>
+    <row r="176" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B176" s="48">
+        <v>2050</v>
+      </c>
+      <c r="C176" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="D176" s="55" t="s">
+      <c r="D176" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="E176" s="55" t="s">
+      <c r="E176" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="F176" s="55" t="s">
+      <c r="F176" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="G176" s="56" t="s">
+      <c r="G176" s="48" t="s">
         <v>195</v>
       </c>
-      <c r="H176" s="55" t="s">
+      <c r="H176" s="6" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="177" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B177" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C177" s="55" t="s">
+      <c r="I176" s="6"/>
+    </row>
+    <row r="177" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B177" s="48">
+        <v>2050</v>
+      </c>
+      <c r="C177" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="D177" s="55" t="s">
+      <c r="D177" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="E177" s="55" t="s">
+      <c r="E177" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="F177" s="55" t="s">
+      <c r="F177" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="G177" s="56" t="s">
+      <c r="G177" s="48" t="s">
         <v>195</v>
       </c>
-      <c r="H177" s="55"/>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A178" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B178" s="56">
-        <v>2050</v>
-      </c>
-      <c r="C178" s="55" t="s">
+      <c r="H177" s="6"/>
+      <c r="I177" s="6"/>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A178" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B178" s="48">
+        <v>2050</v>
+      </c>
+      <c r="C178" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="D178" s="55" t="s">
+      <c r="D178" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="E178" s="55" t="s">
+      <c r="E178" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="F178" s="55" t="s">
+      <c r="F178" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="G178" s="56" t="s">
+      <c r="G178" s="48" t="s">
         <v>195</v>
       </c>
-      <c r="H178" s="55" t="s">
+      <c r="H178" s="6" t="s">
         <v>43</v>
+      </c>
+      <c r="I178" s="6" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>